<commit_message>
ALK Tiles ELOW PI
</commit_message>
<xml_diff>
--- a/Data/Spring_2023/BenthFun_Alkalinity.xlsx
+++ b/Data/Spring_2023/BenthFun_Alkalinity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremy/Library/Mobile Documents/com~apple~CloudDocs/Documents/Documents/Post-Doc/Projets/Villefranche/Projets/BenthFun – Jeremy/BenthFun/Data/Spring_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8577945-3332-2D45-A8D2-2BD25784DD1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325F38BA-CEA0-9C49-B3B2-2A3D7E336709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="231">
   <si>
     <t>Operator</t>
   </si>
@@ -701,9 +701,6 @@
     <t>PI_t1_ELOW_Tile_1b</t>
   </si>
   <si>
-    <t>PI_t1_ELOW_Tile_1c</t>
-  </si>
-  <si>
     <t>PI_t1_ELOW_Tile_2a</t>
   </si>
   <si>
@@ -729,15 +726,6 @@
   </si>
   <si>
     <t>PI_t1_ELOW_blank_c</t>
-  </si>
-  <si>
-    <t>PI_t6_AMB_T0d</t>
-  </si>
-  <si>
-    <t>PI_t7_AMB_T0d</t>
-  </si>
-  <si>
-    <t>PI_t7_AMB_T0e</t>
   </si>
 </sst>
 </file>
@@ -1212,11 +1200,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L271"/>
+  <dimension ref="A1:L267"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="73" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A236" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D256" sqref="D256"/>
+      <pane ySplit="1" topLeftCell="A231" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G259" sqref="G259:K259"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7233,7 +7221,7 @@
         <v>2574.5550000000003</v>
       </c>
     </row>
-    <row r="241" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A241" s="9" t="s">
         <v>11</v>
       </c>
@@ -7253,7 +7241,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="242" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A242" s="9" t="s">
         <v>11</v>
       </c>
@@ -7285,7 +7273,7 @@
         <v>2572.5350000000003</v>
       </c>
     </row>
-    <row r="243" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A243" s="9" t="s">
         <v>11</v>
       </c>
@@ -7305,7 +7293,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="244" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A244" s="9" t="s">
         <v>11</v>
       </c>
@@ -7325,7 +7313,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="245" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A245" s="9" t="s">
         <v>11</v>
       </c>
@@ -7345,7 +7333,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="246" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A246" s="9" t="s">
         <v>11</v>
       </c>
@@ -7377,7 +7365,7 @@
         <v>2567.5250000000001</v>
       </c>
     </row>
-    <row r="247" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A247" s="9" t="s">
         <v>11</v>
       </c>
@@ -7397,7 +7385,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="248" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A248" s="9" t="s">
         <v>11</v>
       </c>
@@ -7411,7 +7399,7 @@
         <v>51.69</v>
       </c>
       <c r="E248" s="5">
-        <v>2595.9299999999998</v>
+        <v>2593.9299999999998</v>
       </c>
       <c r="F248" s="32" t="s">
         <v>213</v>
@@ -7422,14 +7410,14 @@
       </c>
       <c r="H248" s="18">
         <f>STDEV(E248:E249)</f>
-        <v>6.2791082169362973</v>
+        <v>3.4506810921901074</v>
       </c>
       <c r="K248" s="5">
         <f>G248+$J$218</f>
         <v>2580.6</v>
       </c>
     </row>
-    <row r="249" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A249" s="9" t="s">
         <v>11</v>
       </c>
@@ -7443,13 +7431,13 @@
         <v>51.1</v>
       </c>
       <c r="E249" s="5">
-        <v>2587.0500000000002</v>
+        <v>2589.0500000000002</v>
       </c>
       <c r="F249" s="32" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="250" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A250" s="9" t="s">
         <v>11</v>
       </c>
@@ -7460,16 +7448,28 @@
         <v>12</v>
       </c>
       <c r="D250" s="5">
-        <v>49.83</v>
-      </c>
-      <c r="E250" s="5">
-        <v>2613.7199999999998</v>
-      </c>
-      <c r="F250" s="32" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="251" spans="1:11" x14ac:dyDescent="0.2">
+        <v>50.57</v>
+      </c>
+      <c r="E250" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F250" s="17" t="s">
+        <v>216</v>
+      </c>
+      <c r="G250" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="H250" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="K250" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="L250" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="251" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A251" s="9" t="s">
         <v>11</v>
       </c>
@@ -7480,13 +7480,16 @@
         <v>12</v>
       </c>
       <c r="D251" s="5">
-        <v>50.92</v>
-      </c>
-      <c r="F251" s="32" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="252" spans="1:11" x14ac:dyDescent="0.2">
+        <v>50.9</v>
+      </c>
+      <c r="E251" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F251" s="17" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="252" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A252" s="9" t="s">
         <v>11</v>
       </c>
@@ -7497,100 +7500,94 @@
         <v>12</v>
       </c>
       <c r="D252" s="5">
-        <v>50.57</v>
-      </c>
-      <c r="E252" s="5">
-        <v>2319.62</v>
+        <v>50.92</v>
+      </c>
+      <c r="E252" s="5" t="s">
+        <v>155</v>
       </c>
       <c r="F252" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="G252" s="13">
-        <f>AVERAGE(E252:E252)</f>
-        <v>2319.62</v>
-      </c>
-      <c r="H252" s="18" t="e">
-        <f>STDEV(E252:E252)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K252" s="5">
-        <f>G252+$J$218</f>
-        <v>2308.73</v>
-      </c>
-    </row>
-    <row r="253" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A253" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B253" s="31">
-        <v>45079</v>
-      </c>
-      <c r="C253" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D253" s="5">
-        <v>50.9</v>
-      </c>
-      <c r="E253" s="5">
-        <v>2457.2399999999998</v>
-      </c>
-      <c r="F253" s="17" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="254" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E253" s="14"/>
+      <c r="F253" s="1"/>
+    </row>
+    <row r="254" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A254" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B254" s="31">
-        <v>45079</v>
-      </c>
-      <c r="C254" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D254" s="5">
-        <v>50.92</v>
-      </c>
-      <c r="F254" s="17" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="255" spans="1:11" x14ac:dyDescent="0.2">
+        <v>45080</v>
+      </c>
+      <c r="C254" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F254" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="255" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A255" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B255" s="31">
-        <v>45079</v>
+        <v>45080</v>
       </c>
       <c r="C255" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D255" s="5">
-        <v>49.64</v>
-      </c>
-      <c r="F255" s="17" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="256" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E256" s="14"/>
-      <c r="F256" s="1"/>
-    </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F255" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="256" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A256" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B256" s="31">
+        <v>45080</v>
+      </c>
+      <c r="C256" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F256" s="17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="257" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A257" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B257" s="31">
         <v>45079</v>
       </c>
-      <c r="C257" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="F257" s="16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C257" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D257" s="5">
+        <v>49.18</v>
+      </c>
+      <c r="E257" s="5">
+        <v>2690.49</v>
+      </c>
+      <c r="F257" s="32" t="s">
+        <v>220</v>
+      </c>
+      <c r="G257" s="13">
+        <f>AVERAGE(E257:E258)</f>
+        <v>2690.89</v>
+      </c>
+      <c r="H257" s="18">
+        <f>STDEV(E257:E258)</f>
+        <v>0.56568542494936658</v>
+      </c>
+      <c r="K257" s="5">
+        <f>G257+$J$218</f>
+        <v>2680</v>
+      </c>
+    </row>
+    <row r="258" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A258" s="9" t="s">
         <v>11</v>
       </c>
@@ -7600,11 +7597,17 @@
       <c r="C258" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F258" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D258" s="5">
+        <v>51.14</v>
+      </c>
+      <c r="E258" s="5">
+        <v>2691.29</v>
+      </c>
+      <c r="F258" s="32" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="259" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A259" s="9" t="s">
         <v>11</v>
       </c>
@@ -7614,11 +7617,26 @@
       <c r="C259" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F259" s="17" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D259" s="5">
+        <v>50.77</v>
+      </c>
+      <c r="F259" s="32" t="s">
+        <v>222</v>
+      </c>
+      <c r="G259" s="13" t="e">
+        <f>AVERAGE(E259:E260)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H259" s="18" t="e">
+        <f>STDEV(E259:E260)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K259" s="5" t="e">
+        <f>G259+$J$218</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="260" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A260" s="9" t="s">
         <v>11</v>
       </c>
@@ -7628,11 +7646,14 @@
       <c r="C260" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D260" s="5">
+        <v>49.14</v>
+      </c>
       <c r="F260" s="32" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="261" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A261" s="9" t="s">
         <v>11</v>
       </c>
@@ -7642,148 +7663,95 @@
       <c r="C261" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D261" s="5">
+        <v>49.79</v>
+      </c>
       <c r="F261" s="32" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.2">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="262" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A262" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B262" s="31">
-        <v>45079</v>
+        <v>45080</v>
       </c>
       <c r="C262" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F262" s="32" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.2">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="263" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A263" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B263" s="31">
-        <v>45079</v>
+        <v>45080</v>
       </c>
       <c r="C263" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F263" s="32" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.2">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="264" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A264" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B264" s="31">
-        <v>45079</v>
+        <v>45080</v>
       </c>
       <c r="C264" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F264" s="32" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.2">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="265" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A265" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B265" s="31">
-        <v>45079</v>
+        <v>45080</v>
       </c>
       <c r="C265" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F265" s="32" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.2">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="266" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A266" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B266" s="31">
-        <v>45079</v>
+        <v>45080</v>
       </c>
       <c r="C266" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F266" s="32" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.2">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="267" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A267" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B267" s="31">
-        <v>45079</v>
+        <v>45080</v>
       </c>
       <c r="C267" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F267" s="32" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A268" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B268" s="31">
-        <v>45079</v>
-      </c>
-      <c r="C268" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F268" s="32" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A269" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B269" s="31">
-        <v>45079</v>
-      </c>
-      <c r="C269" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F269" s="32" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A270" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B270" s="31">
-        <v>45079</v>
-      </c>
-      <c r="C270" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F270" s="32" t="s">
         <v>230</v>
-      </c>
-    </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A271" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B271" s="31">
-        <v>45079</v>
-      </c>
-      <c r="C271" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F271" s="32" t="s">
-        <v>231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tile 2 A, B ELOW T1
</commit_message>
<xml_diff>
--- a/Data/Spring_2023/BenthFun_Alkalinity.xlsx
+++ b/Data/Spring_2023/BenthFun_Alkalinity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremy/Library/Mobile Documents/com~apple~CloudDocs/Documents/Documents/Post-Doc/Projets/Villefranche/Projets/BenthFun – Jeremy/BenthFun/Data/Spring_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325F38BA-CEA0-9C49-B3B2-2A3D7E336709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5D2EC4-ABB7-3E48-9F84-B6B0C5F1A0A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="238">
   <si>
     <t>Operator</t>
   </si>
@@ -726,6 +726,27 @@
   </si>
   <si>
     <t>PI_t1_ELOW_blank_c</t>
+  </si>
+  <si>
+    <t>PI_t5_AMB_T0a</t>
+  </si>
+  <si>
+    <t>PI_t5_AMB_T0b</t>
+  </si>
+  <si>
+    <t>PI_t5_AMB_T0c</t>
+  </si>
+  <si>
+    <t>Broken bottle</t>
+  </si>
+  <si>
+    <t>PI_t1_LOW_T0c</t>
+  </si>
+  <si>
+    <t>PI_t1_LOW_T0b</t>
+  </si>
+  <si>
+    <t>PI_t1_LOW_T0a</t>
   </si>
 </sst>
 </file>
@@ -1200,11 +1221,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L267"/>
+  <dimension ref="A1:L273"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="73" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A231" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G259" sqref="G259:K259"/>
+      <pane ySplit="1" topLeftCell="A244" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E267" sqref="E267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6755,26 +6776,26 @@
       <c r="C221" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D221" s="5">
-        <v>50.4</v>
-      </c>
-      <c r="E221" s="5">
-        <v>2568.9899999999998</v>
+      <c r="D221" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="E221" s="5" t="s">
+        <v>155</v>
       </c>
       <c r="F221" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="G221" s="13">
-        <f>AVERAGE(E221:E222)</f>
-        <v>2569.0649999999996</v>
-      </c>
-      <c r="H221" s="18">
-        <f>STDEV(E221:E222)</f>
-        <v>0.10606601717804644</v>
-      </c>
-      <c r="K221" s="5">
-        <f>G221+$J$218</f>
-        <v>2558.1749999999997</v>
+        <v>237</v>
+      </c>
+      <c r="G221" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="H221" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="K221" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="L221" s="1" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="222" spans="1:12" x14ac:dyDescent="0.2">
@@ -6787,15 +6808,20 @@
       <c r="C222" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D222" s="5">
-        <v>50.8</v>
-      </c>
-      <c r="E222" s="5">
-        <v>2569.14</v>
+      <c r="D222" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="E222" s="5" t="s">
+        <v>155</v>
       </c>
       <c r="F222" s="17" t="s">
-        <v>187</v>
-      </c>
+        <v>236</v>
+      </c>
+      <c r="G222" s="1"/>
+      <c r="H222" s="1"/>
+      <c r="I222" s="1"/>
+      <c r="J222" s="1"/>
+      <c r="K222" s="1"/>
     </row>
     <row r="223" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A223" s="9" t="s">
@@ -6807,27 +6833,20 @@
       <c r="C223" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D223" s="5">
-        <v>48.18</v>
-      </c>
-      <c r="E223" s="5">
-        <v>2573.29</v>
+      <c r="D223" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="E223" s="5" t="s">
+        <v>155</v>
       </c>
       <c r="F223" s="17" t="s">
-        <v>188</v>
-      </c>
-      <c r="G223" s="13">
-        <f>AVERAGE(E224:E225)</f>
-        <v>2568.3900000000003</v>
-      </c>
-      <c r="H223" s="18">
-        <f>STDEV(E223,E225)</f>
-        <v>0.77781745930513801</v>
-      </c>
-      <c r="K223" s="5">
-        <f>G223+$J$218</f>
-        <v>2557.5000000000005</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="G223" s="1"/>
+      <c r="H223" s="1"/>
+      <c r="I223" s="1"/>
+      <c r="J223" s="1"/>
+      <c r="K223" s="1"/>
     </row>
     <row r="224" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A224" s="9" t="s">
@@ -6840,13 +6859,25 @@
         <v>12</v>
       </c>
       <c r="D224" s="5">
-        <v>50.08</v>
-      </c>
-      <c r="E224" s="14">
-        <v>2564.59</v>
+        <v>50.4</v>
+      </c>
+      <c r="E224" s="5">
+        <v>2568.9899999999998</v>
       </c>
       <c r="F224" s="17" t="s">
-        <v>189</v>
+        <v>186</v>
+      </c>
+      <c r="G224" s="13">
+        <f>AVERAGE(E224:E225)</f>
+        <v>2569.0649999999996</v>
+      </c>
+      <c r="H224" s="18">
+        <f>STDEV(E224:E225)</f>
+        <v>0.10606601717804644</v>
+      </c>
+      <c r="K224" s="5">
+        <f>G224+$J$218</f>
+        <v>2558.1749999999997</v>
       </c>
     </row>
     <row r="225" spans="1:11" x14ac:dyDescent="0.2">
@@ -6860,13 +6891,13 @@
         <v>12</v>
       </c>
       <c r="D225" s="5">
-        <v>50.64</v>
+        <v>50.8</v>
       </c>
       <c r="E225" s="5">
-        <v>2572.19</v>
+        <v>2569.14</v>
       </c>
       <c r="F225" s="17" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="226" spans="1:11" x14ac:dyDescent="0.2">
@@ -6880,25 +6911,25 @@
         <v>12</v>
       </c>
       <c r="D226" s="5">
-        <v>51.27</v>
+        <v>48.18</v>
       </c>
       <c r="E226" s="5">
-        <v>2569.29</v>
+        <v>2573.29</v>
       </c>
       <c r="F226" s="17" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G226" s="13">
-        <f>AVERAGE(E226:E227)</f>
-        <v>2570.1350000000002</v>
+        <f>AVERAGE(E227:E228)</f>
+        <v>2568.3900000000003</v>
       </c>
       <c r="H226" s="18">
-        <f>STDEV(E226:E227)</f>
-        <v>1.195010460205304</v>
+        <f>STDEV(E226,E228)</f>
+        <v>0.77781745930513801</v>
       </c>
       <c r="K226" s="5">
         <f>G226+$J$218</f>
-        <v>2559.2450000000003</v>
+        <v>2557.5000000000005</v>
       </c>
     </row>
     <row r="227" spans="1:11" x14ac:dyDescent="0.2">
@@ -6912,13 +6943,13 @@
         <v>12</v>
       </c>
       <c r="D227" s="5">
-        <v>49.89</v>
-      </c>
-      <c r="E227" s="5">
-        <v>2570.98</v>
+        <v>50.08</v>
+      </c>
+      <c r="E227" s="14">
+        <v>2564.59</v>
       </c>
       <c r="F227" s="17" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="228" spans="1:11" x14ac:dyDescent="0.2">
@@ -6932,25 +6963,13 @@
         <v>12</v>
       </c>
       <c r="D228" s="5">
-        <v>50.77</v>
-      </c>
-      <c r="E228" s="14">
-        <v>2578.58</v>
+        <v>50.64</v>
+      </c>
+      <c r="E228" s="5">
+        <v>2572.19</v>
       </c>
       <c r="F228" s="17" t="s">
-        <v>193</v>
-      </c>
-      <c r="G228" s="13">
-        <f>AVERAGE(E229:E230)</f>
-        <v>2563.94</v>
-      </c>
-      <c r="H228" s="18">
-        <f>STDEV(E229:E230)</f>
-        <v>2.0081832585698978</v>
-      </c>
-      <c r="K228" s="5">
-        <f>G228+$J$218</f>
-        <v>2553.0500000000002</v>
+        <v>190</v>
       </c>
     </row>
     <row r="229" spans="1:11" x14ac:dyDescent="0.2">
@@ -6964,13 +6983,25 @@
         <v>12</v>
       </c>
       <c r="D229" s="5">
-        <v>51.5</v>
+        <v>51.27</v>
       </c>
       <c r="E229" s="5">
-        <v>2562.52</v>
+        <v>2569.29</v>
       </c>
       <c r="F229" s="17" t="s">
-        <v>194</v>
+        <v>191</v>
+      </c>
+      <c r="G229" s="13">
+        <f>AVERAGE(E229:E230)</f>
+        <v>2570.1350000000002</v>
+      </c>
+      <c r="H229" s="18">
+        <f>STDEV(E229:E230)</f>
+        <v>1.195010460205304</v>
+      </c>
+      <c r="K229" s="5">
+        <f>G229+$J$218</f>
+        <v>2559.2450000000003</v>
       </c>
     </row>
     <row r="230" spans="1:11" x14ac:dyDescent="0.2">
@@ -6984,13 +7015,13 @@
         <v>12</v>
       </c>
       <c r="D230" s="5">
-        <v>50.94</v>
+        <v>49.89</v>
       </c>
       <c r="E230" s="5">
-        <v>2565.36</v>
+        <v>2570.98</v>
       </c>
       <c r="F230" s="17" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="231" spans="1:11" x14ac:dyDescent="0.2">
@@ -7004,25 +7035,25 @@
         <v>12</v>
       </c>
       <c r="D231" s="5">
-        <v>49.65</v>
-      </c>
-      <c r="E231" s="5">
-        <v>2587.7399999999998</v>
-      </c>
-      <c r="F231" s="32" t="s">
-        <v>196</v>
+        <v>50.77</v>
+      </c>
+      <c r="E231" s="14">
+        <v>2578.58</v>
+      </c>
+      <c r="F231" s="17" t="s">
+        <v>193</v>
       </c>
       <c r="G231" s="13">
-        <f>AVERAGE(E231,E233)</f>
-        <v>2586.5</v>
+        <f>AVERAGE(E232:E233)</f>
+        <v>2563.94</v>
       </c>
       <c r="H231" s="18">
-        <f>STDEV(E231,E233)</f>
-        <v>1.7536248173423292</v>
+        <f>STDEV(E232:E233)</f>
+        <v>2.0081832585698978</v>
       </c>
       <c r="K231" s="5">
         <f>G231+$J$218</f>
-        <v>2575.61</v>
+        <v>2553.0500000000002</v>
       </c>
     </row>
     <row r="232" spans="1:11" x14ac:dyDescent="0.2">
@@ -7036,13 +7067,13 @@
         <v>12</v>
       </c>
       <c r="D232" s="5">
-        <v>49.82</v>
-      </c>
-      <c r="E232" s="14">
-        <v>2575.98</v>
-      </c>
-      <c r="F232" s="32" t="s">
-        <v>197</v>
+        <v>51.5</v>
+      </c>
+      <c r="E232" s="5">
+        <v>2562.52</v>
+      </c>
+      <c r="F232" s="17" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="233" spans="1:11" x14ac:dyDescent="0.2">
@@ -7056,13 +7087,13 @@
         <v>12</v>
       </c>
       <c r="D233" s="5">
-        <v>49.37</v>
+        <v>50.94</v>
       </c>
       <c r="E233" s="5">
-        <v>2585.2600000000002</v>
-      </c>
-      <c r="F233" s="32" t="s">
-        <v>198</v>
+        <v>2565.36</v>
+      </c>
+      <c r="F233" s="17" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="234" spans="1:11" x14ac:dyDescent="0.2">
@@ -7076,25 +7107,25 @@
         <v>12</v>
       </c>
       <c r="D234" s="5">
-        <v>50.38</v>
+        <v>49.65</v>
       </c>
       <c r="E234" s="5">
-        <v>2571.42</v>
-      </c>
-      <c r="F234" s="17" t="s">
-        <v>199</v>
+        <v>2587.7399999999998</v>
+      </c>
+      <c r="F234" s="32" t="s">
+        <v>196</v>
       </c>
       <c r="G234" s="13">
-        <f>AVERAGE(E234:E235)</f>
-        <v>2572.7600000000002</v>
+        <f>AVERAGE(E234,E236)</f>
+        <v>2586.5</v>
       </c>
       <c r="H234" s="18">
-        <f>STDEV(E234:E235)</f>
-        <v>1.8950461735798316</v>
+        <f>STDEV(E234,E236)</f>
+        <v>1.7536248173423292</v>
       </c>
       <c r="K234" s="5">
         <f>G234+$J$218</f>
-        <v>2561.8700000000003</v>
+        <v>2575.61</v>
       </c>
     </row>
     <row r="235" spans="1:11" x14ac:dyDescent="0.2">
@@ -7108,13 +7139,33 @@
         <v>12</v>
       </c>
       <c r="D235" s="5">
-        <v>48.94</v>
-      </c>
-      <c r="E235" s="5">
-        <v>2574.1</v>
-      </c>
-      <c r="F235" s="17" t="s">
-        <v>200</v>
+        <v>49.82</v>
+      </c>
+      <c r="E235" s="14">
+        <v>2575.98</v>
+      </c>
+      <c r="F235" s="32" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="236" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A236" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B236" s="31">
+        <v>45079</v>
+      </c>
+      <c r="C236" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D236" s="5">
+        <v>49.37</v>
+      </c>
+      <c r="E236" s="5">
+        <v>2585.2600000000002</v>
+      </c>
+      <c r="F236" s="32" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="237" spans="1:11" x14ac:dyDescent="0.2">
@@ -7128,25 +7179,25 @@
         <v>12</v>
       </c>
       <c r="D237" s="5">
-        <v>51.96</v>
-      </c>
-      <c r="E237" s="14">
-        <v>2589.33</v>
+        <v>50.38</v>
+      </c>
+      <c r="E237" s="5">
+        <v>2571.42</v>
       </c>
       <c r="F237" s="17" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G237" s="13">
-        <f>AVERAGE(E238:E239)</f>
-        <v>2607.5250000000001</v>
+        <f>AVERAGE(E237:E238)</f>
+        <v>2572.7600000000002</v>
       </c>
       <c r="H237" s="18">
-        <f>STDEV(E238:E239)</f>
-        <v>4.9143921292463766</v>
+        <f>STDEV(E237:E238)</f>
+        <v>1.8950461735798316</v>
       </c>
       <c r="K237" s="5">
         <f>G237+$J$218</f>
-        <v>2596.6350000000002</v>
+        <v>2561.8700000000003</v>
       </c>
     </row>
     <row r="238" spans="1:11" x14ac:dyDescent="0.2">
@@ -7160,33 +7211,13 @@
         <v>12</v>
       </c>
       <c r="D238" s="5">
-        <v>51.12</v>
+        <v>48.94</v>
       </c>
       <c r="E238" s="5">
-        <v>2604.0500000000002</v>
+        <v>2574.1</v>
       </c>
       <c r="F238" s="17" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="239" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A239" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B239" s="31">
-        <v>45079</v>
-      </c>
-      <c r="C239" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D239" s="5">
-        <v>50.19</v>
-      </c>
-      <c r="E239" s="5">
-        <v>2611</v>
-      </c>
-      <c r="F239" s="17" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="240" spans="1:11" x14ac:dyDescent="0.2">
@@ -7200,25 +7231,25 @@
         <v>12</v>
       </c>
       <c r="D240" s="5">
-        <v>50.01</v>
-      </c>
-      <c r="E240" s="22">
-        <v>2587.63</v>
+        <v>51.96</v>
+      </c>
+      <c r="E240" s="14">
+        <v>2589.33</v>
       </c>
       <c r="F240" s="17" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="G240" s="13">
-        <f>AVERAGE(E240:E241)</f>
-        <v>2585.4450000000002</v>
+        <f>AVERAGE(E241:E242)</f>
+        <v>2607.5250000000001</v>
       </c>
       <c r="H240" s="18">
-        <f>STDEV(E240:E241)</f>
-        <v>3.0900566337851356</v>
+        <f>STDEV(E241:E242)</f>
+        <v>4.9143921292463766</v>
       </c>
       <c r="K240" s="5">
         <f>G240+$J$218</f>
-        <v>2574.5550000000003</v>
+        <v>2596.6350000000002</v>
       </c>
     </row>
     <row r="241" spans="1:12" x14ac:dyDescent="0.2">
@@ -7232,13 +7263,13 @@
         <v>12</v>
       </c>
       <c r="D241" s="5">
-        <v>50.78</v>
+        <v>51.12</v>
       </c>
       <c r="E241" s="5">
-        <v>2583.2600000000002</v>
+        <v>2604.0500000000002</v>
       </c>
       <c r="F241" s="17" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="242" spans="1:12" x14ac:dyDescent="0.2">
@@ -7252,25 +7283,13 @@
         <v>12</v>
       </c>
       <c r="D242" s="5">
-        <v>48.04</v>
-      </c>
-      <c r="E242" s="14">
-        <v>3171.62</v>
+        <v>50.19</v>
+      </c>
+      <c r="E242" s="5">
+        <v>2611</v>
       </c>
       <c r="F242" s="17" t="s">
-        <v>207</v>
-      </c>
-      <c r="G242" s="13">
-        <f>AVERAGE(E243,E245)</f>
-        <v>2583.4250000000002</v>
-      </c>
-      <c r="H242" s="18">
-        <f>STDEV(E241,E243)</f>
-        <v>0.16263455967259724</v>
-      </c>
-      <c r="K242" s="5">
-        <f>G242+$J$218</f>
-        <v>2572.5350000000003</v>
+        <v>203</v>
       </c>
     </row>
     <row r="243" spans="1:12" x14ac:dyDescent="0.2">
@@ -7284,13 +7303,25 @@
         <v>12</v>
       </c>
       <c r="D243" s="5">
-        <v>50.59</v>
-      </c>
-      <c r="E243" s="5">
-        <v>2583.4899999999998</v>
+        <v>50.01</v>
+      </c>
+      <c r="E243" s="22">
+        <v>2587.63</v>
       </c>
       <c r="F243" s="17" t="s">
-        <v>208</v>
+        <v>204</v>
+      </c>
+      <c r="G243" s="13">
+        <f>AVERAGE(E243:E244)</f>
+        <v>2585.4450000000002</v>
+      </c>
+      <c r="H243" s="18">
+        <f>STDEV(E243:E244)</f>
+        <v>3.0900566337851356</v>
+      </c>
+      <c r="K243" s="5">
+        <f>G243+$J$218</f>
+        <v>2574.5550000000003</v>
       </c>
     </row>
     <row r="244" spans="1:12" x14ac:dyDescent="0.2">
@@ -7304,13 +7335,13 @@
         <v>12</v>
       </c>
       <c r="D244" s="5">
-        <v>50.55</v>
-      </c>
-      <c r="E244" s="14">
-        <v>2598.48</v>
+        <v>50.78</v>
+      </c>
+      <c r="E244" s="5">
+        <v>2583.2600000000002</v>
       </c>
       <c r="F244" s="17" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="245" spans="1:12" x14ac:dyDescent="0.2">
@@ -7324,13 +7355,25 @@
         <v>12</v>
       </c>
       <c r="D245" s="5">
-        <v>49.51</v>
-      </c>
-      <c r="E245" s="5">
-        <v>2583.36</v>
+        <v>48.04</v>
+      </c>
+      <c r="E245" s="14">
+        <v>3171.62</v>
       </c>
       <c r="F245" s="17" t="s">
-        <v>219</v>
+        <v>207</v>
+      </c>
+      <c r="G245" s="13">
+        <f>AVERAGE(E246,E248)</f>
+        <v>2583.4250000000002</v>
+      </c>
+      <c r="H245" s="18">
+        <f>STDEV(E244,E246)</f>
+        <v>0.16263455967259724</v>
+      </c>
+      <c r="K245" s="5">
+        <f>G245+$J$218</f>
+        <v>2572.5350000000003</v>
       </c>
     </row>
     <row r="246" spans="1:12" x14ac:dyDescent="0.2">
@@ -7344,25 +7387,13 @@
         <v>12</v>
       </c>
       <c r="D246" s="5">
-        <v>50.07</v>
+        <v>50.59</v>
       </c>
       <c r="E246" s="5">
-        <v>2576</v>
+        <v>2583.4899999999998</v>
       </c>
       <c r="F246" s="17" t="s">
-        <v>210</v>
-      </c>
-      <c r="G246" s="13">
-        <f>AVERAGE(E246:E247)</f>
-        <v>2578.415</v>
-      </c>
-      <c r="H246" s="18">
-        <f>STDEV(E246:E247)</f>
-        <v>3.4153257531309733</v>
-      </c>
-      <c r="K246" s="5">
-        <f>G246+$J$218</f>
-        <v>2567.5250000000001</v>
+        <v>208</v>
       </c>
     </row>
     <row r="247" spans="1:12" x14ac:dyDescent="0.2">
@@ -7376,13 +7407,13 @@
         <v>12</v>
       </c>
       <c r="D247" s="5">
-        <v>48.8</v>
-      </c>
-      <c r="E247" s="5">
-        <v>2580.83</v>
+        <v>50.55</v>
+      </c>
+      <c r="E247" s="14">
+        <v>2598.48</v>
       </c>
       <c r="F247" s="17" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="248" spans="1:12" x14ac:dyDescent="0.2">
@@ -7396,25 +7427,13 @@
         <v>12</v>
       </c>
       <c r="D248" s="5">
-        <v>51.69</v>
+        <v>49.51</v>
       </c>
       <c r="E248" s="5">
-        <v>2593.9299999999998</v>
-      </c>
-      <c r="F248" s="32" t="s">
-        <v>213</v>
-      </c>
-      <c r="G248" s="13">
-        <f>AVERAGE(E248:E249)</f>
-        <v>2591.4899999999998</v>
-      </c>
-      <c r="H248" s="18">
-        <f>STDEV(E248:E249)</f>
-        <v>3.4506810921901074</v>
-      </c>
-      <c r="K248" s="5">
-        <f>G248+$J$218</f>
-        <v>2580.6</v>
+        <v>2583.36</v>
+      </c>
+      <c r="F248" s="17" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="249" spans="1:12" x14ac:dyDescent="0.2">
@@ -7428,13 +7447,25 @@
         <v>12</v>
       </c>
       <c r="D249" s="5">
-        <v>51.1</v>
+        <v>50.07</v>
       </c>
       <c r="E249" s="5">
-        <v>2589.0500000000002</v>
-      </c>
-      <c r="F249" s="32" t="s">
-        <v>214</v>
+        <v>2576</v>
+      </c>
+      <c r="F249" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="G249" s="13">
+        <f>AVERAGE(E249:E250)</f>
+        <v>2578.415</v>
+      </c>
+      <c r="H249" s="18">
+        <f>STDEV(E249:E250)</f>
+        <v>3.4153257531309733</v>
+      </c>
+      <c r="K249" s="5">
+        <f>G249+$J$218</f>
+        <v>2567.5250000000001</v>
       </c>
     </row>
     <row r="250" spans="1:12" x14ac:dyDescent="0.2">
@@ -7448,25 +7479,13 @@
         <v>12</v>
       </c>
       <c r="D250" s="5">
-        <v>50.57</v>
-      </c>
-      <c r="E250" s="5" t="s">
-        <v>155</v>
+        <v>48.8</v>
+      </c>
+      <c r="E250" s="5">
+        <v>2580.83</v>
       </c>
       <c r="F250" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="G250" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="H250" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="K250" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="L250" s="1" t="s">
-        <v>184</v>
+        <v>211</v>
       </c>
     </row>
     <row r="251" spans="1:12" x14ac:dyDescent="0.2">
@@ -7479,14 +7498,26 @@
       <c r="C251" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D251" s="5">
-        <v>50.9</v>
+      <c r="D251" s="5" t="s">
+        <v>155</v>
       </c>
       <c r="E251" s="5" t="s">
         <v>155</v>
       </c>
       <c r="F251" s="17" t="s">
-        <v>217</v>
+        <v>231</v>
+      </c>
+      <c r="G251" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="H251" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="K251" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="L251" s="1" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="252" spans="1:12" x14ac:dyDescent="0.2">
@@ -7499,32 +7530,76 @@
       <c r="C252" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D252" s="5">
-        <v>50.92</v>
+      <c r="D252" s="5" t="s">
+        <v>155</v>
       </c>
       <c r="E252" s="5" t="s">
         <v>155</v>
       </c>
       <c r="F252" s="17" t="s">
-        <v>218</v>
-      </c>
+        <v>232</v>
+      </c>
+      <c r="G252" s="1"/>
+      <c r="H252" s="1"/>
+      <c r="I252" s="1"/>
+      <c r="J252" s="1"/>
+      <c r="K252" s="1"/>
     </row>
     <row r="253" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="E253" s="14"/>
-      <c r="F253" s="1"/>
+      <c r="A253" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B253" s="31">
+        <v>45079</v>
+      </c>
+      <c r="C253" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D253" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="E253" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F253" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="G253" s="1"/>
+      <c r="H253" s="1"/>
+      <c r="I253" s="1"/>
+      <c r="J253" s="1"/>
+      <c r="K253" s="1"/>
     </row>
     <row r="254" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A254" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B254" s="31">
-        <v>45080</v>
-      </c>
-      <c r="C254" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="F254" s="16" t="s">
-        <v>8</v>
+        <v>45079</v>
+      </c>
+      <c r="C254" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D254" s="5">
+        <v>51.69</v>
+      </c>
+      <c r="E254" s="5">
+        <v>2593.9299999999998</v>
+      </c>
+      <c r="F254" s="32" t="s">
+        <v>213</v>
+      </c>
+      <c r="G254" s="13">
+        <f>AVERAGE(E254:E255)</f>
+        <v>2591.4899999999998</v>
+      </c>
+      <c r="H254" s="18">
+        <f>STDEV(E254:E255)</f>
+        <v>3.4506810921901074</v>
+      </c>
+      <c r="K254" s="5">
+        <f>G254+$J$218</f>
+        <v>2580.6</v>
       </c>
     </row>
     <row r="255" spans="1:12" x14ac:dyDescent="0.2">
@@ -7532,13 +7607,19 @@
         <v>11</v>
       </c>
       <c r="B255" s="31">
-        <v>45080</v>
+        <v>45079</v>
       </c>
       <c r="C255" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F255" s="16" t="s">
-        <v>9</v>
+      <c r="D255" s="5">
+        <v>51.1</v>
+      </c>
+      <c r="E255" s="5">
+        <v>2589.0500000000002</v>
+      </c>
+      <c r="F255" s="32" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="256" spans="1:12" x14ac:dyDescent="0.2">
@@ -7546,13 +7627,31 @@
         <v>11</v>
       </c>
       <c r="B256" s="31">
-        <v>45080</v>
+        <v>45079</v>
       </c>
       <c r="C256" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D256" s="5">
+        <v>50.57</v>
+      </c>
+      <c r="E256" s="5" t="s">
+        <v>155</v>
+      </c>
       <c r="F256" s="17" t="s">
-        <v>98</v>
+        <v>216</v>
+      </c>
+      <c r="G256" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="H256" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="K256" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="L256" s="1" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="257" spans="1:11" x14ac:dyDescent="0.2">
@@ -7566,25 +7665,13 @@
         <v>12</v>
       </c>
       <c r="D257" s="5">
-        <v>49.18</v>
-      </c>
-      <c r="E257" s="5">
-        <v>2690.49</v>
-      </c>
-      <c r="F257" s="32" t="s">
-        <v>220</v>
-      </c>
-      <c r="G257" s="13">
-        <f>AVERAGE(E257:E258)</f>
-        <v>2690.89</v>
-      </c>
-      <c r="H257" s="18">
-        <f>STDEV(E257:E258)</f>
-        <v>0.56568542494936658</v>
-      </c>
-      <c r="K257" s="5">
-        <f>G257+$J$218</f>
-        <v>2680</v>
+        <v>50.9</v>
+      </c>
+      <c r="E257" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F257" s="17" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="258" spans="1:11" x14ac:dyDescent="0.2">
@@ -7598,59 +7685,31 @@
         <v>12</v>
       </c>
       <c r="D258" s="5">
-        <v>51.14</v>
-      </c>
-      <c r="E258" s="5">
-        <v>2691.29</v>
-      </c>
-      <c r="F258" s="32" t="s">
-        <v>221</v>
+        <v>50.92</v>
+      </c>
+      <c r="E258" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F258" s="17" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="259" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A259" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B259" s="31">
-        <v>45079</v>
-      </c>
-      <c r="C259" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D259" s="5">
-        <v>50.77</v>
-      </c>
-      <c r="F259" s="32" t="s">
-        <v>222</v>
-      </c>
-      <c r="G259" s="13" t="e">
-        <f>AVERAGE(E259:E260)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H259" s="18" t="e">
-        <f>STDEV(E259:E260)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K259" s="5" t="e">
-        <f>G259+$J$218</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E259" s="14"/>
+      <c r="F259" s="1"/>
     </row>
     <row r="260" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A260" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B260" s="31">
-        <v>45079</v>
-      </c>
-      <c r="C260" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D260" s="5">
-        <v>49.14</v>
-      </c>
-      <c r="F260" s="32" t="s">
-        <v>223</v>
+        <v>45080</v>
+      </c>
+      <c r="C260" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F260" s="16" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="261" spans="1:11" x14ac:dyDescent="0.2">
@@ -7658,16 +7717,13 @@
         <v>11</v>
       </c>
       <c r="B261" s="31">
-        <v>45079</v>
+        <v>45080</v>
       </c>
       <c r="C261" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D261" s="5">
-        <v>49.79</v>
-      </c>
-      <c r="F261" s="32" t="s">
-        <v>224</v>
+      <c r="F261" s="16" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="262" spans="1:11" x14ac:dyDescent="0.2">
@@ -7680,8 +7736,8 @@
       <c r="C262" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F262" s="32" t="s">
-        <v>225</v>
+      <c r="F262" s="17" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="263" spans="1:11" x14ac:dyDescent="0.2">
@@ -7689,13 +7745,31 @@
         <v>11</v>
       </c>
       <c r="B263" s="31">
-        <v>45080</v>
+        <v>45079</v>
       </c>
       <c r="C263" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D263" s="5">
+        <v>49.18</v>
+      </c>
+      <c r="E263" s="5">
+        <v>2690.49</v>
+      </c>
       <c r="F263" s="32" t="s">
-        <v>226</v>
+        <v>220</v>
+      </c>
+      <c r="G263" s="13">
+        <f>AVERAGE(E263:E264)</f>
+        <v>2690.89</v>
+      </c>
+      <c r="H263" s="18">
+        <f>STDEV(E263:E264)</f>
+        <v>0.56568542494936658</v>
+      </c>
+      <c r="K263" s="5">
+        <f>G263+$J$218</f>
+        <v>2680</v>
       </c>
     </row>
     <row r="264" spans="1:11" x14ac:dyDescent="0.2">
@@ -7703,13 +7777,19 @@
         <v>11</v>
       </c>
       <c r="B264" s="31">
-        <v>45080</v>
+        <v>45079</v>
       </c>
       <c r="C264" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D264" s="5">
+        <v>51.14</v>
+      </c>
+      <c r="E264" s="5">
+        <v>2691.29</v>
+      </c>
       <c r="F264" s="32" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="265" spans="1:11" x14ac:dyDescent="0.2">
@@ -7717,13 +7797,31 @@
         <v>11</v>
       </c>
       <c r="B265" s="31">
-        <v>45080</v>
+        <v>45079</v>
       </c>
       <c r="C265" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D265" s="5">
+        <v>50.77</v>
+      </c>
+      <c r="E265" s="5">
+        <v>2851.54</v>
+      </c>
       <c r="F265" s="32" t="s">
-        <v>228</v>
+        <v>222</v>
+      </c>
+      <c r="G265" s="13">
+        <f>AVERAGE(E265:E266)</f>
+        <v>2844.71</v>
+      </c>
+      <c r="H265" s="18">
+        <f>STDEV(E265:E266)</f>
+        <v>9.6590786310081356</v>
+      </c>
+      <c r="K265" s="5">
+        <f>G265+$J$218</f>
+        <v>2833.82</v>
       </c>
     </row>
     <row r="266" spans="1:11" x14ac:dyDescent="0.2">
@@ -7731,13 +7829,19 @@
         <v>11</v>
       </c>
       <c r="B266" s="31">
-        <v>45080</v>
+        <v>45079</v>
       </c>
       <c r="C266" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D266" s="5">
+        <v>49.14</v>
+      </c>
+      <c r="E266" s="5">
+        <v>2837.88</v>
+      </c>
       <c r="F266" s="32" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
     <row r="267" spans="1:11" x14ac:dyDescent="0.2">
@@ -7745,12 +7849,99 @@
         <v>11</v>
       </c>
       <c r="B267" s="31">
+        <v>45079</v>
+      </c>
+      <c r="C267" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D267" s="5">
+        <v>49.79</v>
+      </c>
+      <c r="F267" s="32" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="268" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A268" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B268" s="31">
         <v>45080</v>
       </c>
-      <c r="C267" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F267" s="32" t="s">
+      <c r="C268" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F268" s="32" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="269" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A269" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B269" s="31">
+        <v>45080</v>
+      </c>
+      <c r="C269" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F269" s="32" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="270" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A270" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B270" s="31">
+        <v>45080</v>
+      </c>
+      <c r="C270" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F270" s="32" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="271" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A271" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B271" s="31">
+        <v>45080</v>
+      </c>
+      <c r="C271" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F271" s="32" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="272" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A272" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B272" s="31">
+        <v>45080</v>
+      </c>
+      <c r="C272" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F272" s="32" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A273" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B273" s="31">
+        <v>45080</v>
+      </c>
+      <c r="C273" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F273" s="32" t="s">
         <v>230</v>
       </c>
     </row>

</xml_diff>

<commit_message>
End ALK 2/6/23 Tile 2 T1 ELOW
</commit_message>
<xml_diff>
--- a/Data/Spring_2023/BenthFun_Alkalinity.xlsx
+++ b/Data/Spring_2023/BenthFun_Alkalinity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremy/Library/Mobile Documents/com~apple~CloudDocs/Documents/Documents/Post-Doc/Projets/Villefranche/Projets/BenthFun – Jeremy/BenthFun/Data/Spring_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5D2EC4-ABB7-3E48-9F84-B6B0C5F1A0A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC1ED1B-CDB7-2641-A565-0BA21A99FB0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1224,8 +1224,8 @@
   <dimension ref="A1:L273"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="73" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A244" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E267" sqref="E267"/>
+      <pane ySplit="1" topLeftCell="A254" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N267" sqref="N267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7805,23 +7805,23 @@
       <c r="D265" s="5">
         <v>50.77</v>
       </c>
-      <c r="E265" s="5">
+      <c r="E265" s="14">
         <v>2851.54</v>
       </c>
       <c r="F265" s="32" t="s">
         <v>222</v>
       </c>
       <c r="G265" s="13">
-        <f>AVERAGE(E265:E266)</f>
-        <v>2844.71</v>
+        <f>AVERAGE(E266:E267)</f>
+        <v>2834.8150000000001</v>
       </c>
       <c r="H265" s="18">
-        <f>STDEV(E265:E266)</f>
-        <v>9.6590786310081356</v>
+        <f>STDEV(E266:E267)</f>
+        <v>4.3345645686736134</v>
       </c>
       <c r="K265" s="5">
         <f>G265+$J$218</f>
-        <v>2833.82</v>
+        <v>2823.9250000000002</v>
       </c>
     </row>
     <row r="266" spans="1:11" x14ac:dyDescent="0.2">
@@ -7856,6 +7856,9 @@
       </c>
       <c r="D267" s="5">
         <v>49.79</v>
+      </c>
+      <c r="E267" s="5">
+        <v>2831.75</v>
       </c>
       <c r="F267" s="32" t="s">
         <v>224</v>

</xml_diff>

<commit_message>
CRM init 3/6 ALK
</commit_message>
<xml_diff>
--- a/Data/Spring_2023/BenthFun_Alkalinity.xlsx
+++ b/Data/Spring_2023/BenthFun_Alkalinity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremy/Library/Mobile Documents/com~apple~CloudDocs/Documents/Documents/Post-Doc/Projets/Villefranche/Projets/BenthFun – Jeremy/BenthFun/Data/Spring_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC1ED1B-CDB7-2641-A565-0BA21A99FB0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C04F3CD3-41F7-9E4C-AA76-99F0124165FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="428">
   <si>
     <t>Operator</t>
   </si>
@@ -653,9 +653,6 @@
     <t>PI_t2_AMB_T0b</t>
   </si>
   <si>
-    <t>PI_t2_AMB_T0c</t>
-  </si>
-  <si>
     <t>PI_t3_AMB_T0a</t>
   </si>
   <si>
@@ -671,18 +668,12 @@
     <t>PI_t4_AMB_T0b</t>
   </si>
   <si>
-    <t>PI_t4_AMB_T0c</t>
-  </si>
-  <si>
     <t>PI_t6_AMB_T0a</t>
   </si>
   <si>
     <t>PI_t6_AMB_T0b</t>
   </si>
   <si>
-    <t>PI_t6_AMB_T0c</t>
-  </si>
-  <si>
     <t>PI_t7_AMB_T0a</t>
   </si>
   <si>
@@ -747,13 +738,592 @@
   </si>
   <si>
     <t>PI_t1_LOW_T0a</t>
+  </si>
+  <si>
+    <t>PI_t2_ELOW_Tile_1a</t>
+  </si>
+  <si>
+    <t>PI_t2_ELOW_Tile_1b</t>
+  </si>
+  <si>
+    <t>PI_t2_ELOW_Tile_2a</t>
+  </si>
+  <si>
+    <t>PI_t2_ELOW_Tile_2b</t>
+  </si>
+  <si>
+    <t>PI_t2_ELOW_Tile_2c</t>
+  </si>
+  <si>
+    <t>PI_t2_ELOW_Tile_3a</t>
+  </si>
+  <si>
+    <t>PI_t2_ELOW_Tile_3b</t>
+  </si>
+  <si>
+    <t>PI_t2_ELOW_Tile_3c</t>
+  </si>
+  <si>
+    <t>PI_t3_ELOW_Tile_1a</t>
+  </si>
+  <si>
+    <t>PI_t3_ELOW_Tile_1b</t>
+  </si>
+  <si>
+    <t>PI_t3_ELOW_Tile_2a</t>
+  </si>
+  <si>
+    <t>PI_t3_ELOW_Tile_2b</t>
+  </si>
+  <si>
+    <t>PI_t3_ELOW_Tile_2c</t>
+  </si>
+  <si>
+    <t>PI_t3_ELOW_Tile_3a</t>
+  </si>
+  <si>
+    <t>PI_t3_ELOW_Tile_3b</t>
+  </si>
+  <si>
+    <t>PI_t3_ELOW_Tile_3c</t>
+  </si>
+  <si>
+    <t>PI_t4_ELOW_Tile_1a</t>
+  </si>
+  <si>
+    <t>PI_t4_ELOW_Tile_1b</t>
+  </si>
+  <si>
+    <t>PI_t4_ELOW_Tile_2a</t>
+  </si>
+  <si>
+    <t>PI_t4_ELOW_Tile_2b</t>
+  </si>
+  <si>
+    <t>PI_t4_ELOW_Tile_2c</t>
+  </si>
+  <si>
+    <t>PI_t4_ELOW_Tile_3a</t>
+  </si>
+  <si>
+    <t>PI_t4_ELOW_Tile_3b</t>
+  </si>
+  <si>
+    <t>PI_t4_ELOW_Tile_3c</t>
+  </si>
+  <si>
+    <t>PI_t5_ELOW_Tile_1a</t>
+  </si>
+  <si>
+    <t>PI_t5_ELOW_Tile_1b</t>
+  </si>
+  <si>
+    <t>PI_t5_ELOW_Tile_2a</t>
+  </si>
+  <si>
+    <t>PI_t5_ELOW_Tile_2b</t>
+  </si>
+  <si>
+    <t>PI_t5_ELOW_Tile_2c</t>
+  </si>
+  <si>
+    <t>PI_t5_ELOW_Tile_3a</t>
+  </si>
+  <si>
+    <t>PI_t5_ELOW_Tile_3b</t>
+  </si>
+  <si>
+    <t>PI_t5_ELOW_Tile_3c</t>
+  </si>
+  <si>
+    <t>PI_t2_ELOW_Tile_1c</t>
+  </si>
+  <si>
+    <t>PI_t3_ELOW_Tile_1c</t>
+  </si>
+  <si>
+    <t>PI_t4_ELOW_Tile_1c</t>
+  </si>
+  <si>
+    <t>PI_t5_ELOW_Tile_1c</t>
+  </si>
+  <si>
+    <t>PI_t6_ELOW_Tile_1a</t>
+  </si>
+  <si>
+    <t>PI_t6_ELOW_Tile_1b</t>
+  </si>
+  <si>
+    <t>PI_t6_ELOW_Tile_1c</t>
+  </si>
+  <si>
+    <t>PI_t6_ELOW_Tile_2a</t>
+  </si>
+  <si>
+    <t>PI_t6_ELOW_Tile_2b</t>
+  </si>
+  <si>
+    <t>PI_t6_ELOW_Tile_2c</t>
+  </si>
+  <si>
+    <t>PI_t6_ELOW_Tile_3a</t>
+  </si>
+  <si>
+    <t>PI_t6_ELOW_Tile_3b</t>
+  </si>
+  <si>
+    <t>PI_t6_ELOW_Tile_3c</t>
+  </si>
+  <si>
+    <t>PI_t7_ELOW_Tile_1a</t>
+  </si>
+  <si>
+    <t>PI_t7_ELOW_Tile_1b</t>
+  </si>
+  <si>
+    <t>PI_t7_ELOW_Tile_1c</t>
+  </si>
+  <si>
+    <t>PI_t7_ELOW_Tile_2a</t>
+  </si>
+  <si>
+    <t>PI_t7_ELOW_Tile_2b</t>
+  </si>
+  <si>
+    <t>PI_t7_ELOW_Tile_2c</t>
+  </si>
+  <si>
+    <t>PI_t7_ELOW_Tile_3a</t>
+  </si>
+  <si>
+    <t>PI_t7_ELOW_Tile_3b</t>
+  </si>
+  <si>
+    <t>PI_t7_ELOW_Tile_3c</t>
+  </si>
+  <si>
+    <t>PI_t8_ELOW_Tile_1a</t>
+  </si>
+  <si>
+    <t>PI_t8_ELOW_Tile_1b</t>
+  </si>
+  <si>
+    <t>PI_t8_ELOW_Tile_1c</t>
+  </si>
+  <si>
+    <t>PI_t8_ELOW_Tile_2a</t>
+  </si>
+  <si>
+    <t>PI_t8_ELOW_Tile_2b</t>
+  </si>
+  <si>
+    <t>PI_t8_ELOW_Tile_2c</t>
+  </si>
+  <si>
+    <t>PI_t8_ELOW_Tile_3a</t>
+  </si>
+  <si>
+    <t>PI_t8_ELOW_Tile_3b</t>
+  </si>
+  <si>
+    <t>PI_t8_ELOW_Tile_3c</t>
+  </si>
+  <si>
+    <t>PI_t1_LOW_Tile_1a</t>
+  </si>
+  <si>
+    <t>PI_t1_LOW_Tile_1b</t>
+  </si>
+  <si>
+    <t>PI_t1_LOW_Tile_2a</t>
+  </si>
+  <si>
+    <t>PI_t1_LOW_Tile_2b</t>
+  </si>
+  <si>
+    <t>PI_t1_LOW_Tile_2c</t>
+  </si>
+  <si>
+    <t>PI_t1_LOW_Tile_3a</t>
+  </si>
+  <si>
+    <t>PI_t1_LOW_Tile_3b</t>
+  </si>
+  <si>
+    <t>PI_t1_LOW_Tile_3c</t>
+  </si>
+  <si>
+    <t>PI_t1_LOW_blank_a</t>
+  </si>
+  <si>
+    <t>PI_t1_LOW_blank_b</t>
+  </si>
+  <si>
+    <t>PI_t1_LOW_blank_c</t>
+  </si>
+  <si>
+    <t>PI_t2_LOW_Tile_1a</t>
+  </si>
+  <si>
+    <t>PI_t2_LOW_Tile_1b</t>
+  </si>
+  <si>
+    <t>PI_t2_LOW_Tile_1c</t>
+  </si>
+  <si>
+    <t>PI_t2_LOW_Tile_2a</t>
+  </si>
+  <si>
+    <t>PI_t2_LOW_Tile_2b</t>
+  </si>
+  <si>
+    <t>PI_t2_LOW_Tile_2c</t>
+  </si>
+  <si>
+    <t>PI_t2_LOW_Tile_3a</t>
+  </si>
+  <si>
+    <t>PI_t2_LOW_Tile_3b</t>
+  </si>
+  <si>
+    <t>PI_t2_LOW_Tile_3c</t>
+  </si>
+  <si>
+    <t>PI_t3_LOW_Tile_1a</t>
+  </si>
+  <si>
+    <t>PI_t3_LOW_Tile_1b</t>
+  </si>
+  <si>
+    <t>PI_t3_LOW_Tile_1c</t>
+  </si>
+  <si>
+    <t>PI_t3_LOW_Tile_2a</t>
+  </si>
+  <si>
+    <t>PI_t3_LOW_Tile_2b</t>
+  </si>
+  <si>
+    <t>PI_t3_LOW_Tile_2c</t>
+  </si>
+  <si>
+    <t>PI_t3_LOW_Tile_3a</t>
+  </si>
+  <si>
+    <t>PI_t3_LOW_Tile_3b</t>
+  </si>
+  <si>
+    <t>PI_t3_LOW_Tile_3c</t>
+  </si>
+  <si>
+    <t>PI_t4_LOW_Tile_1a</t>
+  </si>
+  <si>
+    <t>PI_t4_LOW_Tile_1b</t>
+  </si>
+  <si>
+    <t>PI_t4_LOW_Tile_1c</t>
+  </si>
+  <si>
+    <t>PI_t4_LOW_Tile_2a</t>
+  </si>
+  <si>
+    <t>PI_t4_LOW_Tile_2b</t>
+  </si>
+  <si>
+    <t>PI_t4_LOW_Tile_2c</t>
+  </si>
+  <si>
+    <t>PI_t4_LOW_Tile_3a</t>
+  </si>
+  <si>
+    <t>PI_t4_LOW_Tile_3b</t>
+  </si>
+  <si>
+    <t>PI_t4_LOW_Tile_3c</t>
+  </si>
+  <si>
+    <t>PI_t5_LOW_Tile_1a</t>
+  </si>
+  <si>
+    <t>PI_t5_LOW_Tile_1b</t>
+  </si>
+  <si>
+    <t>PI_t5_LOW_Tile_1c</t>
+  </si>
+  <si>
+    <t>PI_t5_LOW_Tile_2a</t>
+  </si>
+  <si>
+    <t>PI_t5_LOW_Tile_2b</t>
+  </si>
+  <si>
+    <t>PI_t5_LOW_Tile_2c</t>
+  </si>
+  <si>
+    <t>PI_t5_LOW_Tile_3a</t>
+  </si>
+  <si>
+    <t>PI_t5_LOW_Tile_3b</t>
+  </si>
+  <si>
+    <t>PI_t5_LOW_Tile_3c</t>
+  </si>
+  <si>
+    <t>PI_t6_LOW_Tile_1a</t>
+  </si>
+  <si>
+    <t>PI_t6_LOW_Tile_1b</t>
+  </si>
+  <si>
+    <t>PI_t6_LOW_Tile_1c</t>
+  </si>
+  <si>
+    <t>PI_t6_LOW_Tile_2a</t>
+  </si>
+  <si>
+    <t>PI_t6_LOW_Tile_2b</t>
+  </si>
+  <si>
+    <t>PI_t6_LOW_Tile_2c</t>
+  </si>
+  <si>
+    <t>PI_t6_LOW_Tile_3a</t>
+  </si>
+  <si>
+    <t>PI_t6_LOW_Tile_3b</t>
+  </si>
+  <si>
+    <t>PI_t6_LOW_Tile_3c</t>
+  </si>
+  <si>
+    <t>PI_t7_LOW_Tile_1a</t>
+  </si>
+  <si>
+    <t>PI_t7_LOW_Tile_1b</t>
+  </si>
+  <si>
+    <t>PI_t7_LOW_Tile_1c</t>
+  </si>
+  <si>
+    <t>PI_t7_LOW_Tile_2a</t>
+  </si>
+  <si>
+    <t>PI_t7_LOW_Tile_2b</t>
+  </si>
+  <si>
+    <t>PI_t7_LOW_Tile_2c</t>
+  </si>
+  <si>
+    <t>PI_t7_LOW_Tile_3a</t>
+  </si>
+  <si>
+    <t>PI_t7_LOW_Tile_3b</t>
+  </si>
+  <si>
+    <t>PI_t7_LOW_Tile_3c</t>
+  </si>
+  <si>
+    <t>PI_t1_AMB_Tile_1a</t>
+  </si>
+  <si>
+    <t>PI_t1_AMB_Tile_1b</t>
+  </si>
+  <si>
+    <t>PI_t1_AMB_Tile_2a</t>
+  </si>
+  <si>
+    <t>PI_t1_AMB_Tile_2b</t>
+  </si>
+  <si>
+    <t>PI_t1_AMB_Tile_2c</t>
+  </si>
+  <si>
+    <t>PI_t1_AMB_Tile_3a</t>
+  </si>
+  <si>
+    <t>PI_t1_AMB_Tile_3b</t>
+  </si>
+  <si>
+    <t>PI_t1_AMB_Tile_3c</t>
+  </si>
+  <si>
+    <t>PI_t1_AMB_blank_a</t>
+  </si>
+  <si>
+    <t>PI_t1_AMB_blank_b</t>
+  </si>
+  <si>
+    <t>PI_t1_AMB_blank_c</t>
+  </si>
+  <si>
+    <t>PI_t2_AMB_Tile_1a</t>
+  </si>
+  <si>
+    <t>PI_t2_AMB_Tile_1b</t>
+  </si>
+  <si>
+    <t>PI_t2_AMB_Tile_1c</t>
+  </si>
+  <si>
+    <t>PI_t2_AMB_Tile_2a</t>
+  </si>
+  <si>
+    <t>PI_t2_AMB_Tile_2b</t>
+  </si>
+  <si>
+    <t>PI_t2_AMB_Tile_2c</t>
+  </si>
+  <si>
+    <t>PI_t2_AMB_Tile_3a</t>
+  </si>
+  <si>
+    <t>PI_t2_AMB_Tile_3b</t>
+  </si>
+  <si>
+    <t>PI_t2_AMB_Tile_3c</t>
+  </si>
+  <si>
+    <t>PI_t3_AMB_Tile_1a</t>
+  </si>
+  <si>
+    <t>PI_t3_AMB_Tile_1b</t>
+  </si>
+  <si>
+    <t>PI_t3_AMB_Tile_1c</t>
+  </si>
+  <si>
+    <t>PI_t3_AMB_Tile_2a</t>
+  </si>
+  <si>
+    <t>PI_t3_AMB_Tile_2b</t>
+  </si>
+  <si>
+    <t>PI_t3_AMB_Tile_2c</t>
+  </si>
+  <si>
+    <t>PI_t3_AMB_Tile_3a</t>
+  </si>
+  <si>
+    <t>PI_t3_AMB_Tile_3b</t>
+  </si>
+  <si>
+    <t>PI_t3_AMB_Tile_3c</t>
+  </si>
+  <si>
+    <t>PI_t4_AMB_Tile_1a</t>
+  </si>
+  <si>
+    <t>PI_t4_AMB_Tile_1b</t>
+  </si>
+  <si>
+    <t>PI_t4_AMB_Tile_1c</t>
+  </si>
+  <si>
+    <t>PI_t4_AMB_Tile_2a</t>
+  </si>
+  <si>
+    <t>PI_t4_AMB_Tile_2b</t>
+  </si>
+  <si>
+    <t>PI_t4_AMB_Tile_2c</t>
+  </si>
+  <si>
+    <t>PI_t4_AMB_Tile_3a</t>
+  </si>
+  <si>
+    <t>PI_t4_AMB_Tile_3b</t>
+  </si>
+  <si>
+    <t>PI_t4_AMB_Tile_3c</t>
+  </si>
+  <si>
+    <t>PI_t5_AMB_Tile_1a</t>
+  </si>
+  <si>
+    <t>PI_t5_AMB_Tile_1b</t>
+  </si>
+  <si>
+    <t>PI_t5_AMB_Tile_1c</t>
+  </si>
+  <si>
+    <t>PI_t5_AMB_Tile_2a</t>
+  </si>
+  <si>
+    <t>PI_t5_AMB_Tile_2b</t>
+  </si>
+  <si>
+    <t>PI_t5_AMB_Tile_2c</t>
+  </si>
+  <si>
+    <t>PI_t5_AMB_Tile_3a</t>
+  </si>
+  <si>
+    <t>PI_t5_AMB_Tile_3b</t>
+  </si>
+  <si>
+    <t>PI_t5_AMB_Tile_3c</t>
+  </si>
+  <si>
+    <t>PI_t6_AMB_Tile_1a</t>
+  </si>
+  <si>
+    <t>PI_t6_AMB_Tile_1b</t>
+  </si>
+  <si>
+    <t>PI_t6_AMB_Tile_1c</t>
+  </si>
+  <si>
+    <t>PI_t6_AMB_Tile_2a</t>
+  </si>
+  <si>
+    <t>PI_t6_AMB_Tile_2b</t>
+  </si>
+  <si>
+    <t>PI_t6_AMB_Tile_2c</t>
+  </si>
+  <si>
+    <t>PI_t6_AMB_Tile_3a</t>
+  </si>
+  <si>
+    <t>PI_t6_AMB_Tile_3b</t>
+  </si>
+  <si>
+    <t>PI_t6_AMB_Tile_3c</t>
+  </si>
+  <si>
+    <t>PI_t7_AMB_Tile_1a</t>
+  </si>
+  <si>
+    <t>PI_t7_AMB_Tile_1b</t>
+  </si>
+  <si>
+    <t>PI_t7_AMB_Tile_1c</t>
+  </si>
+  <si>
+    <t>PI_t7_AMB_Tile_2a</t>
+  </si>
+  <si>
+    <t>PI_t7_AMB_Tile_2b</t>
+  </si>
+  <si>
+    <t>PI_t7_AMB_Tile_2c</t>
+  </si>
+  <si>
+    <t>PI_t7_AMB_Tile_3a</t>
+  </si>
+  <si>
+    <t>PI_t7_AMB_Tile_3b</t>
+  </si>
+  <si>
+    <t>PI_t7_AMB_Tile_3c</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -830,6 +1400,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -852,7 +1428,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -938,6 +1514,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1221,11 +1800,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L273"/>
+  <dimension ref="A1:L486"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="73" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A254" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N267" sqref="N267"/>
+      <pane ySplit="1" topLeftCell="A245" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D274" sqref="D274"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6783,7 +7362,7 @@
         <v>155</v>
       </c>
       <c r="F221" s="17" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="G221" s="5" t="s">
         <v>155</v>
@@ -6795,7 +7374,7 @@
         <v>155</v>
       </c>
       <c r="L221" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="222" spans="1:12" x14ac:dyDescent="0.2">
@@ -6815,7 +7394,7 @@
         <v>155</v>
       </c>
       <c r="F222" s="17" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="G222" s="1"/>
       <c r="H222" s="1"/>
@@ -6840,7 +7419,7 @@
         <v>155</v>
       </c>
       <c r="F223" s="17" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="G223" s="1"/>
       <c r="H223" s="1"/>
@@ -7361,7 +7940,7 @@
         <v>3171.62</v>
       </c>
       <c r="F245" s="17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G245" s="13">
         <f>AVERAGE(E246,E248)</f>
@@ -7393,7 +7972,7 @@
         <v>2583.4899999999998</v>
       </c>
       <c r="F246" s="17" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="247" spans="1:12" x14ac:dyDescent="0.2">
@@ -7413,7 +7992,7 @@
         <v>2598.48</v>
       </c>
       <c r="F247" s="17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="248" spans="1:12" x14ac:dyDescent="0.2">
@@ -7433,7 +8012,7 @@
         <v>2583.36</v>
       </c>
       <c r="F248" s="17" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="249" spans="1:12" x14ac:dyDescent="0.2">
@@ -7453,7 +8032,7 @@
         <v>2576</v>
       </c>
       <c r="F249" s="17" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G249" s="13">
         <f>AVERAGE(E249:E250)</f>
@@ -7485,7 +8064,7 @@
         <v>2580.83</v>
       </c>
       <c r="F250" s="17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="251" spans="1:12" x14ac:dyDescent="0.2">
@@ -7505,7 +8084,7 @@
         <v>155</v>
       </c>
       <c r="F251" s="17" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="G251" s="5" t="s">
         <v>155</v>
@@ -7517,7 +8096,7 @@
         <v>155</v>
       </c>
       <c r="L251" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="252" spans="1:12" x14ac:dyDescent="0.2">
@@ -7537,7 +8116,7 @@
         <v>155</v>
       </c>
       <c r="F252" s="17" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="G252" s="1"/>
       <c r="H252" s="1"/>
@@ -7562,7 +8141,7 @@
         <v>155</v>
       </c>
       <c r="F253" s="17" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="G253" s="1"/>
       <c r="H253" s="1"/>
@@ -7587,7 +8166,7 @@
         <v>2593.9299999999998</v>
       </c>
       <c r="F254" s="32" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G254" s="13">
         <f>AVERAGE(E254:E255)</f>
@@ -7619,7 +8198,7 @@
         <v>2589.0500000000002</v>
       </c>
       <c r="F255" s="32" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="256" spans="1:12" x14ac:dyDescent="0.2">
@@ -7639,7 +8218,7 @@
         <v>155</v>
       </c>
       <c r="F256" s="17" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="G256" s="5" t="s">
         <v>155</v>
@@ -7654,7 +8233,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="257" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A257" s="9" t="s">
         <v>11</v>
       </c>
@@ -7671,10 +8250,10 @@
         <v>155</v>
       </c>
       <c r="F257" s="17" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="258" spans="1:11" x14ac:dyDescent="0.2">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="258" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A258" s="9" t="s">
         <v>11</v>
       </c>
@@ -7691,14 +8270,14 @@
         <v>155</v>
       </c>
       <c r="F258" s="17" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="259" spans="1:11" x14ac:dyDescent="0.2">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="259" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E259" s="14"/>
       <c r="F259" s="1"/>
     </row>
-    <row r="260" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A260" s="9" t="s">
         <v>11</v>
       </c>
@@ -7708,11 +8287,39 @@
       <c r="C260" s="25" t="s">
         <v>12</v>
       </c>
+      <c r="D260" s="5">
+        <v>49.53</v>
+      </c>
+      <c r="E260" s="5">
+        <v>2239.6799999999998</v>
+      </c>
       <c r="F260" s="16" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="261" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G260" s="13">
+        <f>AVERAGE(E260,E262)</f>
+        <v>2236.9849999999997</v>
+      </c>
+      <c r="H260" s="18">
+        <f>STDEV(E260,E262)</f>
+        <v>3.8113055505954012</v>
+      </c>
+      <c r="I260" s="3">
+        <v>2226.44</v>
+      </c>
+      <c r="J260" s="4">
+        <f>I260-G260</f>
+        <v>-10.544999999999618</v>
+      </c>
+      <c r="K260" s="5">
+        <f>G260+J260</f>
+        <v>2226.44</v>
+      </c>
+      <c r="L260" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="261" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A261" s="9" t="s">
         <v>11</v>
       </c>
@@ -7722,11 +8329,17 @@
       <c r="C261" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D261" s="5">
+        <v>49.91</v>
+      </c>
+      <c r="E261" s="5">
+        <v>2246.6</v>
+      </c>
       <c r="F261" s="16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="262" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A262" s="9" t="s">
         <v>11</v>
       </c>
@@ -7736,11 +8349,17 @@
       <c r="C262" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D262" s="5">
+        <v>50.71</v>
+      </c>
+      <c r="E262" s="5">
+        <v>2234.29</v>
+      </c>
       <c r="F262" s="17" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="263" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A263" s="9" t="s">
         <v>11</v>
       </c>
@@ -7757,7 +8376,7 @@
         <v>2690.49</v>
       </c>
       <c r="F263" s="32" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="G263" s="13">
         <f>AVERAGE(E263:E264)</f>
@@ -7772,7 +8391,7 @@
         <v>2680</v>
       </c>
     </row>
-    <row r="264" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A264" s="9" t="s">
         <v>11</v>
       </c>
@@ -7789,10 +8408,10 @@
         <v>2691.29</v>
       </c>
       <c r="F264" s="32" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="265" spans="1:11" x14ac:dyDescent="0.2">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="265" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A265" s="9" t="s">
         <v>11</v>
       </c>
@@ -7809,7 +8428,7 @@
         <v>2851.54</v>
       </c>
       <c r="F265" s="32" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G265" s="13">
         <f>AVERAGE(E266:E267)</f>
@@ -7824,7 +8443,7 @@
         <v>2823.9250000000002</v>
       </c>
     </row>
-    <row r="266" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A266" s="9" t="s">
         <v>11</v>
       </c>
@@ -7841,10 +8460,10 @@
         <v>2837.88</v>
       </c>
       <c r="F266" s="32" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="267" spans="1:11" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="267" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A267" s="9" t="s">
         <v>11</v>
       </c>
@@ -7861,10 +8480,10 @@
         <v>2831.75</v>
       </c>
       <c r="F267" s="32" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="268" spans="1:11" x14ac:dyDescent="0.2">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="268" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A268" s="9" t="s">
         <v>11</v>
       </c>
@@ -7874,11 +8493,26 @@
       <c r="C268" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D268" s="5">
+        <v>50.99</v>
+      </c>
       <c r="F268" s="32" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="269" spans="1:11" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+      <c r="G268" s="13" t="e">
+        <f>AVERAGE(E269:E270)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H268" s="18" t="e">
+        <f>STDEV(E269:E270)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K268" s="5" t="e">
+        <f>G268+$J$260</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="269" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A269" s="9" t="s">
         <v>11</v>
       </c>
@@ -7888,11 +8522,14 @@
       <c r="C269" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D269" s="5">
+        <v>51.23</v>
+      </c>
       <c r="F269" s="32" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="270" spans="1:11" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="270" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A270" s="9" t="s">
         <v>11</v>
       </c>
@@ -7902,11 +8539,14 @@
       <c r="C270" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D270" s="5">
+        <v>49.15</v>
+      </c>
       <c r="F270" s="32" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="271" spans="1:11" x14ac:dyDescent="0.2">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="271" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A271" s="9" t="s">
         <v>11</v>
       </c>
@@ -7916,11 +8556,26 @@
       <c r="C271" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D271" s="5">
+        <v>49.81</v>
+      </c>
       <c r="F271" s="32" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="272" spans="1:11" x14ac:dyDescent="0.2">
+        <v>225</v>
+      </c>
+      <c r="G271" s="13" t="e">
+        <f>AVERAGE(E272:E273)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H271" s="18" t="e">
+        <f>STDEV(E272:E273)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K271" s="5" t="e">
+        <f>G271+$J$260</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="272" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A272" s="9" t="s">
         <v>11</v>
       </c>
@@ -7930,11 +8585,14 @@
       <c r="C272" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D272" s="5">
+        <v>48.54</v>
+      </c>
       <c r="F272" s="32" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.2">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="273" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A273" s="9" t="s">
         <v>11</v>
       </c>
@@ -7944,8 +8602,1411 @@
       <c r="C273" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D273" s="5">
+        <v>49.29</v>
+      </c>
       <c r="F273" s="32" t="s">
-        <v>230</v>
+        <v>227</v>
+      </c>
+    </row>
+    <row r="274" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A274" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B274" s="31">
+        <v>45081</v>
+      </c>
+      <c r="C274" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F274" s="32" t="s">
+        <v>235</v>
+      </c>
+      <c r="G274" s="13" t="e">
+        <f>AVERAGE(E275:E276)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H274" s="18" t="e">
+        <f>STDEV(E275:E276)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K274" s="5" t="e">
+        <f>G274+$J$260</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="275" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A275" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B275" s="31">
+        <v>45081</v>
+      </c>
+      <c r="C275" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F275" s="32" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="276" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A276" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B276" s="31">
+        <v>45081</v>
+      </c>
+      <c r="C276" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F276" s="32" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="277" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A277" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B277" s="31">
+        <v>45081</v>
+      </c>
+      <c r="C277" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F277" s="32" t="s">
+        <v>237</v>
+      </c>
+      <c r="G277" s="13" t="e">
+        <f>AVERAGE(E278:E279)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H277" s="18" t="e">
+        <f>STDEV(E278:E279)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K277" s="5" t="e">
+        <f>G277+$J$260</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="278" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A278" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B278" s="31">
+        <v>45081</v>
+      </c>
+      <c r="C278" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F278" s="32" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="279" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A279" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B279" s="31">
+        <v>45081</v>
+      </c>
+      <c r="C279" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F279" s="32" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="280" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A280" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B280" s="31">
+        <v>45081</v>
+      </c>
+      <c r="C280" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F280" s="32" t="s">
+        <v>240</v>
+      </c>
+      <c r="G280" s="13" t="e">
+        <f>AVERAGE(E281:E282)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H280" s="18" t="e">
+        <f>STDEV(E281:E282)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K280" s="5" t="e">
+        <f>G280+$J$260</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="281" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A281" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B281" s="31">
+        <v>45081</v>
+      </c>
+      <c r="C281" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F281" s="32" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="282" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A282" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B282" s="31">
+        <v>45081</v>
+      </c>
+      <c r="C282" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F282" s="32" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="283" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A283" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B283" s="31">
+        <v>45081</v>
+      </c>
+      <c r="C283" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F283" s="32" t="s">
+        <v>243</v>
+      </c>
+      <c r="G283" s="13" t="e">
+        <f>AVERAGE(E284:E285)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H283" s="18" t="e">
+        <f>STDEV(E284:E285)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K283" s="5" t="e">
+        <f>G283+$J$260</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="284" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A284" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B284" s="31">
+        <v>45081</v>
+      </c>
+      <c r="C284" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F284" s="32" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="285" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A285" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B285" s="31">
+        <v>45081</v>
+      </c>
+      <c r="C285" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F285" s="32" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="286" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A286" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B286" s="31">
+        <v>45081</v>
+      </c>
+      <c r="C286" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F286" s="32" t="s">
+        <v>245</v>
+      </c>
+      <c r="G286" s="13" t="e">
+        <f>AVERAGE(E287:E288)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H286" s="18" t="e">
+        <f>STDEV(E287:E288)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K286" s="5" t="e">
+        <f>G286+$J$260</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="287" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A287" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B287" s="31">
+        <v>45081</v>
+      </c>
+      <c r="C287" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F287" s="32" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="288" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A288" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B288" s="31">
+        <v>45081</v>
+      </c>
+      <c r="C288" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F288" s="32" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="289" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A289" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B289" s="31">
+        <v>45081</v>
+      </c>
+      <c r="C289" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F289" s="32" t="s">
+        <v>248</v>
+      </c>
+      <c r="G289" s="13" t="e">
+        <f>AVERAGE(E290:E291)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H289" s="18" t="e">
+        <f>STDEV(E290:E291)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K289" s="5" t="e">
+        <f>G289+$J$260</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="290" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A290" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B290" s="31">
+        <v>45081</v>
+      </c>
+      <c r="C290" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F290" s="32" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="291" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A291" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B291" s="31">
+        <v>45081</v>
+      </c>
+      <c r="C291" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F291" s="32" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="292" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A292" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B292" s="31">
+        <v>45081</v>
+      </c>
+      <c r="C292" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F292" s="32" t="s">
+        <v>251</v>
+      </c>
+      <c r="G292" s="13" t="e">
+        <f>AVERAGE(E293:E294)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H292" s="18" t="e">
+        <f>STDEV(E293:E294)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K292" s="5" t="e">
+        <f>G292+$J$260</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="293" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A293" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B293" s="31">
+        <v>45081</v>
+      </c>
+      <c r="C293" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F293" s="32" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="294" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A294" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B294" s="31">
+        <v>45081</v>
+      </c>
+      <c r="C294" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F294" s="33" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="295" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A295" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B295" s="31">
+        <v>45081</v>
+      </c>
+      <c r="C295" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F295" s="32" t="s">
+        <v>253</v>
+      </c>
+      <c r="G295" s="13" t="e">
+        <f>AVERAGE(E296:E297)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H295" s="18" t="e">
+        <f>STDEV(E296:E297)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K295" s="5" t="e">
+        <f>G295+$J$260</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="296" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A296" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B296" s="31">
+        <v>45081</v>
+      </c>
+      <c r="C296" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F296" s="32" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="297" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A297" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B297" s="31">
+        <v>45081</v>
+      </c>
+      <c r="C297" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F297" s="32" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="298" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A298" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B298" s="31">
+        <v>45081</v>
+      </c>
+      <c r="C298" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F298" s="32" t="s">
+        <v>256</v>
+      </c>
+      <c r="G298" s="13" t="e">
+        <f>AVERAGE(E299:E300)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H298" s="18" t="e">
+        <f>STDEV(E299:E300)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K298" s="5" t="e">
+        <f>G298+$J$260</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="299" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A299" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B299" s="31">
+        <v>45081</v>
+      </c>
+      <c r="C299" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F299" s="32" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="300" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A300" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B300" s="31">
+        <v>45081</v>
+      </c>
+      <c r="C300" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F300" s="32" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="301" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F301" s="32"/>
+    </row>
+    <row r="302" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F302" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="303" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F303" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="304" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F304" s="17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="305" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F305" s="32" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="306" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F306" s="32" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="307" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F307" s="32" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="308" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F308" s="32" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="309" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F309" s="32" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="310" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F310" s="32" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="311" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F311" s="32" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="312" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F312" s="32" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="313" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F313" s="32" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="314" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F314" s="32" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="315" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F315" s="32" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="316" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F316" s="32" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="317" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F317" s="32" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="318" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F318" s="32" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="319" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F319" s="32" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="320" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F320" s="32" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="321" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F321" s="32" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="322" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F322" s="32" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="323" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F323" s="32" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="324" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F324" s="32" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="325" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F325" s="32" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="326" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F326" s="32" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="327" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F327" s="32" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="328" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F328" s="32" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="329" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F329" s="32" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="330" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F330" s="32" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="331" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F331" s="32" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="332" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F332" s="32" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="333" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F333" s="32" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="334" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F334" s="32" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="335" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F335" s="32" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="336" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F336" s="32" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="337" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F337" s="32" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="338" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F338" s="32" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="339" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F339" s="32" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="340" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F340" s="32" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="342" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F342" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="343" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F343" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="344" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F344" s="17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="345" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F345" s="32" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="346" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F346" s="32" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="347" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F347" s="32" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="348" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F348" s="32" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="349" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F349" s="32" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="350" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F350" s="32" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="351" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F351" s="32" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="352" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F352" s="32" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="353" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F353" s="32" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="354" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F354" s="32" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="355" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F355" s="32" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="356" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F356" s="32" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="357" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F357" s="32" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="358" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F358" s="32" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="359" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F359" s="32" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="360" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F360" s="32" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="361" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F361" s="32" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="362" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F362" s="32" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="363" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F363" s="32" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="364" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F364" s="32" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="365" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F365" s="32" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="366" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F366" s="32" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="367" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F367" s="32" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="368" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F368" s="32" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="369" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F369" s="32" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="370" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F370" s="32" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="371" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F371" s="32" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="372" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F372" s="32" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="373" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F373" s="32" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="374" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F374" s="32" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="375" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F375" s="32" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="376" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F376" s="33" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="377" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F377" s="32" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="378" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F378" s="32" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="379" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F379" s="32" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="380" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F380" s="32" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="381" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F381" s="32" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="382" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F382" s="32" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="383" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F383" s="32"/>
+    </row>
+    <row r="384" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F384" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="385" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F385" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="386" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F386" s="17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="387" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F387" s="32" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="388" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F388" s="32" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="389" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F389" s="32" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="390" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F390" s="32" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="391" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F391" s="32" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="392" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F392" s="32" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="393" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F393" s="32" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="394" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F394" s="32" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="395" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F395" s="32" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="396" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F396" s="32" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="397" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F397" s="32" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="398" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F398" s="32" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="399" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F399" s="32" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="400" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F400" s="32" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="401" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F401" s="32" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="402" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F402" s="32" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="403" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F403" s="32" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="404" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F404" s="32" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="405" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F405" s="32" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="406" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F406" s="32" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="407" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F407" s="32" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="408" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F408" s="32" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="409" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F409" s="32" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="410" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F410" s="32" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="411" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F411" s="32" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="412" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F412" s="32" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="413" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F413" s="32" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="415" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F415" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="416" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F416" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="417" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F417" s="17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="418" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F418" s="32" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="419" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F419" s="32" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="420" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F420" s="32" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="421" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F421" s="32" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="422" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F422" s="32" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="423" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F423" s="32" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="424" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F424" s="32" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="425" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F425" s="32" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="426" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F426" s="32" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="427" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F427" s="32" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="428" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F428" s="32" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="429" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F429" s="32" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="430" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F430" s="32" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="431" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F431" s="32" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="432" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F432" s="32" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="433" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F433" s="32" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="434" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F434" s="32" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="435" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F435" s="32" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="436" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F436" s="32" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="437" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F437" s="32" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="438" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F438" s="32" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="439" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F439" s="32" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="440" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F440" s="32" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="441" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F441" s="32" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="442" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F442" s="32" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="443" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F443" s="32" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="444" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F444" s="32" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="445" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F445" s="32" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="446" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F446" s="32" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="447" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F447" s="32" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="448" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F448" s="32" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="449" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F449" s="33" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="450" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F450" s="32" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="451" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F451" s="32" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="452" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F452" s="32" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="453" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F453" s="32" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="454" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F454" s="32" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="455" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F455" s="32" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="456" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F456" s="32"/>
+    </row>
+    <row r="457" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F457" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="458" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F458" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="459" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F459" s="17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="460" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F460" s="32" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="461" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F461" s="32" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="462" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F462" s="32" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="463" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F463" s="32" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="464" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F464" s="32" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="465" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F465" s="32" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="466" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F466" s="32" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="467" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F467" s="32" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="468" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F468" s="32" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="469" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F469" s="32" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="470" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F470" s="32" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="471" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F471" s="32" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="472" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F472" s="32" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="473" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F473" s="32" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="474" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F474" s="32" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="475" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F475" s="32" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="476" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F476" s="32" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="477" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F477" s="32" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="478" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F478" s="32" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="479" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F479" s="32" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="480" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F480" s="32" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="481" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F481" s="32" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="482" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F482" s="32" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="483" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F483" s="32" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="484" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F484" s="32" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="485" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F485" s="32" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="486" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F486" s="32" t="s">
+        <v>427</v>
       </c>
     </row>
   </sheetData>
@@ -7957,103 +10018,398 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5D882B6-30B5-6742-81C6-39D5A67D008A}">
-  <dimension ref="A1:A18"/>
+  <dimension ref="A1:A81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A18"/>
+    <sheetView topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="A72" sqref="A1:A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
-        <v>201</v>
+      <c r="A1" s="16" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
-        <v>202</v>
+      <c r="A2" s="16" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>203</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
-        <v>204</v>
+      <c r="A4" s="32" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="17" t="s">
-        <v>205</v>
+      <c r="A5" s="32" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
-        <v>206</v>
+      <c r="A6" s="32" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="17" t="s">
-        <v>207</v>
+      <c r="A7" s="32" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="17" t="s">
-        <v>208</v>
+      <c r="A8" s="32" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="17" t="s">
-        <v>209</v>
+      <c r="A9" s="32" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="17" t="s">
-        <v>210</v>
+      <c r="A10" s="32" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="17" t="s">
-        <v>211</v>
+      <c r="A11" s="32" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="17" t="s">
-        <v>212</v>
+      <c r="A12" s="32" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="32" t="s">
-        <v>213</v>
+        <v>372</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="32" t="s">
-        <v>214</v>
+        <v>373</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" s="32" t="s">
-        <v>215</v>
+        <v>374</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="17" t="s">
-        <v>216</v>
+      <c r="A16" s="32" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="17" t="s">
-        <v>217</v>
+      <c r="A17" s="32" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="17" t="s">
-        <v>218</v>
-      </c>
+      <c r="A18" s="32" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="32" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="32" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="32" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="32" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="32" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="32" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="32" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="32" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="32" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="32" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="32" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="32" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="32" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="32" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="32" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="32" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="33" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="32" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="32" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="32" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="32" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="32" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="32" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" s="32"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" s="17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" s="32" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" s="32" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" s="32" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="32" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="32" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" s="32" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" s="32" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" s="32" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" s="32" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" s="32" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" s="32" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" s="32" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" s="32" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" s="32" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" s="32" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" s="32" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" s="32" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" s="32" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" s="32" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" s="32" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" s="32" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" s="32" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" s="32" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" s="32" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" s="32" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" s="32" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" s="32" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" s="32"/>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" s="32"/>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" s="32"/>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" s="32"/>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" s="32"/>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" s="32"/>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" s="32"/>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" s="32"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ALK ELOW 1st part
</commit_message>
<xml_diff>
--- a/Data/Spring_2023/BenthFun_Alkalinity.xlsx
+++ b/Data/Spring_2023/BenthFun_Alkalinity.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremy/Library/Mobile Documents/com~apple~CloudDocs/Documents/Documents/Post-Doc/Projets/Villefranche/Projets/BenthFun – Jeremy/BenthFun/Data/Spring_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C04F3CD3-41F7-9E4C-AA76-99F0124165FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EDC1610-CEC2-9C46-A450-DE7E2154CCAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1305" uniqueCount="425">
   <si>
     <t>Operator</t>
   </si>
@@ -752,15 +754,9 @@
     <t>PI_t2_ELOW_Tile_2b</t>
   </si>
   <si>
-    <t>PI_t2_ELOW_Tile_2c</t>
-  </si>
-  <si>
     <t>PI_t2_ELOW_Tile_3a</t>
   </si>
   <si>
-    <t>PI_t2_ELOW_Tile_3b</t>
-  </si>
-  <si>
     <t>PI_t2_ELOW_Tile_3c</t>
   </si>
   <si>
@@ -776,9 +772,6 @@
     <t>PI_t3_ELOW_Tile_2b</t>
   </si>
   <si>
-    <t>PI_t3_ELOW_Tile_2c</t>
-  </si>
-  <si>
     <t>PI_t3_ELOW_Tile_3a</t>
   </si>
   <si>
@@ -839,9 +832,6 @@
     <t>PI_t2_ELOW_Tile_1c</t>
   </si>
   <si>
-    <t>PI_t3_ELOW_Tile_1c</t>
-  </si>
-  <si>
     <t>PI_t4_ELOW_Tile_1c</t>
   </si>
   <si>
@@ -1317,6 +1307,9 @@
   </si>
   <si>
     <t>PI_t7_AMB_Tile_3c</t>
+  </si>
+  <si>
+    <t>PI_t2_ELOW_Tile_3e</t>
   </si>
 </sst>
 </file>
@@ -1428,7 +1421,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1518,6 +1511,9 @@
     </xf>
     <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1800,11 +1796,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L486"/>
+  <dimension ref="A1:L523"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="73" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A245" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D274" sqref="D274"/>
+      <pane ySplit="1" topLeftCell="A259" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E277" sqref="E277"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8211,8 +8207,8 @@
       <c r="C256" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D256" s="5">
-        <v>50.57</v>
+      <c r="D256" s="5" t="s">
+        <v>155</v>
       </c>
       <c r="E256" s="5" t="s">
         <v>155</v>
@@ -8243,8 +8239,8 @@
       <c r="C257" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D257" s="5">
-        <v>50.9</v>
+      <c r="D257" s="5" t="s">
+        <v>155</v>
       </c>
       <c r="E257" s="5" t="s">
         <v>155</v>
@@ -8263,8 +8259,8 @@
       <c r="C258" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D258" s="5">
-        <v>50.92</v>
+      <c r="D258" s="5" t="s">
+        <v>155</v>
       </c>
       <c r="E258" s="5" t="s">
         <v>155</v>
@@ -8332,7 +8328,7 @@
       <c r="D261" s="5">
         <v>49.91</v>
       </c>
-      <c r="E261" s="5">
+      <c r="E261" s="14">
         <v>2246.6</v>
       </c>
       <c r="F261" s="16" t="s">
@@ -8496,20 +8492,23 @@
       <c r="D268" s="5">
         <v>50.99</v>
       </c>
+      <c r="E268" s="14">
+        <v>2690.59</v>
+      </c>
       <c r="F268" s="32" t="s">
         <v>222</v>
       </c>
-      <c r="G268" s="13" t="e">
+      <c r="G268" s="13">
         <f>AVERAGE(E269:E270)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H268" s="18" t="e">
+        <v>2704.4399999999996</v>
+      </c>
+      <c r="H268" s="18">
         <f>STDEV(E269:E270)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K268" s="5" t="e">
+        <v>2.842569260369908</v>
+      </c>
+      <c r="K268" s="5">
         <f>G268+$J$260</f>
-        <v>#DIV/0!</v>
+        <v>2693.895</v>
       </c>
     </row>
     <row r="269" spans="1:12" x14ac:dyDescent="0.2">
@@ -8525,6 +8524,9 @@
       <c r="D269" s="5">
         <v>51.23</v>
       </c>
+      <c r="E269" s="5">
+        <v>2702.43</v>
+      </c>
       <c r="F269" s="32" t="s">
         <v>223</v>
       </c>
@@ -8542,6 +8544,9 @@
       <c r="D270" s="5">
         <v>49.15</v>
       </c>
+      <c r="E270" s="5">
+        <v>2706.45</v>
+      </c>
       <c r="F270" s="32" t="s">
         <v>224</v>
       </c>
@@ -8559,20 +8564,23 @@
       <c r="D271" s="5">
         <v>49.81</v>
       </c>
+      <c r="E271" s="5">
+        <v>2605.6</v>
+      </c>
       <c r="F271" s="32" t="s">
         <v>225</v>
       </c>
-      <c r="G271" s="13" t="e">
-        <f>AVERAGE(E272:E273)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H271" s="18" t="e">
-        <f>STDEV(E272:E273)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K271" s="5" t="e">
+      <c r="G271" s="13">
+        <f>AVERAGE(E271,E273)</f>
+        <v>2603.0149999999999</v>
+      </c>
+      <c r="H271" s="18">
+        <f>STDEV(E271,E273)</f>
+        <v>3.6557420587345022</v>
+      </c>
+      <c r="K271" s="5">
         <f>G271+$J$260</f>
-        <v>#DIV/0!</v>
+        <v>2592.4700000000003</v>
       </c>
     </row>
     <row r="272" spans="1:12" x14ac:dyDescent="0.2">
@@ -8588,11 +8596,14 @@
       <c r="D272" s="5">
         <v>48.54</v>
       </c>
+      <c r="E272" s="14">
+        <v>2623.87</v>
+      </c>
       <c r="F272" s="32" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="273" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A273" s="9" t="s">
         <v>11</v>
       </c>
@@ -8605,235 +8616,331 @@
       <c r="D273" s="5">
         <v>49.29</v>
       </c>
+      <c r="E273" s="5">
+        <v>2600.4299999999998</v>
+      </c>
       <c r="F273" s="32" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="274" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A274" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B274" s="31">
-        <v>45081</v>
+        <v>45080</v>
       </c>
       <c r="C274" s="10" t="s">
         <v>12</v>
+      </c>
+      <c r="D274" s="5">
+        <v>51.84</v>
+      </c>
+      <c r="E274" s="14">
+        <v>3045.93</v>
       </c>
       <c r="F274" s="32" t="s">
         <v>235</v>
       </c>
-      <c r="G274" s="13" t="e">
+      <c r="G274" s="13">
         <f>AVERAGE(E275:E276)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H274" s="18" t="e">
+        <v>2970.4549999999999</v>
+      </c>
+      <c r="H274" s="18">
         <f>STDEV(E275:E276)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K274" s="5" t="e">
+        <v>2.3122391744799975</v>
+      </c>
+      <c r="K274" s="5">
         <f>G274+$J$260</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="275" spans="1:11" x14ac:dyDescent="0.2">
+        <v>2959.9100000000003</v>
+      </c>
+    </row>
+    <row r="275" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A275" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B275" s="31">
-        <v>45081</v>
+        <v>45080</v>
       </c>
       <c r="C275" s="10" t="s">
         <v>12</v>
+      </c>
+      <c r="D275" s="5">
+        <v>49.31</v>
+      </c>
+      <c r="E275" s="5">
+        <v>2972.09</v>
       </c>
       <c r="F275" s="32" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="276" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A276" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B276" s="31">
-        <v>45081</v>
+        <v>45080</v>
       </c>
       <c r="C276" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D276" s="5">
+        <v>49.67</v>
+      </c>
+      <c r="E276" s="5">
+        <v>2968.82</v>
+      </c>
       <c r="F276" s="32" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="277" spans="1:11" x14ac:dyDescent="0.2">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="277" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A277" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B277" s="31">
-        <v>45081</v>
+        <v>45080</v>
       </c>
       <c r="C277" s="10" t="s">
         <v>12</v>
+      </c>
+      <c r="D277" s="5">
+        <v>48.84</v>
+      </c>
+      <c r="E277" s="5">
+        <v>2879.28</v>
       </c>
       <c r="F277" s="32" t="s">
         <v>237</v>
       </c>
-      <c r="G277" s="13" t="e">
-        <f>AVERAGE(E278:E279)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H277" s="18" t="e">
-        <f>STDEV(E278:E279)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K277" s="5" t="e">
+      <c r="G277" s="13">
+        <f>AVERAGE(E277:E278)</f>
+        <v>2880.085</v>
+      </c>
+      <c r="H277" s="18">
+        <f>STDEV(E277:E278)</f>
+        <v>1.1384419177101099</v>
+      </c>
+      <c r="K277" s="5">
         <f>G277+$J$260</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="278" spans="1:11" x14ac:dyDescent="0.2">
+        <v>2869.5400000000004</v>
+      </c>
+    </row>
+    <row r="278" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A278" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B278" s="31">
-        <v>45081</v>
+        <v>45080</v>
       </c>
       <c r="C278" s="10" t="s">
         <v>12</v>
+      </c>
+      <c r="D278" s="5">
+        <v>49.22</v>
+      </c>
+      <c r="E278" s="5">
+        <v>2880.89</v>
       </c>
       <c r="F278" s="32" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="279" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A279" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B279" s="31">
-        <v>45081</v>
+        <v>45080</v>
       </c>
       <c r="C279" s="10" t="s">
         <v>12</v>
+      </c>
+      <c r="D279" s="5">
+        <v>49.01</v>
+      </c>
+      <c r="E279" s="14">
+        <v>2725.15</v>
       </c>
       <c r="F279" s="32" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="280" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G279" s="34">
+        <f>AVERAGE(E280,E281)</f>
+        <v>2886.1800000000003</v>
+      </c>
+      <c r="H279" s="34">
+        <f>STDEV(E280,E281)</f>
+        <v>14.806815998046345</v>
+      </c>
+      <c r="K279" s="5">
+        <f>G279+$J$260</f>
+        <v>2875.6350000000007</v>
+      </c>
+      <c r="L279" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="280" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A280" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B280" s="31">
-        <v>45081</v>
+        <v>45080</v>
       </c>
       <c r="C280" s="10" t="s">
         <v>12</v>
+      </c>
+      <c r="D280" s="5">
+        <v>50.67</v>
+      </c>
+      <c r="E280" s="5">
+        <v>2875.71</v>
       </c>
       <c r="F280" s="32" t="s">
         <v>240</v>
       </c>
-      <c r="G280" s="13" t="e">
-        <f>AVERAGE(E281:E282)</f>
+    </row>
+    <row r="281" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A281" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B281" s="31">
+        <v>45080</v>
+      </c>
+      <c r="C281" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D281" s="5">
+        <v>49.95</v>
+      </c>
+      <c r="E281" s="5">
+        <v>2896.65</v>
+      </c>
+      <c r="F281" s="32" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="282" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A282" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B282" s="31">
+        <v>45080</v>
+      </c>
+      <c r="C282" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D282" s="5">
+        <v>49.71</v>
+      </c>
+      <c r="E282" s="5">
+        <v>2879.81</v>
+      </c>
+      <c r="F282" s="32" t="s">
+        <v>241</v>
+      </c>
+      <c r="G282" s="13">
+        <f>AVERAGE(E282:E283)</f>
+        <v>2877.66</v>
+      </c>
+      <c r="H282" s="18">
+        <f>STDEV(E282:E283)</f>
+        <v>3.0405591591019614</v>
+      </c>
+      <c r="K282" s="5">
+        <f>G282+$J$260</f>
+        <v>2867.1150000000002</v>
+      </c>
+    </row>
+    <row r="283" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A283" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B283" s="31">
+        <v>45080</v>
+      </c>
+      <c r="C283" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D283" s="5">
+        <v>49.14</v>
+      </c>
+      <c r="E283" s="5">
+        <v>2875.51</v>
+      </c>
+      <c r="F283" s="32" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="284" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A284" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B284" s="31">
+        <v>45080</v>
+      </c>
+      <c r="C284" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D284" s="5">
+        <v>50.9</v>
+      </c>
+      <c r="E284" s="5">
+        <v>2876.26</v>
+      </c>
+      <c r="F284" s="32" t="s">
+        <v>243</v>
+      </c>
+      <c r="G284" s="13">
+        <f>AVERAGE(E285:E285)</f>
+        <v>2876.68</v>
+      </c>
+      <c r="H284" s="18" t="e">
+        <f>STDEV(E285:E285)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H280" s="18" t="e">
-        <f>STDEV(E281:E282)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K280" s="5" t="e">
-        <f>G280+$J$260</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="281" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A281" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B281" s="31">
-        <v>45081</v>
-      </c>
-      <c r="C281" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F281" s="32" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="282" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A282" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B282" s="31">
-        <v>45081</v>
-      </c>
-      <c r="C282" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F282" s="32" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="283" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A283" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B283" s="31">
-        <v>45081</v>
-      </c>
-      <c r="C283" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F283" s="32" t="s">
-        <v>243</v>
-      </c>
-      <c r="G283" s="13" t="e">
-        <f>AVERAGE(E284:E285)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H283" s="18" t="e">
-        <f>STDEV(E284:E285)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K283" s="5" t="e">
-        <f>G283+$J$260</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="284" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A284" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B284" s="31">
-        <v>45081</v>
-      </c>
-      <c r="C284" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F284" s="32" t="s">
+      <c r="K284" s="5">
+        <f>G284+$J$260</f>
+        <v>2866.1350000000002</v>
+      </c>
+    </row>
+    <row r="285" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A285" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B285" s="31">
+        <v>45080</v>
+      </c>
+      <c r="C285" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D285" s="5">
+        <v>49.12</v>
+      </c>
+      <c r="E285" s="5">
+        <v>2876.68</v>
+      </c>
+      <c r="F285" s="32" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="285" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A285" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B285" s="31">
-        <v>45081</v>
-      </c>
-      <c r="C285" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F285" s="32" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="286" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A286" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B286" s="31">
-        <v>45081</v>
+        <v>45080</v>
       </c>
       <c r="C286" s="10" t="s">
         <v>12</v>
+      </c>
+      <c r="D286" s="5">
+        <v>50.67</v>
+      </c>
+      <c r="E286" s="5">
+        <v>2687.18</v>
       </c>
       <c r="F286" s="32" t="s">
         <v>245</v>
@@ -8851,29 +8958,35 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="287" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A287" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B287" s="31">
-        <v>45081</v>
+        <v>45080</v>
       </c>
       <c r="C287" s="10" t="s">
         <v>12</v>
+      </c>
+      <c r="D287" s="5">
+        <v>51.89</v>
       </c>
       <c r="F287" s="32" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="288" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A288" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B288" s="31">
-        <v>45081</v>
+        <v>45080</v>
       </c>
       <c r="C288" s="10" t="s">
         <v>12</v>
+      </c>
+      <c r="D288" s="5">
+        <v>49.27</v>
       </c>
       <c r="F288" s="32" t="s">
         <v>247</v>
@@ -8884,10 +8997,13 @@
         <v>11</v>
       </c>
       <c r="B289" s="31">
-        <v>45081</v>
+        <v>45080</v>
       </c>
       <c r="C289" s="10" t="s">
         <v>12</v>
+      </c>
+      <c r="D289" s="5">
+        <v>48.93</v>
       </c>
       <c r="F289" s="32" t="s">
         <v>248</v>
@@ -8910,10 +9026,13 @@
         <v>11</v>
       </c>
       <c r="B290" s="31">
-        <v>45081</v>
+        <v>45080</v>
       </c>
       <c r="C290" s="10" t="s">
         <v>12</v>
+      </c>
+      <c r="D290" s="5">
+        <v>49.89</v>
       </c>
       <c r="F290" s="32" t="s">
         <v>249</v>
@@ -8924,13 +9043,16 @@
         <v>11</v>
       </c>
       <c r="B291" s="31">
-        <v>45081</v>
+        <v>45080</v>
       </c>
       <c r="C291" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F291" s="32" t="s">
-        <v>250</v>
+      <c r="D291" s="5">
+        <v>50.5</v>
+      </c>
+      <c r="F291" s="33" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="292" spans="1:11" x14ac:dyDescent="0.2">
@@ -8938,13 +9060,16 @@
         <v>11</v>
       </c>
       <c r="B292" s="31">
-        <v>45081</v>
+        <v>45080</v>
       </c>
       <c r="C292" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D292" s="5">
+        <v>48.54</v>
+      </c>
       <c r="F292" s="32" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G292" s="13" t="e">
         <f>AVERAGE(E293:E294)</f>
@@ -8964,13 +9089,16 @@
         <v>11</v>
       </c>
       <c r="B293" s="31">
-        <v>45081</v>
+        <v>45080</v>
       </c>
       <c r="C293" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D293" s="5">
+        <v>49.74</v>
+      </c>
       <c r="F293" s="32" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="294" spans="1:11" x14ac:dyDescent="0.2">
@@ -8978,13 +9106,16 @@
         <v>11</v>
       </c>
       <c r="B294" s="31">
-        <v>45081</v>
+        <v>45080</v>
       </c>
       <c r="C294" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F294" s="33" t="s">
-        <v>269</v>
+      <c r="D294" s="5">
+        <v>51.38</v>
+      </c>
+      <c r="F294" s="32" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="295" spans="1:11" x14ac:dyDescent="0.2">
@@ -8992,7 +9123,7 @@
         <v>11</v>
       </c>
       <c r="B295" s="31">
-        <v>45081</v>
+        <v>45080</v>
       </c>
       <c r="C295" s="10" t="s">
         <v>12</v>
@@ -9018,7 +9149,7 @@
         <v>11</v>
       </c>
       <c r="B296" s="31">
-        <v>45081</v>
+        <v>45080</v>
       </c>
       <c r="C296" s="10" t="s">
         <v>12</v>
@@ -9032,7 +9163,7 @@
         <v>11</v>
       </c>
       <c r="B297" s="31">
-        <v>45081</v>
+        <v>45080</v>
       </c>
       <c r="C297" s="10" t="s">
         <v>12</v>
@@ -9042,1376 +9173,1589 @@
       </c>
     </row>
     <row r="298" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A298" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B298" s="31">
-        <v>45081</v>
-      </c>
-      <c r="C298" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F298" s="32" t="s">
+      <c r="F298" s="32"/>
+    </row>
+    <row r="299" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C299" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F299" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="300" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C300" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F300" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="301" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C301" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F301" s="17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="302" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C302" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F302" s="32" t="s">
         <v>256</v>
       </c>
-      <c r="G298" s="13" t="e">
-        <f>AVERAGE(E299:E300)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H298" s="18" t="e">
-        <f>STDEV(E299:E300)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K298" s="5" t="e">
-        <f>G298+$J$260</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="299" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A299" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B299" s="31">
-        <v>45081</v>
-      </c>
-      <c r="C299" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F299" s="32" t="s">
+    </row>
+    <row r="303" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C303" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F303" s="32" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="300" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A300" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B300" s="31">
-        <v>45081</v>
-      </c>
-      <c r="C300" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F300" s="32" t="s">
+    <row r="304" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C304" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F304" s="32" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="305" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C305" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F305" s="32" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="301" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F301" s="32"/>
-    </row>
-    <row r="302" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F302" s="16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="303" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F303" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="304" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F304" s="17" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="305" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F305" s="32" t="s">
+    <row r="306" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C306" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F306" s="32" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="306" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F306" s="32" t="s">
+    <row r="307" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C307" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F307" s="32" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="307" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F307" s="32" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="308" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="308" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C308" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="F308" s="32" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="309" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="309" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C309" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="F309" s="32" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="310" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="310" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C310" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="F310" s="32" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="311" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="311" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C311" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="F311" s="32" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="312" spans="6:6" x14ac:dyDescent="0.2">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="312" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C312" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="F312" s="32" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="313" spans="6:6" x14ac:dyDescent="0.2">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="313" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C313" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="F313" s="32" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="314" spans="6:6" x14ac:dyDescent="0.2">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="314" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C314" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="F314" s="32" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="315" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C315" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F315" s="32" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="315" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F315" s="32" t="s">
+    <row r="316" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C316" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F316" s="32" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="316" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F316" s="32" t="s">
+    <row r="317" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C317" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F317" s="32" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="317" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F317" s="32" t="s">
+    <row r="318" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C318" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F318" s="32" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="318" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F318" s="32" t="s">
+    <row r="319" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C319" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F319" s="32" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="319" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F319" s="32" t="s">
+    <row r="320" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C320" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F320" s="32" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="320" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F320" s="32" t="s">
+    <row r="321" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C321" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F321" s="32" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="321" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F321" s="32" t="s">
+    <row r="322" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C322" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F322" s="32" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="322" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F322" s="32" t="s">
+    <row r="323" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C323" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F323" s="32" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="323" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F323" s="32" t="s">
+    <row r="324" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C324" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F324" s="32" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="324" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F324" s="32" t="s">
+    <row r="325" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C325" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F325" s="32" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="325" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F325" s="32" t="s">
+    <row r="326" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C326" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F326" s="32" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="326" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F326" s="32" t="s">
+    <row r="327" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C327" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F327" s="32" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="327" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F327" s="32" t="s">
+    <row r="328" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C328" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F328" s="32" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="328" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F328" s="32" t="s">
+    <row r="329" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C329" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F329" s="32" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="329" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F329" s="32" t="s">
+    <row r="330" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C330" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F330" s="32" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="330" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F330" s="32" t="s">
+    <row r="331" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C331" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F331" s="32" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="331" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F331" s="32" t="s">
+    <row r="332" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C332" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F332" s="32" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="332" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F332" s="32" t="s">
+    <row r="333" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C333" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F333" s="32" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="333" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F333" s="32" t="s">
+    <row r="334" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C334" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F334" s="32" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="334" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F334" s="32" t="s">
+    <row r="335" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C335" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F335" s="32" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="335" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F335" s="32" t="s">
+    <row r="336" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C336" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F336" s="32" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="336" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F336" s="32" t="s">
+    <row r="337" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C337" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F337" s="32" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="337" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F337" s="32" t="s">
+    <row r="338" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C338" s="10"/>
+    </row>
+    <row r="339" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C339" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F339" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="340" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C340" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F340" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="341" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C341" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F341" s="17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="342" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C342" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F342" s="32" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="338" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F338" s="32" t="s">
+    <row r="343" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C343" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F343" s="32" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="339" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F339" s="32" t="s">
+    <row r="344" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C344" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F344" s="32" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="340" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F340" s="32" t="s">
+    <row r="345" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C345" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F345" s="32" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="342" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F342" s="16" t="s">
+    <row r="346" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C346" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F346" s="32" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="347" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C347" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F347" s="32" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="348" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C348" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F348" s="32" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="349" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C349" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F349" s="32" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="350" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C350" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F350" s="32" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="351" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C351" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F351" s="32" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="352" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C352" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F352" s="32" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="353" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C353" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F353" s="32" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="354" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C354" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F354" s="32" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="355" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C355" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F355" s="32" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="356" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C356" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F356" s="32" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="357" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C357" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F357" s="32" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="358" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C358" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F358" s="32" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="359" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C359" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F359" s="32" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="360" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C360" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F360" s="32" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="361" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C361" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F361" s="32" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="362" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C362" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F362" s="32" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="363" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C363" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F363" s="32" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="364" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C364" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F364" s="32" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="365" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C365" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F365" s="32" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="366" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C366" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F366" s="32" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="367" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C367" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F367" s="32" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="368" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C368" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F368" s="32" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="369" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C369" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F369" s="32" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="370" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C370" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F370" s="32" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="371" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C371" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F371" s="32" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="372" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C372" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F372" s="32" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="373" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C373" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F373" s="33" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="374" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C374" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F374" s="32" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="375" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C375" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F375" s="32" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="376" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C376" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F376" s="32" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="377" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C377" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F377" s="32" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="378" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C378" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F378" s="32" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="379" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C379" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F379" s="32" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="380" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="F380" s="32"/>
+    </row>
+    <row r="381" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C381" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F381" s="16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="343" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F343" s="16" t="s">
+    <row r="382" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C382" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F382" s="16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="344" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F344" s="17" t="s">
+    <row r="383" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C383" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F383" s="17" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="345" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F345" s="32" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="346" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F346" s="32" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="347" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F347" s="32" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="348" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F348" s="32" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="349" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F349" s="32" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="350" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F350" s="32" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="351" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F351" s="32" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="352" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F352" s="32" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="353" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F353" s="32" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="354" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F354" s="32" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="355" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F355" s="32" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="356" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F356" s="32" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="357" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F357" s="32" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="358" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F358" s="32" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="359" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F359" s="32" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="360" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F360" s="32" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="361" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F361" s="32" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="362" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F362" s="32" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="363" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F363" s="32" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="364" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F364" s="32" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="365" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F365" s="32" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="366" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F366" s="32" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="367" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F367" s="32" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="368" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F368" s="32" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="369" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F369" s="32" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="370" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F370" s="32" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="371" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F371" s="32" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="372" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F372" s="32" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="373" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F373" s="32" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="374" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F374" s="32" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="375" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F375" s="32" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="376" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F376" s="33" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="377" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F377" s="32" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="378" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F378" s="32" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="379" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F379" s="32" t="s">
+    <row r="384" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C384" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F384" s="32" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="380" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F380" s="32" t="s">
+    <row r="385" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C385" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F385" s="32" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="381" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F381" s="32" t="s">
+    <row r="386" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C386" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F386" s="32" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="382" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F382" s="32" t="s">
+    <row r="387" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C387" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F387" s="32" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="383" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F383" s="32"/>
-    </row>
-    <row r="384" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F384" s="16" t="s">
+    <row r="388" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C388" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F388" s="32" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="389" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C389" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F389" s="32" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="390" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C390" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F390" s="32" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="391" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C391" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F391" s="32" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="392" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C392" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F392" s="32" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="393" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C393" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F393" s="32" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="394" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C394" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F394" s="32" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="395" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C395" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F395" s="32" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="396" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C396" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F396" s="32" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="397" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C397" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F397" s="32" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="398" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C398" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F398" s="32" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="399" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C399" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F399" s="32" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="400" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C400" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F400" s="32" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="401" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C401" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F401" s="32" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="402" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C402" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F402" s="32" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="403" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C403" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F403" s="32" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="404" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C404" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F404" s="32" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="405" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C405" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F405" s="32" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="406" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C406" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F406" s="32" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="407" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C407" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F407" s="32" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="408" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C408" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F408" s="32" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="409" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C409" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F409" s="32" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="410" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C410" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F410" s="32" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="411" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C411" s="10"/>
+    </row>
+    <row r="412" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C412" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F412" s="16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="385" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F385" s="16" t="s">
+    <row r="413" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C413" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F413" s="16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="386" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F386" s="17" t="s">
+    <row r="414" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C414" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F414" s="17" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="387" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F387" s="32" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="388" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F388" s="32" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="389" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F389" s="32" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="390" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F390" s="32" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="391" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F391" s="32" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="392" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F392" s="32" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="393" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F393" s="32" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="394" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F394" s="32" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="395" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F395" s="32" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="396" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F396" s="32" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="397" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F397" s="32" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="398" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F398" s="32" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="399" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F399" s="32" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="400" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F400" s="32" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="401" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F401" s="32" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="402" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F402" s="32" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="403" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F403" s="32" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="404" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F404" s="32" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="405" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F405" s="32" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="406" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F406" s="32" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="407" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F407" s="32" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="408" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F408" s="32" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="409" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F409" s="32" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="410" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F410" s="32" t="s">
+    <row r="415" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C415" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F415" s="32" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="411" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F411" s="32" t="s">
+    <row r="416" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C416" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F416" s="32" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="412" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F412" s="32" t="s">
+    <row r="417" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C417" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F417" s="32" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="413" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F413" s="32" t="s">
+    <row r="418" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C418" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F418" s="32" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="415" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F415" s="16" t="s">
+    <row r="419" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C419" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F419" s="32" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="420" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C420" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F420" s="32" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="421" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C421" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F421" s="32" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="422" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C422" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F422" s="32" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="423" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C423" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F423" s="32" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="424" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C424" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F424" s="32" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="425" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C425" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F425" s="32" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="426" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C426" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F426" s="32" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="427" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C427" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F427" s="32" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="428" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C428" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F428" s="32" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="429" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C429" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F429" s="32" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="430" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C430" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F430" s="32" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="431" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C431" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F431" s="32" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="432" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C432" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F432" s="32" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="433" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C433" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F433" s="32" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="434" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C434" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F434" s="32" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="435" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C435" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F435" s="32" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="436" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C436" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F436" s="32" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="437" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C437" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F437" s="32" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="438" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C438" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F438" s="32" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="439" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C439" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F439" s="32" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="440" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C440" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F440" s="32" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="441" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C441" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F441" s="32" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="442" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C442" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F442" s="32" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="443" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C443" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F443" s="32" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="444" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C444" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F444" s="32" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="445" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C445" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F445" s="32" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="446" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C446" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F446" s="33" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="447" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C447" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F447" s="32" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="448" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C448" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F448" s="32" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="449" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C449" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F449" s="32" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="450" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C450" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F450" s="32" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="451" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C451" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F451" s="32" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="452" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C452" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F452" s="32" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="453" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="F453" s="32"/>
+    </row>
+    <row r="454" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C454" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F454" s="16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="416" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F416" s="16" t="s">
+    <row r="455" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C455" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F455" s="16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="417" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F417" s="17" t="s">
+    <row r="456" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C456" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F456" s="17" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="418" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F418" s="32" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="419" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F419" s="32" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="420" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F420" s="32" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="421" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F421" s="32" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="422" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F422" s="32" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="423" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F423" s="32" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="424" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F424" s="32" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="425" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F425" s="32" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="426" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F426" s="32" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="427" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F427" s="32" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="428" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F428" s="32" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="429" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F429" s="32" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="430" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F430" s="32" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="431" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F431" s="32" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="432" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F432" s="32" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="433" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F433" s="32" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="434" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F434" s="32" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="435" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F435" s="32" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="436" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F436" s="32" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="437" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F437" s="32" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="438" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F438" s="32" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="439" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F439" s="32" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="440" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F440" s="32" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="441" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F441" s="32" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="442" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F442" s="32" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="443" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F443" s="32" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="444" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F444" s="32" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="445" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F445" s="32" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="446" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F446" s="32" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="447" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F447" s="32" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="448" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F448" s="32" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="449" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F449" s="33" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="450" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F450" s="32" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="451" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F451" s="32" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="452" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F452" s="32" t="s">
+    <row r="457" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C457" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F457" s="32" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="453" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F453" s="32" t="s">
+    <row r="458" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C458" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F458" s="32" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="454" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F454" s="32" t="s">
+    <row r="459" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C459" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F459" s="32" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="455" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F455" s="32" t="s">
+    <row r="460" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C460" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F460" s="32" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="456" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F456" s="32"/>
-    </row>
-    <row r="457" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F457" s="16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="458" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F458" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="459" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F459" s="17" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="460" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F460" s="32" t="s">
+    <row r="461" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C461" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F461" s="32" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="461" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F461" s="32" t="s">
+    <row r="462" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C462" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F462" s="32" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="462" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F462" s="32" t="s">
+    <row r="463" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C463" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F463" s="32" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="463" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F463" s="32" t="s">
+    <row r="464" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C464" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F464" s="32" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="464" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F464" s="32" t="s">
+    <row r="465" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C465" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F465" s="32" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="465" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F465" s="32" t="s">
+    <row r="466" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C466" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F466" s="32" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="466" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F466" s="32" t="s">
+    <row r="467" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C467" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F467" s="32" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="467" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F467" s="32" t="s">
+    <row r="468" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C468" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F468" s="32" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="468" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F468" s="32" t="s">
+    <row r="469" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C469" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F469" s="32" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="469" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F469" s="32" t="s">
+    <row r="470" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C470" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F470" s="32" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="470" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F470" s="32" t="s">
+    <row r="471" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C471" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F471" s="32" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="471" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F471" s="32" t="s">
+    <row r="472" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C472" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F472" s="32" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="472" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F472" s="32" t="s">
+    <row r="473" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C473" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F473" s="32" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="473" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F473" s="32" t="s">
+    <row r="474" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C474" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F474" s="32" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="474" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F474" s="32" t="s">
+    <row r="475" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C475" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F475" s="32" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="475" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F475" s="32" t="s">
+    <row r="476" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C476" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F476" s="32" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="476" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F476" s="32" t="s">
+    <row r="477" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C477" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F477" s="32" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="477" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F477" s="32" t="s">
+    <row r="478" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C478" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F478" s="32" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="478" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F478" s="32" t="s">
+    <row r="479" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C479" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F479" s="32" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="479" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F479" s="32" t="s">
+    <row r="480" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C480" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F480" s="32" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="480" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F480" s="32" t="s">
+    <row r="481" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C481" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F481" s="32" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="481" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F481" s="32" t="s">
+    <row r="482" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C482" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F482" s="32" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="482" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F482" s="32" t="s">
+    <row r="483" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C483" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F483" s="32" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="483" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F483" s="32" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="484" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F484" s="32" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="485" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F485" s="32" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="486" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F486" s="32" t="s">
-        <v>427</v>
-      </c>
+    <row r="484" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C484" s="10"/>
+    </row>
+    <row r="485" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C485" s="10"/>
+    </row>
+    <row r="486" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C486" s="10"/>
+    </row>
+    <row r="487" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C487" s="10"/>
+    </row>
+    <row r="488" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C488" s="10"/>
+    </row>
+    <row r="489" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C489" s="10"/>
+    </row>
+    <row r="490" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C490" s="10"/>
+    </row>
+    <row r="491" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C491" s="10"/>
+    </row>
+    <row r="492" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C492" s="10"/>
+    </row>
+    <row r="494" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C494" s="25"/>
+    </row>
+    <row r="495" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C495" s="10"/>
+    </row>
+    <row r="496" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C496" s="10"/>
+    </row>
+    <row r="497" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C497" s="10"/>
+    </row>
+    <row r="498" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C498" s="10"/>
+    </row>
+    <row r="499" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C499" s="10"/>
+    </row>
+    <row r="500" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C500" s="10"/>
+    </row>
+    <row r="501" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C501" s="10"/>
+    </row>
+    <row r="502" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C502" s="10"/>
+    </row>
+    <row r="503" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C503" s="10"/>
+    </row>
+    <row r="504" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C504" s="10"/>
+    </row>
+    <row r="505" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C505" s="10"/>
+    </row>
+    <row r="506" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C506" s="10"/>
+    </row>
+    <row r="507" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C507" s="10"/>
+    </row>
+    <row r="508" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C508" s="10"/>
+    </row>
+    <row r="509" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C509" s="10"/>
+    </row>
+    <row r="510" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C510" s="10"/>
+    </row>
+    <row r="511" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C511" s="10"/>
+    </row>
+    <row r="512" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C512" s="10"/>
+    </row>
+    <row r="513" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C513" s="10"/>
+    </row>
+    <row r="514" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C514" s="10"/>
+    </row>
+    <row r="515" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C515" s="10"/>
+    </row>
+    <row r="516" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C516" s="10"/>
+    </row>
+    <row r="517" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C517" s="10"/>
+    </row>
+    <row r="518" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C518" s="10"/>
+    </row>
+    <row r="519" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C519" s="10"/>
+    </row>
+    <row r="520" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C520" s="10"/>
+    </row>
+    <row r="521" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C521" s="10"/>
+    </row>
+    <row r="522" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C522" s="10"/>
+    </row>
+    <row r="523" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C523" s="10"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5D882B6-30B5-6742-81C6-39D5A67D008A}">
-  <dimension ref="A1:A81"/>
-  <sheetViews>
-    <sheetView topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="A72" sqref="A1:A72"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="32" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="32" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="32" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="32" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="32" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="32" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="32" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="32" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="32" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="32" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="32" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="32" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="32" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="32" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="32" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="32" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="32" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="32" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="32" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="32" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="32" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="32" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="32" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="32" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="32" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="32" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="32" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="32" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="32" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="32" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="32" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="33" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="32" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="32" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="32" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="32" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="32" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="32" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="32"/>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" s="17" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" s="32" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" s="32" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" s="32" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="32" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="32" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" s="32" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" s="32" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" s="32" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" s="32" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" s="32" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" s="32" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" s="32" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" s="32" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A59" s="32" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" s="32" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A61" s="32" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" s="32" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A63" s="32" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" s="32" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" s="32" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" s="32" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" s="32" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68" s="32" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A69" s="32" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A70" s="32" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" s="32" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A72" s="32" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A73" s="32"/>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A74" s="32"/>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A75" s="32"/>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A76" s="32"/>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A77" s="32"/>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A78" s="32"/>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A79" s="32"/>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A80" s="32"/>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A81" s="32"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
ELOW End init LOW
</commit_message>
<xml_diff>
--- a/Data/Spring_2023/BenthFun_Alkalinity.xlsx
+++ b/Data/Spring_2023/BenthFun_Alkalinity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremy/Library/Mobile Documents/com~apple~CloudDocs/Documents/Documents/Post-Doc/Projets/Villefranche/Projets/BenthFun – Jeremy/BenthFun/Data/Spring_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7276D0C3-BC8E-A74B-9859-EC26B11E4310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F98C46B-1648-5A4D-9A85-A6FE26C11823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1339" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1375" uniqueCount="422">
   <si>
     <t>Operator</t>
   </si>
@@ -886,18 +886,12 @@
     <t>PI_t8_ELOW_Tile_1b</t>
   </si>
   <si>
-    <t>PI_t8_ELOW_Tile_1c</t>
-  </si>
-  <si>
     <t>PI_t8_ELOW_Tile_2a</t>
   </si>
   <si>
     <t>PI_t8_ELOW_Tile_2b</t>
   </si>
   <si>
-    <t>PI_t8_ELOW_Tile_2c</t>
-  </si>
-  <si>
     <t>PI_t8_ELOW_Tile_3a</t>
   </si>
   <si>
@@ -1301,6 +1295,12 @@
   </si>
   <si>
     <t>PI_t4_ELOW_Tile_3d</t>
+  </si>
+  <si>
+    <t>PI_t6_ELOW_Tile_3d</t>
+  </si>
+  <si>
+    <t>PI_t1_LOW_Tile_2d</t>
   </si>
 </sst>
 </file>
@@ -1787,11 +1787,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L518"/>
+  <dimension ref="A1:L515"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="73" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A297" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F327" sqref="F327"/>
+      <pane ySplit="1" topLeftCell="A324" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H340" sqref="H340"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8717,7 +8717,7 @@
         <v>2889.65</v>
       </c>
       <c r="F277" s="32" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="278" spans="1:12" x14ac:dyDescent="0.2">
@@ -9109,7 +9109,7 @@
         <v>2678.51</v>
       </c>
       <c r="F293" s="32" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="294" spans="1:12" x14ac:dyDescent="0.2">
@@ -9570,23 +9570,23 @@
       <c r="D313" s="5">
         <v>48.63</v>
       </c>
-      <c r="E313" s="5">
+      <c r="E313" s="14">
         <v>2560.79</v>
       </c>
       <c r="F313" s="32" t="s">
         <v>270</v>
       </c>
-      <c r="G313" s="34">
-        <f>AVERAGE(E313:E314)</f>
-        <v>2553.3850000000002</v>
-      </c>
-      <c r="H313" s="34">
-        <f>STDEV(E313:E314)</f>
-        <v>10.472251429372731</v>
+      <c r="G313" s="13">
+        <f>AVERAGE(E314,E316)</f>
+        <v>2547.31</v>
+      </c>
+      <c r="H313" s="13">
+        <f>STDEV(E314,E316)</f>
+        <v>1.8809040379561135</v>
       </c>
       <c r="K313" s="5">
         <f>G313+$J$295</f>
-        <v>2557.8300000000004</v>
+        <v>2551.7550000000001</v>
       </c>
     </row>
     <row r="314" spans="1:11" x14ac:dyDescent="0.2">
@@ -9622,7 +9622,7 @@
       <c r="D315" s="5">
         <v>51.47</v>
       </c>
-      <c r="E315" s="5">
+      <c r="E315" s="14">
         <v>2522.4699999999998</v>
       </c>
       <c r="F315" s="32" t="s">
@@ -9640,25 +9640,13 @@
         <v>12</v>
       </c>
       <c r="D316" s="5">
-        <v>51.27</v>
-      </c>
-      <c r="E316" s="14">
-        <v>2585.0100000000002</v>
+        <v>50.71</v>
+      </c>
+      <c r="E316" s="5">
+        <v>2548.64</v>
       </c>
       <c r="F316" s="32" t="s">
-        <v>273</v>
-      </c>
-      <c r="G316" s="13">
-        <f>AVERAGE(E317:E318)</f>
-        <v>2604.0349999999999</v>
-      </c>
-      <c r="H316" s="18">
-        <f>STDEV(E317:E318)</f>
-        <v>6.3639610306892178E-2</v>
-      </c>
-      <c r="K316" s="5">
-        <f>G316+$J$295</f>
-        <v>2608.48</v>
+        <v>420</v>
       </c>
     </row>
     <row r="317" spans="1:11" x14ac:dyDescent="0.2">
@@ -9672,13 +9660,25 @@
         <v>12</v>
       </c>
       <c r="D317" s="5">
-        <v>49.07</v>
-      </c>
-      <c r="E317" s="5">
-        <v>2603.9899999999998</v>
+        <v>51.27</v>
+      </c>
+      <c r="E317" s="14">
+        <v>2585.0100000000002</v>
       </c>
       <c r="F317" s="32" t="s">
-        <v>274</v>
+        <v>273</v>
+      </c>
+      <c r="G317" s="13">
+        <f>AVERAGE(E318:E319)</f>
+        <v>2604.0349999999999</v>
+      </c>
+      <c r="H317" s="18">
+        <f>STDEV(E318:E319)</f>
+        <v>6.3639610306892178E-2</v>
+      </c>
+      <c r="K317" s="5">
+        <f>G317+$J$295</f>
+        <v>2608.48</v>
       </c>
     </row>
     <row r="318" spans="1:11" x14ac:dyDescent="0.2">
@@ -9692,13 +9692,13 @@
         <v>12</v>
       </c>
       <c r="D318" s="5">
-        <v>48.74</v>
+        <v>49.07</v>
       </c>
       <c r="E318" s="5">
-        <v>2604.08</v>
+        <v>2603.9899999999998</v>
       </c>
       <c r="F318" s="32" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="319" spans="1:11" x14ac:dyDescent="0.2">
@@ -9712,25 +9712,13 @@
         <v>12</v>
       </c>
       <c r="D319" s="5">
-        <v>50.99</v>
-      </c>
-      <c r="E319" s="14">
-        <v>2658.15</v>
+        <v>48.74</v>
+      </c>
+      <c r="E319" s="5">
+        <v>2604.08</v>
       </c>
       <c r="F319" s="32" t="s">
-        <v>276</v>
-      </c>
-      <c r="G319" s="13">
-        <f>AVERAGE(E320:E321)</f>
-        <v>2646.86</v>
-      </c>
-      <c r="H319" s="18">
-        <f>STDEV(E320:E321)</f>
-        <v>2.3617366491631717</v>
-      </c>
-      <c r="K319" s="5">
-        <f>G319+$J$295</f>
-        <v>2651.3050000000003</v>
+        <v>275</v>
       </c>
     </row>
     <row r="320" spans="1:11" x14ac:dyDescent="0.2">
@@ -9744,16 +9732,28 @@
         <v>12</v>
       </c>
       <c r="D320" s="5">
-        <v>50.89</v>
-      </c>
-      <c r="E320" s="5">
-        <v>2645.19</v>
+        <v>50.99</v>
+      </c>
+      <c r="E320" s="14">
+        <v>2658.15</v>
       </c>
       <c r="F320" s="32" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="321" spans="1:11" x14ac:dyDescent="0.2">
+        <v>276</v>
+      </c>
+      <c r="G320" s="13">
+        <f>AVERAGE(E321:E322)</f>
+        <v>2646.86</v>
+      </c>
+      <c r="H320" s="18">
+        <f>STDEV(E321:E322)</f>
+        <v>2.3617366491631717</v>
+      </c>
+      <c r="K320" s="5">
+        <f>G320+$J$295</f>
+        <v>2651.3050000000003</v>
+      </c>
+    </row>
+    <row r="321" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A321" s="9" t="s">
         <v>11</v>
       </c>
@@ -9764,16 +9764,16 @@
         <v>12</v>
       </c>
       <c r="D321" s="5">
-        <v>49.61</v>
+        <v>50.89</v>
       </c>
       <c r="E321" s="5">
-        <v>2648.53</v>
+        <v>2645.19</v>
       </c>
       <c r="F321" s="32" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="322" spans="1:11" x14ac:dyDescent="0.2">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="322" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A322" s="9" t="s">
         <v>11</v>
       </c>
@@ -9784,28 +9784,16 @@
         <v>12</v>
       </c>
       <c r="D322" s="5">
-        <v>48.94</v>
+        <v>49.61</v>
       </c>
       <c r="E322" s="5">
-        <v>2615.2199999999998</v>
+        <v>2648.53</v>
       </c>
       <c r="F322" s="32" t="s">
-        <v>279</v>
-      </c>
-      <c r="G322" s="13">
-        <f>AVERAGE(E322:E323)</f>
-        <v>2612.37</v>
-      </c>
-      <c r="H322" s="18">
-        <f>STDEV(E322:E323)</f>
-        <v>4.0305086527631921</v>
-      </c>
-      <c r="K322" s="5">
-        <f>G322+$J$295</f>
-        <v>2616.8150000000001</v>
-      </c>
-    </row>
-    <row r="323" spans="1:11" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="323" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A323" s="9" t="s">
         <v>11</v>
       </c>
@@ -9816,16 +9804,28 @@
         <v>12</v>
       </c>
       <c r="D323" s="5">
-        <v>50.77</v>
+        <v>48.94</v>
       </c>
       <c r="E323" s="5">
-        <v>2609.52</v>
+        <v>2614.2199999999998</v>
       </c>
       <c r="F323" s="32" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="324" spans="1:11" x14ac:dyDescent="0.2">
+        <v>279</v>
+      </c>
+      <c r="G323" s="13">
+        <f>AVERAGE(E323:E324)</f>
+        <v>2612.37</v>
+      </c>
+      <c r="H323" s="18">
+        <f>STDEV(E323:E324)</f>
+        <v>2.6162950903900972</v>
+      </c>
+      <c r="K323" s="5">
+        <f>G323+$J$295</f>
+        <v>2616.8150000000001</v>
+      </c>
+    </row>
+    <row r="324" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A324" s="9" t="s">
         <v>11</v>
       </c>
@@ -9836,25 +9836,16 @@
         <v>12</v>
       </c>
       <c r="D324" s="5">
-        <v>52.43</v>
+        <v>50.77</v>
+      </c>
+      <c r="E324" s="5">
+        <v>2610.52</v>
       </c>
       <c r="F324" s="32" t="s">
-        <v>281</v>
-      </c>
-      <c r="G324" s="13" t="e">
-        <f>AVERAGE(E324:E325)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H324" s="18" t="e">
-        <f>STDEV(E324:E325)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K324" s="5" t="e">
-        <f>G324+$J$295</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="325" spans="1:11" x14ac:dyDescent="0.2">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="325" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A325" s="9" t="s">
         <v>11</v>
       </c>
@@ -9865,13 +9856,28 @@
         <v>12</v>
       </c>
       <c r="D325" s="5">
-        <v>49.17</v>
+        <v>52.43</v>
+      </c>
+      <c r="E325" s="5">
+        <v>2530.13</v>
       </c>
       <c r="F325" s="32" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="326" spans="1:11" x14ac:dyDescent="0.2">
+        <v>281</v>
+      </c>
+      <c r="G325" s="13">
+        <f>AVERAGE(E325:E326)</f>
+        <v>2528.3500000000004</v>
+      </c>
+      <c r="H325" s="18">
+        <f>STDEV(E325:E326)</f>
+        <v>2.5173001410240707</v>
+      </c>
+      <c r="K325" s="5">
+        <f>G325+$J$295</f>
+        <v>2532.7950000000005</v>
+      </c>
+    </row>
+    <row r="326" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A326" s="9" t="s">
         <v>11</v>
       </c>
@@ -9882,13 +9888,16 @@
         <v>12</v>
       </c>
       <c r="D326" s="5">
-        <v>50.06</v>
+        <v>49.17</v>
+      </c>
+      <c r="E326" s="5">
+        <v>2526.5700000000002</v>
       </c>
       <c r="F326" s="32" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="327" spans="1:11" x14ac:dyDescent="0.2">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="327" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A327" s="9" t="s">
         <v>11</v>
       </c>
@@ -9898,23 +9907,29 @@
       <c r="C327" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D327" s="5">
+        <v>50.31</v>
+      </c>
+      <c r="E327" s="5">
+        <v>2623.15</v>
+      </c>
       <c r="F327" s="32" t="s">
-        <v>284</v>
-      </c>
-      <c r="G327" s="13" t="e">
+        <v>283</v>
+      </c>
+      <c r="G327" s="13">
         <f>AVERAGE(E327:E328)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H327" s="18" t="e">
+        <v>2622.16</v>
+      </c>
+      <c r="H327" s="18">
         <f>STDEV(E327:E328)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K327" s="5" t="e">
+        <v>1.400071426749377</v>
+      </c>
+      <c r="K327" s="5">
         <f>G327+$J$295</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="328" spans="1:11" x14ac:dyDescent="0.2">
+        <v>2626.605</v>
+      </c>
+    </row>
+    <row r="328" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A328" s="9" t="s">
         <v>11</v>
       </c>
@@ -9924,11 +9939,17 @@
       <c r="C328" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D328" s="5">
+        <v>51.67</v>
+      </c>
+      <c r="E328" s="5">
+        <v>2621.17</v>
+      </c>
       <c r="F328" s="32" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="329" spans="1:11" x14ac:dyDescent="0.2">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="329" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A329" s="9" t="s">
         <v>11</v>
       </c>
@@ -9938,11 +9959,29 @@
       <c r="C329" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D329" s="5">
+        <v>50.42</v>
+      </c>
+      <c r="E329" s="14">
+        <v>2585.75</v>
+      </c>
       <c r="F329" s="32" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="330" spans="1:11" x14ac:dyDescent="0.2">
+        <v>285</v>
+      </c>
+      <c r="G329" s="13">
+        <f>AVERAGE(E330:E331)</f>
+        <v>2575.38</v>
+      </c>
+      <c r="H329" s="18">
+        <f>STDEV(E330:E331)</f>
+        <v>4.2426406871192848</v>
+      </c>
+      <c r="K329" s="5">
+        <f>G329+$J$295</f>
+        <v>2579.8250000000003</v>
+      </c>
+    </row>
+    <row r="330" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A330" s="9" t="s">
         <v>11</v>
       </c>
@@ -9952,23 +9991,17 @@
       <c r="C330" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D330" s="5">
+        <v>50.63</v>
+      </c>
+      <c r="E330" s="5">
+        <v>2572.38</v>
+      </c>
       <c r="F330" s="32" t="s">
-        <v>287</v>
-      </c>
-      <c r="G330" s="13" t="e">
-        <f>AVERAGE(E330:E331)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H330" s="18" t="e">
-        <f>STDEV(E330:E331)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K330" s="5" t="e">
-        <f>G330+$J$295</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="331" spans="1:11" x14ac:dyDescent="0.2">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="331" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A331" s="9" t="s">
         <v>11</v>
       </c>
@@ -9978,556 +10011,1157 @@
       <c r="C331" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D331" s="5">
+        <v>49.19</v>
+      </c>
+      <c r="E331" s="5">
+        <v>2578.38</v>
+      </c>
       <c r="F331" s="32" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="332" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C332" s="10"/>
+    </row>
+    <row r="333" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A333" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B333" s="31">
+        <v>45083</v>
+      </c>
+      <c r="C333" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F333" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G333" s="13" t="e">
+        <f>AVERAGE(E334,E335)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H333" s="18" t="e">
+        <f>STDEV(E334,E335)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I333" s="3">
+        <v>2226.44</v>
+      </c>
+      <c r="J333" s="4" t="e">
+        <f>I333-G333</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K333" s="5" t="e">
+        <f>G333+J333</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L333" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="334" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A334" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B334" s="31">
+        <v>45083</v>
+      </c>
+      <c r="C334" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F334" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="335" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A335" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B335" s="31">
+        <v>45083</v>
+      </c>
+      <c r="C335" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F335" s="17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="336" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A336" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B336" s="31">
+        <v>45082</v>
+      </c>
+      <c r="C336" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D336" s="5">
+        <v>48.96</v>
+      </c>
+      <c r="E336" s="5">
+        <v>2601.0100000000002</v>
+      </c>
+      <c r="F336" s="32" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="332" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A332" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B332" s="31">
+      <c r="G336" s="13">
+        <f>AVERAGE(E336:E337)</f>
+        <v>2601.6750000000002</v>
+      </c>
+      <c r="H336" s="18">
+        <f>STDEV(E336:E337)</f>
+        <v>0.94045201897805675</v>
+      </c>
+      <c r="K336" s="5">
+        <f>G336+$J$295</f>
+        <v>2606.1200000000003</v>
+      </c>
+    </row>
+    <row r="337" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A337" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B337" s="31">
         <v>45082</v>
       </c>
-      <c r="C332" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F332" s="32" t="s">
+      <c r="C337" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D337" s="5">
+        <v>52.01</v>
+      </c>
+      <c r="E337" s="5">
+        <v>2602.34</v>
+      </c>
+      <c r="F337" s="32" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="333" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C333" s="10"/>
-    </row>
-    <row r="334" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C334" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="F334" s="16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="335" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C335" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F335" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="336" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C336" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F336" s="17" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="337" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C337" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F337" s="32" t="s">
+    <row r="338" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A338" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B338" s="31">
+        <v>45082</v>
+      </c>
+      <c r="C338" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D338" s="5">
+        <v>50.22</v>
+      </c>
+      <c r="E338" s="5">
+        <v>2534.11</v>
+      </c>
+      <c r="F338" s="32" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="338" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C338" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F338" s="32" t="s">
+      <c r="G338" s="34">
+        <f>AVERAGE(E339:E340)</f>
+        <v>2575.1899999999996</v>
+      </c>
+      <c r="H338" s="34">
+        <f>STDEV(E339:E340)</f>
+        <v>10.974297244015204</v>
+      </c>
+      <c r="K338" s="5">
+        <f>G338+$J$295</f>
+        <v>2579.6349999999998</v>
+      </c>
+    </row>
+    <row r="339" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A339" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B339" s="31">
+        <v>45082</v>
+      </c>
+      <c r="C339" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D339" s="5">
+        <v>49.38</v>
+      </c>
+      <c r="E339" s="5">
+        <v>2567.4299999999998</v>
+      </c>
+      <c r="F339" s="32" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="339" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C339" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F339" s="32" t="s">
+    <row r="340" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A340" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B340" s="31">
+        <v>45082</v>
+      </c>
+      <c r="C340" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D340" s="5">
+        <v>49.96</v>
+      </c>
+      <c r="E340" s="5">
+        <v>2582.9499999999998</v>
+      </c>
+      <c r="F340" s="32" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="340" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C340" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F340" s="32" t="s">
+    <row r="341" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A341" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B341" s="31">
+        <v>45082</v>
+      </c>
+      <c r="C341" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D341" s="5">
+        <v>49.71</v>
+      </c>
+      <c r="F341" s="32" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="342" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A342" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B342" s="31">
+        <v>45082</v>
+      </c>
+      <c r="C342" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D342" s="5">
+        <v>49.6</v>
+      </c>
+      <c r="E342" s="5">
+        <v>2560.94</v>
+      </c>
+      <c r="F342" s="32" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="341" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C341" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F341" s="32" t="s">
+      <c r="G342" s="13">
+        <f>AVERAGE(E342:E343)</f>
+        <v>2554.1149999999998</v>
+      </c>
+      <c r="H342" s="18">
+        <f>STDEV(E342:E343)</f>
+        <v>9.6520075631964382</v>
+      </c>
+      <c r="K342" s="5">
+        <f>G342+$J$295</f>
+        <v>2558.56</v>
+      </c>
+    </row>
+    <row r="343" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A343" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B343" s="31">
+        <v>45082</v>
+      </c>
+      <c r="C343" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D343" s="5">
+        <v>52</v>
+      </c>
+      <c r="E343" s="5">
+        <v>2547.29</v>
+      </c>
+      <c r="F343" s="32" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="342" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C342" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F342" s="32" t="s">
+    <row r="344" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A344" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B344" s="31">
+        <v>45082</v>
+      </c>
+      <c r="C344" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D344" s="5">
+        <v>49.79</v>
+      </c>
+      <c r="F344" s="32" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="343" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C343" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F343" s="32" t="s">
+    <row r="345" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A345" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B345" s="31">
+        <v>45082</v>
+      </c>
+      <c r="C345" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D345" s="5">
+        <v>51.18</v>
+      </c>
+      <c r="E345" s="5">
+        <v>2589.9299999999998</v>
+      </c>
+      <c r="F345" s="32" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="344" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C344" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F344" s="32" t="s">
+      <c r="G345" s="13">
+        <f>AVERAGE(E345:E346)</f>
+        <v>2585.6799999999998</v>
+      </c>
+      <c r="H345" s="18">
+        <f>STDEV(E345:E346)</f>
+        <v>6.0104076400856536</v>
+      </c>
+      <c r="K345" s="5">
+        <f>G345+$J$295</f>
+        <v>2590.125</v>
+      </c>
+    </row>
+    <row r="346" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A346" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B346" s="31">
+        <v>45082</v>
+      </c>
+      <c r="C346" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D346" s="5">
+        <v>50.87</v>
+      </c>
+      <c r="E346" s="5">
+        <v>2581.4299999999998</v>
+      </c>
+      <c r="F346" s="32" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="345" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C345" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F345" s="32" t="s">
+    <row r="347" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A347" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B347" s="31">
+        <v>45082</v>
+      </c>
+      <c r="C347" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D347" s="5">
+        <v>49.3</v>
+      </c>
+      <c r="F347" s="32" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="346" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C346" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F346" s="32" t="s">
+    <row r="348" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A348" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B348" s="31">
+        <v>45083</v>
+      </c>
+      <c r="C348" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F348" s="32" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="347" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C347" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F347" s="32" t="s">
+      <c r="G348" s="13" t="e">
+        <f>AVERAGE(E349:E350)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H348" s="18" t="e">
+        <f>STDEV(E349:E350)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K348" s="5" t="e">
+        <f>G348+$J$333</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="349" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A349" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B349" s="31">
+        <v>45083</v>
+      </c>
+      <c r="C349" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F349" s="32" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="348" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C348" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F348" s="32" t="s">
+    <row r="350" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A350" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B350" s="31">
+        <v>45083</v>
+      </c>
+      <c r="C350" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F350" s="32" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="349" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C349" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F349" s="32" t="s">
+    <row r="351" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A351" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B351" s="31">
+        <v>45083</v>
+      </c>
+      <c r="C351" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F351" s="32" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="350" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C350" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F350" s="32" t="s">
+      <c r="G351" s="13" t="e">
+        <f>AVERAGE(E352:E353)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H351" s="18" t="e">
+        <f>STDEV(E352:E353)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K351" s="5" t="e">
+        <f>G351+$J$333</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="352" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A352" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B352" s="31">
+        <v>45083</v>
+      </c>
+      <c r="C352" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F352" s="32" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="351" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C351" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F351" s="32" t="s">
+    <row r="353" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A353" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B353" s="31">
+        <v>45083</v>
+      </c>
+      <c r="C353" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F353" s="32" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="352" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C352" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F352" s="32" t="s">
+    <row r="354" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A354" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B354" s="31">
+        <v>45083</v>
+      </c>
+      <c r="C354" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F354" s="32" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="353" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C353" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F353" s="32" t="s">
+      <c r="G354" s="13" t="e">
+        <f>AVERAGE(E355:E356)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H354" s="18" t="e">
+        <f>STDEV(E355:E356)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K354" s="5" t="e">
+        <f>G354+$J$333</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="355" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A355" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B355" s="31">
+        <v>45083</v>
+      </c>
+      <c r="C355" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F355" s="32" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="354" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C354" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F354" s="32" t="s">
+    <row r="356" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A356" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B356" s="31">
+        <v>45083</v>
+      </c>
+      <c r="C356" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F356" s="32" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="355" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C355" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F355" s="32" t="s">
+    <row r="357" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A357" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B357" s="31">
+        <v>45083</v>
+      </c>
+      <c r="C357" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F357" s="32" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="356" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C356" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F356" s="32" t="s">
+      <c r="G357" s="13" t="e">
+        <f>AVERAGE(E358:E359)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H357" s="18" t="e">
+        <f>STDEV(E358:E359)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K357" s="5" t="e">
+        <f>G357+$J$333</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="358" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A358" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B358" s="31">
+        <v>45083</v>
+      </c>
+      <c r="C358" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F358" s="32" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="357" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C357" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F357" s="32" t="s">
+    <row r="359" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A359" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B359" s="31">
+        <v>45083</v>
+      </c>
+      <c r="C359" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F359" s="32" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="358" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C358" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F358" s="32" t="s">
+    <row r="360" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A360" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B360" s="31">
+        <v>45083</v>
+      </c>
+      <c r="C360" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F360" s="32" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="359" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C359" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F359" s="32" t="s">
+      <c r="G360" s="13" t="e">
+        <f>AVERAGE(E361:E362)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H360" s="18" t="e">
+        <f>STDEV(E361:E362)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K360" s="5" t="e">
+        <f>G360+$J$333</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="361" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A361" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B361" s="31">
+        <v>45083</v>
+      </c>
+      <c r="C361" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F361" s="32" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="360" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C360" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F360" s="32" t="s">
+    <row r="362" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A362" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B362" s="31">
+        <v>45083</v>
+      </c>
+      <c r="C362" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F362" s="32" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="361" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C361" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F361" s="32" t="s">
+    <row r="363" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A363" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B363" s="31">
+        <v>45083</v>
+      </c>
+      <c r="C363" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F363" s="32" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="362" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C362" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F362" s="32" t="s">
+      <c r="G363" s="13" t="e">
+        <f>AVERAGE(E364:E365)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H363" s="18" t="e">
+        <f>STDEV(E364:E365)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K363" s="5" t="e">
+        <f>G363+$J$333</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="364" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A364" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B364" s="31">
+        <v>45083</v>
+      </c>
+      <c r="C364" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F364" s="32" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="363" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C363" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F363" s="32" t="s">
+    <row r="365" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A365" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B365" s="31">
+        <v>45083</v>
+      </c>
+      <c r="C365" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F365" s="32" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="364" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C364" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F364" s="32" t="s">
+    <row r="366" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A366" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B366" s="31">
+        <v>45083</v>
+      </c>
+      <c r="C366" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F366" s="32" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="365" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C365" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F365" s="32" t="s">
+      <c r="G366" s="13" t="e">
+        <f>AVERAGE(E367:E368)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H366" s="18" t="e">
+        <f>STDEV(E367:E368)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K366" s="5" t="e">
+        <f>G366+$J$333</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="367" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A367" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B367" s="31">
+        <v>45083</v>
+      </c>
+      <c r="C367" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F367" s="32" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="366" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C366" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F366" s="32" t="s">
+    <row r="368" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A368" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B368" s="31">
+        <v>45083</v>
+      </c>
+      <c r="C368" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F368" s="33" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="367" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C367" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F367" s="32" t="s">
+    <row r="369" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A369" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B369" s="31">
+        <v>45083</v>
+      </c>
+      <c r="C369" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F369" s="32" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="368" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C368" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F368" s="33" t="s">
+      <c r="G369" s="13" t="e">
+        <f>AVERAGE(E370:E371)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H369" s="18" t="e">
+        <f>STDEV(E370:E371)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K369" s="5" t="e">
+        <f>G369+$J$333</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="370" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A370" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B370" s="31">
+        <v>45083</v>
+      </c>
+      <c r="C370" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F370" s="32" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="369" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C369" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F369" s="32" t="s">
+    <row r="371" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A371" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B371" s="31">
+        <v>45083</v>
+      </c>
+      <c r="C371" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F371" s="32" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="370" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C370" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F370" s="32" t="s">
+    <row r="372" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A372" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B372" s="31">
+        <v>45083</v>
+      </c>
+      <c r="C372" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F372" s="32" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="371" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C371" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F371" s="32" t="s">
+      <c r="G372" s="13" t="e">
+        <f>AVERAGE(E373:E374)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H372" s="18" t="e">
+        <f>STDEV(E373:E374)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K372" s="5" t="e">
+        <f>G372+$J$333</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="373" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A373" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B373" s="31">
+        <v>45083</v>
+      </c>
+      <c r="C373" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F373" s="32" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="372" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C372" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F372" s="32" t="s">
+    <row r="374" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A374" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B374" s="31">
+        <v>45083</v>
+      </c>
+      <c r="C374" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F374" s="32" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="373" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C373" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F373" s="32" t="s">
+    <row r="375" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F375" s="32"/>
+    </row>
+    <row r="376" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C376" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F376" s="32" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="374" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C374" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F374" s="32" t="s">
+      <c r="G376" s="13" t="e">
+        <f>AVERAGE(E377:E378)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H376" s="18" t="e">
+        <f>STDEV(E377:E378)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K376" s="5" t="e">
+        <f>G376+$J$333</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="377" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C377" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F377" s="32" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="375" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="F375" s="32"/>
-    </row>
-    <row r="376" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C376" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="F376" s="16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="377" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C377" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F377" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="378" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C378" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F378" s="17" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="379" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="F378" s="32" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="379" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C379" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F379" s="32" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="380" spans="3:6" x14ac:dyDescent="0.2">
+        <v>329</v>
+      </c>
+      <c r="G379" s="13" t="e">
+        <f>AVERAGE(E380:E381)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H379" s="18" t="e">
+        <f>STDEV(E380:E381)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K379" s="5" t="e">
+        <f>G379+$J$333</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="380" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C380" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F380" s="32" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="381" spans="3:6" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="381" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C381" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F381" s="32" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="382" spans="3:6" x14ac:dyDescent="0.2">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="382" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C382" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F382" s="32" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="383" spans="3:6" x14ac:dyDescent="0.2">
+        <v>332</v>
+      </c>
+      <c r="G382" s="13" t="e">
+        <f>AVERAGE(E383:E384)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H382" s="18" t="e">
+        <f>STDEV(E383:E384)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K382" s="5" t="e">
+        <f>G382+$J$333</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="383" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C383" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F383" s="32" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="384" spans="3:6" x14ac:dyDescent="0.2">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="384" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C384" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F384" s="32" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="385" spans="3:6" x14ac:dyDescent="0.2">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="385" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C385" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F385" s="32" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="386" spans="3:6" x14ac:dyDescent="0.2">
+        <v>335</v>
+      </c>
+      <c r="G385" s="13" t="e">
+        <f>AVERAGE(E386:E387)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H385" s="18" t="e">
+        <f>STDEV(E386:E387)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K385" s="5" t="e">
+        <f>G385+$J$333</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="386" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C386" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F386" s="32" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="387" spans="3:6" x14ac:dyDescent="0.2">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="387" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C387" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F387" s="32" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="388" spans="3:6" x14ac:dyDescent="0.2">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="388" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C388" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F388" s="32" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="389" spans="3:6" x14ac:dyDescent="0.2">
+        <v>338</v>
+      </c>
+      <c r="G388" s="13" t="e">
+        <f>AVERAGE(E389:E390)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H388" s="18" t="e">
+        <f>STDEV(E389:E390)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K388" s="5" t="e">
+        <f>G388+$J$333</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="389" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C389" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F389" s="32" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="390" spans="3:6" x14ac:dyDescent="0.2">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="390" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C390" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F390" s="32" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="391" spans="3:6" x14ac:dyDescent="0.2">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="391" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C391" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F391" s="32" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="392" spans="3:6" x14ac:dyDescent="0.2">
+        <v>341</v>
+      </c>
+      <c r="G391" s="13" t="e">
+        <f>AVERAGE(E392:E393)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H391" s="18" t="e">
+        <f>STDEV(E392:E393)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K391" s="5" t="e">
+        <f>G391+$J$333</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="392" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C392" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F392" s="32" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="393" spans="3:6" x14ac:dyDescent="0.2">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="393" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C393" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F393" s="32" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="394" spans="3:6" x14ac:dyDescent="0.2">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="394" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C394" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F394" s="32" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="395" spans="3:6" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+      <c r="G394" s="13" t="e">
+        <f>AVERAGE(E395:E396)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H394" s="18" t="e">
+        <f>STDEV(E395:E396)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K394" s="5" t="e">
+        <f>G394+$J$333</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="395" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C395" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F395" s="32" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="396" spans="3:6" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="396" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C396" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F396" s="32" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="397" spans="3:6" x14ac:dyDescent="0.2">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="397" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C397" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F397" s="32" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="398" spans="3:6" x14ac:dyDescent="0.2">
+        <v>347</v>
+      </c>
+      <c r="G397" s="13" t="e">
+        <f>AVERAGE(E398:E399)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H397" s="18" t="e">
+        <f>STDEV(E398:E399)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K397" s="5" t="e">
+        <f>G397+$J$333</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="398" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C398" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F398" s="32" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="399" spans="3:6" x14ac:dyDescent="0.2">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="399" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C399" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F399" s="32" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="400" spans="3:6" x14ac:dyDescent="0.2">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="400" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C400" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F400" s="32" t="s">
-        <v>349</v>
+        <v>350</v>
+      </c>
+      <c r="G400" s="13" t="e">
+        <f>AVERAGE(E401:E402)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H400" s="18" t="e">
+        <f>STDEV(E401:E402)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K400" s="5" t="e">
+        <f>G400+$J$333</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="401" spans="3:6" x14ac:dyDescent="0.2">
@@ -10535,7 +11169,7 @@
         <v>12</v>
       </c>
       <c r="F401" s="32" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="402" spans="3:6" x14ac:dyDescent="0.2">
@@ -10543,58 +11177,58 @@
         <v>12</v>
       </c>
       <c r="F402" s="32" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="403" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C403" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F403" s="32" t="s">
-        <v>352</v>
-      </c>
+      <c r="C403" s="10"/>
     </row>
     <row r="404" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C404" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F404" s="32" t="s">
-        <v>353</v>
+      <c r="C404" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F404" s="16" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="405" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C405" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F405" s="32" t="s">
-        <v>354</v>
+      <c r="F405" s="16" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="406" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C406" s="10"/>
+      <c r="C406" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F406" s="17" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="407" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C407" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="F407" s="16" t="s">
-        <v>8</v>
+      <c r="C407" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F407" s="32" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="408" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C408" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F408" s="16" t="s">
-        <v>9</v>
+      <c r="F408" s="32" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="409" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C409" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F409" s="17" t="s">
-        <v>96</v>
+      <c r="F409" s="32" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="410" spans="3:6" x14ac:dyDescent="0.2">
@@ -10602,7 +11236,7 @@
         <v>12</v>
       </c>
       <c r="F410" s="32" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="411" spans="3:6" x14ac:dyDescent="0.2">
@@ -10610,7 +11244,7 @@
         <v>12</v>
       </c>
       <c r="F411" s="32" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="412" spans="3:6" x14ac:dyDescent="0.2">
@@ -10618,7 +11252,7 @@
         <v>12</v>
       </c>
       <c r="F412" s="32" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="413" spans="3:6" x14ac:dyDescent="0.2">
@@ -10626,7 +11260,7 @@
         <v>12</v>
       </c>
       <c r="F413" s="32" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="414" spans="3:6" x14ac:dyDescent="0.2">
@@ -10634,7 +11268,7 @@
         <v>12</v>
       </c>
       <c r="F414" s="32" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="415" spans="3:6" x14ac:dyDescent="0.2">
@@ -10642,7 +11276,7 @@
         <v>12</v>
       </c>
       <c r="F415" s="32" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="416" spans="3:6" x14ac:dyDescent="0.2">
@@ -10650,7 +11284,7 @@
         <v>12</v>
       </c>
       <c r="F416" s="32" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="417" spans="3:6" x14ac:dyDescent="0.2">
@@ -10658,7 +11292,7 @@
         <v>12</v>
       </c>
       <c r="F417" s="32" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="418" spans="3:6" x14ac:dyDescent="0.2">
@@ -10666,7 +11300,7 @@
         <v>12</v>
       </c>
       <c r="F418" s="32" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="419" spans="3:6" x14ac:dyDescent="0.2">
@@ -10674,7 +11308,7 @@
         <v>12</v>
       </c>
       <c r="F419" s="32" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="420" spans="3:6" x14ac:dyDescent="0.2">
@@ -10682,7 +11316,7 @@
         <v>12</v>
       </c>
       <c r="F420" s="32" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="421" spans="3:6" x14ac:dyDescent="0.2">
@@ -10690,7 +11324,7 @@
         <v>12</v>
       </c>
       <c r="F421" s="32" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="422" spans="3:6" x14ac:dyDescent="0.2">
@@ -10698,7 +11332,7 @@
         <v>12</v>
       </c>
       <c r="F422" s="32" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="423" spans="3:6" x14ac:dyDescent="0.2">
@@ -10706,7 +11340,7 @@
         <v>12</v>
       </c>
       <c r="F423" s="32" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="424" spans="3:6" x14ac:dyDescent="0.2">
@@ -10714,7 +11348,7 @@
         <v>12</v>
       </c>
       <c r="F424" s="32" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="425" spans="3:6" x14ac:dyDescent="0.2">
@@ -10722,7 +11356,7 @@
         <v>12</v>
       </c>
       <c r="F425" s="32" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="426" spans="3:6" x14ac:dyDescent="0.2">
@@ -10730,7 +11364,7 @@
         <v>12</v>
       </c>
       <c r="F426" s="32" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="427" spans="3:6" x14ac:dyDescent="0.2">
@@ -10738,7 +11372,7 @@
         <v>12</v>
       </c>
       <c r="F427" s="32" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="428" spans="3:6" x14ac:dyDescent="0.2">
@@ -10746,7 +11380,7 @@
         <v>12</v>
       </c>
       <c r="F428" s="32" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="429" spans="3:6" x14ac:dyDescent="0.2">
@@ -10754,7 +11388,7 @@
         <v>12</v>
       </c>
       <c r="F429" s="32" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="430" spans="3:6" x14ac:dyDescent="0.2">
@@ -10762,7 +11396,7 @@
         <v>12</v>
       </c>
       <c r="F430" s="32" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="431" spans="3:6" x14ac:dyDescent="0.2">
@@ -10770,7 +11404,7 @@
         <v>12</v>
       </c>
       <c r="F431" s="32" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="432" spans="3:6" x14ac:dyDescent="0.2">
@@ -10778,7 +11412,7 @@
         <v>12</v>
       </c>
       <c r="F432" s="32" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="433" spans="3:6" x14ac:dyDescent="0.2">
@@ -10786,7 +11420,7 @@
         <v>12</v>
       </c>
       <c r="F433" s="32" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="434" spans="3:6" x14ac:dyDescent="0.2">
@@ -10794,7 +11428,7 @@
         <v>12</v>
       </c>
       <c r="F434" s="32" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="435" spans="3:6" x14ac:dyDescent="0.2">
@@ -10802,7 +11436,7 @@
         <v>12</v>
       </c>
       <c r="F435" s="32" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="436" spans="3:6" x14ac:dyDescent="0.2">
@@ -10810,7 +11444,7 @@
         <v>12</v>
       </c>
       <c r="F436" s="32" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="437" spans="3:6" x14ac:dyDescent="0.2">
@@ -10818,15 +11452,15 @@
         <v>12</v>
       </c>
       <c r="F437" s="32" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="438" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C438" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F438" s="32" t="s">
-        <v>383</v>
+      <c r="F438" s="33" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="439" spans="3:6" x14ac:dyDescent="0.2">
@@ -10834,7 +11468,7 @@
         <v>12</v>
       </c>
       <c r="F439" s="32" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="440" spans="3:6" x14ac:dyDescent="0.2">
@@ -10842,15 +11476,15 @@
         <v>12</v>
       </c>
       <c r="F440" s="32" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="441" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C441" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F441" s="33" t="s">
-        <v>386</v>
+      <c r="F441" s="32" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="442" spans="3:6" x14ac:dyDescent="0.2">
@@ -10858,15 +11492,15 @@
         <v>12</v>
       </c>
       <c r="F442" s="32" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="443" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C443" s="10" t="s">
+      <c r="C443" s="25" t="s">
         <v>12</v>
       </c>
       <c r="F443" s="32" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="444" spans="3:6" x14ac:dyDescent="0.2">
@@ -10874,58 +11508,58 @@
         <v>12</v>
       </c>
       <c r="F444" s="32" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="445" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C445" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F445" s="32" t="s">
-        <v>390</v>
-      </c>
+      <c r="F445" s="32"/>
     </row>
     <row r="446" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C446" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="F446" s="32" t="s">
-        <v>391</v>
+      <c r="C446" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F446" s="16" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="447" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C447" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F447" s="32" t="s">
-        <v>392</v>
+      <c r="F447" s="16" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="448" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="F448" s="32"/>
+      <c r="C448" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F448" s="17" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="449" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C449" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F449" s="16" t="s">
-        <v>8</v>
+      <c r="F449" s="32" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="450" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C450" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F450" s="16" t="s">
-        <v>9</v>
+      <c r="F450" s="32" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="451" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C451" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F451" s="17" t="s">
-        <v>96</v>
+      <c r="F451" s="32" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="452" spans="3:6" x14ac:dyDescent="0.2">
@@ -10933,7 +11567,7 @@
         <v>12</v>
       </c>
       <c r="F452" s="32" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="453" spans="3:6" x14ac:dyDescent="0.2">
@@ -10941,7 +11575,7 @@
         <v>12</v>
       </c>
       <c r="F453" s="32" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="454" spans="3:6" x14ac:dyDescent="0.2">
@@ -10949,7 +11583,7 @@
         <v>12</v>
       </c>
       <c r="F454" s="32" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="455" spans="3:6" x14ac:dyDescent="0.2">
@@ -10957,7 +11591,7 @@
         <v>12</v>
       </c>
       <c r="F455" s="32" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="456" spans="3:6" x14ac:dyDescent="0.2">
@@ -10965,7 +11599,7 @@
         <v>12</v>
       </c>
       <c r="F456" s="32" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="457" spans="3:6" x14ac:dyDescent="0.2">
@@ -10973,7 +11607,7 @@
         <v>12</v>
       </c>
       <c r="F457" s="32" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="458" spans="3:6" x14ac:dyDescent="0.2">
@@ -10981,7 +11615,7 @@
         <v>12</v>
       </c>
       <c r="F458" s="32" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="459" spans="3:6" x14ac:dyDescent="0.2">
@@ -10989,7 +11623,7 @@
         <v>12</v>
       </c>
       <c r="F459" s="32" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="460" spans="3:6" x14ac:dyDescent="0.2">
@@ -10997,7 +11631,7 @@
         <v>12</v>
       </c>
       <c r="F460" s="32" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="461" spans="3:6" x14ac:dyDescent="0.2">
@@ -11005,7 +11639,7 @@
         <v>12</v>
       </c>
       <c r="F461" s="32" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="462" spans="3:6" x14ac:dyDescent="0.2">
@@ -11013,7 +11647,7 @@
         <v>12</v>
       </c>
       <c r="F462" s="32" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="463" spans="3:6" x14ac:dyDescent="0.2">
@@ -11021,7 +11655,7 @@
         <v>12</v>
       </c>
       <c r="F463" s="32" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="464" spans="3:6" x14ac:dyDescent="0.2">
@@ -11029,7 +11663,7 @@
         <v>12</v>
       </c>
       <c r="F464" s="32" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="465" spans="3:6" x14ac:dyDescent="0.2">
@@ -11037,7 +11671,7 @@
         <v>12</v>
       </c>
       <c r="F465" s="32" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="466" spans="3:6" x14ac:dyDescent="0.2">
@@ -11045,7 +11679,7 @@
         <v>12</v>
       </c>
       <c r="F466" s="32" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="467" spans="3:6" x14ac:dyDescent="0.2">
@@ -11053,7 +11687,7 @@
         <v>12</v>
       </c>
       <c r="F467" s="32" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="468" spans="3:6" x14ac:dyDescent="0.2">
@@ -11061,7 +11695,7 @@
         <v>12</v>
       </c>
       <c r="F468" s="32" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="469" spans="3:6" x14ac:dyDescent="0.2">
@@ -11069,7 +11703,7 @@
         <v>12</v>
       </c>
       <c r="F469" s="32" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="470" spans="3:6" x14ac:dyDescent="0.2">
@@ -11077,7 +11711,7 @@
         <v>12</v>
       </c>
       <c r="F470" s="32" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="471" spans="3:6" x14ac:dyDescent="0.2">
@@ -11085,7 +11719,7 @@
         <v>12</v>
       </c>
       <c r="F471" s="32" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="472" spans="3:6" x14ac:dyDescent="0.2">
@@ -11093,7 +11727,7 @@
         <v>12</v>
       </c>
       <c r="F472" s="32" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="473" spans="3:6" x14ac:dyDescent="0.2">
@@ -11101,7 +11735,7 @@
         <v>12</v>
       </c>
       <c r="F473" s="32" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="474" spans="3:6" x14ac:dyDescent="0.2">
@@ -11109,7 +11743,7 @@
         <v>12</v>
       </c>
       <c r="F474" s="32" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="475" spans="3:6" x14ac:dyDescent="0.2">
@@ -11117,32 +11751,17 @@
         <v>12</v>
       </c>
       <c r="F475" s="32" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="476" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C476" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F476" s="32" t="s">
-        <v>417</v>
-      </c>
+      <c r="C476" s="10"/>
     </row>
     <row r="477" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C477" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F477" s="32" t="s">
-        <v>418</v>
-      </c>
+      <c r="C477" s="10"/>
     </row>
     <row r="478" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C478" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F478" s="32" t="s">
-        <v>419</v>
-      </c>
+      <c r="C478" s="10"/>
     </row>
     <row r="479" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C479" s="10"/>
@@ -11162,17 +11781,17 @@
     <row r="484" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C484" s="10"/>
     </row>
-    <row r="485" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C485" s="10"/>
-    </row>
     <row r="486" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C486" s="10"/>
+      <c r="C486" s="25"/>
     </row>
     <row r="487" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C487" s="10"/>
     </row>
+    <row r="488" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C488" s="10"/>
+    </row>
     <row r="489" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C489" s="25"/>
+      <c r="C489" s="10"/>
     </row>
     <row r="490" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C490" s="10"/>
@@ -11251,15 +11870,6 @@
     </row>
     <row r="515" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C515" s="10"/>
-    </row>
-    <row r="516" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C516" s="10"/>
-    </row>
-    <row r="517" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C517" s="10"/>
-    </row>
-    <row r="518" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C518" s="10"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:L1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
END 1st day Low 5/6
</commit_message>
<xml_diff>
--- a/Data/Spring_2023/BenthFun_Alkalinity.xlsx
+++ b/Data/Spring_2023/BenthFun_Alkalinity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremy/Library/Mobile Documents/com~apple~CloudDocs/Documents/Documents/Post-Doc/Projets/Villefranche/Projets/BenthFun – Jeremy/BenthFun/Data/Spring_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F98C46B-1648-5A4D-9A85-A6FE26C11823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E39D3C-66CB-1848-B9C6-1D8AC98F75AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1412,7 +1412,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1502,9 +1502,6 @@
     </xf>
     <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1790,8 +1787,8 @@
   <dimension ref="A1:L515"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="73" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A324" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H340" sqref="H340"/>
+      <pane ySplit="1" topLeftCell="A331" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O345" sqref="O345"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10153,23 +10150,23 @@
       <c r="D338" s="5">
         <v>50.22</v>
       </c>
-      <c r="E338" s="5">
+      <c r="E338" s="14">
         <v>2534.11</v>
       </c>
       <c r="F338" s="32" t="s">
         <v>290</v>
       </c>
-      <c r="G338" s="34">
-        <f>AVERAGE(E339:E340)</f>
-        <v>2575.1899999999996</v>
-      </c>
-      <c r="H338" s="34">
-        <f>STDEV(E339:E340)</f>
-        <v>10.974297244015204</v>
+      <c r="G338" s="18">
+        <f>AVERAGE(E340:E341)</f>
+        <v>2582.8850000000002</v>
+      </c>
+      <c r="H338" s="18">
+        <f>STDEV(E340:E341)</f>
+        <v>9.1923881554006784E-2</v>
       </c>
       <c r="K338" s="5">
         <f>G338+$J$295</f>
-        <v>2579.6349999999998</v>
+        <v>2587.3300000000004</v>
       </c>
     </row>
     <row r="339" spans="1:11" x14ac:dyDescent="0.2">
@@ -10185,7 +10182,7 @@
       <c r="D339" s="5">
         <v>49.38</v>
       </c>
-      <c r="E339" s="5">
+      <c r="E339" s="14">
         <v>2567.4299999999998</v>
       </c>
       <c r="F339" s="32" t="s">
@@ -10225,6 +10222,9 @@
       <c r="D341" s="5">
         <v>49.71</v>
       </c>
+      <c r="E341" s="5">
+        <v>2582.8200000000002</v>
+      </c>
       <c r="F341" s="32" t="s">
         <v>421</v>
       </c>
@@ -10243,22 +10243,22 @@
         <v>49.6</v>
       </c>
       <c r="E342" s="5">
-        <v>2560.94</v>
+        <v>2562.94</v>
       </c>
       <c r="F342" s="32" t="s">
         <v>293</v>
       </c>
       <c r="G342" s="13">
         <f>AVERAGE(E342:E343)</f>
-        <v>2554.1149999999998</v>
+        <v>2555.1149999999998</v>
       </c>
       <c r="H342" s="18">
-        <f>STDEV(E342:E343)</f>
-        <v>9.6520075631964382</v>
+        <f>STDEV(E342,E344)</f>
+        <v>2.9698484809833712</v>
       </c>
       <c r="K342" s="5">
         <f>G342+$J$295</f>
-        <v>2558.56</v>
+        <v>2559.56</v>
       </c>
     </row>
     <row r="343" spans="1:11" x14ac:dyDescent="0.2">
@@ -10274,7 +10274,7 @@
       <c r="D343" s="5">
         <v>52</v>
       </c>
-      <c r="E343" s="5">
+      <c r="E343" s="14">
         <v>2547.29</v>
       </c>
       <c r="F343" s="32" t="s">
@@ -10294,6 +10294,9 @@
       <c r="D344" s="5">
         <v>49.79</v>
       </c>
+      <c r="E344" s="5">
+        <v>2567.14</v>
+      </c>
       <c r="F344" s="32" t="s">
         <v>295</v>
       </c>
@@ -10311,23 +10314,23 @@
       <c r="D345" s="5">
         <v>51.18</v>
       </c>
-      <c r="E345" s="5">
+      <c r="E345" s="14">
         <v>2589.9299999999998</v>
       </c>
       <c r="F345" s="32" t="s">
         <v>296</v>
       </c>
       <c r="G345" s="13">
-        <f>AVERAGE(E345:E346)</f>
-        <v>2585.6799999999998</v>
+        <f>AVERAGE(E346:E347)</f>
+        <v>2580.4549999999999</v>
       </c>
       <c r="H345" s="18">
-        <f>STDEV(E345:E346)</f>
-        <v>6.0104076400856536</v>
+        <f>STDEV(E346:E347)</f>
+        <v>1.3788582233136391</v>
       </c>
       <c r="K345" s="5">
         <f>G345+$J$295</f>
-        <v>2590.125</v>
+        <v>2584.9</v>
       </c>
     </row>
     <row r="346" spans="1:11" x14ac:dyDescent="0.2">
@@ -10362,6 +10365,9 @@
       </c>
       <c r="D347" s="5">
         <v>49.3</v>
+      </c>
+      <c r="E347" s="5">
+        <v>2579.48</v>
       </c>
       <c r="F347" s="32" t="s">
         <v>298</v>

</xml_diff>

<commit_message>
I update the file TA
</commit_message>
<xml_diff>
--- a/Data/Spring_2023/BenthFun_Alkalinity.xlsx
+++ b/Data/Spring_2023/BenthFun_Alkalinity.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11010"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremy/Library/Mobile Documents/com~apple~CloudDocs/Documents/Documents/Post-Doc/Projets/Villefranche/Projets/BenthFun – Jeremy/BenthFun/Data/Spring_2023/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SZNHP213\OneDrive\Desktop\SZN\Jeremy project\Data\Spring_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E39D3C-66CB-1848-B9C6-1D8AC98F75AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1306,7 +1305,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1505,8 +1504,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Excel Built-in Normal" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Excel Built-in Normal" xfId="1"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1783,32 +1782,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L515"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="73" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A331" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O345" sqref="O345"/>
+      <pane ySplit="1" topLeftCell="A343" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E353" sqref="E353"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" style="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.36328125" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.36328125" style="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.81640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1796875" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.6640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.6328125" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.81640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6328125" style="15" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" style="15" customWidth="1"/>
-    <col min="10" max="10" width="12.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.1640625" style="1"/>
+    <col min="10" max="10" width="12.453125" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.453125" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1846,7 +1845,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
@@ -1888,7 +1887,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>11</v>
       </c>
@@ -1914,7 +1913,7 @@
       <c r="K3" s="5"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>11</v>
       </c>
@@ -1949,7 +1948,7 @@
       </c>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
@@ -1975,7 +1974,7 @@
       <c r="K5" s="5"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
         <v>11</v>
       </c>
@@ -2001,7 +2000,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>11</v>
       </c>
@@ -2036,7 +2035,7 @@
       </c>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
@@ -2062,7 +2061,7 @@
       <c r="K8" s="5"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
         <v>11</v>
       </c>
@@ -2088,7 +2087,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
         <v>11</v>
       </c>
@@ -2123,7 +2122,7 @@
       </c>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>11</v>
       </c>
@@ -2148,7 +2147,7 @@
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>11</v>
       </c>
@@ -2173,7 +2172,7 @@
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
         <v>11</v>
       </c>
@@ -2207,7 +2206,7 @@
         <v>2592.88</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
         <v>11</v>
       </c>
@@ -2233,7 +2232,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
         <v>11</v>
       </c>
@@ -2268,7 +2267,7 @@
       </c>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
         <v>11</v>
       </c>
@@ -2293,7 +2292,7 @@
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
         <v>11</v>
       </c>
@@ -2327,7 +2326,7 @@
         <v>2621.1999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
         <v>11</v>
       </c>
@@ -2352,7 +2351,7 @@
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
         <v>11</v>
       </c>
@@ -2377,7 +2376,7 @@
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
         <v>11</v>
       </c>
@@ -2411,7 +2410,7 @@
         <v>2553.7799999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
         <v>11</v>
       </c>
@@ -2436,7 +2435,7 @@
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
         <v>11</v>
       </c>
@@ -2461,7 +2460,7 @@
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
         <v>11</v>
       </c>
@@ -2495,7 +2494,7 @@
         <v>2531.04</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
         <v>11</v>
       </c>
@@ -2520,7 +2519,7 @@
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" s="9" t="s">
         <v>11</v>
       </c>
@@ -2554,7 +2553,7 @@
         <v>2487.5749999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="9" t="s">
         <v>11</v>
       </c>
@@ -2579,7 +2578,7 @@
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="9" t="s">
         <v>11</v>
       </c>
@@ -2604,7 +2603,7 @@
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" s="9" t="s">
         <v>11</v>
       </c>
@@ -2638,7 +2637,7 @@
         <v>2606.9649999999997</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
         <v>11</v>
       </c>
@@ -2663,7 +2662,7 @@
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" s="9" t="s">
         <v>11</v>
       </c>
@@ -2688,7 +2687,7 @@
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" s="9"/>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
@@ -2699,7 +2698,7 @@
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
         <v>11</v>
       </c>
@@ -2741,7 +2740,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" s="9" t="s">
         <v>11</v>
       </c>
@@ -2766,7 +2765,7 @@
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" s="9" t="s">
         <v>11</v>
       </c>
@@ -2798,7 +2797,7 @@
         <v>2658.0949999999998</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" s="9" t="s">
         <v>11</v>
       </c>
@@ -2818,7 +2817,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" s="9" t="s">
         <v>11</v>
       </c>
@@ -2850,7 +2849,7 @@
         <v>2655.7449999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" s="9" t="s">
         <v>11</v>
       </c>
@@ -2870,7 +2869,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" s="9" t="s">
         <v>11</v>
       </c>
@@ -2890,7 +2889,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
         <v>11</v>
       </c>
@@ -2922,7 +2921,7 @@
         <v>2591.3400000000006</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" s="9" t="s">
         <v>11</v>
       </c>
@@ -2942,7 +2941,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41" s="9" t="s">
         <v>11</v>
       </c>
@@ -2962,7 +2961,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42" s="9" t="s">
         <v>11</v>
       </c>
@@ -2982,7 +2981,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" s="9" t="s">
         <v>11</v>
       </c>
@@ -3014,7 +3013,7 @@
         <v>2576.5950000000007</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44" s="9" t="s">
         <v>11</v>
       </c>
@@ -3034,7 +3033,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45" s="9" t="s">
         <v>11</v>
       </c>
@@ -3054,7 +3053,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46" s="9" t="s">
         <v>11</v>
       </c>
@@ -3086,7 +3085,7 @@
         <v>2579.6250000000005</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47" s="9" t="s">
         <v>11</v>
       </c>
@@ -3106,7 +3105,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48" s="9" t="s">
         <v>11</v>
       </c>
@@ -3126,7 +3125,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49" s="9" t="s">
         <v>11</v>
       </c>
@@ -3158,7 +3157,7 @@
         <v>2650.0800000000004</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50" s="9" t="s">
         <v>11</v>
       </c>
@@ -3178,7 +3177,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51" s="9" t="s">
         <v>11</v>
       </c>
@@ -3210,7 +3209,7 @@
         <v>2556.6850000000004</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52" s="9" t="s">
         <v>11</v>
       </c>
@@ -3230,7 +3229,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53" s="9" t="s">
         <v>11</v>
       </c>
@@ -3250,7 +3249,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54" s="9" t="s">
         <v>11</v>
       </c>
@@ -3282,7 +3281,7 @@
         <v>2532.8100000000004</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55" s="9" t="s">
         <v>11</v>
       </c>
@@ -3302,7 +3301,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56" s="9" t="s">
         <v>11</v>
       </c>
@@ -3334,7 +3333,7 @@
         <v>2540.77</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57" s="9" t="s">
         <v>11</v>
       </c>
@@ -3354,7 +3353,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58" s="9" t="s">
         <v>11</v>
       </c>
@@ -3386,7 +3385,7 @@
         <v>2633.7750000000001</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59" s="9" t="s">
         <v>11</v>
       </c>
@@ -3406,10 +3405,10 @@
         <v>64</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B60" s="15"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61" s="9" t="s">
         <v>11</v>
       </c>
@@ -3451,7 +3450,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A62" s="9" t="s">
         <v>11</v>
       </c>
@@ -3476,7 +3475,7 @@
       <c r="J62" s="5"/>
       <c r="K62" s="5"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A63" s="9" t="s">
         <v>11</v>
       </c>
@@ -3508,7 +3507,7 @@
         <v>2674.7000000000003</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A64" s="9" t="s">
         <v>11</v>
       </c>
@@ -3528,7 +3527,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A65" s="9" t="s">
         <v>11</v>
       </c>
@@ -3548,7 +3547,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A66" s="9" t="s">
         <v>11</v>
       </c>
@@ -3580,7 +3579,7 @@
         <v>2650.1000000000004</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A67" s="9" t="s">
         <v>11</v>
       </c>
@@ -3600,7 +3599,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A68" s="9" t="s">
         <v>11</v>
       </c>
@@ -3620,7 +3619,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A69" s="9" t="s">
         <v>11</v>
       </c>
@@ -3652,7 +3651,7 @@
         <v>2343.2800000000002</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A70" s="9" t="s">
         <v>11</v>
       </c>
@@ -3672,7 +3671,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A71" s="9" t="s">
         <v>11</v>
       </c>
@@ -3704,7 +3703,7 @@
         <v>2642.0000000000005</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A72" s="9" t="s">
         <v>11</v>
       </c>
@@ -3724,7 +3723,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A73" s="9" t="s">
         <v>11</v>
       </c>
@@ -3756,7 +3755,7 @@
         <v>2620.7650000000003</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A74" s="9" t="s">
         <v>11</v>
       </c>
@@ -3776,7 +3775,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A75" s="9" t="s">
         <v>11</v>
       </c>
@@ -3808,7 +3807,7 @@
         <v>2663.0850000000005</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A76" s="9" t="s">
         <v>11</v>
       </c>
@@ -3828,7 +3827,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A77" s="9" t="s">
         <v>11</v>
       </c>
@@ -3848,7 +3847,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A78" s="9" t="s">
         <v>11</v>
       </c>
@@ -3880,7 +3879,7 @@
         <v>2576.9600000000005</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A79" s="9" t="s">
         <v>11</v>
       </c>
@@ -3900,7 +3899,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A80" s="9" t="s">
         <v>11</v>
       </c>
@@ -3920,7 +3919,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A81" s="9" t="s">
         <v>11</v>
       </c>
@@ -3952,7 +3951,7 @@
         <v>2584.4350000000004</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A82" s="9" t="s">
         <v>11</v>
       </c>
@@ -3972,7 +3971,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A83" s="9" t="s">
         <v>11</v>
       </c>
@@ -3992,7 +3991,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A84" s="9" t="s">
         <v>11</v>
       </c>
@@ -4024,7 +4023,7 @@
         <v>2557.5100000000002</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A85" s="9" t="s">
         <v>11</v>
       </c>
@@ -4044,7 +4043,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A86" s="9" t="s">
         <v>11</v>
       </c>
@@ -4064,7 +4063,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A87" s="9" t="s">
         <v>11</v>
       </c>
@@ -4096,7 +4095,7 @@
         <v>2654.3750000000005</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A88" s="9" t="s">
         <v>11</v>
       </c>
@@ -4116,10 +4115,10 @@
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B89" s="15"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A90" s="9" t="s">
         <v>11</v>
       </c>
@@ -4161,7 +4160,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A91" s="9" t="s">
         <v>11</v>
       </c>
@@ -4181,7 +4180,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A92" s="9" t="s">
         <v>11</v>
       </c>
@@ -4201,7 +4200,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A93" s="9" t="s">
         <v>11</v>
       </c>
@@ -4235,7 +4234,7 @@
         <v>2577.4450000000002</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A94" s="9" t="s">
         <v>11</v>
       </c>
@@ -4255,7 +4254,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A95" s="9" t="s">
         <v>11</v>
       </c>
@@ -4275,7 +4274,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A96" s="9" t="s">
         <v>11</v>
       </c>
@@ -4309,7 +4308,7 @@
         <v>2554.8049999999998</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A97" s="9" t="s">
         <v>11</v>
       </c>
@@ -4329,7 +4328,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A98" s="9" t="s">
         <v>11</v>
       </c>
@@ -4363,7 +4362,7 @@
         <v>3002.58</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A99" s="9" t="s">
         <v>11</v>
       </c>
@@ -4383,7 +4382,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A100" s="9" t="s">
         <v>11</v>
       </c>
@@ -4403,7 +4402,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A101" s="9" t="s">
         <v>11</v>
       </c>
@@ -4437,7 +4436,7 @@
         <v>2990.2099999999996</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A102" s="9" t="s">
         <v>11</v>
       </c>
@@ -4457,7 +4456,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A103" s="9" t="s">
         <v>11</v>
       </c>
@@ -4477,7 +4476,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A104" s="9" t="s">
         <v>11</v>
       </c>
@@ -4511,7 +4510,7 @@
         <v>2976.65</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A105" s="9" t="s">
         <v>11</v>
       </c>
@@ -4531,7 +4530,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A106" s="9" t="s">
         <v>11</v>
       </c>
@@ -4551,7 +4550,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A107" s="9" t="s">
         <v>11</v>
       </c>
@@ -4585,7 +4584,7 @@
         <v>2658.28</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A108" s="9" t="s">
         <v>11</v>
       </c>
@@ -4605,7 +4604,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A109" s="9" t="s">
         <v>11</v>
       </c>
@@ -4625,7 +4624,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A110" s="9" t="s">
         <v>11</v>
       </c>
@@ -4659,7 +4658,7 @@
         <v>2641.56</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A111" s="9" t="s">
         <v>11</v>
       </c>
@@ -4679,7 +4678,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A112" s="9" t="s">
         <v>11</v>
       </c>
@@ -4699,7 +4698,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A113" s="9" t="s">
         <v>11</v>
       </c>
@@ -4733,7 +4732,7 @@
         <v>2651.5699999999997</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A114" s="9" t="s">
         <v>11</v>
       </c>
@@ -4753,7 +4752,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A115" s="9" t="s">
         <v>11</v>
       </c>
@@ -4787,7 +4786,7 @@
         <v>2646.5849999999996</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A116" s="9" t="s">
         <v>11</v>
       </c>
@@ -4807,7 +4806,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A117" s="9" t="s">
         <v>11</v>
       </c>
@@ -4827,7 +4826,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A118" s="9" t="s">
         <v>11</v>
       </c>
@@ -4861,7 +4860,7 @@
         <v>2577.77</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A119" s="9" t="s">
         <v>11</v>
       </c>
@@ -4881,7 +4880,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A120" s="9" t="s">
         <v>11</v>
       </c>
@@ -4901,10 +4900,10 @@
         <v>124</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B121" s="15"/>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A122" s="9" t="s">
         <v>152</v>
       </c>
@@ -4946,7 +4945,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A123" s="9" t="s">
         <v>152</v>
       </c>
@@ -4966,7 +4965,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A124" s="9" t="s">
         <v>152</v>
       </c>
@@ -4986,7 +4985,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A125" s="9" t="s">
         <v>11</v>
       </c>
@@ -5020,7 +5019,7 @@
         <v>2535.7849999999999</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A126" s="9" t="s">
         <v>11</v>
       </c>
@@ -5040,7 +5039,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A127" s="9" t="s">
         <v>11</v>
       </c>
@@ -5060,7 +5059,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A128" s="9" t="s">
         <v>11</v>
       </c>
@@ -5094,7 +5093,7 @@
         <v>2540.9899999999998</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A129" s="9" t="s">
         <v>11</v>
       </c>
@@ -5114,7 +5113,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A130" s="9" t="s">
         <v>11</v>
       </c>
@@ -5134,7 +5133,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A131" s="9" t="s">
         <v>11</v>
       </c>
@@ -5168,7 +5167,7 @@
         <v>2484.7750000000001</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A132" s="9" t="s">
         <v>11</v>
       </c>
@@ -5188,7 +5187,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A133" s="9" t="s">
         <v>11</v>
       </c>
@@ -5222,7 +5221,7 @@
         <v>2483.7199999999998</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A134" s="9" t="s">
         <v>11</v>
       </c>
@@ -5242,7 +5241,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A135" s="9" t="s">
         <v>11</v>
       </c>
@@ -5262,7 +5261,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A136" s="9" t="s">
         <v>11</v>
       </c>
@@ -5296,7 +5295,7 @@
         <v>2488.9699999999998</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A137" s="9" t="s">
         <v>11</v>
       </c>
@@ -5316,7 +5315,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A138" s="9" t="s">
         <v>11</v>
       </c>
@@ -5350,7 +5349,7 @@
         <v>2530.96</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A139" s="9" t="s">
         <v>11</v>
       </c>
@@ -5370,7 +5369,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A140" s="9" t="s">
         <v>11</v>
       </c>
@@ -5390,7 +5389,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A141" s="9" t="s">
         <v>11</v>
       </c>
@@ -5424,7 +5423,7 @@
         <v>2465.5749999999998</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A142" s="9" t="s">
         <v>11</v>
       </c>
@@ -5444,7 +5443,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A143" s="9" t="s">
         <v>11</v>
       </c>
@@ -5478,7 +5477,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A144" s="9" t="s">
         <v>11</v>
       </c>
@@ -5498,7 +5497,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A145" s="9" t="s">
         <v>11</v>
       </c>
@@ -5518,7 +5517,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A146" s="9" t="s">
         <v>152</v>
       </c>
@@ -5552,7 +5551,7 @@
         <v>2488.0249999999996</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A147" s="9" t="s">
         <v>152</v>
       </c>
@@ -5572,7 +5571,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A148" s="9" t="s">
         <v>152</v>
       </c>
@@ -5592,7 +5591,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A149" s="9" t="s">
         <v>152</v>
       </c>
@@ -5626,7 +5625,7 @@
         <v>2545.1</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A150" s="9" t="s">
         <v>152</v>
       </c>
@@ -5646,7 +5645,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A151" s="9" t="s">
         <v>152</v>
       </c>
@@ -5666,14 +5665,14 @@
         <v>149</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A152" s="9"/>
       <c r="B152" s="10"/>
       <c r="C152" s="10"/>
       <c r="E152" s="14"/>
       <c r="F152" s="16"/>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A153" s="9" t="s">
         <v>11</v>
       </c>
@@ -5715,7 +5714,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A154" s="9" t="s">
         <v>11</v>
       </c>
@@ -5735,7 +5734,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A155" s="9" t="s">
         <v>11</v>
       </c>
@@ -5769,7 +5768,7 @@
         <v>2542.6099999999997</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A156" s="9" t="s">
         <v>11</v>
       </c>
@@ -5789,7 +5788,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A157" s="9" t="s">
         <v>11</v>
       </c>
@@ -5809,7 +5808,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A158" s="9" t="s">
         <v>11</v>
       </c>
@@ -5843,7 +5842,7 @@
         <v>2554.4999999999995</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A159" s="9" t="s">
         <v>11</v>
       </c>
@@ -5863,7 +5862,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A160" s="9" t="s">
         <v>11</v>
       </c>
@@ -5883,7 +5882,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A161" s="9" t="s">
         <v>11</v>
       </c>
@@ -5917,7 +5916,7 @@
         <v>2472.7099999999996</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A162" s="9" t="s">
         <v>11</v>
       </c>
@@ -5937,7 +5936,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A163" s="9" t="s">
         <v>11</v>
       </c>
@@ -5957,7 +5956,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A164" s="9" t="s">
         <v>11</v>
       </c>
@@ -5991,7 +5990,7 @@
         <v>2509.61</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A165" s="9" t="s">
         <v>11</v>
       </c>
@@ -6011,7 +6010,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A166" s="9" t="s">
         <v>11</v>
       </c>
@@ -6031,7 +6030,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A167" s="9" t="s">
         <v>11</v>
       </c>
@@ -6065,7 +6064,7 @@
         <v>2514.2399999999998</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A168" s="9" t="s">
         <v>11</v>
       </c>
@@ -6085,7 +6084,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A169" s="9" t="s">
         <v>11</v>
       </c>
@@ -6119,7 +6118,7 @@
         <v>2549.4999999999995</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A170" s="9" t="s">
         <v>11</v>
       </c>
@@ -6139,7 +6138,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A171" s="9" t="s">
         <v>11</v>
       </c>
@@ -6159,7 +6158,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A172" s="9" t="s">
         <v>11</v>
       </c>
@@ -6193,7 +6192,7 @@
         <v>2483.7800000000002</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A173" s="9" t="s">
         <v>11</v>
       </c>
@@ -6213,7 +6212,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A174" s="9" t="s">
         <v>11</v>
       </c>
@@ -6233,7 +6232,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="175" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A175" s="24" t="s">
         <v>11</v>
       </c>
@@ -6267,7 +6266,7 @@
         <v>2442.1749999999997</v>
       </c>
     </row>
-    <row r="176" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A176" s="24" t="s">
         <v>11</v>
       </c>
@@ -6292,7 +6291,7 @@
       <c r="J176" s="29"/>
       <c r="K176" s="29"/>
     </row>
-    <row r="177" spans="1:12" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:12" s="28" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A177" s="24" t="s">
         <v>11</v>
       </c>
@@ -6317,7 +6316,7 @@
       <c r="J177" s="29"/>
       <c r="K177" s="29"/>
     </row>
-    <row r="178" spans="1:12" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:12" s="28" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A178" s="24" t="s">
         <v>11</v>
       </c>
@@ -6351,7 +6350,7 @@
         <v>2454.9850000000001</v>
       </c>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A179" s="9" t="s">
         <v>11</v>
       </c>
@@ -6376,7 +6375,7 @@
       <c r="J179" s="1"/>
       <c r="K179" s="1"/>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A180" s="9" t="s">
         <v>11</v>
       </c>
@@ -6396,7 +6395,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A181" s="9" t="s">
         <v>11</v>
       </c>
@@ -6431,7 +6430,7 @@
       </c>
       <c r="L181" s="28"/>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A182" s="9" t="s">
         <v>11</v>
       </c>
@@ -6451,7 +6450,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A183" s="9" t="s">
         <v>11</v>
       </c>
@@ -6471,10 +6470,10 @@
         <v>156</v>
       </c>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B184" s="15"/>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A185" s="15" t="s">
         <v>152</v>
       </c>
@@ -6516,7 +6515,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A186" s="15" t="s">
         <v>152</v>
       </c>
@@ -6536,7 +6535,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A187" s="15" t="s">
         <v>152</v>
       </c>
@@ -6556,7 +6555,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A188" s="15" t="s">
         <v>152</v>
       </c>
@@ -6588,7 +6587,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A189" s="15" t="s">
         <v>152</v>
       </c>
@@ -6608,7 +6607,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A190" s="15" t="s">
         <v>152</v>
       </c>
@@ -6628,7 +6627,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A191" s="15" t="s">
         <v>152</v>
       </c>
@@ -6660,7 +6659,7 @@
         <v>2575.6150000000002</v>
       </c>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A192" s="15" t="s">
         <v>152</v>
       </c>
@@ -6680,7 +6679,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A193" s="15" t="s">
         <v>152</v>
       </c>
@@ -6700,7 +6699,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A194" s="15" t="s">
         <v>152</v>
       </c>
@@ -6720,7 +6719,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A195" s="15" t="s">
         <v>152</v>
       </c>
@@ -6752,7 +6751,7 @@
         <v>2558.6349999999998</v>
       </c>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A196" s="15" t="s">
         <v>152</v>
       </c>
@@ -6772,7 +6771,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A197" s="15" t="s">
         <v>152</v>
       </c>
@@ -6792,7 +6791,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A198" s="9" t="s">
         <v>11</v>
       </c>
@@ -6824,7 +6823,7 @@
         <v>2583.3199999999997</v>
       </c>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A199" s="9" t="s">
         <v>11</v>
       </c>
@@ -6844,7 +6843,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A200" s="9" t="s">
         <v>11</v>
       </c>
@@ -6864,7 +6863,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A201" s="9" t="s">
         <v>11</v>
       </c>
@@ -6896,7 +6895,7 @@
         <v>2594.98</v>
       </c>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A202" s="9" t="s">
         <v>11</v>
       </c>
@@ -6916,7 +6915,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A203" s="9" t="s">
         <v>11</v>
       </c>
@@ -6936,7 +6935,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A204" s="9" t="s">
         <v>11</v>
       </c>
@@ -6968,7 +6967,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A205" s="9" t="s">
         <v>11</v>
       </c>
@@ -6988,7 +6987,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A206" s="24" t="s">
         <v>11</v>
       </c>
@@ -7008,7 +7007,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A207" s="24" t="s">
         <v>11</v>
       </c>
@@ -7040,7 +7039,7 @@
         <v>2564.5749999999998</v>
       </c>
     </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A208" s="24" t="s">
         <v>11</v>
       </c>
@@ -7060,7 +7059,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A209" s="9" t="s">
         <v>11</v>
       </c>
@@ -7092,7 +7091,7 @@
         <v>2552.5749999999998</v>
       </c>
     </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A210" s="9" t="s">
         <v>11</v>
       </c>
@@ -7112,7 +7111,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A211" s="9" t="s">
         <v>11</v>
       </c>
@@ -7132,7 +7131,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A212" s="9" t="s">
         <v>11</v>
       </c>
@@ -7153,11 +7152,11 @@
       </c>
       <c r="J212" s="5"/>
     </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A213" s="9"/>
       <c r="B213" s="15"/>
     </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A214" s="9" t="s">
         <v>11</v>
       </c>
@@ -7199,7 +7198,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A215" s="9" t="s">
         <v>11</v>
       </c>
@@ -7219,7 +7218,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A216" s="9" t="s">
         <v>11</v>
       </c>
@@ -7239,7 +7238,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A217" s="9" t="s">
         <v>11</v>
       </c>
@@ -7271,7 +7270,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A218" s="9" t="s">
         <v>11</v>
       </c>
@@ -7296,7 +7295,7 @@
       <c r="J218" s="1"/>
       <c r="K218" s="1"/>
     </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A219" s="9" t="s">
         <v>11</v>
       </c>
@@ -7321,7 +7320,7 @@
       <c r="J219" s="1"/>
       <c r="K219" s="1"/>
     </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A220" s="9" t="s">
         <v>11</v>
       </c>
@@ -7353,7 +7352,7 @@
         <v>2558.1749999999997</v>
       </c>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A221" s="9" t="s">
         <v>11</v>
       </c>
@@ -7373,7 +7372,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A222" s="9" t="s">
         <v>11</v>
       </c>
@@ -7405,7 +7404,7 @@
         <v>2557.5000000000005</v>
       </c>
     </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A223" s="9" t="s">
         <v>11</v>
       </c>
@@ -7425,7 +7424,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A224" s="9" t="s">
         <v>11</v>
       </c>
@@ -7445,7 +7444,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A225" s="9" t="s">
         <v>11</v>
       </c>
@@ -7477,7 +7476,7 @@
         <v>2559.2450000000003</v>
       </c>
     </row>
-    <row r="226" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A226" s="9" t="s">
         <v>11</v>
       </c>
@@ -7497,7 +7496,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="227" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A227" s="9" t="s">
         <v>11</v>
       </c>
@@ -7529,7 +7528,7 @@
         <v>2553.0500000000002</v>
       </c>
     </row>
-    <row r="228" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A228" s="9" t="s">
         <v>11</v>
       </c>
@@ -7549,7 +7548,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="229" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A229" s="9" t="s">
         <v>11</v>
       </c>
@@ -7569,7 +7568,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="230" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A230" s="9" t="s">
         <v>11</v>
       </c>
@@ -7601,7 +7600,7 @@
         <v>2575.61</v>
       </c>
     </row>
-    <row r="231" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A231" s="9" t="s">
         <v>11</v>
       </c>
@@ -7621,7 +7620,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="232" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A232" s="9" t="s">
         <v>11</v>
       </c>
@@ -7641,7 +7640,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="233" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A233" s="9" t="s">
         <v>11</v>
       </c>
@@ -7673,7 +7672,7 @@
         <v>2561.8700000000003</v>
       </c>
     </row>
-    <row r="234" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A234" s="9" t="s">
         <v>11</v>
       </c>
@@ -7693,7 +7692,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="236" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A236" s="9" t="s">
         <v>11</v>
       </c>
@@ -7725,7 +7724,7 @@
         <v>2596.6350000000002</v>
       </c>
     </row>
-    <row r="237" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A237" s="9" t="s">
         <v>11</v>
       </c>
@@ -7745,7 +7744,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="238" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A238" s="9" t="s">
         <v>11</v>
       </c>
@@ -7765,7 +7764,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="239" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A239" s="9" t="s">
         <v>11</v>
       </c>
@@ -7797,7 +7796,7 @@
         <v>2574.5550000000003</v>
       </c>
     </row>
-    <row r="240" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A240" s="9" t="s">
         <v>11</v>
       </c>
@@ -7817,7 +7816,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="241" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A241" s="9" t="s">
         <v>11</v>
       </c>
@@ -7849,7 +7848,7 @@
         <v>2572.5350000000003</v>
       </c>
     </row>
-    <row r="242" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A242" s="9" t="s">
         <v>11</v>
       </c>
@@ -7869,7 +7868,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="243" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A243" s="9" t="s">
         <v>11</v>
       </c>
@@ -7889,7 +7888,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="244" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A244" s="9" t="s">
         <v>11</v>
       </c>
@@ -7909,7 +7908,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="245" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A245" s="9" t="s">
         <v>11</v>
       </c>
@@ -7941,7 +7940,7 @@
         <v>2567.5250000000001</v>
       </c>
     </row>
-    <row r="246" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A246" s="9" t="s">
         <v>11</v>
       </c>
@@ -7961,7 +7960,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="247" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A247" s="9" t="s">
         <v>11</v>
       </c>
@@ -7993,7 +7992,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="248" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A248" s="9" t="s">
         <v>11</v>
       </c>
@@ -8018,7 +8017,7 @@
       <c r="J248" s="1"/>
       <c r="K248" s="1"/>
     </row>
-    <row r="249" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A249" s="9" t="s">
         <v>11</v>
       </c>
@@ -8043,7 +8042,7 @@
       <c r="J249" s="1"/>
       <c r="K249" s="1"/>
     </row>
-    <row r="250" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A250" s="9" t="s">
         <v>11</v>
       </c>
@@ -8075,7 +8074,7 @@
         <v>2580.6</v>
       </c>
     </row>
-    <row r="251" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A251" s="9" t="s">
         <v>11</v>
       </c>
@@ -8095,7 +8094,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="252" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A252" s="9" t="s">
         <v>11</v>
       </c>
@@ -8127,7 +8126,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="253" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A253" s="9" t="s">
         <v>11</v>
       </c>
@@ -8147,7 +8146,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="254" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A254" s="9" t="s">
         <v>11</v>
       </c>
@@ -8167,11 +8166,11 @@
         <v>213</v>
       </c>
     </row>
-    <row r="255" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:12" x14ac:dyDescent="0.35">
       <c r="E255" s="14"/>
       <c r="F255" s="1"/>
     </row>
-    <row r="256" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A256" s="9" t="s">
         <v>11</v>
       </c>
@@ -8213,7 +8212,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="257" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A257" s="9" t="s">
         <v>11</v>
       </c>
@@ -8233,7 +8232,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="258" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A258" s="9" t="s">
         <v>11</v>
       </c>
@@ -8253,7 +8252,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="259" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A259" s="9" t="s">
         <v>11</v>
       </c>
@@ -8285,7 +8284,7 @@
         <v>2680</v>
       </c>
     </row>
-    <row r="260" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A260" s="9" t="s">
         <v>11</v>
       </c>
@@ -8305,7 +8304,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="261" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A261" s="9" t="s">
         <v>11</v>
       </c>
@@ -8337,7 +8336,7 @@
         <v>2823.9250000000002</v>
       </c>
     </row>
-    <row r="262" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A262" s="9" t="s">
         <v>11</v>
       </c>
@@ -8357,7 +8356,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="263" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A263" s="9" t="s">
         <v>11</v>
       </c>
@@ -8377,7 +8376,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="264" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A264" s="9" t="s">
         <v>11</v>
       </c>
@@ -8409,7 +8408,7 @@
         <v>2693.895</v>
       </c>
     </row>
-    <row r="265" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A265" s="9" t="s">
         <v>11</v>
       </c>
@@ -8429,7 +8428,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="266" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A266" s="9" t="s">
         <v>11</v>
       </c>
@@ -8449,7 +8448,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="267" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A267" s="9" t="s">
         <v>11</v>
       </c>
@@ -8481,7 +8480,7 @@
         <v>2592.4700000000003</v>
       </c>
     </row>
-    <row r="268" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A268" s="9" t="s">
         <v>11</v>
       </c>
@@ -8501,7 +8500,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="269" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A269" s="9" t="s">
         <v>11</v>
       </c>
@@ -8521,7 +8520,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="270" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A270" s="9" t="s">
         <v>11</v>
       </c>
@@ -8553,7 +8552,7 @@
         <v>2959.9100000000003</v>
       </c>
     </row>
-    <row r="271" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A271" s="9" t="s">
         <v>11</v>
       </c>
@@ -8573,7 +8572,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="272" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A272" s="9" t="s">
         <v>11</v>
       </c>
@@ -8593,7 +8592,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="273" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A273" s="9" t="s">
         <v>11</v>
       </c>
@@ -8625,7 +8624,7 @@
         <v>2869.5400000000004</v>
       </c>
     </row>
-    <row r="274" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A274" s="9" t="s">
         <v>11</v>
       </c>
@@ -8645,7 +8644,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="275" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A275" s="9" t="s">
         <v>11</v>
       </c>
@@ -8677,7 +8676,7 @@
         <v>2875.6350000000007</v>
       </c>
     </row>
-    <row r="276" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A276" s="9" t="s">
         <v>11</v>
       </c>
@@ -8697,7 +8696,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="277" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A277" s="9" t="s">
         <v>11</v>
       </c>
@@ -8717,7 +8716,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="278" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A278" s="9" t="s">
         <v>11</v>
       </c>
@@ -8749,7 +8748,7 @@
         <v>2867.1150000000002</v>
       </c>
     </row>
-    <row r="279" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A279" s="9" t="s">
         <v>11</v>
       </c>
@@ -8769,7 +8768,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="280" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A280" s="9" t="s">
         <v>11</v>
       </c>
@@ -8801,7 +8800,7 @@
         <v>2865.9250000000006</v>
       </c>
     </row>
-    <row r="281" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A281" s="9" t="s">
         <v>11</v>
       </c>
@@ -8821,7 +8820,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="282" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A282" s="9" t="s">
         <v>11</v>
       </c>
@@ -8853,7 +8852,7 @@
         <v>2667.4650000000006</v>
       </c>
     </row>
-    <row r="283" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A283" s="9" t="s">
         <v>11</v>
       </c>
@@ -8873,7 +8872,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="284" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A284" s="9" t="s">
         <v>11</v>
       </c>
@@ -8893,7 +8892,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="285" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A285" s="9" t="s">
         <v>11</v>
       </c>
@@ -8925,7 +8924,7 @@
         <v>2791.6800000000003</v>
       </c>
     </row>
-    <row r="286" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A286" s="9" t="s">
         <v>11</v>
       </c>
@@ -8945,7 +8944,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="287" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A287" s="9" t="s">
         <v>11</v>
       </c>
@@ -8965,7 +8964,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="288" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A288" s="9" t="s">
         <v>11</v>
       </c>
@@ -8997,7 +8996,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="289" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A289" s="9" t="s">
         <v>11</v>
       </c>
@@ -9017,7 +9016,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="290" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A290" s="9" t="s">
         <v>11</v>
       </c>
@@ -9037,7 +9036,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="291" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A291" s="9" t="s">
         <v>11</v>
       </c>
@@ -9069,7 +9068,7 @@
         <v>2665.1500000000005</v>
       </c>
     </row>
-    <row r="292" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A292" s="9" t="s">
         <v>11</v>
       </c>
@@ -9089,7 +9088,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="293" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A293" s="9" t="s">
         <v>11</v>
       </c>
@@ -9109,10 +9108,10 @@
         <v>419</v>
       </c>
     </row>
-    <row r="294" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:12" x14ac:dyDescent="0.35">
       <c r="F294" s="32"/>
     </row>
-    <row r="295" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A295" s="9" t="s">
         <v>11</v>
       </c>
@@ -9154,7 +9153,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="296" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A296" s="9" t="s">
         <v>11</v>
       </c>
@@ -9174,7 +9173,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="297" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A297" s="9" t="s">
         <v>11</v>
       </c>
@@ -9194,7 +9193,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="298" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A298" s="9" t="s">
         <v>11</v>
       </c>
@@ -9226,7 +9225,7 @@
         <v>2683.1600000000003</v>
       </c>
     </row>
-    <row r="299" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A299" s="9" t="s">
         <v>11</v>
       </c>
@@ -9246,7 +9245,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="300" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A300" s="9" t="s">
         <v>11</v>
       </c>
@@ -9266,7 +9265,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="301" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A301" s="9" t="s">
         <v>11</v>
       </c>
@@ -9298,7 +9297,7 @@
         <v>2767.9650000000001</v>
       </c>
     </row>
-    <row r="302" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A302" s="9" t="s">
         <v>11</v>
       </c>
@@ -9318,7 +9317,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="303" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A303" s="9" t="s">
         <v>11</v>
       </c>
@@ -9338,7 +9337,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="304" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A304" s="9" t="s">
         <v>11</v>
       </c>
@@ -9370,7 +9369,7 @@
         <v>2664.9050000000002</v>
       </c>
     </row>
-    <row r="305" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A305" s="9" t="s">
         <v>11</v>
       </c>
@@ -9390,7 +9389,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="306" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A306" s="9" t="s">
         <v>11</v>
       </c>
@@ -9410,7 +9409,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="307" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A307" s="9" t="s">
         <v>11</v>
       </c>
@@ -9442,7 +9441,7 @@
         <v>2507.11</v>
       </c>
     </row>
-    <row r="308" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A308" s="9" t="s">
         <v>11</v>
       </c>
@@ -9462,7 +9461,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="309" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A309" s="9" t="s">
         <v>11</v>
       </c>
@@ -9482,7 +9481,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="310" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A310" s="9" t="s">
         <v>11</v>
       </c>
@@ -9514,7 +9513,7 @@
         <v>2560.5800000000004</v>
       </c>
     </row>
-    <row r="311" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A311" s="9" t="s">
         <v>11</v>
       </c>
@@ -9534,7 +9533,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="312" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A312" s="9" t="s">
         <v>11</v>
       </c>
@@ -9554,7 +9553,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="313" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A313" s="9" t="s">
         <v>11</v>
       </c>
@@ -9586,7 +9585,7 @@
         <v>2551.7550000000001</v>
       </c>
     </row>
-    <row r="314" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A314" s="9" t="s">
         <v>11</v>
       </c>
@@ -9606,7 +9605,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="315" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A315" s="9" t="s">
         <v>11</v>
       </c>
@@ -9626,7 +9625,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="316" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A316" s="9" t="s">
         <v>11</v>
       </c>
@@ -9646,7 +9645,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="317" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A317" s="9" t="s">
         <v>11</v>
       </c>
@@ -9678,7 +9677,7 @@
         <v>2608.48</v>
       </c>
     </row>
-    <row r="318" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A318" s="9" t="s">
         <v>11</v>
       </c>
@@ -9698,7 +9697,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="319" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A319" s="9" t="s">
         <v>11</v>
       </c>
@@ -9718,7 +9717,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="320" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A320" s="9" t="s">
         <v>11</v>
       </c>
@@ -9750,7 +9749,7 @@
         <v>2651.3050000000003</v>
       </c>
     </row>
-    <row r="321" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A321" s="9" t="s">
         <v>11</v>
       </c>
@@ -9770,7 +9769,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="322" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A322" s="9" t="s">
         <v>11</v>
       </c>
@@ -9790,7 +9789,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="323" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A323" s="9" t="s">
         <v>11</v>
       </c>
@@ -9822,7 +9821,7 @@
         <v>2616.8150000000001</v>
       </c>
     </row>
-    <row r="324" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A324" s="9" t="s">
         <v>11</v>
       </c>
@@ -9842,7 +9841,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="325" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A325" s="9" t="s">
         <v>11</v>
       </c>
@@ -9874,7 +9873,7 @@
         <v>2532.7950000000005</v>
       </c>
     </row>
-    <row r="326" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A326" s="9" t="s">
         <v>11</v>
       </c>
@@ -9894,7 +9893,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="327" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A327" s="9" t="s">
         <v>11</v>
       </c>
@@ -9926,7 +9925,7 @@
         <v>2626.605</v>
       </c>
     </row>
-    <row r="328" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A328" s="9" t="s">
         <v>11</v>
       </c>
@@ -9946,7 +9945,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="329" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A329" s="9" t="s">
         <v>11</v>
       </c>
@@ -9978,7 +9977,7 @@
         <v>2579.8250000000003</v>
       </c>
     </row>
-    <row r="330" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A330" s="9" t="s">
         <v>11</v>
       </c>
@@ -9998,7 +9997,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="331" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A331" s="9" t="s">
         <v>11</v>
       </c>
@@ -10018,10 +10017,10 @@
         <v>287</v>
       </c>
     </row>
-    <row r="332" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C332" s="10"/>
     </row>
-    <row r="333" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A333" s="9" t="s">
         <v>11</v>
       </c>
@@ -10057,7 +10056,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="334" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A334" s="9" t="s">
         <v>11</v>
       </c>
@@ -10071,7 +10070,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="335" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A335" s="9" t="s">
         <v>11</v>
       </c>
@@ -10085,7 +10084,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="336" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A336" s="9" t="s">
         <v>11</v>
       </c>
@@ -10117,7 +10116,7 @@
         <v>2606.1200000000003</v>
       </c>
     </row>
-    <row r="337" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A337" s="9" t="s">
         <v>11</v>
       </c>
@@ -10137,7 +10136,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="338" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A338" s="9" t="s">
         <v>11</v>
       </c>
@@ -10169,7 +10168,7 @@
         <v>2587.3300000000004</v>
       </c>
     </row>
-    <row r="339" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A339" s="9" t="s">
         <v>11</v>
       </c>
@@ -10189,7 +10188,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="340" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A340" s="9" t="s">
         <v>11</v>
       </c>
@@ -10209,7 +10208,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="341" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A341" s="9" t="s">
         <v>11</v>
       </c>
@@ -10229,7 +10228,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="342" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A342" s="9" t="s">
         <v>11</v>
       </c>
@@ -10261,7 +10260,7 @@
         <v>2559.56</v>
       </c>
     </row>
-    <row r="343" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A343" s="9" t="s">
         <v>11</v>
       </c>
@@ -10281,7 +10280,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="344" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A344" s="9" t="s">
         <v>11</v>
       </c>
@@ -10301,7 +10300,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="345" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A345" s="9" t="s">
         <v>11</v>
       </c>
@@ -10333,7 +10332,7 @@
         <v>2584.9</v>
       </c>
     </row>
-    <row r="346" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A346" s="9" t="s">
         <v>11</v>
       </c>
@@ -10353,7 +10352,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="347" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A347" s="9" t="s">
         <v>11</v>
       </c>
@@ -10373,7 +10372,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="348" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A348" s="9" t="s">
         <v>11</v>
       </c>
@@ -10382,6 +10381,12 @@
       </c>
       <c r="C348" s="10" t="s">
         <v>12</v>
+      </c>
+      <c r="D348" s="5">
+        <v>51.48</v>
+      </c>
+      <c r="E348" s="5">
+        <v>2483.77</v>
       </c>
       <c r="F348" s="32" t="s">
         <v>299</v>
@@ -10399,7 +10404,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="349" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A349" s="9" t="s">
         <v>11</v>
       </c>
@@ -10413,7 +10418,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="350" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A350" s="9" t="s">
         <v>11</v>
       </c>
@@ -10427,7 +10432,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="351" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A351" s="9" t="s">
         <v>11</v>
       </c>
@@ -10453,7 +10458,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="352" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A352" s="9" t="s">
         <v>11</v>
       </c>
@@ -10467,7 +10472,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="353" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A353" s="9" t="s">
         <v>11</v>
       </c>
@@ -10481,7 +10486,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="354" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A354" s="9" t="s">
         <v>11</v>
       </c>
@@ -10507,7 +10512,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="355" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A355" s="9" t="s">
         <v>11</v>
       </c>
@@ -10521,7 +10526,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="356" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A356" s="9" t="s">
         <v>11</v>
       </c>
@@ -10535,7 +10540,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="357" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A357" s="9" t="s">
         <v>11</v>
       </c>
@@ -10561,7 +10566,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="358" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A358" s="9" t="s">
         <v>11</v>
       </c>
@@ -10575,7 +10580,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="359" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A359" s="9" t="s">
         <v>11</v>
       </c>
@@ -10589,7 +10594,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="360" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A360" s="9" t="s">
         <v>11</v>
       </c>
@@ -10615,7 +10620,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="361" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A361" s="9" t="s">
         <v>11</v>
       </c>
@@ -10629,7 +10634,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="362" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A362" s="9" t="s">
         <v>11</v>
       </c>
@@ -10643,7 +10648,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="363" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A363" s="9" t="s">
         <v>11</v>
       </c>
@@ -10669,7 +10674,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="364" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A364" s="9" t="s">
         <v>11</v>
       </c>
@@ -10683,7 +10688,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="365" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A365" s="9" t="s">
         <v>11</v>
       </c>
@@ -10697,7 +10702,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="366" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A366" s="9" t="s">
         <v>11</v>
       </c>
@@ -10723,7 +10728,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="367" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A367" s="9" t="s">
         <v>11</v>
       </c>
@@ -10737,7 +10742,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="368" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A368" s="9" t="s">
         <v>11</v>
       </c>
@@ -10751,7 +10756,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="369" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A369" s="9" t="s">
         <v>11</v>
       </c>
@@ -10777,7 +10782,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="370" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A370" s="9" t="s">
         <v>11</v>
       </c>
@@ -10791,7 +10796,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="371" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A371" s="9" t="s">
         <v>11</v>
       </c>
@@ -10805,7 +10810,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="372" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A372" s="9" t="s">
         <v>11</v>
       </c>
@@ -10831,7 +10836,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="373" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A373" s="9" t="s">
         <v>11</v>
       </c>
@@ -10845,7 +10850,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="374" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A374" s="9" t="s">
         <v>11</v>
       </c>
@@ -10859,10 +10864,10 @@
         <v>325</v>
       </c>
     </row>
-    <row r="375" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:11" x14ac:dyDescent="0.35">
       <c r="F375" s="32"/>
     </row>
-    <row r="376" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C376" s="10" t="s">
         <v>12</v>
       </c>
@@ -10882,7 +10887,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="377" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C377" s="10" t="s">
         <v>12</v>
       </c>
@@ -10890,7 +10895,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="378" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C378" s="10" t="s">
         <v>12</v>
       </c>
@@ -10898,7 +10903,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="379" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C379" s="10" t="s">
         <v>12</v>
       </c>
@@ -10918,7 +10923,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="380" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C380" s="10" t="s">
         <v>12</v>
       </c>
@@ -10926,7 +10931,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="381" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C381" s="10" t="s">
         <v>12</v>
       </c>
@@ -10934,7 +10939,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="382" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C382" s="10" t="s">
         <v>12</v>
       </c>
@@ -10954,7 +10959,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="383" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C383" s="10" t="s">
         <v>12</v>
       </c>
@@ -10962,7 +10967,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="384" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C384" s="10" t="s">
         <v>12</v>
       </c>
@@ -10970,7 +10975,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="385" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="385" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C385" s="10" t="s">
         <v>12</v>
       </c>
@@ -10990,7 +10995,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="386" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="386" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C386" s="10" t="s">
         <v>12</v>
       </c>
@@ -10998,7 +11003,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="387" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="387" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C387" s="10" t="s">
         <v>12</v>
       </c>
@@ -11006,7 +11011,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="388" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="388" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C388" s="10" t="s">
         <v>12</v>
       </c>
@@ -11026,7 +11031,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="389" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="389" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C389" s="10" t="s">
         <v>12</v>
       </c>
@@ -11034,7 +11039,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="390" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="390" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C390" s="10" t="s">
         <v>12</v>
       </c>
@@ -11042,7 +11047,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="391" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="391" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C391" s="10" t="s">
         <v>12</v>
       </c>
@@ -11062,7 +11067,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="392" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="392" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C392" s="10" t="s">
         <v>12</v>
       </c>
@@ -11070,7 +11075,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="393" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="393" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C393" s="10" t="s">
         <v>12</v>
       </c>
@@ -11078,7 +11083,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="394" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="394" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C394" s="10" t="s">
         <v>12</v>
       </c>
@@ -11098,7 +11103,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="395" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="395" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C395" s="10" t="s">
         <v>12</v>
       </c>
@@ -11106,7 +11111,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="396" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="396" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C396" s="10" t="s">
         <v>12</v>
       </c>
@@ -11114,7 +11119,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="397" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="397" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C397" s="10" t="s">
         <v>12</v>
       </c>
@@ -11134,7 +11139,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="398" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="398" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C398" s="10" t="s">
         <v>12</v>
       </c>
@@ -11142,7 +11147,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="399" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="399" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C399" s="10" t="s">
         <v>12</v>
       </c>
@@ -11150,7 +11155,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="400" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="400" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C400" s="10" t="s">
         <v>12</v>
       </c>
@@ -11170,7 +11175,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="401" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="401" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C401" s="10" t="s">
         <v>12</v>
       </c>
@@ -11178,7 +11183,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="402" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="402" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C402" s="10" t="s">
         <v>12</v>
       </c>
@@ -11186,10 +11191,10 @@
         <v>352</v>
       </c>
     </row>
-    <row r="403" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="403" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C403" s="10"/>
     </row>
-    <row r="404" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="404" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C404" s="25" t="s">
         <v>12</v>
       </c>
@@ -11197,7 +11202,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="405" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="405" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C405" s="10" t="s">
         <v>12</v>
       </c>
@@ -11205,7 +11210,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="406" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="406" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C406" s="10" t="s">
         <v>12</v>
       </c>
@@ -11213,7 +11218,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="407" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="407" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C407" s="10" t="s">
         <v>12</v>
       </c>
@@ -11221,7 +11226,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="408" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="408" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C408" s="10" t="s">
         <v>12</v>
       </c>
@@ -11229,7 +11234,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="409" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="409" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C409" s="10" t="s">
         <v>12</v>
       </c>
@@ -11237,7 +11242,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="410" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="410" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C410" s="10" t="s">
         <v>12</v>
       </c>
@@ -11245,7 +11250,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="411" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="411" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C411" s="10" t="s">
         <v>12</v>
       </c>
@@ -11253,7 +11258,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="412" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="412" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C412" s="10" t="s">
         <v>12</v>
       </c>
@@ -11261,7 +11266,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="413" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="413" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C413" s="10" t="s">
         <v>12</v>
       </c>
@@ -11269,7 +11274,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="414" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="414" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C414" s="10" t="s">
         <v>12</v>
       </c>
@@ -11277,7 +11282,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="415" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="415" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C415" s="10" t="s">
         <v>12</v>
       </c>
@@ -11285,7 +11290,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="416" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="416" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C416" s="10" t="s">
         <v>12</v>
       </c>
@@ -11293,7 +11298,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="417" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="417" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C417" s="10" t="s">
         <v>12</v>
       </c>
@@ -11301,7 +11306,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="418" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="418" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C418" s="10" t="s">
         <v>12</v>
       </c>
@@ -11309,7 +11314,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="419" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="419" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C419" s="10" t="s">
         <v>12</v>
       </c>
@@ -11317,7 +11322,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="420" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="420" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C420" s="10" t="s">
         <v>12</v>
       </c>
@@ -11325,7 +11330,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="421" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="421" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C421" s="10" t="s">
         <v>12</v>
       </c>
@@ -11333,7 +11338,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="422" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="422" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C422" s="10" t="s">
         <v>12</v>
       </c>
@@ -11341,7 +11346,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="423" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="423" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C423" s="10" t="s">
         <v>12</v>
       </c>
@@ -11349,7 +11354,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="424" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="424" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C424" s="10" t="s">
         <v>12</v>
       </c>
@@ -11357,7 +11362,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="425" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="425" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C425" s="10" t="s">
         <v>12</v>
       </c>
@@ -11365,7 +11370,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="426" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="426" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C426" s="10" t="s">
         <v>12</v>
       </c>
@@ -11373,7 +11378,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="427" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="427" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C427" s="10" t="s">
         <v>12</v>
       </c>
@@ -11381,7 +11386,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="428" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="428" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C428" s="10" t="s">
         <v>12</v>
       </c>
@@ -11389,7 +11394,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="429" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="429" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C429" s="10" t="s">
         <v>12</v>
       </c>
@@ -11397,7 +11402,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="430" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="430" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C430" s="10" t="s">
         <v>12</v>
       </c>
@@ -11405,7 +11410,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="431" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="431" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C431" s="10" t="s">
         <v>12</v>
       </c>
@@ -11413,7 +11418,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="432" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="432" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C432" s="10" t="s">
         <v>12</v>
       </c>
@@ -11421,7 +11426,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="433" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="433" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C433" s="10" t="s">
         <v>12</v>
       </c>
@@ -11429,7 +11434,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="434" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="434" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C434" s="10" t="s">
         <v>12</v>
       </c>
@@ -11437,7 +11442,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="435" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="435" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C435" s="10" t="s">
         <v>12</v>
       </c>
@@ -11445,7 +11450,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="436" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="436" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C436" s="10" t="s">
         <v>12</v>
       </c>
@@ -11453,7 +11458,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="437" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="437" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C437" s="10" t="s">
         <v>12</v>
       </c>
@@ -11461,7 +11466,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="438" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="438" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C438" s="10" t="s">
         <v>12</v>
       </c>
@@ -11469,7 +11474,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="439" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="439" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C439" s="10" t="s">
         <v>12</v>
       </c>
@@ -11477,7 +11482,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="440" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="440" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C440" s="10" t="s">
         <v>12</v>
       </c>
@@ -11485,7 +11490,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="441" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="441" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C441" s="10" t="s">
         <v>12</v>
       </c>
@@ -11493,7 +11498,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="442" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="442" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C442" s="10" t="s">
         <v>12</v>
       </c>
@@ -11501,7 +11506,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="443" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="443" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C443" s="25" t="s">
         <v>12</v>
       </c>
@@ -11509,7 +11514,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="444" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="444" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C444" s="10" t="s">
         <v>12</v>
       </c>
@@ -11517,10 +11522,10 @@
         <v>390</v>
       </c>
     </row>
-    <row r="445" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="445" spans="3:6" x14ac:dyDescent="0.35">
       <c r="F445" s="32"/>
     </row>
-    <row r="446" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="446" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C446" s="10" t="s">
         <v>12</v>
       </c>
@@ -11528,7 +11533,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="447" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="447" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C447" s="10" t="s">
         <v>12</v>
       </c>
@@ -11536,7 +11541,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="448" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="448" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C448" s="10" t="s">
         <v>12</v>
       </c>
@@ -11544,7 +11549,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="449" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="449" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C449" s="10" t="s">
         <v>12</v>
       </c>
@@ -11552,7 +11557,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="450" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="450" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C450" s="10" t="s">
         <v>12</v>
       </c>
@@ -11560,7 +11565,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="451" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="451" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C451" s="10" t="s">
         <v>12</v>
       </c>
@@ -11568,7 +11573,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="452" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="452" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C452" s="10" t="s">
         <v>12</v>
       </c>
@@ -11576,7 +11581,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="453" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="453" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C453" s="10" t="s">
         <v>12</v>
       </c>
@@ -11584,7 +11589,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="454" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="454" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C454" s="10" t="s">
         <v>12</v>
       </c>
@@ -11592,7 +11597,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="455" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="455" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C455" s="10" t="s">
         <v>12</v>
       </c>
@@ -11600,7 +11605,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="456" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="456" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C456" s="10" t="s">
         <v>12</v>
       </c>
@@ -11608,7 +11613,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="457" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="457" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C457" s="10" t="s">
         <v>12</v>
       </c>
@@ -11616,7 +11621,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="458" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="458" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C458" s="10" t="s">
         <v>12</v>
       </c>
@@ -11624,7 +11629,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="459" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="459" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C459" s="10" t="s">
         <v>12</v>
       </c>
@@ -11632,7 +11637,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="460" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="460" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C460" s="10" t="s">
         <v>12</v>
       </c>
@@ -11640,7 +11645,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="461" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="461" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C461" s="10" t="s">
         <v>12</v>
       </c>
@@ -11648,7 +11653,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="462" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="462" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C462" s="10" t="s">
         <v>12</v>
       </c>
@@ -11656,7 +11661,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="463" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="463" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C463" s="10" t="s">
         <v>12</v>
       </c>
@@ -11664,7 +11669,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="464" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="464" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C464" s="10" t="s">
         <v>12</v>
       </c>
@@ -11672,7 +11677,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="465" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="465" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C465" s="10" t="s">
         <v>12</v>
       </c>
@@ -11680,7 +11685,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="466" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="466" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C466" s="10" t="s">
         <v>12</v>
       </c>
@@ -11688,7 +11693,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="467" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="467" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C467" s="10" t="s">
         <v>12</v>
       </c>
@@ -11696,7 +11701,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="468" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="468" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C468" s="10" t="s">
         <v>12</v>
       </c>
@@ -11704,7 +11709,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="469" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="469" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C469" s="10" t="s">
         <v>12</v>
       </c>
@@ -11712,7 +11717,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="470" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="470" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C470" s="10" t="s">
         <v>12</v>
       </c>
@@ -11720,7 +11725,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="471" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="471" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C471" s="10" t="s">
         <v>12</v>
       </c>
@@ -11728,7 +11733,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="472" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="472" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C472" s="10" t="s">
         <v>12</v>
       </c>
@@ -11736,7 +11741,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="473" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="473" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C473" s="10" t="s">
         <v>12</v>
       </c>
@@ -11744,7 +11749,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="474" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="474" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C474" s="10" t="s">
         <v>12</v>
       </c>
@@ -11752,7 +11757,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="475" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="475" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C475" s="10" t="s">
         <v>12</v>
       </c>
@@ -11760,125 +11765,125 @@
         <v>417</v>
       </c>
     </row>
-    <row r="476" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="476" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C476" s="10"/>
     </row>
-    <row r="477" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="477" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C477" s="10"/>
     </row>
-    <row r="478" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="478" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C478" s="10"/>
     </row>
-    <row r="479" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="479" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C479" s="10"/>
     </row>
-    <row r="480" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="480" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C480" s="10"/>
     </row>
-    <row r="481" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="481" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C481" s="10"/>
     </row>
-    <row r="482" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="482" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C482" s="10"/>
     </row>
-    <row r="483" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="483" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C483" s="10"/>
     </row>
-    <row r="484" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="484" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C484" s="10"/>
     </row>
-    <row r="486" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="486" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C486" s="25"/>
     </row>
-    <row r="487" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="487" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C487" s="10"/>
     </row>
-    <row r="488" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="488" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C488" s="10"/>
     </row>
-    <row r="489" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="489" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C489" s="10"/>
     </row>
-    <row r="490" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="490" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C490" s="10"/>
     </row>
-    <row r="491" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="491" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C491" s="10"/>
     </row>
-    <row r="492" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="492" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C492" s="10"/>
     </row>
-    <row r="493" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="493" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C493" s="10"/>
     </row>
-    <row r="494" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="494" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C494" s="10"/>
     </row>
-    <row r="495" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="495" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C495" s="10"/>
     </row>
-    <row r="496" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="496" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C496" s="10"/>
     </row>
-    <row r="497" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="497" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C497" s="10"/>
     </row>
-    <row r="498" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="498" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C498" s="10"/>
     </row>
-    <row r="499" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="499" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C499" s="10"/>
     </row>
-    <row r="500" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="500" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C500" s="10"/>
     </row>
-    <row r="501" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="501" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C501" s="10"/>
     </row>
-    <row r="502" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="502" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C502" s="10"/>
     </row>
-    <row r="503" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="503" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C503" s="10"/>
     </row>
-    <row r="504" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="504" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C504" s="10"/>
     </row>
-    <row r="505" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="505" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C505" s="10"/>
     </row>
-    <row r="506" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="506" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C506" s="10"/>
     </row>
-    <row r="507" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="507" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C507" s="10"/>
     </row>
-    <row r="508" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="508" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C508" s="10"/>
     </row>
-    <row r="509" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="509" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C509" s="10"/>
     </row>
-    <row r="510" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="510" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C510" s="10"/>
     </row>
-    <row r="511" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="511" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C511" s="10"/>
     </row>
-    <row r="512" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="512" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C512" s="10"/>
     </row>
-    <row r="513" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="513" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C513" s="10"/>
     </row>
-    <row r="514" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="514" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C514" s="10"/>
     </row>
-    <row r="515" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="515" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C515" s="10"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:L1"/>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
LOW until T5 6/6
</commit_message>
<xml_diff>
--- a/Data/Spring_2023/BenthFun_Alkalinity.xlsx
+++ b/Data/Spring_2023/BenthFun_Alkalinity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremy/Library/Mobile Documents/com~apple~CloudDocs/Documents/Documents/Post-Doc/Projets/Villefranche/Projets/BenthFun – Jeremy/BenthFun/Data/Spring_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48732D29-F85B-7F45-A400-0EEF60E8939A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69DB0230-1A0C-804F-9C7B-7CFF8E3F0748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1372" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1366" uniqueCount="416">
   <si>
     <t>Operator</t>
   </si>
@@ -853,9 +853,6 @@
     <t>PI_t6_ELOW_Tile_3b</t>
   </si>
   <si>
-    <t>PI_t6_ELOW_Tile_3c</t>
-  </si>
-  <si>
     <t>PI_t7_ELOW_Tile_1a</t>
   </si>
   <si>
@@ -937,36 +934,24 @@
     <t>PI_t2_LOW_Tile_1b</t>
   </si>
   <si>
-    <t>PI_t2_LOW_Tile_1c</t>
-  </si>
-  <si>
     <t>PI_t2_LOW_Tile_2a</t>
   </si>
   <si>
     <t>PI_t2_LOW_Tile_2b</t>
   </si>
   <si>
-    <t>PI_t2_LOW_Tile_2c</t>
-  </si>
-  <si>
     <t>PI_t2_LOW_Tile_3a</t>
   </si>
   <si>
     <t>PI_t2_LOW_Tile_3b</t>
   </si>
   <si>
-    <t>PI_t2_LOW_Tile_3c</t>
-  </si>
-  <si>
     <t>PI_t3_LOW_Tile_1a</t>
   </si>
   <si>
     <t>PI_t3_LOW_Tile_1b</t>
   </si>
   <si>
-    <t>PI_t3_LOW_Tile_1c</t>
-  </si>
-  <si>
     <t>PI_t3_LOW_Tile_2a</t>
   </si>
   <si>
@@ -982,9 +967,6 @@
     <t>PI_t3_LOW_Tile_3b</t>
   </si>
   <si>
-    <t>PI_t3_LOW_Tile_3c</t>
-  </si>
-  <si>
     <t>PI_t4_LOW_Tile_1a</t>
   </si>
   <si>
@@ -1000,9 +982,6 @@
     <t>PI_t4_LOW_Tile_2b</t>
   </si>
   <si>
-    <t>PI_t4_LOW_Tile_2c</t>
-  </si>
-  <si>
     <t>PI_t4_LOW_Tile_3a</t>
   </si>
   <si>
@@ -1018,9 +997,6 @@
     <t>PI_t5_LOW_Tile_1b</t>
   </si>
   <si>
-    <t>PI_t5_LOW_Tile_1c</t>
-  </si>
-  <si>
     <t>PI_t5_LOW_Tile_2a</t>
   </si>
   <si>
@@ -1298,6 +1274,15 @@
   </si>
   <si>
     <t>PI_t1_LOW_Tile_2d</t>
+  </si>
+  <si>
+    <t>PI_t2_LOW_Tile_3d</t>
+  </si>
+  <si>
+    <t>PI_t3_LOW_Tile_3e</t>
+  </si>
+  <si>
+    <t>PI_t4_LOW_Tile_2d</t>
   </si>
 </sst>
 </file>
@@ -1781,11 +1766,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L514"/>
+  <dimension ref="A1:L509"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="73" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A339" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G346" sqref="G346"/>
+      <pane ySplit="1" topLeftCell="A359" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D388" sqref="D388"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8711,7 +8696,7 @@
         <v>2889.65</v>
       </c>
       <c r="F277" s="32" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
     </row>
     <row r="278" spans="1:12" x14ac:dyDescent="0.2">
@@ -9103,7 +9088,7 @@
         <v>2678.51</v>
       </c>
       <c r="F293" s="32" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
     </row>
     <row r="294" spans="1:12" x14ac:dyDescent="0.2">
@@ -9571,11 +9556,11 @@
         <v>270</v>
       </c>
       <c r="G313" s="13">
-        <f>AVERAGE(E314,E316)</f>
+        <f>AVERAGE(E314,E315)</f>
         <v>2547.31</v>
       </c>
       <c r="H313" s="13">
-        <f>STDEV(E314,E316)</f>
+        <f>STDEV(E314,E315)</f>
         <v>1.8809040379561135</v>
       </c>
       <c r="K313" s="5">
@@ -9614,13 +9599,13 @@
         <v>12</v>
       </c>
       <c r="D315" s="5">
-        <v>51.47</v>
-      </c>
-      <c r="E315" s="14">
-        <v>2522.4699999999998</v>
+        <v>50.71</v>
+      </c>
+      <c r="E315" s="5">
+        <v>2548.64</v>
       </c>
       <c r="F315" s="32" t="s">
-        <v>272</v>
+        <v>411</v>
       </c>
     </row>
     <row r="316" spans="1:11" x14ac:dyDescent="0.2">
@@ -9634,13 +9619,25 @@
         <v>12</v>
       </c>
       <c r="D316" s="5">
-        <v>50.71</v>
-      </c>
-      <c r="E316" s="5">
-        <v>2548.64</v>
+        <v>51.27</v>
+      </c>
+      <c r="E316" s="14">
+        <v>2585.0100000000002</v>
       </c>
       <c r="F316" s="32" t="s">
-        <v>419</v>
+        <v>272</v>
+      </c>
+      <c r="G316" s="13">
+        <f>AVERAGE(E317:E318)</f>
+        <v>2604.0349999999999</v>
+      </c>
+      <c r="H316" s="18">
+        <f>STDEV(E317:E318)</f>
+        <v>6.3639610306892178E-2</v>
+      </c>
+      <c r="K316" s="5">
+        <f>G316+$J$295</f>
+        <v>2608.48</v>
       </c>
     </row>
     <row r="317" spans="1:11" x14ac:dyDescent="0.2">
@@ -9654,26 +9651,14 @@
         <v>12</v>
       </c>
       <c r="D317" s="5">
-        <v>51.27</v>
-      </c>
-      <c r="E317" s="14">
-        <v>2585.0100000000002</v>
+        <v>49.07</v>
+      </c>
+      <c r="E317" s="5">
+        <v>2603.9899999999998</v>
       </c>
       <c r="F317" s="32" t="s">
         <v>273</v>
       </c>
-      <c r="G317" s="13">
-        <f>AVERAGE(E318:E319)</f>
-        <v>2604.0349999999999</v>
-      </c>
-      <c r="H317" s="18">
-        <f>STDEV(E318:E319)</f>
-        <v>6.3639610306892178E-2</v>
-      </c>
-      <c r="K317" s="5">
-        <f>G317+$J$295</f>
-        <v>2608.48</v>
-      </c>
     </row>
     <row r="318" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A318" s="9" t="s">
@@ -9686,10 +9671,10 @@
         <v>12</v>
       </c>
       <c r="D318" s="5">
-        <v>49.07</v>
+        <v>48.74</v>
       </c>
       <c r="E318" s="5">
-        <v>2603.9899999999998</v>
+        <v>2604.08</v>
       </c>
       <c r="F318" s="32" t="s">
         <v>274</v>
@@ -9706,14 +9691,26 @@
         <v>12</v>
       </c>
       <c r="D319" s="5">
-        <v>48.74</v>
-      </c>
-      <c r="E319" s="5">
-        <v>2604.08</v>
+        <v>50.99</v>
+      </c>
+      <c r="E319" s="14">
+        <v>2658.15</v>
       </c>
       <c r="F319" s="32" t="s">
         <v>275</v>
       </c>
+      <c r="G319" s="13">
+        <f>AVERAGE(E320:E321)</f>
+        <v>2646.86</v>
+      </c>
+      <c r="H319" s="18">
+        <f>STDEV(E320:E321)</f>
+        <v>2.3617366491631717</v>
+      </c>
+      <c r="K319" s="5">
+        <f>G319+$J$295</f>
+        <v>2651.3050000000003</v>
+      </c>
     </row>
     <row r="320" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A320" s="9" t="s">
@@ -9726,26 +9723,14 @@
         <v>12</v>
       </c>
       <c r="D320" s="5">
-        <v>50.99</v>
-      </c>
-      <c r="E320" s="14">
-        <v>2658.15</v>
+        <v>50.89</v>
+      </c>
+      <c r="E320" s="5">
+        <v>2645.19</v>
       </c>
       <c r="F320" s="32" t="s">
         <v>276</v>
       </c>
-      <c r="G320" s="13">
-        <f>AVERAGE(E321:E322)</f>
-        <v>2646.86</v>
-      </c>
-      <c r="H320" s="18">
-        <f>STDEV(E321:E322)</f>
-        <v>2.3617366491631717</v>
-      </c>
-      <c r="K320" s="5">
-        <f>G320+$J$295</f>
-        <v>2651.3050000000003</v>
-      </c>
     </row>
     <row r="321" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A321" s="9" t="s">
@@ -9758,10 +9743,10 @@
         <v>12</v>
       </c>
       <c r="D321" s="5">
-        <v>50.89</v>
+        <v>49.61</v>
       </c>
       <c r="E321" s="5">
-        <v>2645.19</v>
+        <v>2648.53</v>
       </c>
       <c r="F321" s="32" t="s">
         <v>277</v>
@@ -9778,14 +9763,26 @@
         <v>12</v>
       </c>
       <c r="D322" s="5">
-        <v>49.61</v>
+        <v>48.94</v>
       </c>
       <c r="E322" s="5">
-        <v>2648.53</v>
+        <v>2614.2199999999998</v>
       </c>
       <c r="F322" s="32" t="s">
         <v>278</v>
       </c>
+      <c r="G322" s="13">
+        <f>AVERAGE(E322:E323)</f>
+        <v>2612.37</v>
+      </c>
+      <c r="H322" s="18">
+        <f>STDEV(E322:E323)</f>
+        <v>2.6162950903900972</v>
+      </c>
+      <c r="K322" s="5">
+        <f>G322+$J$295</f>
+        <v>2616.8150000000001</v>
+      </c>
     </row>
     <row r="323" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A323" s="9" t="s">
@@ -9798,26 +9795,14 @@
         <v>12</v>
       </c>
       <c r="D323" s="5">
-        <v>48.94</v>
+        <v>50.77</v>
       </c>
       <c r="E323" s="5">
-        <v>2614.2199999999998</v>
+        <v>2610.52</v>
       </c>
       <c r="F323" s="32" t="s">
         <v>279</v>
       </c>
-      <c r="G323" s="13">
-        <f>AVERAGE(E323:E324)</f>
-        <v>2612.37</v>
-      </c>
-      <c r="H323" s="18">
-        <f>STDEV(E323:E324)</f>
-        <v>2.6162950903900972</v>
-      </c>
-      <c r="K323" s="5">
-        <f>G323+$J$295</f>
-        <v>2616.8150000000001</v>
-      </c>
     </row>
     <row r="324" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A324" s="9" t="s">
@@ -9830,14 +9815,26 @@
         <v>12</v>
       </c>
       <c r="D324" s="5">
-        <v>50.77</v>
+        <v>52.43</v>
       </c>
       <c r="E324" s="5">
-        <v>2610.52</v>
+        <v>2530.13</v>
       </c>
       <c r="F324" s="32" t="s">
         <v>280</v>
       </c>
+      <c r="G324" s="13">
+        <f>AVERAGE(E324:E325)</f>
+        <v>2528.3500000000004</v>
+      </c>
+      <c r="H324" s="18">
+        <f>STDEV(E324:E325)</f>
+        <v>2.5173001410240707</v>
+      </c>
+      <c r="K324" s="5">
+        <f>G324+$J$295</f>
+        <v>2532.7950000000005</v>
+      </c>
     </row>
     <row r="325" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A325" s="9" t="s">
@@ -9850,26 +9847,14 @@
         <v>12</v>
       </c>
       <c r="D325" s="5">
-        <v>52.43</v>
+        <v>49.17</v>
       </c>
       <c r="E325" s="5">
-        <v>2530.13</v>
+        <v>2526.5700000000002</v>
       </c>
       <c r="F325" s="32" t="s">
         <v>281</v>
       </c>
-      <c r="G325" s="13">
-        <f>AVERAGE(E325:E326)</f>
-        <v>2528.3500000000004</v>
-      </c>
-      <c r="H325" s="18">
-        <f>STDEV(E325:E326)</f>
-        <v>2.5173001410240707</v>
-      </c>
-      <c r="K325" s="5">
-        <f>G325+$J$295</f>
-        <v>2532.7950000000005</v>
-      </c>
     </row>
     <row r="326" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A326" s="9" t="s">
@@ -9882,14 +9867,26 @@
         <v>12</v>
       </c>
       <c r="D326" s="5">
-        <v>49.17</v>
+        <v>50.31</v>
       </c>
       <c r="E326" s="5">
-        <v>2526.5700000000002</v>
+        <v>2623.15</v>
       </c>
       <c r="F326" s="32" t="s">
         <v>282</v>
       </c>
+      <c r="G326" s="13">
+        <f>AVERAGE(E326:E327)</f>
+        <v>2622.16</v>
+      </c>
+      <c r="H326" s="18">
+        <f>STDEV(E326:E327)</f>
+        <v>1.400071426749377</v>
+      </c>
+      <c r="K326" s="5">
+        <f>G326+$J$295</f>
+        <v>2626.605</v>
+      </c>
     </row>
     <row r="327" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A327" s="9" t="s">
@@ -9902,26 +9899,14 @@
         <v>12</v>
       </c>
       <c r="D327" s="5">
-        <v>50.31</v>
+        <v>51.67</v>
       </c>
       <c r="E327" s="5">
-        <v>2623.15</v>
+        <v>2621.17</v>
       </c>
       <c r="F327" s="32" t="s">
         <v>283</v>
       </c>
-      <c r="G327" s="13">
-        <f>AVERAGE(E327:E328)</f>
-        <v>2622.16</v>
-      </c>
-      <c r="H327" s="18">
-        <f>STDEV(E327:E328)</f>
-        <v>1.400071426749377</v>
-      </c>
-      <c r="K327" s="5">
-        <f>G327+$J$295</f>
-        <v>2626.605</v>
-      </c>
     </row>
     <row r="328" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A328" s="9" t="s">
@@ -9934,14 +9919,26 @@
         <v>12</v>
       </c>
       <c r="D328" s="5">
-        <v>51.67</v>
-      </c>
-      <c r="E328" s="5">
-        <v>2621.17</v>
+        <v>50.42</v>
+      </c>
+      <c r="E328" s="14">
+        <v>2585.75</v>
       </c>
       <c r="F328" s="32" t="s">
         <v>284</v>
       </c>
+      <c r="G328" s="13">
+        <f>AVERAGE(E329:E330)</f>
+        <v>2575.38</v>
+      </c>
+      <c r="H328" s="18">
+        <f>STDEV(E329:E330)</f>
+        <v>4.2426406871192848</v>
+      </c>
+      <c r="K328" s="5">
+        <f>G328+$J$295</f>
+        <v>2579.8250000000003</v>
+      </c>
     </row>
     <row r="329" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A329" s="9" t="s">
@@ -9954,26 +9951,14 @@
         <v>12</v>
       </c>
       <c r="D329" s="5">
-        <v>50.42</v>
-      </c>
-      <c r="E329" s="14">
-        <v>2585.75</v>
+        <v>50.63</v>
+      </c>
+      <c r="E329" s="5">
+        <v>2572.38</v>
       </c>
       <c r="F329" s="32" t="s">
         <v>285</v>
       </c>
-      <c r="G329" s="13">
-        <f>AVERAGE(E330:E331)</f>
-        <v>2575.38</v>
-      </c>
-      <c r="H329" s="18">
-        <f>STDEV(E330:E331)</f>
-        <v>4.2426406871192848</v>
-      </c>
-      <c r="K329" s="5">
-        <f>G329+$J$295</f>
-        <v>2579.8250000000003</v>
-      </c>
     </row>
     <row r="330" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A330" s="9" t="s">
@@ -9986,37 +9971,59 @@
         <v>12</v>
       </c>
       <c r="D330" s="5">
-        <v>50.63</v>
+        <v>49.19</v>
       </c>
       <c r="E330" s="5">
-        <v>2572.38</v>
+        <v>2578.38</v>
       </c>
       <c r="F330" s="32" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="331" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A331" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B331" s="31">
-        <v>45082</v>
-      </c>
-      <c r="C331" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D331" s="5">
-        <v>49.19</v>
-      </c>
-      <c r="E331" s="5">
-        <v>2578.38</v>
-      </c>
-      <c r="F331" s="32" t="s">
-        <v>287</v>
-      </c>
+      <c r="C331" s="10"/>
     </row>
     <row r="332" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C332" s="10"/>
+      <c r="A332" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B332" s="31">
+        <v>45083</v>
+      </c>
+      <c r="C332" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D332" s="5">
+        <v>50.52</v>
+      </c>
+      <c r="E332" s="14">
+        <v>2219.19</v>
+      </c>
+      <c r="F332" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G332" s="13">
+        <f>AVERAGE(E333:E334)</f>
+        <v>2238.3050000000003</v>
+      </c>
+      <c r="H332" s="18">
+        <f>STDEV(E333:E334)</f>
+        <v>2.8637824638053244</v>
+      </c>
+      <c r="I332" s="3">
+        <v>2226.44</v>
+      </c>
+      <c r="J332" s="4">
+        <f>I332-G332</f>
+        <v>-11.865000000000236</v>
+      </c>
+      <c r="K332" s="5">
+        <f>G332+J332</f>
+        <v>2226.44</v>
+      </c>
+      <c r="L332" s="2" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="333" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A333" s="9" t="s">
@@ -10025,39 +10032,17 @@
       <c r="B333" s="31">
         <v>45083</v>
       </c>
-      <c r="C333" s="25" t="s">
+      <c r="C333" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D333" s="5">
-        <v>50.52</v>
-      </c>
-      <c r="E333" s="14">
-        <v>2219.19</v>
+        <v>48.27</v>
+      </c>
+      <c r="E333" s="5">
+        <v>2236.2800000000002</v>
       </c>
       <c r="F333" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="G333" s="13">
-        <f>AVERAGE(E334:E335)</f>
-        <v>2238.3050000000003</v>
-      </c>
-      <c r="H333" s="18">
-        <f>STDEV(E334:E335)</f>
-        <v>2.8637824638053244</v>
-      </c>
-      <c r="I333" s="3">
-        <v>2226.44</v>
-      </c>
-      <c r="J333" s="4">
-        <f>I333-G333</f>
-        <v>-11.865000000000236</v>
-      </c>
-      <c r="K333" s="5">
-        <f>G333+J333</f>
-        <v>2226.44</v>
-      </c>
-      <c r="L333" s="2" t="s">
-        <v>94</v>
+        <v>9</v>
       </c>
     </row>
     <row r="334" spans="1:12" x14ac:dyDescent="0.2">
@@ -10071,13 +10056,13 @@
         <v>12</v>
       </c>
       <c r="D334" s="5">
-        <v>48.27</v>
+        <v>50.04</v>
       </c>
       <c r="E334" s="5">
-        <v>2236.2800000000002</v>
-      </c>
-      <c r="F334" s="16" t="s">
-        <v>9</v>
+        <v>2240.33</v>
+      </c>
+      <c r="F334" s="17" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="335" spans="1:12" x14ac:dyDescent="0.2">
@@ -10085,19 +10070,31 @@
         <v>11</v>
       </c>
       <c r="B335" s="31">
-        <v>45083</v>
+        <v>45082</v>
       </c>
       <c r="C335" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D335" s="5">
-        <v>50.04</v>
+        <v>48.96</v>
       </c>
       <c r="E335" s="5">
-        <v>2240.33</v>
-      </c>
-      <c r="F335" s="17" t="s">
-        <v>96</v>
+        <v>2601.0100000000002</v>
+      </c>
+      <c r="F335" s="32" t="s">
+        <v>287</v>
+      </c>
+      <c r="G335" s="13">
+        <f>AVERAGE(E335:E336)</f>
+        <v>2601.6750000000002</v>
+      </c>
+      <c r="H335" s="18">
+        <f>STDEV(E335:E336)</f>
+        <v>0.94045201897805675</v>
+      </c>
+      <c r="K335" s="5">
+        <f>G335+$J$295</f>
+        <v>2606.1200000000003</v>
       </c>
     </row>
     <row r="336" spans="1:12" x14ac:dyDescent="0.2">
@@ -10111,26 +10108,14 @@
         <v>12</v>
       </c>
       <c r="D336" s="5">
-        <v>48.96</v>
+        <v>52.01</v>
       </c>
       <c r="E336" s="5">
-        <v>2601.0100000000002</v>
+        <v>2602.34</v>
       </c>
       <c r="F336" s="32" t="s">
         <v>288</v>
       </c>
-      <c r="G336" s="13">
-        <f>AVERAGE(E336:E337)</f>
-        <v>2601.6750000000002</v>
-      </c>
-      <c r="H336" s="18">
-        <f>STDEV(E336:E337)</f>
-        <v>0.94045201897805675</v>
-      </c>
-      <c r="K336" s="5">
-        <f>G336+$J$295</f>
-        <v>2606.1200000000003</v>
-      </c>
     </row>
     <row r="337" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A337" s="9" t="s">
@@ -10143,14 +10128,26 @@
         <v>12</v>
       </c>
       <c r="D337" s="5">
-        <v>52.01</v>
-      </c>
-      <c r="E337" s="5">
-        <v>2602.34</v>
+        <v>50.22</v>
+      </c>
+      <c r="E337" s="14">
+        <v>2534.11</v>
       </c>
       <c r="F337" s="32" t="s">
         <v>289</v>
       </c>
+      <c r="G337" s="18">
+        <f>AVERAGE(E338:E339)</f>
+        <v>2582.8850000000002</v>
+      </c>
+      <c r="H337" s="18">
+        <f>STDEV(E338:E339)</f>
+        <v>9.1923881554006784E-2</v>
+      </c>
+      <c r="K337" s="5">
+        <f>G337+$J$295</f>
+        <v>2587.3300000000004</v>
+      </c>
     </row>
     <row r="338" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A338" s="9" t="s">
@@ -10163,26 +10160,14 @@
         <v>12</v>
       </c>
       <c r="D338" s="5">
-        <v>50.22</v>
-      </c>
-      <c r="E338" s="14">
-        <v>2534.11</v>
+        <v>49.96</v>
+      </c>
+      <c r="E338" s="5">
+        <v>2582.9499999999998</v>
       </c>
       <c r="F338" s="32" t="s">
         <v>290</v>
       </c>
-      <c r="G338" s="18">
-        <f>AVERAGE(E339:E340)</f>
-        <v>2582.8850000000002</v>
-      </c>
-      <c r="H338" s="18">
-        <f>STDEV(E339:E340)</f>
-        <v>9.1923881554006784E-2</v>
-      </c>
-      <c r="K338" s="5">
-        <f>G338+$J$295</f>
-        <v>2587.3300000000004</v>
-      </c>
     </row>
     <row r="339" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A339" s="9" t="s">
@@ -10195,13 +10180,13 @@
         <v>12</v>
       </c>
       <c r="D339" s="5">
-        <v>49.96</v>
+        <v>49.71</v>
       </c>
       <c r="E339" s="5">
-        <v>2582.9499999999998</v>
+        <v>2582.8200000000002</v>
       </c>
       <c r="F339" s="32" t="s">
-        <v>291</v>
+        <v>412</v>
       </c>
     </row>
     <row r="340" spans="1:11" x14ac:dyDescent="0.2">
@@ -10215,13 +10200,25 @@
         <v>12</v>
       </c>
       <c r="D340" s="5">
-        <v>49.71</v>
+        <v>49.6</v>
       </c>
       <c r="E340" s="5">
-        <v>2582.8200000000002</v>
+        <v>2562.94</v>
       </c>
       <c r="F340" s="32" t="s">
-        <v>420</v>
+        <v>291</v>
+      </c>
+      <c r="G340" s="13">
+        <f>AVERAGE(E340:E341)</f>
+        <v>2555.1149999999998</v>
+      </c>
+      <c r="H340" s="18">
+        <f>STDEV(E340,E342)</f>
+        <v>2.9698484809833712</v>
+      </c>
+      <c r="K340" s="5">
+        <f>G340+$J$295</f>
+        <v>2559.56</v>
       </c>
     </row>
     <row r="341" spans="1:11" x14ac:dyDescent="0.2">
@@ -10235,26 +10232,14 @@
         <v>12</v>
       </c>
       <c r="D341" s="5">
-        <v>49.6</v>
-      </c>
-      <c r="E341" s="5">
-        <v>2562.94</v>
+        <v>52</v>
+      </c>
+      <c r="E341" s="14">
+        <v>2547.29</v>
       </c>
       <c r="F341" s="32" t="s">
         <v>292</v>
       </c>
-      <c r="G341" s="13">
-        <f>AVERAGE(E341:E342)</f>
-        <v>2555.1149999999998</v>
-      </c>
-      <c r="H341" s="18">
-        <f>STDEV(E341,E343)</f>
-        <v>2.9698484809833712</v>
-      </c>
-      <c r="K341" s="5">
-        <f>G341+$J$295</f>
-        <v>2559.56</v>
-      </c>
     </row>
     <row r="342" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A342" s="9" t="s">
@@ -10267,10 +10252,10 @@
         <v>12</v>
       </c>
       <c r="D342" s="5">
-        <v>52</v>
-      </c>
-      <c r="E342" s="14">
-        <v>2547.29</v>
+        <v>49.79</v>
+      </c>
+      <c r="E342" s="5">
+        <v>2567.14</v>
       </c>
       <c r="F342" s="32" t="s">
         <v>293</v>
@@ -10287,14 +10272,26 @@
         <v>12</v>
       </c>
       <c r="D343" s="5">
-        <v>49.79</v>
-      </c>
-      <c r="E343" s="5">
-        <v>2567.14</v>
+        <v>51.18</v>
+      </c>
+      <c r="E343" s="14">
+        <v>2589.9299999999998</v>
       </c>
       <c r="F343" s="32" t="s">
         <v>294</v>
       </c>
+      <c r="G343" s="13">
+        <f>AVERAGE(E344:E345)</f>
+        <v>2580.4549999999999</v>
+      </c>
+      <c r="H343" s="18">
+        <f>STDEV(E344:E345)</f>
+        <v>1.3788582233136391</v>
+      </c>
+      <c r="K343" s="5">
+        <f>G343+$J$295</f>
+        <v>2584.9</v>
+      </c>
     </row>
     <row r="344" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A344" s="9" t="s">
@@ -10307,26 +10304,14 @@
         <v>12</v>
       </c>
       <c r="D344" s="5">
-        <v>51.18</v>
-      </c>
-      <c r="E344" s="14">
-        <v>2589.9299999999998</v>
+        <v>50.87</v>
+      </c>
+      <c r="E344" s="5">
+        <v>2581.4299999999998</v>
       </c>
       <c r="F344" s="32" t="s">
         <v>295</v>
       </c>
-      <c r="G344" s="13">
-        <f>AVERAGE(E345:E346)</f>
-        <v>2580.4549999999999</v>
-      </c>
-      <c r="H344" s="18">
-        <f>STDEV(E345:E346)</f>
-        <v>1.3788582233136391</v>
-      </c>
-      <c r="K344" s="5">
-        <f>G344+$J$295</f>
-        <v>2584.9</v>
-      </c>
     </row>
     <row r="345" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A345" s="9" t="s">
@@ -10339,10 +10324,10 @@
         <v>12</v>
       </c>
       <c r="D345" s="5">
-        <v>50.87</v>
+        <v>49.3</v>
       </c>
       <c r="E345" s="5">
-        <v>2581.4299999999998</v>
+        <v>2579.48</v>
       </c>
       <c r="F345" s="32" t="s">
         <v>296</v>
@@ -10353,20 +10338,32 @@
         <v>11</v>
       </c>
       <c r="B346" s="31">
-        <v>45082</v>
+        <v>45083</v>
       </c>
       <c r="C346" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D346" s="5">
-        <v>49.3</v>
+        <v>51.48</v>
       </c>
       <c r="E346" s="5">
-        <v>2579.48</v>
+        <v>2583.7800000000002</v>
       </c>
       <c r="F346" s="32" t="s">
         <v>297</v>
       </c>
+      <c r="G346" s="13">
+        <f>AVERAGE(E346:E347)</f>
+        <v>2581.6000000000004</v>
+      </c>
+      <c r="H346" s="18">
+        <f>STDEV(E346:E347)</f>
+        <v>3.0829855659734373</v>
+      </c>
+      <c r="K346" s="5">
+        <f>G346+$J$332</f>
+        <v>2569.7350000000001</v>
+      </c>
     </row>
     <row r="347" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A347" s="9" t="s">
@@ -10379,23 +10376,14 @@
         <v>12</v>
       </c>
       <c r="D347" s="5">
-        <v>51.48</v>
+        <v>50.77</v>
+      </c>
+      <c r="E347" s="5">
+        <v>2579.42</v>
       </c>
       <c r="F347" s="32" t="s">
         <v>298</v>
       </c>
-      <c r="G347" s="13" t="e">
-        <f>AVERAGE(E348:E349)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H347" s="18" t="e">
-        <f>STDEV(E348:E349)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K347" s="5" t="e">
-        <f>G347+$J$333</f>
-        <v>#DIV/0!</v>
-      </c>
     </row>
     <row r="348" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A348" s="9" t="s">
@@ -10408,11 +10396,26 @@
         <v>12</v>
       </c>
       <c r="D348" s="5">
-        <v>50.77</v>
+        <v>50.57</v>
+      </c>
+      <c r="E348" s="5">
+        <v>2526.5100000000002</v>
       </c>
       <c r="F348" s="32" t="s">
         <v>299</v>
       </c>
+      <c r="G348" s="13">
+        <f>AVERAGE(E348:E349)</f>
+        <v>2524.2700000000004</v>
+      </c>
+      <c r="H348" s="18">
+        <f>STDEV(E348:E349)</f>
+        <v>3.1678383797157457</v>
+      </c>
+      <c r="K348" s="5">
+        <f>G348+$J$332</f>
+        <v>2512.4050000000002</v>
+      </c>
     </row>
     <row r="349" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A349" s="9" t="s">
@@ -10425,7 +10428,10 @@
         <v>12</v>
       </c>
       <c r="D349" s="5">
-        <v>50.17</v>
+        <v>50.2</v>
+      </c>
+      <c r="E349" s="5">
+        <v>2522.0300000000002</v>
       </c>
       <c r="F349" s="32" t="s">
         <v>300</v>
@@ -10442,22 +10448,25 @@
         <v>12</v>
       </c>
       <c r="D350" s="5">
-        <v>50.57</v>
+        <v>51.23</v>
+      </c>
+      <c r="E350" s="5">
+        <v>2528.85</v>
       </c>
       <c r="F350" s="32" t="s">
         <v>301</v>
       </c>
-      <c r="G350" s="13" t="e">
-        <f>AVERAGE(E351:E352)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H350" s="18" t="e">
-        <f>STDEV(E351:E352)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K350" s="5" t="e">
-        <f>G350+$J$333</f>
-        <v>#DIV/0!</v>
+      <c r="G350" s="13">
+        <f>AVERAGE(E350,E352)</f>
+        <v>2527.4899999999998</v>
+      </c>
+      <c r="H350" s="18">
+        <f>STDEV(E350,E352)</f>
+        <v>1.9233304448272679</v>
+      </c>
+      <c r="K350" s="5">
+        <f>G350+$J$332</f>
+        <v>2515.6249999999995</v>
       </c>
     </row>
     <row r="351" spans="1:11" x14ac:dyDescent="0.2">
@@ -10471,7 +10480,10 @@
         <v>12</v>
       </c>
       <c r="D351" s="5">
-        <v>50.2</v>
+        <v>50.45</v>
+      </c>
+      <c r="E351" s="14">
+        <v>2487.25</v>
       </c>
       <c r="F351" s="32" t="s">
         <v>302</v>
@@ -10488,10 +10500,13 @@
         <v>12</v>
       </c>
       <c r="D352" s="5">
-        <v>49.92</v>
+        <v>50.72</v>
+      </c>
+      <c r="E352" s="5">
+        <v>2526.13</v>
       </c>
       <c r="F352" s="32" t="s">
-        <v>303</v>
+        <v>413</v>
       </c>
     </row>
     <row r="353" spans="1:11" x14ac:dyDescent="0.2">
@@ -10504,20 +10519,26 @@
       <c r="C353" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D353" s="5">
+        <v>49.24</v>
+      </c>
+      <c r="E353" s="5">
+        <v>2442.25</v>
+      </c>
       <c r="F353" s="32" t="s">
-        <v>304</v>
-      </c>
-      <c r="G353" s="13" t="e">
-        <f>AVERAGE(E354:E355)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H353" s="18" t="e">
-        <f>STDEV(E354:E355)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K353" s="5" t="e">
-        <f>G353+$J$333</f>
-        <v>#DIV/0!</v>
+        <v>303</v>
+      </c>
+      <c r="G353" s="13">
+        <f>AVERAGE(E353:E354)</f>
+        <v>2443.69</v>
+      </c>
+      <c r="H353" s="18">
+        <f>STDEV(E353:E354)</f>
+        <v>2.036467529817334</v>
+      </c>
+      <c r="K353" s="5">
+        <f>G353+$J$332</f>
+        <v>2431.8249999999998</v>
       </c>
     </row>
     <row r="354" spans="1:11" x14ac:dyDescent="0.2">
@@ -10530,8 +10551,14 @@
       <c r="C354" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D354" s="5">
+        <v>50.38</v>
+      </c>
+      <c r="E354" s="5">
+        <v>2445.13</v>
+      </c>
       <c r="F354" s="32" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="355" spans="1:11" x14ac:dyDescent="0.2">
@@ -10544,8 +10571,26 @@
       <c r="C355" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D355" s="5">
+        <v>50.66</v>
+      </c>
+      <c r="E355" s="5">
+        <v>2465.79</v>
+      </c>
       <c r="F355" s="32" t="s">
-        <v>306</v>
+        <v>305</v>
+      </c>
+      <c r="G355" s="13">
+        <f>AVERAGE(E355,E357)</f>
+        <v>2464.0450000000001</v>
+      </c>
+      <c r="H355" s="18">
+        <f>STDEV(E355,E357)</f>
+        <v>2.4678026663408965</v>
+      </c>
+      <c r="K355" s="5">
+        <f>G355+$J$332</f>
+        <v>2452.1799999999998</v>
       </c>
     </row>
     <row r="356" spans="1:11" x14ac:dyDescent="0.2">
@@ -10558,20 +10603,14 @@
       <c r="C356" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D356" s="5">
+        <v>50.38</v>
+      </c>
+      <c r="E356" s="14">
+        <v>2473.2600000000002</v>
+      </c>
       <c r="F356" s="32" t="s">
-        <v>307</v>
-      </c>
-      <c r="G356" s="13" t="e">
-        <f>AVERAGE(E357:E358)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H356" s="18" t="e">
-        <f>STDEV(E357:E358)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K356" s="5" t="e">
-        <f>G356+$J$333</f>
-        <v>#DIV/0!</v>
+        <v>306</v>
       </c>
     </row>
     <row r="357" spans="1:11" x14ac:dyDescent="0.2">
@@ -10584,8 +10623,14 @@
       <c r="C357" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D357" s="5">
+        <v>49.58</v>
+      </c>
+      <c r="E357" s="5">
+        <v>2462.3000000000002</v>
+      </c>
       <c r="F357" s="32" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="358" spans="1:11" x14ac:dyDescent="0.2">
@@ -10598,8 +10643,26 @@
       <c r="C358" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D358" s="5">
+        <v>48.57</v>
+      </c>
+      <c r="E358" s="5">
+        <v>2592.0100000000002</v>
+      </c>
       <c r="F358" s="32" t="s">
-        <v>309</v>
+        <v>308</v>
+      </c>
+      <c r="G358" s="13">
+        <f>AVERAGE(E359,E360)</f>
+        <v>2479.8000000000002</v>
+      </c>
+      <c r="H358" s="18">
+        <f>STDEV(E359,E360)</f>
+        <v>3.2385490578343363</v>
+      </c>
+      <c r="K358" s="5">
+        <f>G358+$J$332</f>
+        <v>2467.9349999999999</v>
       </c>
     </row>
     <row r="359" spans="1:11" x14ac:dyDescent="0.2">
@@ -10612,20 +10675,14 @@
       <c r="C359" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D359" s="5">
+        <v>48.07</v>
+      </c>
+      <c r="E359" s="5">
+        <v>2477.5100000000002</v>
+      </c>
       <c r="F359" s="32" t="s">
-        <v>310</v>
-      </c>
-      <c r="G359" s="13" t="e">
-        <f>AVERAGE(E360:E361)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H359" s="18" t="e">
-        <f>STDEV(E360:E361)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K359" s="5" t="e">
-        <f>G359+$J$333</f>
-        <v>#DIV/0!</v>
+        <v>309</v>
       </c>
     </row>
     <row r="360" spans="1:11" x14ac:dyDescent="0.2">
@@ -10638,8 +10695,14 @@
       <c r="C360" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D360" s="5">
+        <v>51.58</v>
+      </c>
+      <c r="E360" s="5">
+        <v>2482.09</v>
+      </c>
       <c r="F360" s="32" t="s">
-        <v>311</v>
+        <v>414</v>
       </c>
     </row>
     <row r="361" spans="1:11" x14ac:dyDescent="0.2">
@@ -10652,8 +10715,26 @@
       <c r="C361" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D361" s="5">
+        <v>49.59</v>
+      </c>
+      <c r="E361" s="5">
+        <v>2471.12</v>
+      </c>
       <c r="F361" s="32" t="s">
-        <v>312</v>
+        <v>310</v>
+      </c>
+      <c r="G361" s="13">
+        <f>AVERAGE(E361,E363)</f>
+        <v>2473.2049999999999</v>
+      </c>
+      <c r="H361" s="18">
+        <f>STDEV(E361,E363)</f>
+        <v>2.9486352775479547</v>
+      </c>
+      <c r="K361" s="5">
+        <f>G361+$J$332</f>
+        <v>2461.3399999999997</v>
       </c>
     </row>
     <row r="362" spans="1:11" x14ac:dyDescent="0.2">
@@ -10666,20 +10747,14 @@
       <c r="C362" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D362" s="5">
+        <v>49.61</v>
+      </c>
+      <c r="E362" s="14">
+        <v>2442.16</v>
+      </c>
       <c r="F362" s="32" t="s">
-        <v>313</v>
-      </c>
-      <c r="G362" s="13" t="e">
-        <f>AVERAGE(E363:E364)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H362" s="18" t="e">
-        <f>STDEV(E363:E364)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K362" s="5" t="e">
-        <f>G362+$J$333</f>
-        <v>#DIV/0!</v>
+        <v>311</v>
       </c>
     </row>
     <row r="363" spans="1:11" x14ac:dyDescent="0.2">
@@ -10692,8 +10767,14 @@
       <c r="C363" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F363" s="32" t="s">
-        <v>314</v>
+      <c r="D363" s="5">
+        <v>50.11</v>
+      </c>
+      <c r="E363" s="5">
+        <v>2475.29</v>
+      </c>
+      <c r="F363" s="33" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="364" spans="1:11" x14ac:dyDescent="0.2">
@@ -10706,8 +10787,26 @@
       <c r="C364" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D364" s="5">
+        <v>50.48</v>
+      </c>
+      <c r="E364" s="14">
+        <v>2497.66</v>
+      </c>
       <c r="F364" s="32" t="s">
-        <v>315</v>
+        <v>313</v>
+      </c>
+      <c r="G364" s="13">
+        <f>AVERAGE(E365:E366)</f>
+        <v>2475.91</v>
+      </c>
+      <c r="H364" s="18">
+        <f>STDEV(E365:E366)</f>
+        <v>1.5980613254814302</v>
+      </c>
+      <c r="K364" s="5">
+        <f>G364+$J$332</f>
+        <v>2464.0449999999996</v>
       </c>
     </row>
     <row r="365" spans="1:11" x14ac:dyDescent="0.2">
@@ -10720,20 +10819,14 @@
       <c r="C365" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D365" s="5">
+        <v>51.38</v>
+      </c>
+      <c r="E365" s="5">
+        <v>2474.7800000000002</v>
+      </c>
       <c r="F365" s="32" t="s">
-        <v>316</v>
-      </c>
-      <c r="G365" s="13" t="e">
-        <f>AVERAGE(E366:E367)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H365" s="18" t="e">
-        <f>STDEV(E366:E367)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K365" s="5" t="e">
-        <f>G365+$J$333</f>
-        <v>#DIV/0!</v>
+        <v>314</v>
       </c>
     </row>
     <row r="366" spans="1:11" x14ac:dyDescent="0.2">
@@ -10746,8 +10839,14 @@
       <c r="C366" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D366" s="5">
+        <v>50.49</v>
+      </c>
+      <c r="E366" s="5">
+        <v>2477.04</v>
+      </c>
       <c r="F366" s="32" t="s">
-        <v>317</v>
+        <v>415</v>
       </c>
     </row>
     <row r="367" spans="1:11" x14ac:dyDescent="0.2">
@@ -10760,8 +10859,26 @@
       <c r="C367" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F367" s="33" t="s">
-        <v>318</v>
+      <c r="D367" s="5">
+        <v>50.73</v>
+      </c>
+      <c r="E367" s="5">
+        <v>2478.58</v>
+      </c>
+      <c r="F367" s="32" t="s">
+        <v>315</v>
+      </c>
+      <c r="G367" s="13">
+        <f>AVERAGE(E367,E369)</f>
+        <v>2481.125</v>
+      </c>
+      <c r="H367" s="18">
+        <f>STDEV(E367,E369)</f>
+        <v>3.5991735162396297</v>
+      </c>
+      <c r="K367" s="5">
+        <f>G367+$J$332</f>
+        <v>2469.2599999999998</v>
       </c>
     </row>
     <row r="368" spans="1:11" x14ac:dyDescent="0.2">
@@ -10774,20 +10891,14 @@
       <c r="C368" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D368" s="5">
+        <v>48.76</v>
+      </c>
+      <c r="E368" s="14">
+        <v>2462.1799999999998</v>
+      </c>
       <c r="F368" s="32" t="s">
-        <v>319</v>
-      </c>
-      <c r="G368" s="13" t="e">
-        <f>AVERAGE(E369:E370)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H368" s="18" t="e">
-        <f>STDEV(E369:E370)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K368" s="5" t="e">
-        <f>G368+$J$333</f>
-        <v>#DIV/0!</v>
+        <v>316</v>
       </c>
     </row>
     <row r="369" spans="1:11" x14ac:dyDescent="0.2">
@@ -10800,23 +10911,18 @@
       <c r="C369" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D369" s="5">
+        <v>49.49</v>
+      </c>
+      <c r="E369" s="5">
+        <v>2483.67</v>
+      </c>
       <c r="F369" s="32" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="370" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A370" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B370" s="31">
-        <v>45083</v>
-      </c>
-      <c r="C370" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F370" s="32" t="s">
-        <v>321</v>
-      </c>
+      <c r="F370" s="32"/>
     </row>
     <row r="371" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A371" s="9" t="s">
@@ -10828,20 +10934,26 @@
       <c r="C371" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D371" s="5">
+        <v>49.57</v>
+      </c>
+      <c r="E371" s="5">
+        <v>2419.6799999999998</v>
+      </c>
       <c r="F371" s="32" t="s">
-        <v>322</v>
-      </c>
-      <c r="G371" s="13" t="e">
-        <f>AVERAGE(E372:E373)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H371" s="18" t="e">
-        <f>STDEV(E372:E373)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K371" s="5" t="e">
-        <f>G371+$J$333</f>
-        <v>#DIV/0!</v>
+        <v>318</v>
+      </c>
+      <c r="G371" s="13">
+        <f>AVERAGE(E371:E372)</f>
+        <v>2421.96</v>
+      </c>
+      <c r="H371" s="18">
+        <f>STDEV(E371:E372)</f>
+        <v>3.2244069222106182</v>
+      </c>
+      <c r="K371" s="5">
+        <f>G371+$J$332</f>
+        <v>2410.0949999999998</v>
       </c>
     </row>
     <row r="372" spans="1:11" x14ac:dyDescent="0.2">
@@ -10854,8 +10966,14 @@
       <c r="C372" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D372" s="5">
+        <v>49.37</v>
+      </c>
+      <c r="E372" s="5">
+        <v>2424.2399999999998</v>
+      </c>
       <c r="F372" s="32" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="373" spans="1:11" x14ac:dyDescent="0.2">
@@ -10868,67 +10986,138 @@
       <c r="C373" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D373" s="5">
+        <v>48.39</v>
+      </c>
+      <c r="E373" s="5">
+        <v>2487.91</v>
+      </c>
       <c r="F373" s="32" t="s">
+        <v>320</v>
+      </c>
+      <c r="G373" s="13">
+        <f>AVERAGE(E373,E375)</f>
+        <v>2488.9749999999999</v>
+      </c>
+      <c r="H373" s="18">
+        <f>STDEV(E373,E375)</f>
+        <v>1.5061374439274233</v>
+      </c>
+      <c r="K373" s="5">
+        <f>G373+$J$332</f>
+        <v>2477.1099999999997</v>
+      </c>
+    </row>
+    <row r="374" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A374" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B374" s="31">
+        <v>45083</v>
+      </c>
+      <c r="C374" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D374" s="5">
+        <v>50.53</v>
+      </c>
+      <c r="E374" s="14">
+        <v>2498.6999999999998</v>
+      </c>
+      <c r="F374" s="32" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="375" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A375" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B375" s="31">
+        <v>45083</v>
+      </c>
+      <c r="C375" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D375" s="5">
+        <v>50.24</v>
+      </c>
+      <c r="E375" s="5">
+        <v>2490.04</v>
+      </c>
+      <c r="F375" s="32" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="376" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A376" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B376" s="31">
+        <v>45083</v>
+      </c>
+      <c r="C376" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D376" s="5">
+        <v>48.99</v>
+      </c>
+      <c r="E376" s="14">
+        <v>2472.96</v>
+      </c>
+      <c r="F376" s="32" t="s">
+        <v>323</v>
+      </c>
+      <c r="G376" s="13">
+        <f>AVERAGE(E377:E378)</f>
+        <v>2465.23</v>
+      </c>
+      <c r="H376" s="18">
+        <f>STDEV(E377:E378)</f>
+        <v>2.6587214972615731</v>
+      </c>
+      <c r="K376" s="5">
+        <f>G376+$J$332</f>
+        <v>2453.3649999999998</v>
+      </c>
+    </row>
+    <row r="377" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A377" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B377" s="31">
+        <v>45083</v>
+      </c>
+      <c r="C377" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D377" s="5">
+        <v>49.26</v>
+      </c>
+      <c r="E377" s="5">
+        <v>2463.35</v>
+      </c>
+      <c r="F377" s="32" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="374" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F374" s="32"/>
-    </row>
-    <row r="375" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C375" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F375" s="32" t="s">
+    <row r="378" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A378" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B378" s="31">
+        <v>45083</v>
+      </c>
+      <c r="C378" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D378" s="5">
+        <v>49.75</v>
+      </c>
+      <c r="E378" s="5">
+        <v>2467.11</v>
+      </c>
+      <c r="F378" s="32" t="s">
         <v>325</v>
-      </c>
-      <c r="G375" s="13" t="e">
-        <f>AVERAGE(E376:E377)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H375" s="18" t="e">
-        <f>STDEV(E376:E377)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K375" s="5" t="e">
-        <f>G375+$J$333</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="376" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C376" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F376" s="32" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="377" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C377" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F377" s="32" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="378" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C378" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F378" s="32" t="s">
-        <v>328</v>
-      </c>
-      <c r="G378" s="13" t="e">
-        <f>AVERAGE(E379:E380)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H378" s="18" t="e">
-        <f>STDEV(E379:E380)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K378" s="5" t="e">
-        <f>G378+$J$333</f>
-        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="379" spans="1:11" x14ac:dyDescent="0.2">
@@ -10936,7 +11125,19 @@
         <v>12</v>
       </c>
       <c r="F379" s="32" t="s">
-        <v>329</v>
+        <v>326</v>
+      </c>
+      <c r="G379" s="13" t="e">
+        <f>AVERAGE(E380:E381)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H379" s="18" t="e">
+        <f>STDEV(E380:E381)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K379" s="5" t="e">
+        <f>G379+$J$332</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="380" spans="1:11" x14ac:dyDescent="0.2">
@@ -10944,7 +11145,7 @@
         <v>12</v>
       </c>
       <c r="F380" s="32" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="381" spans="1:11" x14ac:dyDescent="0.2">
@@ -10952,19 +11153,7 @@
         <v>12</v>
       </c>
       <c r="F381" s="32" t="s">
-        <v>331</v>
-      </c>
-      <c r="G381" s="13" t="e">
-        <f>AVERAGE(E382:E383)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H381" s="18" t="e">
-        <f>STDEV(E382:E383)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K381" s="5" t="e">
-        <f>G381+$J$333</f>
-        <v>#DIV/0!</v>
+        <v>328</v>
       </c>
     </row>
     <row r="382" spans="1:11" x14ac:dyDescent="0.2">
@@ -10972,7 +11161,19 @@
         <v>12</v>
       </c>
       <c r="F382" s="32" t="s">
-        <v>332</v>
+        <v>329</v>
+      </c>
+      <c r="G382" s="13" t="e">
+        <f>AVERAGE(E383:E384)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H382" s="18" t="e">
+        <f>STDEV(E383:E384)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K382" s="5" t="e">
+        <f>G382+$J$332</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="383" spans="1:11" x14ac:dyDescent="0.2">
@@ -10980,7 +11181,7 @@
         <v>12</v>
       </c>
       <c r="F383" s="32" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="384" spans="1:11" x14ac:dyDescent="0.2">
@@ -10988,19 +11189,7 @@
         <v>12</v>
       </c>
       <c r="F384" s="32" t="s">
-        <v>334</v>
-      </c>
-      <c r="G384" s="13" t="e">
-        <f>AVERAGE(E385:E386)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H384" s="18" t="e">
-        <f>STDEV(E385:E386)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K384" s="5" t="e">
-        <f>G384+$J$333</f>
-        <v>#DIV/0!</v>
+        <v>331</v>
       </c>
     </row>
     <row r="385" spans="3:11" x14ac:dyDescent="0.2">
@@ -11008,7 +11197,19 @@
         <v>12</v>
       </c>
       <c r="F385" s="32" t="s">
-        <v>335</v>
+        <v>332</v>
+      </c>
+      <c r="G385" s="13" t="e">
+        <f>AVERAGE(E386:E387)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H385" s="18" t="e">
+        <f>STDEV(E386:E387)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K385" s="5" t="e">
+        <f>G385+$J$332</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="386" spans="3:11" x14ac:dyDescent="0.2">
@@ -11016,7 +11217,7 @@
         <v>12</v>
       </c>
       <c r="F386" s="32" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="387" spans="3:11" x14ac:dyDescent="0.2">
@@ -11024,19 +11225,7 @@
         <v>12</v>
       </c>
       <c r="F387" s="32" t="s">
-        <v>337</v>
-      </c>
-      <c r="G387" s="13" t="e">
-        <f>AVERAGE(E388:E389)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H387" s="18" t="e">
-        <f>STDEV(E388:E389)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K387" s="5" t="e">
-        <f>G387+$J$333</f>
-        <v>#DIV/0!</v>
+        <v>334</v>
       </c>
     </row>
     <row r="388" spans="3:11" x14ac:dyDescent="0.2">
@@ -11044,7 +11233,19 @@
         <v>12</v>
       </c>
       <c r="F388" s="32" t="s">
-        <v>338</v>
+        <v>335</v>
+      </c>
+      <c r="G388" s="13" t="e">
+        <f>AVERAGE(E389:E390)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H388" s="18" t="e">
+        <f>STDEV(E389:E390)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K388" s="5" t="e">
+        <f>G388+$J$332</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="389" spans="3:11" x14ac:dyDescent="0.2">
@@ -11052,7 +11253,7 @@
         <v>12</v>
       </c>
       <c r="F389" s="32" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="390" spans="3:11" x14ac:dyDescent="0.2">
@@ -11060,19 +11261,7 @@
         <v>12</v>
       </c>
       <c r="F390" s="32" t="s">
-        <v>340</v>
-      </c>
-      <c r="G390" s="13" t="e">
-        <f>AVERAGE(E391:E392)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H390" s="18" t="e">
-        <f>STDEV(E391:E392)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K390" s="5" t="e">
-        <f>G390+$J$333</f>
-        <v>#DIV/0!</v>
+        <v>337</v>
       </c>
     </row>
     <row r="391" spans="3:11" x14ac:dyDescent="0.2">
@@ -11080,7 +11269,19 @@
         <v>12</v>
       </c>
       <c r="F391" s="32" t="s">
-        <v>341</v>
+        <v>338</v>
+      </c>
+      <c r="G391" s="13" t="e">
+        <f>AVERAGE(E392:E393)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H391" s="18" t="e">
+        <f>STDEV(E392:E393)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K391" s="5" t="e">
+        <f>G391+$J$332</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="392" spans="3:11" x14ac:dyDescent="0.2">
@@ -11088,7 +11289,7 @@
         <v>12</v>
       </c>
       <c r="F392" s="32" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="393" spans="3:11" x14ac:dyDescent="0.2">
@@ -11096,19 +11297,7 @@
         <v>12</v>
       </c>
       <c r="F393" s="32" t="s">
-        <v>343</v>
-      </c>
-      <c r="G393" s="13" t="e">
-        <f>AVERAGE(E394:E395)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H393" s="18" t="e">
-        <f>STDEV(E394:E395)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K393" s="5" t="e">
-        <f>G393+$J$333</f>
-        <v>#DIV/0!</v>
+        <v>340</v>
       </c>
     </row>
     <row r="394" spans="3:11" x14ac:dyDescent="0.2">
@@ -11116,7 +11305,19 @@
         <v>12</v>
       </c>
       <c r="F394" s="32" t="s">
-        <v>344</v>
+        <v>341</v>
+      </c>
+      <c r="G394" s="13" t="e">
+        <f>AVERAGE(E395:E396)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H394" s="18" t="e">
+        <f>STDEV(E395:E396)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K394" s="5" t="e">
+        <f>G394+$J$332</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="395" spans="3:11" x14ac:dyDescent="0.2">
@@ -11124,7 +11325,7 @@
         <v>12</v>
       </c>
       <c r="F395" s="32" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="396" spans="3:11" x14ac:dyDescent="0.2">
@@ -11132,63 +11333,34 @@
         <v>12</v>
       </c>
       <c r="F396" s="32" t="s">
-        <v>346</v>
-      </c>
-      <c r="G396" s="13" t="e">
-        <f>AVERAGE(E397:E398)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H396" s="18" t="e">
-        <f>STDEV(E397:E398)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K396" s="5" t="e">
-        <f>G396+$J$333</f>
-        <v>#DIV/0!</v>
+        <v>343</v>
       </c>
     </row>
     <row r="397" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C397" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F397" s="32" t="s">
-        <v>347</v>
-      </c>
+      <c r="C397" s="10"/>
     </row>
     <row r="398" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C398" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F398" s="32" t="s">
-        <v>348</v>
+      <c r="C398" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F398" s="16" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="399" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C399" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F399" s="32" t="s">
-        <v>349</v>
-      </c>
-      <c r="G399" s="13" t="e">
-        <f>AVERAGE(E400:E401)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H399" s="18" t="e">
-        <f>STDEV(E400:E401)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K399" s="5" t="e">
-        <f>G399+$J$333</f>
-        <v>#DIV/0!</v>
+      <c r="F399" s="16" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="400" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C400" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F400" s="32" t="s">
-        <v>350</v>
+      <c r="F400" s="17" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="401" spans="3:6" x14ac:dyDescent="0.2">
@@ -11196,34 +11368,39 @@
         <v>12</v>
       </c>
       <c r="F401" s="32" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
     </row>
     <row r="402" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C402" s="10"/>
+      <c r="C402" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F402" s="32" t="s">
+        <v>345</v>
+      </c>
     </row>
     <row r="403" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C403" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="F403" s="16" t="s">
-        <v>8</v>
+      <c r="C403" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F403" s="32" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="404" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C404" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F404" s="16" t="s">
-        <v>9</v>
+      <c r="F404" s="32" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="405" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C405" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F405" s="17" t="s">
-        <v>96</v>
+      <c r="F405" s="32" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="406" spans="3:6" x14ac:dyDescent="0.2">
@@ -11231,7 +11408,7 @@
         <v>12</v>
       </c>
       <c r="F406" s="32" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="407" spans="3:6" x14ac:dyDescent="0.2">
@@ -11239,7 +11416,7 @@
         <v>12</v>
       </c>
       <c r="F407" s="32" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="408" spans="3:6" x14ac:dyDescent="0.2">
@@ -11247,7 +11424,7 @@
         <v>12</v>
       </c>
       <c r="F408" s="32" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="409" spans="3:6" x14ac:dyDescent="0.2">
@@ -11255,7 +11432,7 @@
         <v>12</v>
       </c>
       <c r="F409" s="32" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="410" spans="3:6" x14ac:dyDescent="0.2">
@@ -11263,7 +11440,7 @@
         <v>12</v>
       </c>
       <c r="F410" s="32" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="411" spans="3:6" x14ac:dyDescent="0.2">
@@ -11271,7 +11448,7 @@
         <v>12</v>
       </c>
       <c r="F411" s="32" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="412" spans="3:6" x14ac:dyDescent="0.2">
@@ -11279,7 +11456,7 @@
         <v>12</v>
       </c>
       <c r="F412" s="32" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="413" spans="3:6" x14ac:dyDescent="0.2">
@@ -11287,7 +11464,7 @@
         <v>12</v>
       </c>
       <c r="F413" s="32" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="414" spans="3:6" x14ac:dyDescent="0.2">
@@ -11295,7 +11472,7 @@
         <v>12</v>
       </c>
       <c r="F414" s="32" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="415" spans="3:6" x14ac:dyDescent="0.2">
@@ -11303,7 +11480,7 @@
         <v>12</v>
       </c>
       <c r="F415" s="32" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="416" spans="3:6" x14ac:dyDescent="0.2">
@@ -11311,7 +11488,7 @@
         <v>12</v>
       </c>
       <c r="F416" s="32" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="417" spans="3:6" x14ac:dyDescent="0.2">
@@ -11319,7 +11496,7 @@
         <v>12</v>
       </c>
       <c r="F417" s="32" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="418" spans="3:6" x14ac:dyDescent="0.2">
@@ -11327,7 +11504,7 @@
         <v>12</v>
       </c>
       <c r="F418" s="32" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="419" spans="3:6" x14ac:dyDescent="0.2">
@@ -11335,7 +11512,7 @@
         <v>12</v>
       </c>
       <c r="F419" s="32" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="420" spans="3:6" x14ac:dyDescent="0.2">
@@ -11343,7 +11520,7 @@
         <v>12</v>
       </c>
       <c r="F420" s="32" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="421" spans="3:6" x14ac:dyDescent="0.2">
@@ -11351,7 +11528,7 @@
         <v>12</v>
       </c>
       <c r="F421" s="32" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="422" spans="3:6" x14ac:dyDescent="0.2">
@@ -11359,7 +11536,7 @@
         <v>12</v>
       </c>
       <c r="F422" s="32" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="423" spans="3:6" x14ac:dyDescent="0.2">
@@ -11367,7 +11544,7 @@
         <v>12</v>
       </c>
       <c r="F423" s="32" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="424" spans="3:6" x14ac:dyDescent="0.2">
@@ -11375,7 +11552,7 @@
         <v>12</v>
       </c>
       <c r="F424" s="32" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="425" spans="3:6" x14ac:dyDescent="0.2">
@@ -11383,7 +11560,7 @@
         <v>12</v>
       </c>
       <c r="F425" s="32" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="426" spans="3:6" x14ac:dyDescent="0.2">
@@ -11391,7 +11568,7 @@
         <v>12</v>
       </c>
       <c r="F426" s="32" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="427" spans="3:6" x14ac:dyDescent="0.2">
@@ -11399,7 +11576,7 @@
         <v>12</v>
       </c>
       <c r="F427" s="32" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="428" spans="3:6" x14ac:dyDescent="0.2">
@@ -11407,7 +11584,7 @@
         <v>12</v>
       </c>
       <c r="F428" s="32" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="429" spans="3:6" x14ac:dyDescent="0.2">
@@ -11415,7 +11592,7 @@
         <v>12</v>
       </c>
       <c r="F429" s="32" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="430" spans="3:6" x14ac:dyDescent="0.2">
@@ -11423,7 +11600,7 @@
         <v>12</v>
       </c>
       <c r="F430" s="32" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="431" spans="3:6" x14ac:dyDescent="0.2">
@@ -11431,15 +11608,15 @@
         <v>12</v>
       </c>
       <c r="F431" s="32" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="432" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C432" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F432" s="32" t="s">
-        <v>378</v>
+      <c r="F432" s="33" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="433" spans="3:6" x14ac:dyDescent="0.2">
@@ -11447,7 +11624,7 @@
         <v>12</v>
       </c>
       <c r="F433" s="32" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="434" spans="3:6" x14ac:dyDescent="0.2">
@@ -11455,7 +11632,7 @@
         <v>12</v>
       </c>
       <c r="F434" s="32" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="435" spans="3:6" x14ac:dyDescent="0.2">
@@ -11463,7 +11640,7 @@
         <v>12</v>
       </c>
       <c r="F435" s="32" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="436" spans="3:6" x14ac:dyDescent="0.2">
@@ -11471,15 +11648,15 @@
         <v>12</v>
       </c>
       <c r="F436" s="32" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="437" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C437" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F437" s="33" t="s">
-        <v>383</v>
+      <c r="C437" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F437" s="32" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="438" spans="3:6" x14ac:dyDescent="0.2">
@@ -11487,39 +11664,34 @@
         <v>12</v>
       </c>
       <c r="F438" s="32" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="439" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C439" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F439" s="32" t="s">
-        <v>385</v>
-      </c>
+      <c r="F439" s="32"/>
     </row>
     <row r="440" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C440" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F440" s="32" t="s">
-        <v>386</v>
+      <c r="F440" s="16" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="441" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C441" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F441" s="32" t="s">
-        <v>387</v>
+      <c r="F441" s="16" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="442" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C442" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="F442" s="32" t="s">
-        <v>388</v>
+      <c r="C442" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F442" s="17" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="443" spans="3:6" x14ac:dyDescent="0.2">
@@ -11527,34 +11699,39 @@
         <v>12</v>
       </c>
       <c r="F443" s="32" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
     </row>
     <row r="444" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="F444" s="32"/>
+      <c r="C444" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F444" s="32" t="s">
+        <v>383</v>
+      </c>
     </row>
     <row r="445" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C445" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F445" s="16" t="s">
-        <v>8</v>
+      <c r="F445" s="32" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="446" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C446" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F446" s="16" t="s">
-        <v>9</v>
+      <c r="F446" s="32" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="447" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C447" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F447" s="17" t="s">
-        <v>96</v>
+      <c r="F447" s="32" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="448" spans="3:6" x14ac:dyDescent="0.2">
@@ -11562,7 +11739,7 @@
         <v>12</v>
       </c>
       <c r="F448" s="32" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="449" spans="3:6" x14ac:dyDescent="0.2">
@@ -11570,7 +11747,7 @@
         <v>12</v>
       </c>
       <c r="F449" s="32" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="450" spans="3:6" x14ac:dyDescent="0.2">
@@ -11578,7 +11755,7 @@
         <v>12</v>
       </c>
       <c r="F450" s="32" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="451" spans="3:6" x14ac:dyDescent="0.2">
@@ -11586,7 +11763,7 @@
         <v>12</v>
       </c>
       <c r="F451" s="32" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="452" spans="3:6" x14ac:dyDescent="0.2">
@@ -11594,7 +11771,7 @@
         <v>12</v>
       </c>
       <c r="F452" s="32" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="453" spans="3:6" x14ac:dyDescent="0.2">
@@ -11602,7 +11779,7 @@
         <v>12</v>
       </c>
       <c r="F453" s="32" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="454" spans="3:6" x14ac:dyDescent="0.2">
@@ -11610,7 +11787,7 @@
         <v>12</v>
       </c>
       <c r="F454" s="32" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="455" spans="3:6" x14ac:dyDescent="0.2">
@@ -11618,7 +11795,7 @@
         <v>12</v>
       </c>
       <c r="F455" s="32" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="456" spans="3:6" x14ac:dyDescent="0.2">
@@ -11626,7 +11803,7 @@
         <v>12</v>
       </c>
       <c r="F456" s="32" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="457" spans="3:6" x14ac:dyDescent="0.2">
@@ -11634,7 +11811,7 @@
         <v>12</v>
       </c>
       <c r="F457" s="32" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="458" spans="3:6" x14ac:dyDescent="0.2">
@@ -11642,7 +11819,7 @@
         <v>12</v>
       </c>
       <c r="F458" s="32" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="459" spans="3:6" x14ac:dyDescent="0.2">
@@ -11650,7 +11827,7 @@
         <v>12</v>
       </c>
       <c r="F459" s="32" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="460" spans="3:6" x14ac:dyDescent="0.2">
@@ -11658,7 +11835,7 @@
         <v>12</v>
       </c>
       <c r="F460" s="32" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="461" spans="3:6" x14ac:dyDescent="0.2">
@@ -11666,7 +11843,7 @@
         <v>12</v>
       </c>
       <c r="F461" s="32" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
     </row>
     <row r="462" spans="3:6" x14ac:dyDescent="0.2">
@@ -11674,7 +11851,7 @@
         <v>12</v>
       </c>
       <c r="F462" s="32" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="463" spans="3:6" x14ac:dyDescent="0.2">
@@ -11682,7 +11859,7 @@
         <v>12</v>
       </c>
       <c r="F463" s="32" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="464" spans="3:6" x14ac:dyDescent="0.2">
@@ -11690,7 +11867,7 @@
         <v>12</v>
       </c>
       <c r="F464" s="32" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="465" spans="3:6" x14ac:dyDescent="0.2">
@@ -11698,7 +11875,7 @@
         <v>12</v>
       </c>
       <c r="F465" s="32" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="466" spans="3:6" x14ac:dyDescent="0.2">
@@ -11706,7 +11883,7 @@
         <v>12</v>
       </c>
       <c r="F466" s="32" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="467" spans="3:6" x14ac:dyDescent="0.2">
@@ -11714,7 +11891,7 @@
         <v>12</v>
       </c>
       <c r="F467" s="32" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
     </row>
     <row r="468" spans="3:6" x14ac:dyDescent="0.2">
@@ -11722,7 +11899,7 @@
         <v>12</v>
       </c>
       <c r="F468" s="32" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="469" spans="3:6" x14ac:dyDescent="0.2">
@@ -11730,48 +11907,23 @@
         <v>12</v>
       </c>
       <c r="F469" s="32" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="470" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C470" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F470" s="32" t="s">
-        <v>412</v>
-      </c>
+      <c r="C470" s="10"/>
     </row>
     <row r="471" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C471" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F471" s="32" t="s">
-        <v>413</v>
-      </c>
+      <c r="C471" s="10"/>
     </row>
     <row r="472" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C472" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F472" s="32" t="s">
-        <v>414</v>
-      </c>
+      <c r="C472" s="10"/>
     </row>
     <row r="473" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C473" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F473" s="32" t="s">
-        <v>415</v>
-      </c>
+      <c r="C473" s="10"/>
     </row>
     <row r="474" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C474" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F474" s="32" t="s">
-        <v>416</v>
-      </c>
+      <c r="C474" s="10"/>
     </row>
     <row r="475" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C475" s="10"/>
@@ -11785,11 +11937,8 @@
     <row r="478" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C478" s="10"/>
     </row>
-    <row r="479" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C479" s="10"/>
-    </row>
     <row r="480" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C480" s="10"/>
+      <c r="C480" s="25"/>
     </row>
     <row r="481" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C481" s="10"/>
@@ -11800,8 +11949,11 @@
     <row r="483" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C483" s="10"/>
     </row>
+    <row r="484" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C484" s="10"/>
+    </row>
     <row r="485" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C485" s="25"/>
+      <c r="C485" s="10"/>
     </row>
     <row r="486" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C486" s="10"/>
@@ -11874,21 +12026,6 @@
     </row>
     <row r="509" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C509" s="10"/>
-    </row>
-    <row r="510" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C510" s="10"/>
-    </row>
-    <row r="511" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C511" s="10"/>
-    </row>
-    <row r="512" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C512" s="10"/>
-    </row>
-    <row r="513" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C513" s="10"/>
-    </row>
-    <row r="514" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C514" s="10"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:L1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Photosynthesis PAR experiment + END LOW ALK 7/6 Start AMB
</commit_message>
<xml_diff>
--- a/Data/Spring_2023/BenthFun_Alkalinity.xlsx
+++ b/Data/Spring_2023/BenthFun_Alkalinity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremy/Library/Mobile Documents/com~apple~CloudDocs/Documents/Documents/Post-Doc/Projets/Villefranche/Projets/BenthFun – Jeremy/BenthFun/Data/Spring_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69DB0230-1A0C-804F-9C7B-7CFF8E3F0748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322BCAB3-3013-0E48-8B76-5684751376AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1366" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1440" uniqueCount="411">
   <si>
     <t>Operator</t>
   </si>
@@ -1030,9 +1030,6 @@
     <t>PI_t6_LOW_Tile_2b</t>
   </si>
   <si>
-    <t>PI_t6_LOW_Tile_2c</t>
-  </si>
-  <si>
     <t>PI_t6_LOW_Tile_3a</t>
   </si>
   <si>
@@ -1048,9 +1045,6 @@
     <t>PI_t7_LOW_Tile_1b</t>
   </si>
   <si>
-    <t>PI_t7_LOW_Tile_1c</t>
-  </si>
-  <si>
     <t>PI_t7_LOW_Tile_2a</t>
   </si>
   <si>
@@ -1081,18 +1075,12 @@
     <t>PI_t1_AMB_Tile_2b</t>
   </si>
   <si>
-    <t>PI_t1_AMB_Tile_2c</t>
-  </si>
-  <si>
     <t>PI_t1_AMB_Tile_3a</t>
   </si>
   <si>
     <t>PI_t1_AMB_Tile_3b</t>
   </si>
   <si>
-    <t>PI_t1_AMB_Tile_3c</t>
-  </si>
-  <si>
     <t>PI_t1_AMB_blank_a</t>
   </si>
   <si>
@@ -1115,9 +1103,6 @@
   </si>
   <si>
     <t>PI_t2_AMB_Tile_2b</t>
-  </si>
-  <si>
-    <t>PI_t2_AMB_Tile_2c</t>
   </si>
   <si>
     <t>PI_t2_AMB_Tile_3a</t>
@@ -1766,11 +1751,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L509"/>
+  <dimension ref="A1:L500"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="73" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A359" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D388" sqref="D388"/>
+      <pane ySplit="1" topLeftCell="A425" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D420" sqref="D420"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8696,7 +8681,7 @@
         <v>2889.65</v>
       </c>
       <c r="F277" s="32" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
     </row>
     <row r="278" spans="1:12" x14ac:dyDescent="0.2">
@@ -9088,11 +9073,50 @@
         <v>2678.51</v>
       </c>
       <c r="F293" s="32" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
     </row>
     <row r="294" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="F294" s="32"/>
+      <c r="A294" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B294" s="31">
+        <v>45082</v>
+      </c>
+      <c r="C294" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D294" s="5">
+        <v>50.09</v>
+      </c>
+      <c r="E294" s="14">
+        <v>2229.2600000000002</v>
+      </c>
+      <c r="F294" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G294" s="13">
+        <f>AVERAGE(E295,E296)</f>
+        <v>2221.9949999999999</v>
+      </c>
+      <c r="H294" s="18">
+        <f>STDEV(E295,E296)</f>
+        <v>1.0111626970966472</v>
+      </c>
+      <c r="I294" s="3">
+        <v>2226.44</v>
+      </c>
+      <c r="J294" s="4">
+        <f>I294-G294</f>
+        <v>4.4450000000001637</v>
+      </c>
+      <c r="K294" s="5">
+        <f>G294+J294</f>
+        <v>2226.44</v>
+      </c>
+      <c r="L294" s="2" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="295" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A295" s="9" t="s">
@@ -9101,39 +9125,17 @@
       <c r="B295" s="31">
         <v>45082</v>
       </c>
-      <c r="C295" s="25" t="s">
+      <c r="C295" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D295" s="5">
-        <v>50.09</v>
-      </c>
-      <c r="E295" s="14">
-        <v>2229.2600000000002</v>
+        <v>50.52</v>
+      </c>
+      <c r="E295" s="5">
+        <v>2221.2800000000002</v>
       </c>
       <c r="F295" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="G295" s="13">
-        <f>AVERAGE(E296,E297)</f>
-        <v>2221.9949999999999</v>
-      </c>
-      <c r="H295" s="18">
-        <f>STDEV(E296,E297)</f>
-        <v>1.0111626970966472</v>
-      </c>
-      <c r="I295" s="3">
-        <v>2226.44</v>
-      </c>
-      <c r="J295" s="4">
-        <f>I295-G295</f>
-        <v>4.4450000000001637</v>
-      </c>
-      <c r="K295" s="5">
-        <f>G295+J295</f>
-        <v>2226.44</v>
-      </c>
-      <c r="L295" s="2" t="s">
-        <v>94</v>
+        <v>9</v>
       </c>
     </row>
     <row r="296" spans="1:12" x14ac:dyDescent="0.2">
@@ -9147,13 +9149,13 @@
         <v>12</v>
       </c>
       <c r="D296" s="5">
-        <v>50.52</v>
+        <v>50.23</v>
       </c>
       <c r="E296" s="5">
-        <v>2221.2800000000002</v>
-      </c>
-      <c r="F296" s="16" t="s">
-        <v>9</v>
+        <v>2222.71</v>
+      </c>
+      <c r="F296" s="17" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="297" spans="1:12" x14ac:dyDescent="0.2">
@@ -9167,13 +9169,25 @@
         <v>12</v>
       </c>
       <c r="D297" s="5">
-        <v>50.23</v>
+        <v>50.19</v>
       </c>
       <c r="E297" s="5">
-        <v>2222.71</v>
-      </c>
-      <c r="F297" s="17" t="s">
-        <v>96</v>
+        <v>2675.99</v>
+      </c>
+      <c r="F297" s="32" t="s">
+        <v>253</v>
+      </c>
+      <c r="G297" s="13">
+        <f>AVERAGE(E297,E299)</f>
+        <v>2678.7150000000001</v>
+      </c>
+      <c r="H297" s="18">
+        <f>STDEV(E297,E299)</f>
+        <v>3.8537319574668771</v>
+      </c>
+      <c r="K297" s="5">
+        <f>G297+$J$294</f>
+        <v>2683.1600000000003</v>
       </c>
     </row>
     <row r="298" spans="1:12" x14ac:dyDescent="0.2">
@@ -9187,25 +9201,13 @@
         <v>12</v>
       </c>
       <c r="D298" s="5">
-        <v>50.19</v>
-      </c>
-      <c r="E298" s="5">
-        <v>2675.99</v>
+        <v>49.27</v>
+      </c>
+      <c r="E298" s="14">
+        <v>2689.84</v>
       </c>
       <c r="F298" s="32" t="s">
-        <v>253</v>
-      </c>
-      <c r="G298" s="13">
-        <f>AVERAGE(E298,E300)</f>
-        <v>2678.7150000000001</v>
-      </c>
-      <c r="H298" s="18">
-        <f>STDEV(E298,E300)</f>
-        <v>3.8537319574668771</v>
-      </c>
-      <c r="K298" s="5">
-        <f>G298+$J$295</f>
-        <v>2683.1600000000003</v>
+        <v>254</v>
       </c>
     </row>
     <row r="299" spans="1:12" x14ac:dyDescent="0.2">
@@ -9219,13 +9221,13 @@
         <v>12</v>
       </c>
       <c r="D299" s="5">
-        <v>49.27</v>
-      </c>
-      <c r="E299" s="14">
-        <v>2689.84</v>
+        <v>50.54</v>
+      </c>
+      <c r="E299" s="5">
+        <v>2681.44</v>
       </c>
       <c r="F299" s="32" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
     </row>
     <row r="300" spans="1:12" x14ac:dyDescent="0.2">
@@ -9239,13 +9241,25 @@
         <v>12</v>
       </c>
       <c r="D300" s="5">
-        <v>50.54</v>
+        <v>50.97</v>
       </c>
       <c r="E300" s="5">
-        <v>2681.44</v>
+        <v>2763.97</v>
       </c>
       <c r="F300" s="32" t="s">
-        <v>263</v>
+        <v>255</v>
+      </c>
+      <c r="G300" s="13">
+        <f>AVERAGE(E300,E302)</f>
+        <v>2763.52</v>
+      </c>
+      <c r="H300" s="18">
+        <f>STDEV(E300,E302)</f>
+        <v>0.6363961030676355</v>
+      </c>
+      <c r="K300" s="5">
+        <f>G300+$J$294</f>
+        <v>2767.9650000000001</v>
       </c>
     </row>
     <row r="301" spans="1:12" x14ac:dyDescent="0.2">
@@ -9259,25 +9273,13 @@
         <v>12</v>
       </c>
       <c r="D301" s="5">
-        <v>50.97</v>
-      </c>
-      <c r="E301" s="5">
-        <v>2763.97</v>
+        <v>51.25</v>
+      </c>
+      <c r="E301" s="14">
+        <v>2775.93</v>
       </c>
       <c r="F301" s="32" t="s">
-        <v>255</v>
-      </c>
-      <c r="G301" s="13">
-        <f>AVERAGE(E301,E303)</f>
-        <v>2763.52</v>
-      </c>
-      <c r="H301" s="18">
-        <f>STDEV(E301,E303)</f>
-        <v>0.6363961030676355</v>
-      </c>
-      <c r="K301" s="5">
-        <f>G301+$J$295</f>
-        <v>2767.9650000000001</v>
+        <v>256</v>
       </c>
     </row>
     <row r="302" spans="1:12" x14ac:dyDescent="0.2">
@@ -9291,13 +9293,13 @@
         <v>12</v>
       </c>
       <c r="D302" s="5">
-        <v>51.25</v>
-      </c>
-      <c r="E302" s="14">
-        <v>2775.93</v>
+        <v>50.53</v>
+      </c>
+      <c r="E302" s="5">
+        <v>2763.07</v>
       </c>
       <c r="F302" s="32" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="303" spans="1:12" x14ac:dyDescent="0.2">
@@ -9311,13 +9313,25 @@
         <v>12</v>
       </c>
       <c r="D303" s="5">
-        <v>50.53</v>
-      </c>
-      <c r="E303" s="5">
-        <v>2763.07</v>
+        <v>50.84</v>
+      </c>
+      <c r="E303" s="14">
+        <v>2677.87</v>
       </c>
       <c r="F303" s="32" t="s">
-        <v>257</v>
+        <v>258</v>
+      </c>
+      <c r="G303" s="13">
+        <f>AVERAGE(E304:E305)</f>
+        <v>2660.46</v>
+      </c>
+      <c r="H303" s="18">
+        <f>STDEV(E304:E305)</f>
+        <v>0.4525483399596219</v>
+      </c>
+      <c r="K303" s="5">
+        <f>G303+$J$294</f>
+        <v>2664.9050000000002</v>
       </c>
     </row>
     <row r="304" spans="1:12" x14ac:dyDescent="0.2">
@@ -9331,25 +9345,13 @@
         <v>12</v>
       </c>
       <c r="D304" s="5">
-        <v>50.84</v>
-      </c>
-      <c r="E304" s="14">
-        <v>2677.87</v>
+        <v>51.25</v>
+      </c>
+      <c r="E304" s="5">
+        <v>2660.78</v>
       </c>
       <c r="F304" s="32" t="s">
-        <v>258</v>
-      </c>
-      <c r="G304" s="13">
-        <f>AVERAGE(E305:E306)</f>
-        <v>2660.46</v>
-      </c>
-      <c r="H304" s="18">
-        <f>STDEV(E305:E306)</f>
-        <v>0.4525483399596219</v>
-      </c>
-      <c r="K304" s="5">
-        <f>G304+$J$295</f>
-        <v>2664.9050000000002</v>
+        <v>259</v>
       </c>
     </row>
     <row r="305" spans="1:11" x14ac:dyDescent="0.2">
@@ -9363,13 +9365,13 @@
         <v>12</v>
       </c>
       <c r="D305" s="5">
-        <v>51.25</v>
+        <v>50.59</v>
       </c>
       <c r="E305" s="5">
-        <v>2660.78</v>
+        <v>2660.14</v>
       </c>
       <c r="F305" s="32" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="306" spans="1:11" x14ac:dyDescent="0.2">
@@ -9383,13 +9385,25 @@
         <v>12</v>
       </c>
       <c r="D306" s="5">
-        <v>50.59</v>
-      </c>
-      <c r="E306" s="5">
-        <v>2660.14</v>
+        <v>48.28</v>
+      </c>
+      <c r="E306" s="14">
+        <v>2519.1799999999998</v>
       </c>
       <c r="F306" s="32" t="s">
-        <v>260</v>
+        <v>264</v>
+      </c>
+      <c r="G306" s="13">
+        <f>AVERAGE(E307:E308)</f>
+        <v>2502.665</v>
+      </c>
+      <c r="H306" s="18">
+        <f>STDEV(E307:E308)</f>
+        <v>0.27577164466298504</v>
+      </c>
+      <c r="K306" s="5">
+        <f>G306+$J$294</f>
+        <v>2507.11</v>
       </c>
     </row>
     <row r="307" spans="1:11" x14ac:dyDescent="0.2">
@@ -9403,25 +9417,13 @@
         <v>12</v>
       </c>
       <c r="D307" s="5">
-        <v>48.28</v>
-      </c>
-      <c r="E307" s="14">
-        <v>2519.1799999999998</v>
+        <v>50.97</v>
+      </c>
+      <c r="E307" s="5">
+        <v>2502.86</v>
       </c>
       <c r="F307" s="32" t="s">
-        <v>264</v>
-      </c>
-      <c r="G307" s="13">
-        <f>AVERAGE(E308:E309)</f>
-        <v>2502.665</v>
-      </c>
-      <c r="H307" s="18">
-        <f>STDEV(E308:E309)</f>
-        <v>0.27577164466298504</v>
-      </c>
-      <c r="K307" s="5">
-        <f>G307+$J$295</f>
-        <v>2507.11</v>
+        <v>265</v>
       </c>
     </row>
     <row r="308" spans="1:11" x14ac:dyDescent="0.2">
@@ -9435,13 +9437,13 @@
         <v>12</v>
       </c>
       <c r="D308" s="5">
-        <v>50.97</v>
+        <v>50.3</v>
       </c>
       <c r="E308" s="5">
-        <v>2502.86</v>
+        <v>2502.4699999999998</v>
       </c>
       <c r="F308" s="32" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="309" spans="1:11" x14ac:dyDescent="0.2">
@@ -9455,13 +9457,25 @@
         <v>12</v>
       </c>
       <c r="D309" s="5">
-        <v>50.3</v>
-      </c>
-      <c r="E309" s="5">
-        <v>2502.4699999999998</v>
+        <v>50.71</v>
+      </c>
+      <c r="E309" s="14">
+        <v>2568.89</v>
       </c>
       <c r="F309" s="32" t="s">
-        <v>266</v>
+        <v>267</v>
+      </c>
+      <c r="G309" s="13">
+        <f>AVERAGE(E310:E311)</f>
+        <v>2556.1350000000002</v>
+      </c>
+      <c r="H309" s="18">
+        <f>STDEV(E310:E311)</f>
+        <v>0.91216774773094211</v>
+      </c>
+      <c r="K309" s="5">
+        <f>G309+$J$294</f>
+        <v>2560.5800000000004</v>
       </c>
     </row>
     <row r="310" spans="1:11" x14ac:dyDescent="0.2">
@@ -9475,25 +9489,13 @@
         <v>12</v>
       </c>
       <c r="D310" s="5">
-        <v>50.71</v>
-      </c>
-      <c r="E310" s="14">
-        <v>2568.89</v>
+        <v>51.81</v>
+      </c>
+      <c r="E310" s="5">
+        <v>2555.4899999999998</v>
       </c>
       <c r="F310" s="32" t="s">
-        <v>267</v>
-      </c>
-      <c r="G310" s="13">
-        <f>AVERAGE(E311:E312)</f>
-        <v>2556.1350000000002</v>
-      </c>
-      <c r="H310" s="18">
-        <f>STDEV(E311:E312)</f>
-        <v>0.91216774773094211</v>
-      </c>
-      <c r="K310" s="5">
-        <f>G310+$J$295</f>
-        <v>2560.5800000000004</v>
+        <v>268</v>
       </c>
     </row>
     <row r="311" spans="1:11" x14ac:dyDescent="0.2">
@@ -9507,13 +9509,13 @@
         <v>12</v>
       </c>
       <c r="D311" s="5">
-        <v>51.81</v>
+        <v>50</v>
       </c>
       <c r="E311" s="5">
-        <v>2555.4899999999998</v>
+        <v>2556.7800000000002</v>
       </c>
       <c r="F311" s="32" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="312" spans="1:11" x14ac:dyDescent="0.2">
@@ -9527,13 +9529,25 @@
         <v>12</v>
       </c>
       <c r="D312" s="5">
-        <v>50</v>
-      </c>
-      <c r="E312" s="5">
-        <v>2556.7800000000002</v>
+        <v>48.63</v>
+      </c>
+      <c r="E312" s="14">
+        <v>2560.79</v>
       </c>
       <c r="F312" s="32" t="s">
-        <v>269</v>
+        <v>270</v>
+      </c>
+      <c r="G312" s="13">
+        <f>AVERAGE(E313,E314)</f>
+        <v>2547.31</v>
+      </c>
+      <c r="H312" s="13">
+        <f>STDEV(E313,E314)</f>
+        <v>1.8809040379561135</v>
+      </c>
+      <c r="K312" s="5">
+        <f>G312+$J$294</f>
+        <v>2551.7550000000001</v>
       </c>
     </row>
     <row r="313" spans="1:11" x14ac:dyDescent="0.2">
@@ -9547,25 +9561,13 @@
         <v>12</v>
       </c>
       <c r="D313" s="5">
-        <v>48.63</v>
-      </c>
-      <c r="E313" s="14">
-        <v>2560.79</v>
+        <v>51.07</v>
+      </c>
+      <c r="E313" s="5">
+        <v>2545.98</v>
       </c>
       <c r="F313" s="32" t="s">
-        <v>270</v>
-      </c>
-      <c r="G313" s="13">
-        <f>AVERAGE(E314,E315)</f>
-        <v>2547.31</v>
-      </c>
-      <c r="H313" s="13">
-        <f>STDEV(E314,E315)</f>
-        <v>1.8809040379561135</v>
-      </c>
-      <c r="K313" s="5">
-        <f>G313+$J$295</f>
-        <v>2551.7550000000001</v>
+        <v>271</v>
       </c>
     </row>
     <row r="314" spans="1:11" x14ac:dyDescent="0.2">
@@ -9579,13 +9581,13 @@
         <v>12</v>
       </c>
       <c r="D314" s="5">
-        <v>51.07</v>
+        <v>50.71</v>
       </c>
       <c r="E314" s="5">
-        <v>2545.98</v>
+        <v>2548.64</v>
       </c>
       <c r="F314" s="32" t="s">
-        <v>271</v>
+        <v>406</v>
       </c>
     </row>
     <row r="315" spans="1:11" x14ac:dyDescent="0.2">
@@ -9599,13 +9601,25 @@
         <v>12</v>
       </c>
       <c r="D315" s="5">
-        <v>50.71</v>
-      </c>
-      <c r="E315" s="5">
-        <v>2548.64</v>
+        <v>51.27</v>
+      </c>
+      <c r="E315" s="14">
+        <v>2585.0100000000002</v>
       </c>
       <c r="F315" s="32" t="s">
-        <v>411</v>
+        <v>272</v>
+      </c>
+      <c r="G315" s="13">
+        <f>AVERAGE(E316:E317)</f>
+        <v>2604.0349999999999</v>
+      </c>
+      <c r="H315" s="18">
+        <f>STDEV(E316:E317)</f>
+        <v>6.3639610306892178E-2</v>
+      </c>
+      <c r="K315" s="5">
+        <f>G315+$J$294</f>
+        <v>2608.48</v>
       </c>
     </row>
     <row r="316" spans="1:11" x14ac:dyDescent="0.2">
@@ -9619,25 +9633,13 @@
         <v>12</v>
       </c>
       <c r="D316" s="5">
-        <v>51.27</v>
-      </c>
-      <c r="E316" s="14">
-        <v>2585.0100000000002</v>
+        <v>49.07</v>
+      </c>
+      <c r="E316" s="5">
+        <v>2603.9899999999998</v>
       </c>
       <c r="F316" s="32" t="s">
-        <v>272</v>
-      </c>
-      <c r="G316" s="13">
-        <f>AVERAGE(E317:E318)</f>
-        <v>2604.0349999999999</v>
-      </c>
-      <c r="H316" s="18">
-        <f>STDEV(E317:E318)</f>
-        <v>6.3639610306892178E-2</v>
-      </c>
-      <c r="K316" s="5">
-        <f>G316+$J$295</f>
-        <v>2608.48</v>
+        <v>273</v>
       </c>
     </row>
     <row r="317" spans="1:11" x14ac:dyDescent="0.2">
@@ -9651,13 +9653,13 @@
         <v>12</v>
       </c>
       <c r="D317" s="5">
-        <v>49.07</v>
+        <v>48.74</v>
       </c>
       <c r="E317" s="5">
-        <v>2603.9899999999998</v>
+        <v>2604.08</v>
       </c>
       <c r="F317" s="32" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="318" spans="1:11" x14ac:dyDescent="0.2">
@@ -9671,13 +9673,25 @@
         <v>12</v>
       </c>
       <c r="D318" s="5">
-        <v>48.74</v>
-      </c>
-      <c r="E318" s="5">
-        <v>2604.08</v>
+        <v>50.99</v>
+      </c>
+      <c r="E318" s="14">
+        <v>2658.15</v>
       </c>
       <c r="F318" s="32" t="s">
-        <v>274</v>
+        <v>275</v>
+      </c>
+      <c r="G318" s="13">
+        <f>AVERAGE(E319:E320)</f>
+        <v>2646.86</v>
+      </c>
+      <c r="H318" s="18">
+        <f>STDEV(E319:E320)</f>
+        <v>2.3617366491631717</v>
+      </c>
+      <c r="K318" s="5">
+        <f>G318+$J$294</f>
+        <v>2651.3050000000003</v>
       </c>
     </row>
     <row r="319" spans="1:11" x14ac:dyDescent="0.2">
@@ -9691,25 +9705,13 @@
         <v>12</v>
       </c>
       <c r="D319" s="5">
-        <v>50.99</v>
-      </c>
-      <c r="E319" s="14">
-        <v>2658.15</v>
+        <v>50.89</v>
+      </c>
+      <c r="E319" s="5">
+        <v>2645.19</v>
       </c>
       <c r="F319" s="32" t="s">
-        <v>275</v>
-      </c>
-      <c r="G319" s="13">
-        <f>AVERAGE(E320:E321)</f>
-        <v>2646.86</v>
-      </c>
-      <c r="H319" s="18">
-        <f>STDEV(E320:E321)</f>
-        <v>2.3617366491631717</v>
-      </c>
-      <c r="K319" s="5">
-        <f>G319+$J$295</f>
-        <v>2651.3050000000003</v>
+        <v>276</v>
       </c>
     </row>
     <row r="320" spans="1:11" x14ac:dyDescent="0.2">
@@ -9723,13 +9725,13 @@
         <v>12</v>
       </c>
       <c r="D320" s="5">
-        <v>50.89</v>
+        <v>49.61</v>
       </c>
       <c r="E320" s="5">
-        <v>2645.19</v>
+        <v>2648.53</v>
       </c>
       <c r="F320" s="32" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="321" spans="1:12" x14ac:dyDescent="0.2">
@@ -9743,13 +9745,25 @@
         <v>12</v>
       </c>
       <c r="D321" s="5">
-        <v>49.61</v>
+        <v>48.94</v>
       </c>
       <c r="E321" s="5">
-        <v>2648.53</v>
+        <v>2614.2199999999998</v>
       </c>
       <c r="F321" s="32" t="s">
-        <v>277</v>
+        <v>278</v>
+      </c>
+      <c r="G321" s="13">
+        <f>AVERAGE(E321:E322)</f>
+        <v>2612.37</v>
+      </c>
+      <c r="H321" s="18">
+        <f>STDEV(E321:E322)</f>
+        <v>2.6162950903900972</v>
+      </c>
+      <c r="K321" s="5">
+        <f>G321+$J$294</f>
+        <v>2616.8150000000001</v>
       </c>
     </row>
     <row r="322" spans="1:12" x14ac:dyDescent="0.2">
@@ -9763,25 +9777,13 @@
         <v>12</v>
       </c>
       <c r="D322" s="5">
-        <v>48.94</v>
+        <v>50.77</v>
       </c>
       <c r="E322" s="5">
-        <v>2614.2199999999998</v>
+        <v>2610.52</v>
       </c>
       <c r="F322" s="32" t="s">
-        <v>278</v>
-      </c>
-      <c r="G322" s="13">
-        <f>AVERAGE(E322:E323)</f>
-        <v>2612.37</v>
-      </c>
-      <c r="H322" s="18">
-        <f>STDEV(E322:E323)</f>
-        <v>2.6162950903900972</v>
-      </c>
-      <c r="K322" s="5">
-        <f>G322+$J$295</f>
-        <v>2616.8150000000001</v>
+        <v>279</v>
       </c>
     </row>
     <row r="323" spans="1:12" x14ac:dyDescent="0.2">
@@ -9795,13 +9797,25 @@
         <v>12</v>
       </c>
       <c r="D323" s="5">
-        <v>50.77</v>
+        <v>52.43</v>
       </c>
       <c r="E323" s="5">
-        <v>2610.52</v>
+        <v>2530.13</v>
       </c>
       <c r="F323" s="32" t="s">
-        <v>279</v>
+        <v>280</v>
+      </c>
+      <c r="G323" s="13">
+        <f>AVERAGE(E323:E324)</f>
+        <v>2528.3500000000004</v>
+      </c>
+      <c r="H323" s="18">
+        <f>STDEV(E323:E324)</f>
+        <v>2.5173001410240707</v>
+      </c>
+      <c r="K323" s="5">
+        <f>G323+$J$294</f>
+        <v>2532.7950000000005</v>
       </c>
     </row>
     <row r="324" spans="1:12" x14ac:dyDescent="0.2">
@@ -9815,25 +9829,13 @@
         <v>12</v>
       </c>
       <c r="D324" s="5">
-        <v>52.43</v>
+        <v>49.17</v>
       </c>
       <c r="E324" s="5">
-        <v>2530.13</v>
+        <v>2526.5700000000002</v>
       </c>
       <c r="F324" s="32" t="s">
-        <v>280</v>
-      </c>
-      <c r="G324" s="13">
-        <f>AVERAGE(E324:E325)</f>
-        <v>2528.3500000000004</v>
-      </c>
-      <c r="H324" s="18">
-        <f>STDEV(E324:E325)</f>
-        <v>2.5173001410240707</v>
-      </c>
-      <c r="K324" s="5">
-        <f>G324+$J$295</f>
-        <v>2532.7950000000005</v>
+        <v>281</v>
       </c>
     </row>
     <row r="325" spans="1:12" x14ac:dyDescent="0.2">
@@ -9847,13 +9849,25 @@
         <v>12</v>
       </c>
       <c r="D325" s="5">
-        <v>49.17</v>
+        <v>50.31</v>
       </c>
       <c r="E325" s="5">
-        <v>2526.5700000000002</v>
+        <v>2623.15</v>
       </c>
       <c r="F325" s="32" t="s">
-        <v>281</v>
+        <v>282</v>
+      </c>
+      <c r="G325" s="13">
+        <f>AVERAGE(E325:E326)</f>
+        <v>2622.16</v>
+      </c>
+      <c r="H325" s="18">
+        <f>STDEV(E325:E326)</f>
+        <v>1.400071426749377</v>
+      </c>
+      <c r="K325" s="5">
+        <f>G325+$J$294</f>
+        <v>2626.605</v>
       </c>
     </row>
     <row r="326" spans="1:12" x14ac:dyDescent="0.2">
@@ -9867,25 +9881,13 @@
         <v>12</v>
       </c>
       <c r="D326" s="5">
-        <v>50.31</v>
+        <v>51.67</v>
       </c>
       <c r="E326" s="5">
-        <v>2623.15</v>
+        <v>2621.17</v>
       </c>
       <c r="F326" s="32" t="s">
-        <v>282</v>
-      </c>
-      <c r="G326" s="13">
-        <f>AVERAGE(E326:E327)</f>
-        <v>2622.16</v>
-      </c>
-      <c r="H326" s="18">
-        <f>STDEV(E326:E327)</f>
-        <v>1.400071426749377</v>
-      </c>
-      <c r="K326" s="5">
-        <f>G326+$J$295</f>
-        <v>2626.605</v>
+        <v>283</v>
       </c>
     </row>
     <row r="327" spans="1:12" x14ac:dyDescent="0.2">
@@ -9899,13 +9901,25 @@
         <v>12</v>
       </c>
       <c r="D327" s="5">
-        <v>51.67</v>
-      </c>
-      <c r="E327" s="5">
-        <v>2621.17</v>
+        <v>50.42</v>
+      </c>
+      <c r="E327" s="14">
+        <v>2585.75</v>
       </c>
       <c r="F327" s="32" t="s">
-        <v>283</v>
+        <v>284</v>
+      </c>
+      <c r="G327" s="13">
+        <f>AVERAGE(E328:E329)</f>
+        <v>2575.38</v>
+      </c>
+      <c r="H327" s="18">
+        <f>STDEV(E328:E329)</f>
+        <v>4.2426406871192848</v>
+      </c>
+      <c r="K327" s="5">
+        <f>G327+$J$294</f>
+        <v>2579.8250000000003</v>
       </c>
     </row>
     <row r="328" spans="1:12" x14ac:dyDescent="0.2">
@@ -9919,25 +9933,13 @@
         <v>12</v>
       </c>
       <c r="D328" s="5">
-        <v>50.42</v>
-      </c>
-      <c r="E328" s="14">
-        <v>2585.75</v>
+        <v>50.63</v>
+      </c>
+      <c r="E328" s="5">
+        <v>2572.38</v>
       </c>
       <c r="F328" s="32" t="s">
-        <v>284</v>
-      </c>
-      <c r="G328" s="13">
-        <f>AVERAGE(E329:E330)</f>
-        <v>2575.38</v>
-      </c>
-      <c r="H328" s="18">
-        <f>STDEV(E329:E330)</f>
-        <v>4.2426406871192848</v>
-      </c>
-      <c r="K328" s="5">
-        <f>G328+$J$295</f>
-        <v>2579.8250000000003</v>
+        <v>285</v>
       </c>
     </row>
     <row r="329" spans="1:12" x14ac:dyDescent="0.2">
@@ -9951,37 +9953,59 @@
         <v>12</v>
       </c>
       <c r="D329" s="5">
-        <v>50.63</v>
+        <v>49.19</v>
       </c>
       <c r="E329" s="5">
-        <v>2572.38</v>
+        <v>2578.38</v>
       </c>
       <c r="F329" s="32" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="330" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A330" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B330" s="31">
-        <v>45082</v>
-      </c>
-      <c r="C330" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D330" s="5">
-        <v>49.19</v>
-      </c>
-      <c r="E330" s="5">
-        <v>2578.38</v>
-      </c>
-      <c r="F330" s="32" t="s">
-        <v>286</v>
-      </c>
+      <c r="C330" s="10"/>
     </row>
     <row r="331" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C331" s="10"/>
+      <c r="A331" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B331" s="31">
+        <v>45083</v>
+      </c>
+      <c r="C331" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D331" s="5">
+        <v>50.52</v>
+      </c>
+      <c r="E331" s="14">
+        <v>2219.19</v>
+      </c>
+      <c r="F331" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G331" s="13">
+        <f>AVERAGE(E332:E333)</f>
+        <v>2238.3050000000003</v>
+      </c>
+      <c r="H331" s="18">
+        <f>STDEV(E332:E333)</f>
+        <v>2.8637824638053244</v>
+      </c>
+      <c r="I331" s="3">
+        <v>2226.44</v>
+      </c>
+      <c r="J331" s="4">
+        <f>I331-G331</f>
+        <v>-11.865000000000236</v>
+      </c>
+      <c r="K331" s="5">
+        <f>G331+J331</f>
+        <v>2226.44</v>
+      </c>
+      <c r="L331" s="2" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="332" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A332" s="9" t="s">
@@ -9990,39 +10014,17 @@
       <c r="B332" s="31">
         <v>45083</v>
       </c>
-      <c r="C332" s="25" t="s">
+      <c r="C332" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D332" s="5">
-        <v>50.52</v>
-      </c>
-      <c r="E332" s="14">
-        <v>2219.19</v>
+        <v>48.27</v>
+      </c>
+      <c r="E332" s="5">
+        <v>2236.2800000000002</v>
       </c>
       <c r="F332" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="G332" s="13">
-        <f>AVERAGE(E333:E334)</f>
-        <v>2238.3050000000003</v>
-      </c>
-      <c r="H332" s="18">
-        <f>STDEV(E333:E334)</f>
-        <v>2.8637824638053244</v>
-      </c>
-      <c r="I332" s="3">
-        <v>2226.44</v>
-      </c>
-      <c r="J332" s="4">
-        <f>I332-G332</f>
-        <v>-11.865000000000236</v>
-      </c>
-      <c r="K332" s="5">
-        <f>G332+J332</f>
-        <v>2226.44</v>
-      </c>
-      <c r="L332" s="2" t="s">
-        <v>94</v>
+        <v>9</v>
       </c>
     </row>
     <row r="333" spans="1:12" x14ac:dyDescent="0.2">
@@ -10036,13 +10038,13 @@
         <v>12</v>
       </c>
       <c r="D333" s="5">
-        <v>48.27</v>
+        <v>50.04</v>
       </c>
       <c r="E333" s="5">
-        <v>2236.2800000000002</v>
-      </c>
-      <c r="F333" s="16" t="s">
-        <v>9</v>
+        <v>2240.33</v>
+      </c>
+      <c r="F333" s="17" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="334" spans="1:12" x14ac:dyDescent="0.2">
@@ -10050,19 +10052,31 @@
         <v>11</v>
       </c>
       <c r="B334" s="31">
-        <v>45083</v>
+        <v>45082</v>
       </c>
       <c r="C334" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D334" s="5">
-        <v>50.04</v>
+        <v>48.96</v>
       </c>
       <c r="E334" s="5">
-        <v>2240.33</v>
-      </c>
-      <c r="F334" s="17" t="s">
-        <v>96</v>
+        <v>2601.0100000000002</v>
+      </c>
+      <c r="F334" s="32" t="s">
+        <v>287</v>
+      </c>
+      <c r="G334" s="13">
+        <f>AVERAGE(E334:E335)</f>
+        <v>2601.6750000000002</v>
+      </c>
+      <c r="H334" s="18">
+        <f>STDEV(E334:E335)</f>
+        <v>0.94045201897805675</v>
+      </c>
+      <c r="K334" s="5">
+        <f>G334+$J$294</f>
+        <v>2606.1200000000003</v>
       </c>
     </row>
     <row r="335" spans="1:12" x14ac:dyDescent="0.2">
@@ -10076,25 +10090,13 @@
         <v>12</v>
       </c>
       <c r="D335" s="5">
-        <v>48.96</v>
+        <v>52.01</v>
       </c>
       <c r="E335" s="5">
-        <v>2601.0100000000002</v>
+        <v>2602.34</v>
       </c>
       <c r="F335" s="32" t="s">
-        <v>287</v>
-      </c>
-      <c r="G335" s="13">
-        <f>AVERAGE(E335:E336)</f>
-        <v>2601.6750000000002</v>
-      </c>
-      <c r="H335" s="18">
-        <f>STDEV(E335:E336)</f>
-        <v>0.94045201897805675</v>
-      </c>
-      <c r="K335" s="5">
-        <f>G335+$J$295</f>
-        <v>2606.1200000000003</v>
+        <v>288</v>
       </c>
     </row>
     <row r="336" spans="1:12" x14ac:dyDescent="0.2">
@@ -10108,13 +10110,25 @@
         <v>12</v>
       </c>
       <c r="D336" s="5">
-        <v>52.01</v>
-      </c>
-      <c r="E336" s="5">
-        <v>2602.34</v>
+        <v>50.22</v>
+      </c>
+      <c r="E336" s="14">
+        <v>2534.11</v>
       </c>
       <c r="F336" s="32" t="s">
-        <v>288</v>
+        <v>289</v>
+      </c>
+      <c r="G336" s="18">
+        <f>AVERAGE(E337:E338)</f>
+        <v>2582.8850000000002</v>
+      </c>
+      <c r="H336" s="18">
+        <f>STDEV(E337:E338)</f>
+        <v>9.1923881554006784E-2</v>
+      </c>
+      <c r="K336" s="5">
+        <f>G336+$J$294</f>
+        <v>2587.3300000000004</v>
       </c>
     </row>
     <row r="337" spans="1:11" x14ac:dyDescent="0.2">
@@ -10128,25 +10142,13 @@
         <v>12</v>
       </c>
       <c r="D337" s="5">
-        <v>50.22</v>
-      </c>
-      <c r="E337" s="14">
-        <v>2534.11</v>
+        <v>49.96</v>
+      </c>
+      <c r="E337" s="5">
+        <v>2582.9499999999998</v>
       </c>
       <c r="F337" s="32" t="s">
-        <v>289</v>
-      </c>
-      <c r="G337" s="18">
-        <f>AVERAGE(E338:E339)</f>
-        <v>2582.8850000000002</v>
-      </c>
-      <c r="H337" s="18">
-        <f>STDEV(E338:E339)</f>
-        <v>9.1923881554006784E-2</v>
-      </c>
-      <c r="K337" s="5">
-        <f>G337+$J$295</f>
-        <v>2587.3300000000004</v>
+        <v>290</v>
       </c>
     </row>
     <row r="338" spans="1:11" x14ac:dyDescent="0.2">
@@ -10160,13 +10162,13 @@
         <v>12</v>
       </c>
       <c r="D338" s="5">
-        <v>49.96</v>
+        <v>49.71</v>
       </c>
       <c r="E338" s="5">
-        <v>2582.9499999999998</v>
+        <v>2582.8200000000002</v>
       </c>
       <c r="F338" s="32" t="s">
-        <v>290</v>
+        <v>407</v>
       </c>
     </row>
     <row r="339" spans="1:11" x14ac:dyDescent="0.2">
@@ -10180,13 +10182,25 @@
         <v>12</v>
       </c>
       <c r="D339" s="5">
-        <v>49.71</v>
+        <v>49.6</v>
       </c>
       <c r="E339" s="5">
-        <v>2582.8200000000002</v>
+        <v>2562.94</v>
       </c>
       <c r="F339" s="32" t="s">
-        <v>412</v>
+        <v>291</v>
+      </c>
+      <c r="G339" s="13">
+        <f>AVERAGE(E339:E340)</f>
+        <v>2555.1149999999998</v>
+      </c>
+      <c r="H339" s="18">
+        <f>STDEV(E339,E341)</f>
+        <v>2.9698484809833712</v>
+      </c>
+      <c r="K339" s="5">
+        <f>G339+$J$294</f>
+        <v>2559.56</v>
       </c>
     </row>
     <row r="340" spans="1:11" x14ac:dyDescent="0.2">
@@ -10200,25 +10214,13 @@
         <v>12</v>
       </c>
       <c r="D340" s="5">
-        <v>49.6</v>
-      </c>
-      <c r="E340" s="5">
-        <v>2562.94</v>
+        <v>52</v>
+      </c>
+      <c r="E340" s="14">
+        <v>2547.29</v>
       </c>
       <c r="F340" s="32" t="s">
-        <v>291</v>
-      </c>
-      <c r="G340" s="13">
-        <f>AVERAGE(E340:E341)</f>
-        <v>2555.1149999999998</v>
-      </c>
-      <c r="H340" s="18">
-        <f>STDEV(E340,E342)</f>
-        <v>2.9698484809833712</v>
-      </c>
-      <c r="K340" s="5">
-        <f>G340+$J$295</f>
-        <v>2559.56</v>
+        <v>292</v>
       </c>
     </row>
     <row r="341" spans="1:11" x14ac:dyDescent="0.2">
@@ -10232,13 +10234,13 @@
         <v>12</v>
       </c>
       <c r="D341" s="5">
-        <v>52</v>
-      </c>
-      <c r="E341" s="14">
-        <v>2547.29</v>
+        <v>49.79</v>
+      </c>
+      <c r="E341" s="5">
+        <v>2567.14</v>
       </c>
       <c r="F341" s="32" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="342" spans="1:11" x14ac:dyDescent="0.2">
@@ -10252,13 +10254,25 @@
         <v>12</v>
       </c>
       <c r="D342" s="5">
-        <v>49.79</v>
-      </c>
-      <c r="E342" s="5">
-        <v>2567.14</v>
+        <v>51.18</v>
+      </c>
+      <c r="E342" s="14">
+        <v>2589.9299999999998</v>
       </c>
       <c r="F342" s="32" t="s">
-        <v>293</v>
+        <v>294</v>
+      </c>
+      <c r="G342" s="13">
+        <f>AVERAGE(E343:E344)</f>
+        <v>2580.4549999999999</v>
+      </c>
+      <c r="H342" s="18">
+        <f>STDEV(E343:E344)</f>
+        <v>1.3788582233136391</v>
+      </c>
+      <c r="K342" s="5">
+        <f>G342+$J$294</f>
+        <v>2584.9</v>
       </c>
     </row>
     <row r="343" spans="1:11" x14ac:dyDescent="0.2">
@@ -10272,25 +10286,13 @@
         <v>12</v>
       </c>
       <c r="D343" s="5">
-        <v>51.18</v>
-      </c>
-      <c r="E343" s="14">
-        <v>2589.9299999999998</v>
+        <v>50.87</v>
+      </c>
+      <c r="E343" s="5">
+        <v>2581.4299999999998</v>
       </c>
       <c r="F343" s="32" t="s">
-        <v>294</v>
-      </c>
-      <c r="G343" s="13">
-        <f>AVERAGE(E344:E345)</f>
-        <v>2580.4549999999999</v>
-      </c>
-      <c r="H343" s="18">
-        <f>STDEV(E344:E345)</f>
-        <v>1.3788582233136391</v>
-      </c>
-      <c r="K343" s="5">
-        <f>G343+$J$295</f>
-        <v>2584.9</v>
+        <v>295</v>
       </c>
     </row>
     <row r="344" spans="1:11" x14ac:dyDescent="0.2">
@@ -10304,13 +10306,13 @@
         <v>12</v>
       </c>
       <c r="D344" s="5">
-        <v>50.87</v>
+        <v>49.3</v>
       </c>
       <c r="E344" s="5">
-        <v>2581.4299999999998</v>
+        <v>2579.48</v>
       </c>
       <c r="F344" s="32" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="345" spans="1:11" x14ac:dyDescent="0.2">
@@ -10318,19 +10320,31 @@
         <v>11</v>
       </c>
       <c r="B345" s="31">
-        <v>45082</v>
+        <v>45083</v>
       </c>
       <c r="C345" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D345" s="5">
-        <v>49.3</v>
+        <v>51.48</v>
       </c>
       <c r="E345" s="5">
-        <v>2579.48</v>
+        <v>2583.7800000000002</v>
       </c>
       <c r="F345" s="32" t="s">
-        <v>296</v>
+        <v>297</v>
+      </c>
+      <c r="G345" s="13">
+        <f>AVERAGE(E345:E346)</f>
+        <v>2581.6000000000004</v>
+      </c>
+      <c r="H345" s="18">
+        <f>STDEV(E345:E346)</f>
+        <v>3.0829855659734373</v>
+      </c>
+      <c r="K345" s="5">
+        <f>G345+$J$331</f>
+        <v>2569.7350000000001</v>
       </c>
     </row>
     <row r="346" spans="1:11" x14ac:dyDescent="0.2">
@@ -10344,25 +10358,13 @@
         <v>12</v>
       </c>
       <c r="D346" s="5">
-        <v>51.48</v>
+        <v>50.77</v>
       </c>
       <c r="E346" s="5">
-        <v>2583.7800000000002</v>
+        <v>2579.42</v>
       </c>
       <c r="F346" s="32" t="s">
-        <v>297</v>
-      </c>
-      <c r="G346" s="13">
-        <f>AVERAGE(E346:E347)</f>
-        <v>2581.6000000000004</v>
-      </c>
-      <c r="H346" s="18">
-        <f>STDEV(E346:E347)</f>
-        <v>3.0829855659734373</v>
-      </c>
-      <c r="K346" s="5">
-        <f>G346+$J$332</f>
-        <v>2569.7350000000001</v>
+        <v>298</v>
       </c>
     </row>
     <row r="347" spans="1:11" x14ac:dyDescent="0.2">
@@ -10376,13 +10378,25 @@
         <v>12</v>
       </c>
       <c r="D347" s="5">
-        <v>50.77</v>
+        <v>50.57</v>
       </c>
       <c r="E347" s="5">
-        <v>2579.42</v>
+        <v>2526.5100000000002</v>
       </c>
       <c r="F347" s="32" t="s">
-        <v>298</v>
+        <v>299</v>
+      </c>
+      <c r="G347" s="13">
+        <f>AVERAGE(E347:E348)</f>
+        <v>2524.2700000000004</v>
+      </c>
+      <c r="H347" s="18">
+        <f>STDEV(E347:E348)</f>
+        <v>3.1678383797157457</v>
+      </c>
+      <c r="K347" s="5">
+        <f>G347+$J$331</f>
+        <v>2512.4050000000002</v>
       </c>
     </row>
     <row r="348" spans="1:11" x14ac:dyDescent="0.2">
@@ -10396,25 +10410,13 @@
         <v>12</v>
       </c>
       <c r="D348" s="5">
-        <v>50.57</v>
+        <v>50.2</v>
       </c>
       <c r="E348" s="5">
-        <v>2526.5100000000002</v>
+        <v>2522.0300000000002</v>
       </c>
       <c r="F348" s="32" t="s">
-        <v>299</v>
-      </c>
-      <c r="G348" s="13">
-        <f>AVERAGE(E348:E349)</f>
-        <v>2524.2700000000004</v>
-      </c>
-      <c r="H348" s="18">
-        <f>STDEV(E348:E349)</f>
-        <v>3.1678383797157457</v>
-      </c>
-      <c r="K348" s="5">
-        <f>G348+$J$332</f>
-        <v>2512.4050000000002</v>
+        <v>300</v>
       </c>
     </row>
     <row r="349" spans="1:11" x14ac:dyDescent="0.2">
@@ -10428,13 +10430,25 @@
         <v>12</v>
       </c>
       <c r="D349" s="5">
-        <v>50.2</v>
+        <v>51.23</v>
       </c>
       <c r="E349" s="5">
-        <v>2522.0300000000002</v>
+        <v>2528.85</v>
       </c>
       <c r="F349" s="32" t="s">
-        <v>300</v>
+        <v>301</v>
+      </c>
+      <c r="G349" s="13">
+        <f>AVERAGE(E349,E351)</f>
+        <v>2527.4899999999998</v>
+      </c>
+      <c r="H349" s="18">
+        <f>STDEV(E349,E351)</f>
+        <v>1.9233304448272679</v>
+      </c>
+      <c r="K349" s="5">
+        <f>G349+$J$331</f>
+        <v>2515.6249999999995</v>
       </c>
     </row>
     <row r="350" spans="1:11" x14ac:dyDescent="0.2">
@@ -10448,25 +10462,13 @@
         <v>12</v>
       </c>
       <c r="D350" s="5">
-        <v>51.23</v>
-      </c>
-      <c r="E350" s="5">
-        <v>2528.85</v>
+        <v>50.45</v>
+      </c>
+      <c r="E350" s="14">
+        <v>2487.25</v>
       </c>
       <c r="F350" s="32" t="s">
-        <v>301</v>
-      </c>
-      <c r="G350" s="13">
-        <f>AVERAGE(E350,E352)</f>
-        <v>2527.4899999999998</v>
-      </c>
-      <c r="H350" s="18">
-        <f>STDEV(E350,E352)</f>
-        <v>1.9233304448272679</v>
-      </c>
-      <c r="K350" s="5">
-        <f>G350+$J$332</f>
-        <v>2515.6249999999995</v>
+        <v>302</v>
       </c>
     </row>
     <row r="351" spans="1:11" x14ac:dyDescent="0.2">
@@ -10480,13 +10482,13 @@
         <v>12</v>
       </c>
       <c r="D351" s="5">
-        <v>50.45</v>
-      </c>
-      <c r="E351" s="14">
-        <v>2487.25</v>
+        <v>50.72</v>
+      </c>
+      <c r="E351" s="5">
+        <v>2526.13</v>
       </c>
       <c r="F351" s="32" t="s">
-        <v>302</v>
+        <v>408</v>
       </c>
     </row>
     <row r="352" spans="1:11" x14ac:dyDescent="0.2">
@@ -10500,13 +10502,25 @@
         <v>12</v>
       </c>
       <c r="D352" s="5">
-        <v>50.72</v>
+        <v>49.24</v>
       </c>
       <c r="E352" s="5">
-        <v>2526.13</v>
+        <v>2442.25</v>
       </c>
       <c r="F352" s="32" t="s">
-        <v>413</v>
+        <v>303</v>
+      </c>
+      <c r="G352" s="13">
+        <f>AVERAGE(E352:E353)</f>
+        <v>2443.69</v>
+      </c>
+      <c r="H352" s="18">
+        <f>STDEV(E352:E353)</f>
+        <v>2.036467529817334</v>
+      </c>
+      <c r="K352" s="5">
+        <f>G352+$J$331</f>
+        <v>2431.8249999999998</v>
       </c>
     </row>
     <row r="353" spans="1:11" x14ac:dyDescent="0.2">
@@ -10520,25 +10534,13 @@
         <v>12</v>
       </c>
       <c r="D353" s="5">
-        <v>49.24</v>
+        <v>50.38</v>
       </c>
       <c r="E353" s="5">
-        <v>2442.25</v>
+        <v>2445.13</v>
       </c>
       <c r="F353" s="32" t="s">
-        <v>303</v>
-      </c>
-      <c r="G353" s="13">
-        <f>AVERAGE(E353:E354)</f>
-        <v>2443.69</v>
-      </c>
-      <c r="H353" s="18">
-        <f>STDEV(E353:E354)</f>
-        <v>2.036467529817334</v>
-      </c>
-      <c r="K353" s="5">
-        <f>G353+$J$332</f>
-        <v>2431.8249999999998</v>
+        <v>304</v>
       </c>
     </row>
     <row r="354" spans="1:11" x14ac:dyDescent="0.2">
@@ -10552,13 +10554,25 @@
         <v>12</v>
       </c>
       <c r="D354" s="5">
-        <v>50.38</v>
+        <v>50.66</v>
       </c>
       <c r="E354" s="5">
-        <v>2445.13</v>
+        <v>2465.79</v>
       </c>
       <c r="F354" s="32" t="s">
-        <v>304</v>
+        <v>305</v>
+      </c>
+      <c r="G354" s="13">
+        <f>AVERAGE(E354,E356)</f>
+        <v>2464.0450000000001</v>
+      </c>
+      <c r="H354" s="18">
+        <f>STDEV(E354,E356)</f>
+        <v>2.4678026663408965</v>
+      </c>
+      <c r="K354" s="5">
+        <f>G354+$J$331</f>
+        <v>2452.1799999999998</v>
       </c>
     </row>
     <row r="355" spans="1:11" x14ac:dyDescent="0.2">
@@ -10572,25 +10586,13 @@
         <v>12</v>
       </c>
       <c r="D355" s="5">
-        <v>50.66</v>
-      </c>
-      <c r="E355" s="5">
-        <v>2465.79</v>
+        <v>50.38</v>
+      </c>
+      <c r="E355" s="14">
+        <v>2473.2600000000002</v>
       </c>
       <c r="F355" s="32" t="s">
-        <v>305</v>
-      </c>
-      <c r="G355" s="13">
-        <f>AVERAGE(E355,E357)</f>
-        <v>2464.0450000000001</v>
-      </c>
-      <c r="H355" s="18">
-        <f>STDEV(E355,E357)</f>
-        <v>2.4678026663408965</v>
-      </c>
-      <c r="K355" s="5">
-        <f>G355+$J$332</f>
-        <v>2452.1799999999998</v>
+        <v>306</v>
       </c>
     </row>
     <row r="356" spans="1:11" x14ac:dyDescent="0.2">
@@ -10604,13 +10606,13 @@
         <v>12</v>
       </c>
       <c r="D356" s="5">
-        <v>50.38</v>
-      </c>
-      <c r="E356" s="14">
-        <v>2473.2600000000002</v>
+        <v>49.58</v>
+      </c>
+      <c r="E356" s="5">
+        <v>2462.3000000000002</v>
       </c>
       <c r="F356" s="32" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="357" spans="1:11" x14ac:dyDescent="0.2">
@@ -10624,13 +10626,25 @@
         <v>12</v>
       </c>
       <c r="D357" s="5">
-        <v>49.58</v>
+        <v>48.57</v>
       </c>
       <c r="E357" s="5">
-        <v>2462.3000000000002</v>
+        <v>2592.0100000000002</v>
       </c>
       <c r="F357" s="32" t="s">
-        <v>307</v>
+        <v>308</v>
+      </c>
+      <c r="G357" s="13">
+        <f>AVERAGE(E358,E359)</f>
+        <v>2479.8000000000002</v>
+      </c>
+      <c r="H357" s="18">
+        <f>STDEV(E358,E359)</f>
+        <v>3.2385490578343363</v>
+      </c>
+      <c r="K357" s="5">
+        <f>G357+$J$331</f>
+        <v>2467.9349999999999</v>
       </c>
     </row>
     <row r="358" spans="1:11" x14ac:dyDescent="0.2">
@@ -10644,25 +10658,13 @@
         <v>12</v>
       </c>
       <c r="D358" s="5">
-        <v>48.57</v>
+        <v>48.07</v>
       </c>
       <c r="E358" s="5">
-        <v>2592.0100000000002</v>
+        <v>2477.5100000000002</v>
       </c>
       <c r="F358" s="32" t="s">
-        <v>308</v>
-      </c>
-      <c r="G358" s="13">
-        <f>AVERAGE(E359,E360)</f>
-        <v>2479.8000000000002</v>
-      </c>
-      <c r="H358" s="18">
-        <f>STDEV(E359,E360)</f>
-        <v>3.2385490578343363</v>
-      </c>
-      <c r="K358" s="5">
-        <f>G358+$J$332</f>
-        <v>2467.9349999999999</v>
+        <v>309</v>
       </c>
     </row>
     <row r="359" spans="1:11" x14ac:dyDescent="0.2">
@@ -10676,13 +10678,13 @@
         <v>12</v>
       </c>
       <c r="D359" s="5">
-        <v>48.07</v>
+        <v>51.58</v>
       </c>
       <c r="E359" s="5">
-        <v>2477.5100000000002</v>
+        <v>2482.09</v>
       </c>
       <c r="F359" s="32" t="s">
-        <v>309</v>
+        <v>409</v>
       </c>
     </row>
     <row r="360" spans="1:11" x14ac:dyDescent="0.2">
@@ -10696,13 +10698,25 @@
         <v>12</v>
       </c>
       <c r="D360" s="5">
-        <v>51.58</v>
+        <v>49.59</v>
       </c>
       <c r="E360" s="5">
-        <v>2482.09</v>
+        <v>2471.12</v>
       </c>
       <c r="F360" s="32" t="s">
-        <v>414</v>
+        <v>310</v>
+      </c>
+      <c r="G360" s="13">
+        <f>AVERAGE(E360,E362)</f>
+        <v>2473.2049999999999</v>
+      </c>
+      <c r="H360" s="18">
+        <f>STDEV(E360,E362)</f>
+        <v>2.9486352775479547</v>
+      </c>
+      <c r="K360" s="5">
+        <f>G360+$J$331</f>
+        <v>2461.3399999999997</v>
       </c>
     </row>
     <row r="361" spans="1:11" x14ac:dyDescent="0.2">
@@ -10716,25 +10730,13 @@
         <v>12</v>
       </c>
       <c r="D361" s="5">
-        <v>49.59</v>
-      </c>
-      <c r="E361" s="5">
-        <v>2471.12</v>
+        <v>49.61</v>
+      </c>
+      <c r="E361" s="14">
+        <v>2442.16</v>
       </c>
       <c r="F361" s="32" t="s">
-        <v>310</v>
-      </c>
-      <c r="G361" s="13">
-        <f>AVERAGE(E361,E363)</f>
-        <v>2473.2049999999999</v>
-      </c>
-      <c r="H361" s="18">
-        <f>STDEV(E361,E363)</f>
-        <v>2.9486352775479547</v>
-      </c>
-      <c r="K361" s="5">
-        <f>G361+$J$332</f>
-        <v>2461.3399999999997</v>
+        <v>311</v>
       </c>
     </row>
     <row r="362" spans="1:11" x14ac:dyDescent="0.2">
@@ -10748,13 +10750,13 @@
         <v>12</v>
       </c>
       <c r="D362" s="5">
-        <v>49.61</v>
-      </c>
-      <c r="E362" s="14">
-        <v>2442.16</v>
-      </c>
-      <c r="F362" s="32" t="s">
-        <v>311</v>
+        <v>50.11</v>
+      </c>
+      <c r="E362" s="5">
+        <v>2475.29</v>
+      </c>
+      <c r="F362" s="33" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="363" spans="1:11" x14ac:dyDescent="0.2">
@@ -10768,13 +10770,25 @@
         <v>12</v>
       </c>
       <c r="D363" s="5">
-        <v>50.11</v>
-      </c>
-      <c r="E363" s="5">
-        <v>2475.29</v>
-      </c>
-      <c r="F363" s="33" t="s">
-        <v>312</v>
+        <v>50.48</v>
+      </c>
+      <c r="E363" s="14">
+        <v>2497.66</v>
+      </c>
+      <c r="F363" s="32" t="s">
+        <v>313</v>
+      </c>
+      <c r="G363" s="13">
+        <f>AVERAGE(E364:E365)</f>
+        <v>2475.91</v>
+      </c>
+      <c r="H363" s="18">
+        <f>STDEV(E364:E365)</f>
+        <v>1.5980613254814302</v>
+      </c>
+      <c r="K363" s="5">
+        <f>G363+$J$331</f>
+        <v>2464.0449999999996</v>
       </c>
     </row>
     <row r="364" spans="1:11" x14ac:dyDescent="0.2">
@@ -10788,25 +10802,13 @@
         <v>12</v>
       </c>
       <c r="D364" s="5">
-        <v>50.48</v>
-      </c>
-      <c r="E364" s="14">
-        <v>2497.66</v>
+        <v>51.38</v>
+      </c>
+      <c r="E364" s="5">
+        <v>2474.7800000000002</v>
       </c>
       <c r="F364" s="32" t="s">
-        <v>313</v>
-      </c>
-      <c r="G364" s="13">
-        <f>AVERAGE(E365:E366)</f>
-        <v>2475.91</v>
-      </c>
-      <c r="H364" s="18">
-        <f>STDEV(E365:E366)</f>
-        <v>1.5980613254814302</v>
-      </c>
-      <c r="K364" s="5">
-        <f>G364+$J$332</f>
-        <v>2464.0449999999996</v>
+        <v>314</v>
       </c>
     </row>
     <row r="365" spans="1:11" x14ac:dyDescent="0.2">
@@ -10820,13 +10822,13 @@
         <v>12</v>
       </c>
       <c r="D365" s="5">
-        <v>51.38</v>
+        <v>50.49</v>
       </c>
       <c r="E365" s="5">
-        <v>2474.7800000000002</v>
+        <v>2477.04</v>
       </c>
       <c r="F365" s="32" t="s">
-        <v>314</v>
+        <v>410</v>
       </c>
     </row>
     <row r="366" spans="1:11" x14ac:dyDescent="0.2">
@@ -10840,13 +10842,25 @@
         <v>12</v>
       </c>
       <c r="D366" s="5">
-        <v>50.49</v>
+        <v>50.73</v>
       </c>
       <c r="E366" s="5">
-        <v>2477.04</v>
+        <v>2478.58</v>
       </c>
       <c r="F366" s="32" t="s">
-        <v>415</v>
+        <v>315</v>
+      </c>
+      <c r="G366" s="13">
+        <f>AVERAGE(E366,E368)</f>
+        <v>2481.125</v>
+      </c>
+      <c r="H366" s="18">
+        <f>STDEV(E366,E368)</f>
+        <v>3.5991735162396297</v>
+      </c>
+      <c r="K366" s="5">
+        <f>G366+$J$331</f>
+        <v>2469.2599999999998</v>
       </c>
     </row>
     <row r="367" spans="1:11" x14ac:dyDescent="0.2">
@@ -10860,25 +10874,13 @@
         <v>12</v>
       </c>
       <c r="D367" s="5">
-        <v>50.73</v>
-      </c>
-      <c r="E367" s="5">
-        <v>2478.58</v>
+        <v>48.76</v>
+      </c>
+      <c r="E367" s="14">
+        <v>2462.1799999999998</v>
       </c>
       <c r="F367" s="32" t="s">
-        <v>315</v>
-      </c>
-      <c r="G367" s="13">
-        <f>AVERAGE(E367,E369)</f>
-        <v>2481.125</v>
-      </c>
-      <c r="H367" s="18">
-        <f>STDEV(E367,E369)</f>
-        <v>3.5991735162396297</v>
-      </c>
-      <c r="K367" s="5">
-        <f>G367+$J$332</f>
-        <v>2469.2599999999998</v>
+        <v>316</v>
       </c>
     </row>
     <row r="368" spans="1:11" x14ac:dyDescent="0.2">
@@ -10892,13 +10894,13 @@
         <v>12</v>
       </c>
       <c r="D368" s="5">
-        <v>48.76</v>
-      </c>
-      <c r="E368" s="14">
-        <v>2462.1799999999998</v>
+        <v>49.49</v>
+      </c>
+      <c r="E368" s="5">
+        <v>2483.67</v>
       </c>
       <c r="F368" s="32" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="369" spans="1:11" x14ac:dyDescent="0.2">
@@ -10912,17 +10914,46 @@
         <v>12</v>
       </c>
       <c r="D369" s="5">
-        <v>49.49</v>
+        <v>49.57</v>
       </c>
       <c r="E369" s="5">
-        <v>2483.67</v>
+        <v>2419.6799999999998</v>
       </c>
       <c r="F369" s="32" t="s">
-        <v>317</v>
+        <v>318</v>
+      </c>
+      <c r="G369" s="13">
+        <f>AVERAGE(E369:E370)</f>
+        <v>2421.96</v>
+      </c>
+      <c r="H369" s="18">
+        <f>STDEV(E369:E370)</f>
+        <v>3.2244069222106182</v>
+      </c>
+      <c r="K369" s="5">
+        <f>G369+$J$331</f>
+        <v>2410.0949999999998</v>
       </c>
     </row>
     <row r="370" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F370" s="32"/>
+      <c r="A370" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B370" s="31">
+        <v>45083</v>
+      </c>
+      <c r="C370" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D370" s="5">
+        <v>49.37</v>
+      </c>
+      <c r="E370" s="5">
+        <v>2424.2399999999998</v>
+      </c>
+      <c r="F370" s="32" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="371" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A371" s="9" t="s">
@@ -10935,25 +10966,25 @@
         <v>12</v>
       </c>
       <c r="D371" s="5">
-        <v>49.57</v>
+        <v>48.39</v>
       </c>
       <c r="E371" s="5">
-        <v>2419.6799999999998</v>
+        <v>2487.91</v>
       </c>
       <c r="F371" s="32" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="G371" s="13">
-        <f>AVERAGE(E371:E372)</f>
-        <v>2421.96</v>
+        <f>AVERAGE(E371,E373)</f>
+        <v>2488.9749999999999</v>
       </c>
       <c r="H371" s="18">
-        <f>STDEV(E371:E372)</f>
-        <v>3.2244069222106182</v>
+        <f>STDEV(E371,E373)</f>
+        <v>1.5061374439274233</v>
       </c>
       <c r="K371" s="5">
-        <f>G371+$J$332</f>
-        <v>2410.0949999999998</v>
+        <f>G371+$J$331</f>
+        <v>2477.1099999999997</v>
       </c>
     </row>
     <row r="372" spans="1:11" x14ac:dyDescent="0.2">
@@ -10967,13 +10998,13 @@
         <v>12</v>
       </c>
       <c r="D372" s="5">
-        <v>49.37</v>
-      </c>
-      <c r="E372" s="5">
-        <v>2424.2399999999998</v>
+        <v>50.53</v>
+      </c>
+      <c r="E372" s="14">
+        <v>2498.6999999999998</v>
       </c>
       <c r="F372" s="32" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
     </row>
     <row r="373" spans="1:11" x14ac:dyDescent="0.2">
@@ -10987,25 +11018,13 @@
         <v>12</v>
       </c>
       <c r="D373" s="5">
-        <v>48.39</v>
+        <v>50.24</v>
       </c>
       <c r="E373" s="5">
-        <v>2487.91</v>
+        <v>2490.04</v>
       </c>
       <c r="F373" s="32" t="s">
-        <v>320</v>
-      </c>
-      <c r="G373" s="13">
-        <f>AVERAGE(E373,E375)</f>
-        <v>2488.9749999999999</v>
-      </c>
-      <c r="H373" s="18">
-        <f>STDEV(E373,E375)</f>
-        <v>1.5061374439274233</v>
-      </c>
-      <c r="K373" s="5">
-        <f>G373+$J$332</f>
-        <v>2477.1099999999997</v>
+        <v>322</v>
       </c>
     </row>
     <row r="374" spans="1:11" x14ac:dyDescent="0.2">
@@ -11019,13 +11038,25 @@
         <v>12</v>
       </c>
       <c r="D374" s="5">
-        <v>50.53</v>
+        <v>48.99</v>
       </c>
       <c r="E374" s="14">
-        <v>2498.6999999999998</v>
+        <v>2472.96</v>
       </c>
       <c r="F374" s="32" t="s">
-        <v>321</v>
+        <v>323</v>
+      </c>
+      <c r="G374" s="13">
+        <f>AVERAGE(E375:E376)</f>
+        <v>2465.23</v>
+      </c>
+      <c r="H374" s="18">
+        <f>STDEV(E375:E376)</f>
+        <v>2.6587214972615731</v>
+      </c>
+      <c r="K374" s="5">
+        <f>G374+$J$331</f>
+        <v>2453.3649999999998</v>
       </c>
     </row>
     <row r="375" spans="1:11" x14ac:dyDescent="0.2">
@@ -11039,13 +11070,13 @@
         <v>12</v>
       </c>
       <c r="D375" s="5">
-        <v>50.24</v>
+        <v>49.26</v>
       </c>
       <c r="E375" s="5">
-        <v>2490.04</v>
+        <v>2463.35</v>
       </c>
       <c r="F375" s="32" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="376" spans="1:11" x14ac:dyDescent="0.2">
@@ -11059,25 +11090,13 @@
         <v>12</v>
       </c>
       <c r="D376" s="5">
-        <v>48.99</v>
-      </c>
-      <c r="E376" s="14">
-        <v>2472.96</v>
+        <v>49.75</v>
+      </c>
+      <c r="E376" s="5">
+        <v>2467.11</v>
       </c>
       <c r="F376" s="32" t="s">
-        <v>323</v>
-      </c>
-      <c r="G376" s="13">
-        <f>AVERAGE(E377:E378)</f>
-        <v>2465.23</v>
-      </c>
-      <c r="H376" s="18">
-        <f>STDEV(E377:E378)</f>
-        <v>2.6587214972615731</v>
-      </c>
-      <c r="K376" s="5">
-        <f>G376+$J$332</f>
-        <v>2453.3649999999998</v>
+        <v>325</v>
       </c>
     </row>
     <row r="377" spans="1:11" x14ac:dyDescent="0.2">
@@ -11085,19 +11104,31 @@
         <v>11</v>
       </c>
       <c r="B377" s="31">
-        <v>45083</v>
+        <v>45084</v>
       </c>
       <c r="C377" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D377" s="5">
-        <v>49.26</v>
+        <v>49.88</v>
       </c>
       <c r="E377" s="5">
-        <v>2463.35</v>
+        <v>2557.1799999999998</v>
       </c>
       <c r="F377" s="32" t="s">
-        <v>324</v>
+        <v>326</v>
+      </c>
+      <c r="G377" s="13">
+        <f>AVERAGE(E377,E379)</f>
+        <v>2554.3850000000002</v>
+      </c>
+      <c r="H377" s="18">
+        <f>STDEV(E377,E379)</f>
+        <v>3.9527269068325821</v>
+      </c>
+      <c r="K377" s="5">
+        <f>G377+$J$394</f>
+        <v>2557.395</v>
       </c>
     </row>
     <row r="378" spans="1:11" x14ac:dyDescent="0.2">
@@ -11105,537 +11136,1298 @@
         <v>11</v>
       </c>
       <c r="B378" s="31">
-        <v>45083</v>
+        <v>45084</v>
       </c>
       <c r="C378" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D378" s="5">
-        <v>49.75</v>
-      </c>
-      <c r="E378" s="5">
-        <v>2467.11</v>
+        <v>49.71</v>
+      </c>
+      <c r="E378" s="14">
+        <v>2569.42</v>
       </c>
       <c r="F378" s="32" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
     </row>
     <row r="379" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A379" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B379" s="31">
+        <v>45084</v>
+      </c>
       <c r="C379" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D379" s="5">
+        <v>50.58</v>
+      </c>
+      <c r="E379" s="5">
+        <v>2551.59</v>
+      </c>
       <c r="F379" s="32" t="s">
-        <v>326</v>
-      </c>
-      <c r="G379" s="13" t="e">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="380" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A380" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B380" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C380" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D380" s="5">
+        <v>49.55</v>
+      </c>
+      <c r="E380" s="5">
+        <v>2526.6799999999998</v>
+      </c>
+      <c r="F380" s="32" t="s">
+        <v>329</v>
+      </c>
+      <c r="G380" s="13">
         <f>AVERAGE(E380:E381)</f>
+        <v>2528.5249999999996</v>
+      </c>
+      <c r="H380" s="18">
+        <f>STDEV(E380:E381)</f>
+        <v>2.6092240225783989</v>
+      </c>
+      <c r="K380" s="5">
+        <f>G380+$J$394</f>
+        <v>2531.5349999999994</v>
+      </c>
+    </row>
+    <row r="381" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A381" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B381" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C381" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D381" s="5">
+        <v>50.17</v>
+      </c>
+      <c r="E381" s="5">
+        <v>2530.37</v>
+      </c>
+      <c r="F381" s="32" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="382" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A382" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B382" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C382" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D382" s="5">
+        <v>50.25</v>
+      </c>
+      <c r="E382" s="14">
+        <v>2551.3000000000002</v>
+      </c>
+      <c r="F382" s="32" t="s">
+        <v>331</v>
+      </c>
+      <c r="G382" s="13">
+        <f>AVERAGE(E383:E384)</f>
+        <v>2560.7350000000001</v>
+      </c>
+      <c r="H382" s="18">
+        <f>STDEV(E383:E384)</f>
+        <v>1.7041273426594767</v>
+      </c>
+      <c r="K382" s="5">
+        <f>G382+$J$394</f>
+        <v>2563.7449999999999</v>
+      </c>
+    </row>
+    <row r="383" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A383" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B383" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C383" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D383" s="5">
+        <v>50.42</v>
+      </c>
+      <c r="E383" s="5">
+        <v>2559.5300000000002</v>
+      </c>
+      <c r="F383" s="32" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="384" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A384" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B384" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C384" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D384" s="5">
+        <v>51.75</v>
+      </c>
+      <c r="E384" s="5">
+        <v>2561.94</v>
+      </c>
+      <c r="F384" s="32" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="385" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A385" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B385" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C385" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D385" s="5">
+        <v>50.52</v>
+      </c>
+      <c r="E385" s="5">
+        <v>2550.35</v>
+      </c>
+      <c r="F385" s="32" t="s">
+        <v>334</v>
+      </c>
+      <c r="G385" s="13">
+        <f>AVERAGE(E386:E386)</f>
+        <v>2547.5500000000002</v>
+      </c>
+      <c r="H385" s="18">
+        <f>STDEV(E385:E386)</f>
+        <v>1.9798989873221402</v>
+      </c>
+      <c r="K385" s="5">
+        <f>G385+$J$394</f>
+        <v>2550.56</v>
+      </c>
+    </row>
+    <row r="386" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A386" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B386" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C386" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D386" s="5">
+        <v>50.42</v>
+      </c>
+      <c r="E386" s="5">
+        <v>2547.5500000000002</v>
+      </c>
+      <c r="F386" s="32" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="387" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A387" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B387" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C387" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D387" s="5">
+        <v>49.88</v>
+      </c>
+      <c r="E387" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="F387" s="32" t="s">
+        <v>336</v>
+      </c>
+      <c r="G387" s="13">
+        <f>AVERAGE(E388:E389)</f>
+        <v>2530.77</v>
+      </c>
+      <c r="H387" s="18">
+        <f>STDEV(E388:E389)</f>
+        <v>1.2869343417593107</v>
+      </c>
+      <c r="K387" s="5">
+        <f>G387+$J$394</f>
+        <v>2533.7799999999997</v>
+      </c>
+    </row>
+    <row r="388" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A388" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B388" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C388" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D388" s="5">
+        <v>50.59</v>
+      </c>
+      <c r="E388" s="5">
+        <v>2529.86</v>
+      </c>
+      <c r="F388" s="32" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="389" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A389" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B389" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C389" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D389" s="5">
+        <v>50.92</v>
+      </c>
+      <c r="E389" s="5">
+        <v>2531.6799999999998</v>
+      </c>
+      <c r="F389" s="32" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="390" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A390" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B390" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C390" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D390" s="5">
+        <v>49.68</v>
+      </c>
+      <c r="E390" s="5">
+        <v>2544.84</v>
+      </c>
+      <c r="F390" s="32" t="s">
+        <v>339</v>
+      </c>
+      <c r="G390" s="13">
+        <f>AVERAGE(E390,E392)</f>
+        <v>2546.91</v>
+      </c>
+      <c r="H390" s="18">
+        <f>STDEV(E390,E392)</f>
+        <v>2.9274220741122168</v>
+      </c>
+      <c r="K390" s="5">
+        <f>G390+$J$394</f>
+        <v>2549.9199999999996</v>
+      </c>
+    </row>
+    <row r="391" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A391" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B391" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C391" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D391" s="5">
+        <v>50.52</v>
+      </c>
+      <c r="E391" s="14">
+        <v>2560.81</v>
+      </c>
+      <c r="F391" s="32" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="392" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A392" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B392" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C392" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D392" s="5">
+        <v>51.62</v>
+      </c>
+      <c r="E392" s="5">
+        <v>2548.98</v>
+      </c>
+      <c r="F392" s="32" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="393" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C393" s="10"/>
+    </row>
+    <row r="394" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A394" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B394" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C394" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D394" s="14">
+        <v>50.58</v>
+      </c>
+      <c r="E394" s="14">
+        <v>2251.12</v>
+      </c>
+      <c r="F394" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G394" s="13">
+        <f>AVERAGE(E395:E396)</f>
+        <v>2223.4300000000003</v>
+      </c>
+      <c r="H394" s="18">
+        <f>STDEV(E395:E396)</f>
+        <v>0.22627416997981095</v>
+      </c>
+      <c r="I394" s="3">
+        <v>2226.44</v>
+      </c>
+      <c r="J394" s="4">
+        <f>I394-G394</f>
+        <v>3.0099999999997635</v>
+      </c>
+      <c r="K394" s="5">
+        <f>G394+J394</f>
+        <v>2226.44</v>
+      </c>
+      <c r="L394" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="395" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A395" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B395" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C395" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D395" s="5">
+        <v>49.7</v>
+      </c>
+      <c r="E395" s="5">
+        <v>2223.27</v>
+      </c>
+      <c r="F395" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="396" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A396" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B396" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C396" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D396" s="5">
+        <v>48.62</v>
+      </c>
+      <c r="E396" s="5">
+        <v>2223.59</v>
+      </c>
+      <c r="F396" s="17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="397" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A397" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B397" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C397" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D397" s="5">
+        <v>50.21</v>
+      </c>
+      <c r="E397" s="5">
+        <v>2556.63</v>
+      </c>
+      <c r="F397" s="32" t="s">
+        <v>342</v>
+      </c>
+      <c r="G397" s="13">
+        <f>AVERAGE(E397:E398)</f>
+        <v>2556.88</v>
+      </c>
+      <c r="H397" s="18">
+        <f>STDEV(E397:E398)</f>
+        <v>0.35355339059327379</v>
+      </c>
+      <c r="K397" s="5">
+        <f>G397+$J$394</f>
+        <v>2559.89</v>
+      </c>
+    </row>
+    <row r="398" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A398" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B398" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C398" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D398" s="5">
+        <v>51.83</v>
+      </c>
+      <c r="E398" s="5">
+        <v>2557.13</v>
+      </c>
+      <c r="F398" s="32" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="399" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A399" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B399" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C399" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D399" s="5">
+        <v>49.33</v>
+      </c>
+      <c r="E399" s="5">
+        <v>2576.39</v>
+      </c>
+      <c r="F399" s="32" t="s">
+        <v>344</v>
+      </c>
+      <c r="G399" s="13">
+        <f>AVERAGE(E399:E400)</f>
+        <v>2575.5500000000002</v>
+      </c>
+      <c r="H399" s="18">
+        <f>STDEV(E399:E400)</f>
+        <v>1.1879393923932842</v>
+      </c>
+      <c r="K399" s="5">
+        <f>G399+$J$394</f>
+        <v>2578.56</v>
+      </c>
+    </row>
+    <row r="400" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A400" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B400" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C400" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D400" s="5">
+        <v>51.19</v>
+      </c>
+      <c r="E400" s="5">
+        <v>2574.71</v>
+      </c>
+      <c r="F400" s="32" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="401" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A401" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B401" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C401" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D401" s="5">
+        <v>50.11</v>
+      </c>
+      <c r="E401" s="5">
+        <v>2584.3000000000002</v>
+      </c>
+      <c r="F401" s="32" t="s">
+        <v>346</v>
+      </c>
+      <c r="G401" s="13">
+        <f>AVERAGE(E401:E402)</f>
+        <v>2586.9949999999999</v>
+      </c>
+      <c r="H401" s="18">
+        <f>STDEV(E401:E402)</f>
+        <v>3.8113055505954012</v>
+      </c>
+      <c r="K401" s="5">
+        <f>G401+$J$394</f>
+        <v>2590.0049999999997</v>
+      </c>
+    </row>
+    <row r="402" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A402" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B402" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C402" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D402" s="5">
+        <v>51.16</v>
+      </c>
+      <c r="E402" s="5">
+        <v>2589.69</v>
+      </c>
+      <c r="F402" s="32" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="403" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A403" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B403" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C403" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D403" s="5">
+        <v>51.03</v>
+      </c>
+      <c r="E403" s="14">
+        <v>2580.5300000000002</v>
+      </c>
+      <c r="F403" s="32" t="s">
+        <v>348</v>
+      </c>
+      <c r="G403" s="13">
+        <f>AVERAGE(E404:E405)</f>
+        <v>2592.87</v>
+      </c>
+      <c r="H403" s="18">
+        <f>STDEV(E404:E405)</f>
+        <v>4.2426406871192848</v>
+      </c>
+      <c r="K403" s="5">
+        <f>G403+$J$394</f>
+        <v>2595.8799999999997</v>
+      </c>
+    </row>
+    <row r="404" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A404" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B404" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C404" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D404" s="5">
+        <v>49.23</v>
+      </c>
+      <c r="E404" s="5">
+        <v>2595.87</v>
+      </c>
+      <c r="F404" s="32" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="405" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A405" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B405" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C405" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D405" s="5">
+        <v>51.58</v>
+      </c>
+      <c r="E405" s="5">
+        <v>2589.87</v>
+      </c>
+      <c r="F405" s="32" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="406" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A406" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B406" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C406" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D406" s="5">
+        <v>51.53</v>
+      </c>
+      <c r="E406" s="14">
+        <v>2539.8200000000002</v>
+      </c>
+      <c r="F406" s="32" t="s">
+        <v>351</v>
+      </c>
+      <c r="G406" s="13">
+        <f>AVERAGE(E407:E408)</f>
+        <v>2556.105</v>
+      </c>
+      <c r="H406" s="18">
+        <f>STDEV(E407:E408)</f>
+        <v>1.2374368670764582</v>
+      </c>
+      <c r="K406" s="5">
+        <f>G406+$J$394</f>
+        <v>2559.1149999999998</v>
+      </c>
+    </row>
+    <row r="407" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A407" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B407" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C407" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D407" s="5">
+        <v>51.05</v>
+      </c>
+      <c r="E407" s="5">
+        <v>2555.23</v>
+      </c>
+      <c r="F407" s="32" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="408" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A408" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B408" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C408" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D408" s="5">
+        <v>49.5</v>
+      </c>
+      <c r="E408" s="5">
+        <v>2556.98</v>
+      </c>
+      <c r="F408" s="32" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="409" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A409" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B409" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C409" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D409" s="5">
+        <v>50.5</v>
+      </c>
+      <c r="E409" s="5">
+        <v>2573.62</v>
+      </c>
+      <c r="F409" s="32" t="s">
+        <v>354</v>
+      </c>
+      <c r="G409" s="13">
+        <f>AVERAGE(E409:E410)</f>
+        <v>2571.7150000000001</v>
+      </c>
+      <c r="H409" s="18">
+        <f>STDEV(E409:E410)</f>
+        <v>2.6940768363207073</v>
+      </c>
+      <c r="K409" s="5">
+        <f>G409+$J$432</f>
+        <v>2568.17</v>
+      </c>
+    </row>
+    <row r="410" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A410" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B410" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C410" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D410" s="5">
+        <v>50.84</v>
+      </c>
+      <c r="E410" s="5">
+        <v>2569.81</v>
+      </c>
+      <c r="F410" s="32" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="411" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A411" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B411" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C411" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D411" s="5">
+        <v>50.26</v>
+      </c>
+      <c r="F411" s="32" t="s">
+        <v>356</v>
+      </c>
+      <c r="G411" s="13" t="e">
+        <f>AVERAGE(E412:E413)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H379" s="18" t="e">
-        <f>STDEV(E380:E381)</f>
+      <c r="H411" s="18" t="e">
+        <f>STDEV(E412:E413)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K379" s="5" t="e">
-        <f>G379+$J$332</f>
+      <c r="K411" s="5" t="e">
+        <f>G411+$J$432</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="380" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C380" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F380" s="32" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="381" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C381" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F381" s="32" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="382" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C382" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F382" s="32" t="s">
-        <v>329</v>
-      </c>
-      <c r="G382" s="13" t="e">
-        <f>AVERAGE(E383:E384)</f>
+    <row r="412" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A412" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B412" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C412" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D412" s="5">
+        <v>49.6</v>
+      </c>
+      <c r="F412" s="32" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="413" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A413" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B413" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C413" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D413" s="5">
+        <v>48.01</v>
+      </c>
+      <c r="F413" s="32" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="414" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A414" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B414" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C414" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D414" s="5">
+        <v>51.72</v>
+      </c>
+      <c r="F414" s="32" t="s">
+        <v>359</v>
+      </c>
+      <c r="G414" s="13" t="e">
+        <f>AVERAGE(E415:E416)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H382" s="18" t="e">
-        <f>STDEV(E383:E384)</f>
+      <c r="H414" s="18" t="e">
+        <f>STDEV(E415:E416)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K382" s="5" t="e">
-        <f>G382+$J$332</f>
+      <c r="K414" s="5" t="e">
+        <f>G414+$J$432</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="383" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C383" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F383" s="32" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="384" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C384" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F384" s="32" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="385" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C385" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F385" s="32" t="s">
-        <v>332</v>
-      </c>
-      <c r="G385" s="13" t="e">
-        <f>AVERAGE(E386:E387)</f>
+    <row r="415" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A415" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B415" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C415" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D415" s="5">
+        <v>51.74</v>
+      </c>
+      <c r="F415" s="32" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="416" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A416" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B416" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C416" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D416" s="5">
+        <v>50.54</v>
+      </c>
+      <c r="F416" s="32" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="417" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A417" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B417" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C417" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D417" s="5">
+        <v>49.45</v>
+      </c>
+      <c r="F417" s="32" t="s">
+        <v>362</v>
+      </c>
+      <c r="G417" s="13" t="e">
+        <f>AVERAGE(E418:E419)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H385" s="18" t="e">
-        <f>STDEV(E386:E387)</f>
+      <c r="H417" s="18" t="e">
+        <f>STDEV(E418:E419)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K385" s="5" t="e">
-        <f>G385+$J$332</f>
+      <c r="K417" s="5" t="e">
+        <f>G417+$J$432</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="386" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C386" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F386" s="32" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="387" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C387" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F387" s="32" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="388" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C388" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F388" s="32" t="s">
-        <v>335</v>
-      </c>
-      <c r="G388" s="13" t="e">
-        <f>AVERAGE(E389:E390)</f>
+    <row r="418" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A418" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B418" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C418" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D418" s="5">
+        <v>48.52</v>
+      </c>
+      <c r="F418" s="32" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="419" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A419" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B419" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C419" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D419" s="5">
+        <v>49.32</v>
+      </c>
+      <c r="F419" s="32" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="420" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A420" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B420" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C420" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F420" s="32" t="s">
+        <v>365</v>
+      </c>
+      <c r="G420" s="13" t="e">
+        <f>AVERAGE(E421:E422)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H388" s="18" t="e">
-        <f>STDEV(E389:E390)</f>
+      <c r="H420" s="18" t="e">
+        <f>STDEV(E421:E422)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K388" s="5" t="e">
-        <f>G388+$J$332</f>
+      <c r="K420" s="5" t="e">
+        <f>G420+$J$432</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="389" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C389" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F389" s="32" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="390" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C390" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F390" s="32" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="391" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C391" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F391" s="32" t="s">
-        <v>338</v>
-      </c>
-      <c r="G391" s="13" t="e">
-        <f>AVERAGE(E392:E393)</f>
+    <row r="421" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A421" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B421" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C421" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F421" s="32" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="422" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A422" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B422" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C422" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F422" s="32" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="423" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A423" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B423" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C423" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F423" s="32" t="s">
+        <v>368</v>
+      </c>
+      <c r="G423" s="13" t="e">
+        <f>AVERAGE(E424:E425)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H391" s="18" t="e">
-        <f>STDEV(E392:E393)</f>
+      <c r="H423" s="18" t="e">
+        <f>STDEV(E424:E425)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K391" s="5" t="e">
-        <f>G391+$J$332</f>
+      <c r="K423" s="5" t="e">
+        <f>G423+$J$432</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="392" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C392" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F392" s="32" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="393" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C393" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F393" s="32" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="394" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C394" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F394" s="32" t="s">
-        <v>341</v>
-      </c>
-      <c r="G394" s="13" t="e">
-        <f>AVERAGE(E395:E396)</f>
+    <row r="424" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A424" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B424" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C424" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F424" s="32" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="425" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A425" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B425" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C425" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F425" s="33" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="426" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A426" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B426" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C426" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F426" s="32" t="s">
+        <v>371</v>
+      </c>
+      <c r="G426" s="13" t="e">
+        <f>AVERAGE(E427:E428)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H394" s="18" t="e">
-        <f>STDEV(E395:E396)</f>
+      <c r="H426" s="18" t="e">
+        <f>STDEV(E427:E428)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K394" s="5" t="e">
-        <f>G394+$J$332</f>
+      <c r="K426" s="5" t="e">
+        <f>G426+$J$432</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="395" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C395" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F395" s="32" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="396" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C396" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F396" s="32" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="397" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C397" s="10"/>
-    </row>
-    <row r="398" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C398" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="F398" s="16" t="s">
+    <row r="427" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A427" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B427" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C427" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F427" s="32" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="428" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A428" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B428" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C428" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F428" s="32" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="429" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A429" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B429" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C429" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F429" s="32" t="s">
+        <v>374</v>
+      </c>
+      <c r="G429" s="13" t="e">
+        <f>AVERAGE(E430:E431)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H429" s="18" t="e">
+        <f>STDEV(E430:E431)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K429" s="5" t="e">
+        <f>G429+$J$432</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="430" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A430" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B430" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C430" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F430" s="32" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="431" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A431" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B431" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C431" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F431" s="32" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="432" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A432" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B432" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C432" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D432" s="5">
+        <v>49.82</v>
+      </c>
+      <c r="E432" s="5">
+        <v>2228.86</v>
+      </c>
+      <c r="F432" s="16" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="399" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C399" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F399" s="16" t="s">
+      <c r="G432" s="13">
+        <f>AVERAGE(E432:E433)</f>
+        <v>2229.9850000000001</v>
+      </c>
+      <c r="H432" s="18">
+        <f>STDEV(E432:E433)</f>
+        <v>1.5909902576697319</v>
+      </c>
+      <c r="I432" s="3">
+        <v>2226.44</v>
+      </c>
+      <c r="J432" s="4">
+        <f>I432-G432</f>
+        <v>-3.5450000000000728</v>
+      </c>
+      <c r="K432" s="5">
+        <f>G432+J432</f>
+        <v>2226.44</v>
+      </c>
+      <c r="L432" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="433" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A433" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B433" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C433" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D433" s="5">
+        <v>49.88</v>
+      </c>
+      <c r="E433" s="5">
+        <v>2231.11</v>
+      </c>
+      <c r="F433" s="16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="400" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C400" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F400" s="17" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="401" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C401" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F401" s="32" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="402" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C402" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F402" s="32" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="403" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C403" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F403" s="32" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="404" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C404" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F404" s="32" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="405" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C405" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F405" s="32" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="406" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C406" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F406" s="32" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="407" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C407" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F407" s="32" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="408" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C408" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F408" s="32" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="409" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C409" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F409" s="32" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="410" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C410" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F410" s="32" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="411" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C411" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F411" s="32" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="412" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C412" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F412" s="32" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="413" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C413" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F413" s="32" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="414" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C414" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F414" s="32" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="415" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C415" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F415" s="32" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="416" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C416" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F416" s="32" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="417" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C417" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F417" s="32" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="418" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C418" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F418" s="32" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="419" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C419" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F419" s="32" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="420" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C420" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F420" s="32" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="421" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C421" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F421" s="32" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="422" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C422" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F422" s="32" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="423" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C423" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F423" s="32" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="424" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C424" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F424" s="32" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="425" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C425" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F425" s="32" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="426" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C426" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F426" s="32" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="427" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C427" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F427" s="32" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="428" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C428" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F428" s="32" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="429" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C429" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F429" s="32" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="430" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C430" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F430" s="32" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="431" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C431" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F431" s="32" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="432" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C432" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F432" s="33" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="433" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C433" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F433" s="32" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="434" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="434" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A434" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B434" s="31">
+        <v>45084</v>
+      </c>
       <c r="C434" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F434" s="32" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="435" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="G434" s="13" t="e">
+        <f>AVERAGE(E435:E436)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H434" s="18" t="e">
+        <f>STDEV(E435:E436)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K434" s="5" t="e">
+        <f>G434+$J$432</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="435" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A435" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B435" s="31">
+        <v>45084</v>
+      </c>
       <c r="C435" s="10" t="s">
         <v>12</v>
       </c>
@@ -11643,7 +12435,13 @@
         <v>378</v>
       </c>
     </row>
-    <row r="436" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="436" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A436" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B436" s="31">
+        <v>45084</v>
+      </c>
       <c r="C436" s="10" t="s">
         <v>12</v>
       </c>
@@ -11651,15 +12449,39 @@
         <v>379</v>
       </c>
     </row>
-    <row r="437" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C437" s="25" t="s">
+    <row r="437" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A437" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B437" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C437" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F437" s="32" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="438" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="G437" s="13" t="e">
+        <f>AVERAGE(E438:E439)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H437" s="18" t="e">
+        <f>STDEV(E438:E439)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K437" s="5" t="e">
+        <f>G437+$J$432</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="438" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A438" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B438" s="31">
+        <v>45084</v>
+      </c>
       <c r="C438" s="10" t="s">
         <v>12</v>
       </c>
@@ -11667,278 +12489,325 @@
         <v>381</v>
       </c>
     </row>
-    <row r="439" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="F439" s="32"/>
-    </row>
-    <row r="440" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="439" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A439" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B439" s="31">
+        <v>45084</v>
+      </c>
+      <c r="C439" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F439" s="32" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="440" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A440" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B440" s="31">
+        <v>45084</v>
+      </c>
       <c r="C440" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F440" s="16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="441" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="F440" s="32" t="s">
+        <v>383</v>
+      </c>
+      <c r="G440" s="13" t="e">
+        <f>AVERAGE(E441:E442)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H440" s="18" t="e">
+        <f>STDEV(E441:E442)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K440" s="5" t="e">
+        <f>G440+$J$432</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="441" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A441" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B441" s="31">
+        <v>45084</v>
+      </c>
       <c r="C441" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F441" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="442" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="F441" s="32" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="442" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A442" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="C442" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F442" s="17" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="443" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="F442" s="32" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="443" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A443" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="C443" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F443" s="32" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="444" spans="3:6" x14ac:dyDescent="0.2">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="444" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A444" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="C444" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F444" s="32" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="445" spans="3:6" x14ac:dyDescent="0.2">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="445" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A445" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="C445" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F445" s="32" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="446" spans="3:6" x14ac:dyDescent="0.2">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="446" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A446" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="C446" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F446" s="32" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="447" spans="3:6" x14ac:dyDescent="0.2">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="447" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A447" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="C447" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F447" s="32" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="448" spans="3:6" x14ac:dyDescent="0.2">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="448" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A448" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="C448" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F448" s="32" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="449" spans="3:6" x14ac:dyDescent="0.2">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="449" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A449" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="C449" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F449" s="32" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="450" spans="3:6" x14ac:dyDescent="0.2">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="450" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A450" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="C450" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F450" s="32" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="451" spans="3:6" x14ac:dyDescent="0.2">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="451" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A451" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="C451" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F451" s="32" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="452" spans="3:6" x14ac:dyDescent="0.2">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="452" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A452" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="C452" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F452" s="32" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="453" spans="3:6" x14ac:dyDescent="0.2">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="453" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A453" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="C453" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F453" s="32" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="454" spans="3:6" x14ac:dyDescent="0.2">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="454" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A454" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="C454" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F454" s="32" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="455" spans="3:6" x14ac:dyDescent="0.2">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="455" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A455" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="C455" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F455" s="32" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="456" spans="3:6" x14ac:dyDescent="0.2">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="456" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A456" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="C456" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F456" s="32" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="457" spans="3:6" x14ac:dyDescent="0.2">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="457" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A457" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="C457" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F457" s="32" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="458" spans="3:6" x14ac:dyDescent="0.2">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="458" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A458" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="C458" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F458" s="32" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="459" spans="3:6" x14ac:dyDescent="0.2">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="459" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A459" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="C459" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F459" s="32" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="460" spans="3:6" x14ac:dyDescent="0.2">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="460" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A460" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="C460" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F460" s="32" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="461" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C461" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F461" s="32" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="462" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C462" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F462" s="32" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="463" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C463" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F463" s="32" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="464" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C464" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F464" s="32" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="465" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C465" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F465" s="32" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="466" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C466" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F466" s="32" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="467" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C467" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F467" s="32" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="468" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C468" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F468" s="32" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="469" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C469" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F469" s="32" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="470" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C470" s="10"/>
-    </row>
-    <row r="471" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C471" s="10"/>
-    </row>
-    <row r="472" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="461" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C461" s="10"/>
+    </row>
+    <row r="462" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C462" s="10"/>
+    </row>
+    <row r="463" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C463" s="10"/>
+    </row>
+    <row r="464" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C464" s="10"/>
+    </row>
+    <row r="465" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C465" s="10"/>
+    </row>
+    <row r="466" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C466" s="10"/>
+    </row>
+    <row r="467" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C467" s="10"/>
+    </row>
+    <row r="468" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C468" s="10"/>
+    </row>
+    <row r="469" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C469" s="10"/>
+    </row>
+    <row r="471" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C471" s="25"/>
+    </row>
+    <row r="472" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C472" s="10"/>
     </row>
-    <row r="473" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="473" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C473" s="10"/>
     </row>
-    <row r="474" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="474" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C474" s="10"/>
     </row>
-    <row r="475" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="475" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C475" s="10"/>
     </row>
-    <row r="476" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="476" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C476" s="10"/>
     </row>
-    <row r="477" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="477" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C477" s="10"/>
     </row>
-    <row r="478" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="478" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C478" s="10"/>
     </row>
-    <row r="480" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C480" s="25"/>
+    <row r="479" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C479" s="10"/>
+    </row>
+    <row r="480" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C480" s="10"/>
     </row>
     <row r="481" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C481" s="10"/>
@@ -11999,33 +12868,6 @@
     </row>
     <row r="500" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C500" s="10"/>
-    </row>
-    <row r="501" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C501" s="10"/>
-    </row>
-    <row r="502" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C502" s="10"/>
-    </row>
-    <row r="503" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C503" s="10"/>
-    </row>
-    <row r="504" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C504" s="10"/>
-    </row>
-    <row r="505" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C505" s="10"/>
-    </row>
-    <row r="506" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C506" s="10"/>
-    </row>
-    <row r="507" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C507" s="10"/>
-    </row>
-    <row r="508" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C508" s="10"/>
-    </row>
-    <row r="509" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C509" s="10"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:L1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
ALK ELOW 40% Historic
</commit_message>
<xml_diff>
--- a/Data/Spring_2023/BenthFun_Alkalinity.xlsx
+++ b/Data/Spring_2023/BenthFun_Alkalinity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremy/Library/Mobile Documents/com~apple~CloudDocs/Documents/Documents/Post-Doc/Projets/Villefranche/Projets/BenthFun – Jeremy/BenthFun/Data/Spring_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996D05F8-B76E-E240-A6F1-E4C80D816F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7DC91F-4C92-0740-85B3-B453A66A543D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1825" uniqueCount="582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1819" uniqueCount="580">
   <si>
     <t>Operator</t>
   </si>
@@ -1243,16 +1243,10 @@
     <t>Tn_t1_ELOW_tile_01b</t>
   </si>
   <si>
-    <t>Tn_t1_ELOW_tile_01c</t>
-  </si>
-  <si>
     <t>Tn_t1_ELOW_tile_02a</t>
   </si>
   <si>
     <t>Tn_t1_ELOW_tile_02b</t>
-  </si>
-  <si>
-    <t>Tn_t1_ELOW_tile_02c</t>
   </si>
   <si>
     <t>Tn_t1_ELOW_tile_03a</t>
@@ -2264,11 +2258,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L644"/>
+  <dimension ref="A1:L642"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="73" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A435" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D457" sqref="D457"/>
+      <selection pane="bottomLeft" activeCell="G451" sqref="G451"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13036,7 +13030,7 @@
         <v>2468.38</v>
       </c>
       <c r="F424" s="32" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="425" spans="1:11" x14ac:dyDescent="0.2">
@@ -13232,7 +13226,7 @@
         <v>2530.84</v>
       </c>
       <c r="F432" s="32" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="433" spans="1:12" x14ac:dyDescent="0.2">
@@ -13530,22 +13524,22 @@
         <v>49.72</v>
       </c>
       <c r="E445" s="5">
-        <v>2798.88</v>
+        <v>2797.88</v>
       </c>
       <c r="F445" s="16" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="G445" s="13">
-        <f>AVERAGE(E446,E447)</f>
-        <v>2892.7</v>
-      </c>
-      <c r="H445" s="18" t="e">
-        <f>STDEV(E446,E447)</f>
-        <v>#DIV/0!</v>
+        <f>AVERAGE(E445,E447)</f>
+        <v>2794.82</v>
+      </c>
+      <c r="H445" s="18">
+        <f>STDEV(E445,E447)</f>
+        <v>4.3274935008615936</v>
       </c>
       <c r="K445" s="5">
         <f>G445+$J$416</f>
-        <v>2889.1549999999997</v>
+        <v>2791.2750000000001</v>
       </c>
     </row>
     <row r="446" spans="1:12" x14ac:dyDescent="0.2">
@@ -13561,11 +13555,11 @@
       <c r="D446" s="5">
         <v>48.28</v>
       </c>
-      <c r="E446" s="5">
+      <c r="E446" s="14">
         <v>2892.7</v>
       </c>
       <c r="F446" s="16" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="447" spans="1:12" x14ac:dyDescent="0.2">
@@ -13581,8 +13575,11 @@
       <c r="D447" s="5">
         <v>50.26</v>
       </c>
+      <c r="E447" s="5">
+        <v>2791.76</v>
+      </c>
       <c r="F447" s="16" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="448" spans="1:12" x14ac:dyDescent="0.2">
@@ -13598,20 +13595,23 @@
       <c r="D448" s="5">
         <v>50.21</v>
       </c>
+      <c r="E448" s="14">
+        <v>2776.09</v>
+      </c>
       <c r="F448" s="16" t="s">
-        <v>475</v>
-      </c>
-      <c r="G448" s="13" t="e">
+        <v>473</v>
+      </c>
+      <c r="G448" s="13">
         <f>AVERAGE(E449,E450)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H448" s="18" t="e">
+        <v>2792.2950000000001</v>
+      </c>
+      <c r="H448" s="18">
         <f>STDEV(E449,E450)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K448" s="5" t="e">
+        <v>3.995153313704058</v>
+      </c>
+      <c r="K448" s="5">
         <f>G448+$J$416</f>
-        <v>#DIV/0!</v>
+        <v>2788.75</v>
       </c>
     </row>
     <row r="449" spans="1:11" x14ac:dyDescent="0.2">
@@ -13627,8 +13627,11 @@
       <c r="D449" s="5">
         <v>48.31</v>
       </c>
+      <c r="E449" s="5">
+        <v>2789.47</v>
+      </c>
       <c r="F449" s="16" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="450" spans="1:11" x14ac:dyDescent="0.2">
@@ -13644,8 +13647,11 @@
       <c r="D450" s="5">
         <v>51.2</v>
       </c>
+      <c r="E450" s="5">
+        <v>2795.12</v>
+      </c>
       <c r="F450" s="16" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="451" spans="1:11" x14ac:dyDescent="0.2">
@@ -13661,20 +13667,23 @@
       <c r="D451" s="5">
         <v>50.61</v>
       </c>
+      <c r="E451" s="5">
+        <v>2738.11</v>
+      </c>
       <c r="F451" s="16" t="s">
         <v>400</v>
       </c>
-      <c r="G451" s="13" t="e">
-        <f>AVERAGE(E452,E453)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H451" s="18" t="e">
-        <f>STDEV(E452,E453)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K451" s="5" t="e">
+      <c r="G451" s="13">
+        <f>AVERAGE(E452,E451)</f>
+        <v>2736.45</v>
+      </c>
+      <c r="H451" s="18">
+        <f>STDEV(E452,E451)</f>
+        <v>2.3475945135394536</v>
+      </c>
+      <c r="K451" s="5">
         <f>G451+$J$416</f>
-        <v>#DIV/0!</v>
+        <v>2732.9049999999997</v>
       </c>
     </row>
     <row r="452" spans="1:11" x14ac:dyDescent="0.2">
@@ -13690,6 +13699,9 @@
       <c r="D452" s="5">
         <v>50.35</v>
       </c>
+      <c r="E452" s="5">
+        <v>2734.79</v>
+      </c>
       <c r="F452" s="16" t="s">
         <v>401</v>
       </c>
@@ -13705,11 +13717,26 @@
         <v>12</v>
       </c>
       <c r="D453" s="5">
-        <v>48.89</v>
+        <v>51.43</v>
+      </c>
+      <c r="E453" s="5">
+        <v>2773.66</v>
       </c>
       <c r="F453" s="16" t="s">
         <v>402</v>
       </c>
+      <c r="G453" s="13">
+        <f>AVERAGE(E453:E454)</f>
+        <v>2775.7049999999999</v>
+      </c>
+      <c r="H453" s="18">
+        <f>STDEV(E453:E454)</f>
+        <v>2.8920667350530822</v>
+      </c>
+      <c r="K453" s="5">
+        <f>G453+$J$416</f>
+        <v>2772.16</v>
+      </c>
     </row>
     <row r="454" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A454" s="9" t="s">
@@ -13722,53 +13749,38 @@
         <v>12</v>
       </c>
       <c r="D454" s="5">
-        <v>51.43</v>
+        <v>51.73</v>
+      </c>
+      <c r="E454" s="5">
+        <v>2777.75</v>
       </c>
       <c r="F454" s="16" t="s">
         <v>403</v>
       </c>
-      <c r="G454" s="13" t="e">
-        <f>AVERAGE(E455,E456)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H454" s="18" t="e">
-        <f>STDEV(E455,E456)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K454" s="5" t="e">
-        <f>G454+$J$416</f>
-        <v>#DIV/0!</v>
-      </c>
     </row>
     <row r="455" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A455" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B455" s="31">
-        <v>45090</v>
-      </c>
       <c r="C455" s="10" t="s">
         <v>12</v>
-      </c>
-      <c r="D455" s="5">
-        <v>51.73</v>
       </c>
       <c r="F455" s="16" t="s">
         <v>404</v>
       </c>
+      <c r="G455" s="13" t="e">
+        <f>AVERAGE(E456,E457)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H455" s="18" t="e">
+        <f>STDEV(E456,E457)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K455" s="5" t="e">
+        <f>G455+$J$416</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="456" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A456" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B456" s="31">
-        <v>45090</v>
-      </c>
       <c r="C456" s="10" t="s">
         <v>12</v>
-      </c>
-      <c r="D456" s="5">
-        <v>51.37</v>
       </c>
       <c r="F456" s="16" t="s">
         <v>405</v>
@@ -13781,18 +13793,6 @@
       <c r="F457" s="16" t="s">
         <v>406</v>
       </c>
-      <c r="G457" s="13" t="e">
-        <f>AVERAGE(E458,E459)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H457" s="18" t="e">
-        <f>STDEV(E458,E459)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K457" s="5" t="e">
-        <f>G457+$J$416</f>
-        <v>#DIV/0!</v>
-      </c>
     </row>
     <row r="458" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C458" s="10" t="s">
@@ -13801,6 +13801,18 @@
       <c r="F458" s="16" t="s">
         <v>407</v>
       </c>
+      <c r="G458" s="13" t="e">
+        <f>AVERAGE(E459,E460)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H458" s="18" t="e">
+        <f>STDEV(E459,E460)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K458" s="5" t="e">
+        <f>G458+$J$416</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="459" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C459" s="10" t="s">
@@ -13817,18 +13829,6 @@
       <c r="F460" s="16" t="s">
         <v>409</v>
       </c>
-      <c r="G460" s="13" t="e">
-        <f>AVERAGE(E461,E462)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H460" s="18" t="e">
-        <f>STDEV(E461,E462)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K460" s="5" t="e">
-        <f>G460+$J$416</f>
-        <v>#DIV/0!</v>
-      </c>
     </row>
     <row r="461" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C461" s="10" t="s">
@@ -13837,6 +13837,18 @@
       <c r="F461" s="16" t="s">
         <v>410</v>
       </c>
+      <c r="G461" s="13" t="e">
+        <f>AVERAGE(E462,E463)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H461" s="18" t="e">
+        <f>STDEV(E462,E463)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K461" s="5" t="e">
+        <f>G461+$J$416</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="462" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C462" s="10" t="s">
@@ -13853,18 +13865,6 @@
       <c r="F463" s="16" t="s">
         <v>412</v>
       </c>
-      <c r="G463" s="13" t="e">
-        <f>AVERAGE(E464,E465)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H463" s="18" t="e">
-        <f>STDEV(E464,E465)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K463" s="5" t="e">
-        <f>G463+$J$416</f>
-        <v>#DIV/0!</v>
-      </c>
     </row>
     <row r="464" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C464" s="10" t="s">
@@ -13873,6 +13873,18 @@
       <c r="F464" s="16" t="s">
         <v>413</v>
       </c>
+      <c r="G464" s="13" t="e">
+        <f>AVERAGE(E465,E466)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H464" s="18" t="e">
+        <f>STDEV(E465,E466)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K464" s="5" t="e">
+        <f>G464+$J$416</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="465" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C465" s="10" t="s">
@@ -13889,18 +13901,6 @@
       <c r="F466" s="16" t="s">
         <v>415</v>
       </c>
-      <c r="G466" s="13" t="e">
-        <f>AVERAGE(E467,E468)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H466" s="18" t="e">
-        <f>STDEV(E467,E468)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K466" s="5" t="e">
-        <f>G466+$J$416</f>
-        <v>#DIV/0!</v>
-      </c>
     </row>
     <row r="467" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C467" s="10" t="s">
@@ -13909,6 +13909,18 @@
       <c r="F467" s="16" t="s">
         <v>416</v>
       </c>
+      <c r="G467" s="13" t="e">
+        <f>AVERAGE(E468,E469)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H467" s="18" t="e">
+        <f>STDEV(E468,E469)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K467" s="5" t="e">
+        <f>G467+$J$416</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="468" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C468" s="10" t="s">
@@ -13925,18 +13937,6 @@
       <c r="F469" s="16" t="s">
         <v>418</v>
       </c>
-      <c r="G469" s="13" t="e">
-        <f>AVERAGE(E470,E471)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H469" s="18" t="e">
-        <f>STDEV(E470,E471)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K469" s="5" t="e">
-        <f>G469+$J$416</f>
-        <v>#DIV/0!</v>
-      </c>
     </row>
     <row r="470" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C470" s="10" t="s">
@@ -13945,6 +13945,18 @@
       <c r="F470" s="16" t="s">
         <v>419</v>
       </c>
+      <c r="G470" s="13" t="e">
+        <f>AVERAGE(E471,E472)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H470" s="18" t="e">
+        <f>STDEV(E471,E472)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K470" s="5" t="e">
+        <f>G470+$J$416</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="471" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C471" s="10" t="s">
@@ -13961,45 +13973,33 @@
       <c r="F472" s="16" t="s">
         <v>421</v>
       </c>
-      <c r="G472" s="13" t="e">
-        <f>AVERAGE(E473,E474)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H472" s="18" t="e">
-        <f>STDEV(E473,E474)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K472" s="5" t="e">
-        <f>G472+$J$416</f>
-        <v>#DIV/0!</v>
-      </c>
     </row>
     <row r="473" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C473" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F473" s="16" t="s">
-        <v>422</v>
-      </c>
+      <c r="C473" s="10"/>
+      <c r="F473" s="16"/>
     </row>
     <row r="474" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C474" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F474" s="16" t="s">
-        <v>423</v>
+        <v>8</v>
       </c>
     </row>
     <row r="475" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C475" s="10"/>
-      <c r="F475" s="16"/>
+      <c r="C475" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F475" s="16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="476" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C476" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F476" s="16" t="s">
-        <v>8</v>
+        <v>96</v>
       </c>
     </row>
     <row r="477" spans="3:11" x14ac:dyDescent="0.2">
@@ -14007,7 +14007,7 @@
         <v>12</v>
       </c>
       <c r="F477" s="16" t="s">
-        <v>9</v>
+        <v>476</v>
       </c>
     </row>
     <row r="478" spans="3:11" x14ac:dyDescent="0.2">
@@ -14015,7 +14015,7 @@
         <v>12</v>
       </c>
       <c r="F478" s="16" t="s">
-        <v>96</v>
+        <v>477</v>
       </c>
     </row>
     <row r="479" spans="3:11" x14ac:dyDescent="0.2">
@@ -14055,7 +14055,7 @@
         <v>12</v>
       </c>
       <c r="F483" s="16" t="s">
-        <v>482</v>
+        <v>422</v>
       </c>
     </row>
     <row r="484" spans="3:6" x14ac:dyDescent="0.2">
@@ -14063,7 +14063,7 @@
         <v>12</v>
       </c>
       <c r="F484" s="16" t="s">
-        <v>483</v>
+        <v>423</v>
       </c>
     </row>
     <row r="485" spans="3:6" x14ac:dyDescent="0.2">
@@ -14242,20 +14242,20 @@
         <v>445</v>
       </c>
     </row>
-    <row r="507" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C507" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F507" s="16" t="s">
-        <v>446</v>
-      </c>
-    </row>
     <row r="508" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C508" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F508" s="16" t="s">
-        <v>447</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="509" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C509" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F509" s="16" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="510" spans="3:6" x14ac:dyDescent="0.2">
@@ -14263,7 +14263,7 @@
         <v>12</v>
       </c>
       <c r="F510" s="16" t="s">
-        <v>8</v>
+        <v>96</v>
       </c>
     </row>
     <row r="511" spans="3:6" x14ac:dyDescent="0.2">
@@ -14271,7 +14271,7 @@
         <v>12</v>
       </c>
       <c r="F511" s="16" t="s">
-        <v>9</v>
+        <v>482</v>
       </c>
     </row>
     <row r="512" spans="3:6" x14ac:dyDescent="0.2">
@@ -14279,7 +14279,7 @@
         <v>12</v>
       </c>
       <c r="F512" s="16" t="s">
-        <v>96</v>
+        <v>483</v>
       </c>
     </row>
     <row r="513" spans="3:6" x14ac:dyDescent="0.2">
@@ -14319,7 +14319,7 @@
         <v>12</v>
       </c>
       <c r="F517" s="16" t="s">
-        <v>488</v>
+        <v>446</v>
       </c>
     </row>
     <row r="518" spans="3:6" x14ac:dyDescent="0.2">
@@ -14327,7 +14327,7 @@
         <v>12</v>
       </c>
       <c r="F518" s="16" t="s">
-        <v>489</v>
+        <v>447</v>
       </c>
     </row>
     <row r="519" spans="3:6" x14ac:dyDescent="0.2">
@@ -14506,20 +14506,20 @@
         <v>469</v>
       </c>
     </row>
-    <row r="541" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C541" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F541" s="16" t="s">
-        <v>470</v>
-      </c>
-    </row>
     <row r="542" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C542" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F542" s="16" t="s">
-        <v>471</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="543" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C543" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F543" s="16" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="544" spans="3:6" x14ac:dyDescent="0.2">
@@ -14527,7 +14527,7 @@
         <v>12</v>
       </c>
       <c r="F544" s="16" t="s">
-        <v>8</v>
+        <v>96</v>
       </c>
     </row>
     <row r="545" spans="3:6" x14ac:dyDescent="0.2">
@@ -14535,7 +14535,7 @@
         <v>12</v>
       </c>
       <c r="F545" s="16" t="s">
-        <v>9</v>
+        <v>488</v>
       </c>
     </row>
     <row r="546" spans="3:6" x14ac:dyDescent="0.2">
@@ -14543,7 +14543,7 @@
         <v>12</v>
       </c>
       <c r="F546" s="16" t="s">
-        <v>96</v>
+        <v>489</v>
       </c>
     </row>
     <row r="547" spans="3:6" x14ac:dyDescent="0.2">
@@ -14771,30 +14771,30 @@
       </c>
     </row>
     <row r="575" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C575" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F575" s="16" t="s">
-        <v>518</v>
-      </c>
+      <c r="F575" s="16"/>
     </row>
     <row r="576" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C576" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F576" s="16" t="s">
-        <v>519</v>
+        <v>8</v>
       </c>
     </row>
     <row r="577" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="F577" s="16"/>
+      <c r="C577" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F577" s="16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="578" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C578" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F578" s="16" t="s">
-        <v>8</v>
+        <v>96</v>
       </c>
     </row>
     <row r="579" spans="3:6" x14ac:dyDescent="0.2">
@@ -14802,7 +14802,7 @@
         <v>12</v>
       </c>
       <c r="F579" s="16" t="s">
-        <v>9</v>
+        <v>518</v>
       </c>
     </row>
     <row r="580" spans="3:6" x14ac:dyDescent="0.2">
@@ -14810,7 +14810,7 @@
         <v>12</v>
       </c>
       <c r="F580" s="16" t="s">
-        <v>96</v>
+        <v>519</v>
       </c>
     </row>
     <row r="581" spans="3:6" x14ac:dyDescent="0.2">
@@ -15037,20 +15037,20 @@
         <v>547</v>
       </c>
     </row>
-    <row r="609" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C609" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F609" s="16" t="s">
-        <v>548</v>
-      </c>
-    </row>
     <row r="610" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C610" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F610" s="16" t="s">
-        <v>549</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="611" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C611" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F611" s="16" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="612" spans="3:6" x14ac:dyDescent="0.2">
@@ -15058,7 +15058,7 @@
         <v>12</v>
       </c>
       <c r="F612" s="16" t="s">
-        <v>8</v>
+        <v>96</v>
       </c>
     </row>
     <row r="613" spans="3:6" x14ac:dyDescent="0.2">
@@ -15066,7 +15066,7 @@
         <v>12</v>
       </c>
       <c r="F613" s="16" t="s">
-        <v>9</v>
+        <v>548</v>
       </c>
     </row>
     <row r="614" spans="3:6" x14ac:dyDescent="0.2">
@@ -15074,7 +15074,7 @@
         <v>12</v>
       </c>
       <c r="F614" s="16" t="s">
-        <v>96</v>
+        <v>549</v>
       </c>
     </row>
     <row r="615" spans="3:6" x14ac:dyDescent="0.2">
@@ -15299,22 +15299,6 @@
       </c>
       <c r="F642" s="16" t="s">
         <v>577</v>
-      </c>
-    </row>
-    <row r="643" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C643" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F643" s="16" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="644" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C644" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F644" s="16" t="s">
-        <v>579</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Alice ELOW ALK 100%
</commit_message>
<xml_diff>
--- a/Data/Spring_2023/BenthFun_Alkalinity.xlsx
+++ b/Data/Spring_2023/BenthFun_Alkalinity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremy/Library/Mobile Documents/com~apple~CloudDocs/Documents/Documents/Post-Doc/Projets/Villefranche/Projets/BenthFun – Jeremy/BenthFun/Data/Spring_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7DC91F-4C92-0740-85B3-B453A66A543D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD89542-41E5-B34F-AA33-854F93F8A6B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1819" uniqueCount="580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1841" uniqueCount="580">
   <si>
     <t>Operator</t>
   </si>
@@ -2261,8 +2261,8 @@
   <dimension ref="A1:L642"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="73" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A435" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G451" sqref="G451"/>
+      <pane ySplit="1" topLeftCell="A430" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N464" sqref="N464"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13759,6 +13759,12 @@
       </c>
     </row>
     <row r="455" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A455" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B455" s="31">
+        <v>45091</v>
+      </c>
       <c r="C455" s="10" t="s">
         <v>12</v>
       </c>
@@ -13774,11 +13780,17 @@
         <v>#DIV/0!</v>
       </c>
       <c r="K455" s="5" t="e">
-        <f>G455+$J$416</f>
+        <f>G455+$J$474</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="456" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A456" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B456" s="31">
+        <v>45091</v>
+      </c>
       <c r="C456" s="10" t="s">
         <v>12</v>
       </c>
@@ -13787,6 +13799,12 @@
       </c>
     </row>
     <row r="457" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A457" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B457" s="31">
+        <v>45091</v>
+      </c>
       <c r="C457" s="10" t="s">
         <v>12</v>
       </c>
@@ -13795,6 +13813,12 @@
       </c>
     </row>
     <row r="458" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A458" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B458" s="31">
+        <v>45091</v>
+      </c>
       <c r="C458" s="10" t="s">
         <v>12</v>
       </c>
@@ -13810,11 +13834,17 @@
         <v>#DIV/0!</v>
       </c>
       <c r="K458" s="5" t="e">
-        <f>G458+$J$416</f>
+        <f>G458+$J$474</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="459" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A459" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B459" s="31">
+        <v>45091</v>
+      </c>
       <c r="C459" s="10" t="s">
         <v>12</v>
       </c>
@@ -13823,6 +13853,12 @@
       </c>
     </row>
     <row r="460" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A460" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B460" s="31">
+        <v>45091</v>
+      </c>
       <c r="C460" s="10" t="s">
         <v>12</v>
       </c>
@@ -13831,6 +13867,12 @@
       </c>
     </row>
     <row r="461" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A461" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B461" s="31">
+        <v>45091</v>
+      </c>
       <c r="C461" s="10" t="s">
         <v>12</v>
       </c>
@@ -13846,11 +13888,17 @@
         <v>#DIV/0!</v>
       </c>
       <c r="K461" s="5" t="e">
-        <f>G461+$J$416</f>
+        <f>G461+$J$474</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="462" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A462" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B462" s="31">
+        <v>45091</v>
+      </c>
       <c r="C462" s="10" t="s">
         <v>12</v>
       </c>
@@ -13859,6 +13907,12 @@
       </c>
     </row>
     <row r="463" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A463" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B463" s="31">
+        <v>45091</v>
+      </c>
       <c r="C463" s="10" t="s">
         <v>12</v>
       </c>
@@ -13867,6 +13921,12 @@
       </c>
     </row>
     <row r="464" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A464" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B464" s="31">
+        <v>45091</v>
+      </c>
       <c r="C464" s="10" t="s">
         <v>12</v>
       </c>
@@ -13882,11 +13942,17 @@
         <v>#DIV/0!</v>
       </c>
       <c r="K464" s="5" t="e">
-        <f>G464+$J$416</f>
+        <f>G464+$J$474</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="465" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="465" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A465" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B465" s="31">
+        <v>45091</v>
+      </c>
       <c r="C465" s="10" t="s">
         <v>12</v>
       </c>
@@ -13894,7 +13960,13 @@
         <v>414</v>
       </c>
     </row>
-    <row r="466" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="466" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A466" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B466" s="31">
+        <v>45091</v>
+      </c>
       <c r="C466" s="10" t="s">
         <v>12</v>
       </c>
@@ -13902,7 +13974,13 @@
         <v>415</v>
       </c>
     </row>
-    <row r="467" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="467" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A467" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B467" s="31">
+        <v>45091</v>
+      </c>
       <c r="C467" s="10" t="s">
         <v>12</v>
       </c>
@@ -13918,11 +13996,17 @@
         <v>#DIV/0!</v>
       </c>
       <c r="K467" s="5" t="e">
-        <f>G467+$J$416</f>
+        <f>G467+$J$474</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="468" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="468" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A468" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B468" s="31">
+        <v>45091</v>
+      </c>
       <c r="C468" s="10" t="s">
         <v>12</v>
       </c>
@@ -13930,7 +14014,13 @@
         <v>417</v>
       </c>
     </row>
-    <row r="469" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="469" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A469" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B469" s="31">
+        <v>45091</v>
+      </c>
       <c r="C469" s="10" t="s">
         <v>12</v>
       </c>
@@ -13938,7 +14028,13 @@
         <v>418</v>
       </c>
     </row>
-    <row r="470" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="470" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A470" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B470" s="31">
+        <v>45091</v>
+      </c>
       <c r="C470" s="10" t="s">
         <v>12</v>
       </c>
@@ -13954,11 +14050,17 @@
         <v>#DIV/0!</v>
       </c>
       <c r="K470" s="5" t="e">
-        <f>G470+$J$416</f>
+        <f>G470+$J$474</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="471" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="471" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A471" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B471" s="31">
+        <v>45091</v>
+      </c>
       <c r="C471" s="10" t="s">
         <v>12</v>
       </c>
@@ -13966,7 +14068,13 @@
         <v>420</v>
       </c>
     </row>
-    <row r="472" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="472" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A472" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B472" s="31">
+        <v>45091</v>
+      </c>
       <c r="C472" s="10" t="s">
         <v>12</v>
       </c>
@@ -13974,19 +14082,53 @@
         <v>421</v>
       </c>
     </row>
-    <row r="473" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="473" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C473" s="10"/>
       <c r="F473" s="16"/>
     </row>
-    <row r="474" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="474" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A474" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B474" s="31">
+        <v>45091</v>
+      </c>
       <c r="C474" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F474" s="16" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="475" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="G474" s="13" t="e">
+        <f>AVERAGE(E475,E476)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H474" s="18" t="e">
+        <f>STDEV(E475,E476)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I474" s="3">
+        <v>2226.44</v>
+      </c>
+      <c r="J474" s="4" t="e">
+        <f>I474-G474</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K474" s="5" t="e">
+        <f>G474+J474</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L474" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="475" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A475" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B475" s="31">
+        <v>45091</v>
+      </c>
       <c r="C475" s="10" t="s">
         <v>12</v>
       </c>
@@ -13994,7 +14136,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="476" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="476" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A476" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B476" s="31">
+        <v>45091</v>
+      </c>
       <c r="C476" s="10" t="s">
         <v>12</v>
       </c>
@@ -14002,7 +14150,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="477" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="477" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C477" s="10" t="s">
         <v>12</v>
       </c>
@@ -14010,7 +14158,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="478" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="478" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C478" s="10" t="s">
         <v>12</v>
       </c>
@@ -14018,7 +14166,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="479" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="479" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C479" s="10" t="s">
         <v>12</v>
       </c>
@@ -14026,7 +14174,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="480" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="480" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C480" s="10" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
LOW 60% Historic Jerem
</commit_message>
<xml_diff>
--- a/Data/Spring_2023/BenthFun_Alkalinity.xlsx
+++ b/Data/Spring_2023/BenthFun_Alkalinity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremy/Library/Mobile Documents/com~apple~CloudDocs/Documents/Documents/Post-Doc/Projets/Villefranche/Projets/BenthFun – Jeremy/BenthFun/Data/Spring_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1AB45CC-4308-8640-B021-6F4A6491D029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF810D2E-C701-004C-8273-FC81E93EFE0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1840" uniqueCount="580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1846" uniqueCount="576">
   <si>
     <t>Operator</t>
   </si>
@@ -1318,18 +1318,12 @@
     <t>Tn_t1_LOW_tile_02b</t>
   </si>
   <si>
-    <t>Tn_t1_LOW_tile_02c</t>
-  </si>
-  <si>
     <t>Tn_t1_LOW_tile_03a</t>
   </si>
   <si>
     <t>Tn_t1_LOW_tile_03b</t>
   </si>
   <si>
-    <t>Tn_t1_LOW_tile_03c</t>
-  </si>
-  <si>
     <t>Tn_t1_LOW_blank_01a</t>
   </si>
   <si>
@@ -1471,16 +1465,10 @@
     <t>Tn_t0_LOW_blank_01b</t>
   </si>
   <si>
-    <t>Tn_t0_LOW_blank_01c</t>
-  </si>
-  <si>
     <t>Tn_t0_LOW_blank_02a</t>
   </si>
   <si>
     <t>Tn_t0_LOW_blank_02b</t>
-  </si>
-  <si>
-    <t>Tn_t0_LOW_blank_02c</t>
   </si>
   <si>
     <t>Tn_t0_AMB_blank_01a</t>
@@ -2258,11 +2246,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L641"/>
+  <dimension ref="A1:L637"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="73" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A446" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G453" sqref="G453"/>
+      <pane ySplit="1" topLeftCell="A471" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H488" sqref="H488"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13030,7 +13018,7 @@
         <v>2468.38</v>
       </c>
       <c r="F424" s="32" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
     </row>
     <row r="425" spans="1:11" x14ac:dyDescent="0.2">
@@ -13226,7 +13214,7 @@
         <v>2530.84</v>
       </c>
       <c r="F432" s="32" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
     </row>
     <row r="433" spans="1:12" x14ac:dyDescent="0.2">
@@ -13524,7 +13512,7 @@
         <v>2797.88</v>
       </c>
       <c r="F444" s="16" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="G444" s="13">
         <f>AVERAGE(E444,E446)</f>
@@ -13556,7 +13544,7 @@
         <v>2892.7</v>
       </c>
       <c r="F445" s="16" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="446" spans="1:12" x14ac:dyDescent="0.2">
@@ -13576,7 +13564,7 @@
         <v>2791.76</v>
       </c>
       <c r="F446" s="16" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="447" spans="1:12" x14ac:dyDescent="0.2">
@@ -13596,7 +13584,7 @@
         <v>2776.09</v>
       </c>
       <c r="F447" s="16" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="G447" s="13">
         <f>AVERAGE(E448,E449)</f>
@@ -13628,7 +13616,7 @@
         <v>2789.47</v>
       </c>
       <c r="F448" s="16" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="449" spans="1:11" x14ac:dyDescent="0.2">
@@ -13648,7 +13636,7 @@
         <v>2795.12</v>
       </c>
       <c r="F449" s="16" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="450" spans="1:11" x14ac:dyDescent="0.2">
@@ -13784,7 +13772,7 @@
       </c>
       <c r="K454" s="5">
         <f>G454+$J$473</f>
-        <v>2758.4116666666669</v>
+        <v>2756.6450000000004</v>
       </c>
     </row>
     <row r="455" spans="1:11" x14ac:dyDescent="0.2">
@@ -13856,7 +13844,7 @@
       </c>
       <c r="K457" s="5">
         <f>G457+$J$473</f>
-        <v>2788.416666666667</v>
+        <v>2786.6500000000005</v>
       </c>
     </row>
     <row r="458" spans="1:11" x14ac:dyDescent="0.2">
@@ -13928,7 +13916,7 @@
       </c>
       <c r="K460" s="5">
         <f>G460+$J$473</f>
-        <v>2809.3116666666665</v>
+        <v>2807.5450000000001</v>
       </c>
     </row>
     <row r="461" spans="1:11" x14ac:dyDescent="0.2">
@@ -14000,7 +13988,7 @@
       </c>
       <c r="K463" s="5">
         <f>G463+$J$473</f>
-        <v>2827.6233333333334</v>
+        <v>2825.856666666667</v>
       </c>
     </row>
     <row r="464" spans="1:11" x14ac:dyDescent="0.2">
@@ -14072,7 +14060,7 @@
       </c>
       <c r="K466" s="5">
         <f>G466+$J$473</f>
-        <v>2810.9866666666667</v>
+        <v>2809.2200000000003</v>
       </c>
     </row>
     <row r="467" spans="1:11" x14ac:dyDescent="0.2">
@@ -14144,7 +14132,7 @@
       </c>
       <c r="K469" s="5">
         <f>G469+$J$473</f>
-        <v>2789.7716666666665</v>
+        <v>2788.0050000000001</v>
       </c>
     </row>
     <row r="470" spans="1:11" x14ac:dyDescent="0.2">
@@ -14211,19 +14199,19 @@
         <v>8</v>
       </c>
       <c r="G473" s="13">
-        <f>AVERAGE(E473,E474,E475)</f>
-        <v>2233.8733333333334</v>
+        <f>AVERAGE(E473,E475)</f>
+        <v>2235.64</v>
       </c>
       <c r="H473" s="18">
-        <f>STDEV(E473,E474,E475)</f>
-        <v>3.2689192913457772</v>
+        <f>STDEV(E473,E475)</f>
+        <v>1.626345596729188</v>
       </c>
       <c r="I473" s="3">
         <v>2226.44</v>
       </c>
       <c r="J473" s="4">
         <f>I473-G473</f>
-        <v>-7.433333333333394</v>
+        <v>-9.1999999999998181</v>
       </c>
       <c r="K473" s="5">
         <f>G473+J473</f>
@@ -14271,171 +14259,411 @@
       </c>
     </row>
     <row r="476" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A476" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B476" s="31">
+        <v>45091</v>
+      </c>
       <c r="C476" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D476" s="5">
+        <v>50.54</v>
+      </c>
+      <c r="E476" s="5">
+        <v>2724.69</v>
+      </c>
       <c r="F476" s="16" t="s">
+        <v>474</v>
+      </c>
+      <c r="G476" s="13">
+        <f>AVERAGE(E476:E477)</f>
+        <v>2723.1849999999999</v>
+      </c>
+      <c r="H476" s="18">
+        <f>STDEV(E476,E477)</f>
+        <v>2.1283914113716627</v>
+      </c>
+      <c r="K476" s="5">
+        <f>G476+$J$473</f>
+        <v>2713.9850000000001</v>
+      </c>
+    </row>
+    <row r="477" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A477" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B477" s="31">
+        <v>45091</v>
+      </c>
+      <c r="C477" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D477" s="5">
+        <v>48.78</v>
+      </c>
+      <c r="E477" s="5">
+        <v>2721.68</v>
+      </c>
+      <c r="F477" s="16" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="478" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A478" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B478" s="31">
+        <v>45091</v>
+      </c>
+      <c r="C478" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D478" s="5">
+        <v>49.21</v>
+      </c>
+      <c r="E478" s="5">
+        <v>2703.56</v>
+      </c>
+      <c r="F478" s="16" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="477" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C477" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F477" s="16" t="s">
+      <c r="G478" s="13">
+        <f>AVERAGE(E478,E480)</f>
+        <v>2680.0749999999998</v>
+      </c>
+      <c r="H478" s="18">
+        <f>STDEV(E478,E479)</f>
+        <v>4.0305086527631921</v>
+      </c>
+      <c r="K478" s="5">
+        <f>G478+$J$473</f>
+        <v>2670.875</v>
+      </c>
+    </row>
+    <row r="479" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A479" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B479" s="31">
+        <v>45091</v>
+      </c>
+      <c r="C479" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D479" s="5">
+        <v>49.8</v>
+      </c>
+      <c r="E479" s="5">
+        <v>2697.86</v>
+      </c>
+      <c r="F479" s="16" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="478" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C478" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F478" s="16" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="479" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C479" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F479" s="16" t="s">
-        <v>479</v>
-      </c>
-    </row>
     <row r="480" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A480" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B480" s="31">
+        <v>45091</v>
+      </c>
       <c r="C480" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D480" s="5">
+        <v>51.62</v>
+      </c>
+      <c r="E480" s="14">
+        <v>2656.59</v>
+      </c>
       <c r="F480" s="16" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="481" spans="3:6" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+      <c r="G480" s="13">
+        <f>AVERAGE(E481,E482)</f>
+        <v>2647.81</v>
+      </c>
+      <c r="H480" s="18">
+        <f>STDEV(E481,E482)</f>
+        <v>0.82024386617629219</v>
+      </c>
+      <c r="K480" s="5">
+        <f>G480+$J$473</f>
+        <v>2638.61</v>
+      </c>
+    </row>
+    <row r="481" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A481" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B481" s="31">
+        <v>45091</v>
+      </c>
       <c r="C481" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D481" s="5">
+        <v>49.21</v>
+      </c>
+      <c r="E481" s="5">
+        <v>2647.23</v>
+      </c>
       <c r="F481" s="16" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="482" spans="3:6" x14ac:dyDescent="0.2">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="482" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A482" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B482" s="31">
+        <v>45091</v>
+      </c>
       <c r="C482" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D482" s="5">
+        <v>48.69</v>
+      </c>
+      <c r="E482" s="5">
+        <v>2648.39</v>
+      </c>
       <c r="F482" s="16" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="483" spans="3:6" x14ac:dyDescent="0.2">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="483" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A483" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B483" s="31">
+        <v>45091</v>
+      </c>
       <c r="C483" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D483" s="5">
+        <v>51.12</v>
+      </c>
+      <c r="E483" s="5">
+        <v>2656.91</v>
+      </c>
       <c r="F483" s="16" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="484" spans="3:6" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G483" s="13">
+        <f>AVERAGE(E483,E484)</f>
+        <v>2656.1099999999997</v>
+      </c>
+      <c r="H483" s="18">
+        <f>STDEV(E483,E484)</f>
+        <v>1.1313708498984119</v>
+      </c>
+      <c r="K483" s="5">
+        <f>G483+$J$473</f>
+        <v>2646.91</v>
+      </c>
+    </row>
+    <row r="484" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A484" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B484" s="31">
+        <v>45091</v>
+      </c>
       <c r="C484" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D484" s="5">
+        <v>51.4</v>
+      </c>
+      <c r="E484" s="5">
+        <v>2655.31</v>
+      </c>
       <c r="F484" s="16" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="485" spans="3:6" x14ac:dyDescent="0.2">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="485" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A485" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B485" s="31">
+        <v>45091</v>
+      </c>
       <c r="C485" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D485" s="5">
+        <v>49.41</v>
+      </c>
+      <c r="E485" s="5">
+        <v>2684.74</v>
+      </c>
       <c r="F485" s="16" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="486" spans="3:6" x14ac:dyDescent="0.2">
+        <v>427</v>
+      </c>
+      <c r="G485" s="13">
+        <f>AVERAGE(E485,E486)</f>
+        <v>2684.2649999999999</v>
+      </c>
+      <c r="H485" s="18">
+        <f>STDEV(E485,E486)</f>
+        <v>0.67175144212709148</v>
+      </c>
+      <c r="K485" s="5">
+        <f>G485+$J$473</f>
+        <v>2675.0650000000001</v>
+      </c>
+    </row>
+    <row r="486" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A486" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B486" s="31">
+        <v>45091</v>
+      </c>
       <c r="C486" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D486" s="5">
+        <v>49.72</v>
+      </c>
+      <c r="E486" s="5">
+        <v>2683.79</v>
+      </c>
       <c r="F486" s="16" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="487" spans="3:6" x14ac:dyDescent="0.2">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="487" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A487" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B487" s="31">
+        <v>45091</v>
+      </c>
       <c r="C487" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D487" s="5">
+        <v>50.83</v>
+      </c>
+      <c r="E487" s="14">
+        <v>2735.14</v>
+      </c>
       <c r="F487" s="16" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="488" spans="3:6" x14ac:dyDescent="0.2">
+        <v>429</v>
+      </c>
+      <c r="G487" s="13">
+        <f>AVERAGE(E487,E488)</f>
+        <v>2729.2150000000001</v>
+      </c>
+      <c r="H487" s="18">
+        <f>STDEV(E487,E488)</f>
+        <v>8.3792153570605237</v>
+      </c>
+      <c r="K487" s="5">
+        <f>G487+$J$473</f>
+        <v>2720.0150000000003</v>
+      </c>
+    </row>
+    <row r="488" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A488" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B488" s="31">
+        <v>45091</v>
+      </c>
       <c r="C488" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D488" s="5">
+        <v>48.96</v>
+      </c>
+      <c r="E488" s="5">
+        <v>2723.29</v>
+      </c>
       <c r="F488" s="16" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="489" spans="3:6" x14ac:dyDescent="0.2">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="489" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A489" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B489" s="31">
+        <v>45091</v>
+      </c>
       <c r="C489" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D489" s="5">
+        <v>50.39</v>
+      </c>
+      <c r="E489" s="14">
+        <v>2558.9699999999998</v>
+      </c>
       <c r="F489" s="16" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="490" spans="3:6" x14ac:dyDescent="0.2">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="490" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C490" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F490" s="16" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="491" spans="3:6" x14ac:dyDescent="0.2">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="491" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C491" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F491" s="16" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="492" spans="3:6" x14ac:dyDescent="0.2">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="492" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C492" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F492" s="16" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="493" spans="3:6" x14ac:dyDescent="0.2">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="493" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C493" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F493" s="16" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="494" spans="3:6" x14ac:dyDescent="0.2">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="494" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C494" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F494" s="16" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="495" spans="3:6" x14ac:dyDescent="0.2">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="495" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C495" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F495" s="16" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="496" spans="3:6" x14ac:dyDescent="0.2">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="496" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C496" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F496" s="16" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
     </row>
     <row r="497" spans="3:6" x14ac:dyDescent="0.2">
@@ -14443,7 +14671,7 @@
         <v>12</v>
       </c>
       <c r="F497" s="16" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
     </row>
     <row r="498" spans="3:6" x14ac:dyDescent="0.2">
@@ -14451,7 +14679,7 @@
         <v>12</v>
       </c>
       <c r="F498" s="16" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
     </row>
     <row r="499" spans="3:6" x14ac:dyDescent="0.2">
@@ -14459,7 +14687,7 @@
         <v>12</v>
       </c>
       <c r="F499" s="16" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
     </row>
     <row r="500" spans="3:6" x14ac:dyDescent="0.2">
@@ -14467,7 +14695,7 @@
         <v>12</v>
       </c>
       <c r="F500" s="16" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="501" spans="3:6" x14ac:dyDescent="0.2">
@@ -14475,15 +14703,7 @@
         <v>12</v>
       </c>
       <c r="F501" s="16" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="502" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C502" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F502" s="16" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="503" spans="3:6" x14ac:dyDescent="0.2">
@@ -14491,7 +14711,7 @@
         <v>12</v>
       </c>
       <c r="F503" s="16" t="s">
-        <v>443</v>
+        <v>8</v>
       </c>
     </row>
     <row r="504" spans="3:6" x14ac:dyDescent="0.2">
@@ -14499,7 +14719,7 @@
         <v>12</v>
       </c>
       <c r="F504" s="16" t="s">
-        <v>444</v>
+        <v>9</v>
       </c>
     </row>
     <row r="505" spans="3:6" x14ac:dyDescent="0.2">
@@ -14507,7 +14727,15 @@
         <v>12</v>
       </c>
       <c r="F505" s="16" t="s">
-        <v>445</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="506" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C506" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F506" s="16" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="507" spans="3:6" x14ac:dyDescent="0.2">
@@ -14515,7 +14743,7 @@
         <v>12</v>
       </c>
       <c r="F507" s="16" t="s">
-        <v>8</v>
+        <v>479</v>
       </c>
     </row>
     <row r="508" spans="3:6" x14ac:dyDescent="0.2">
@@ -14523,7 +14751,7 @@
         <v>12</v>
       </c>
       <c r="F508" s="16" t="s">
-        <v>9</v>
+        <v>480</v>
       </c>
     </row>
     <row r="509" spans="3:6" x14ac:dyDescent="0.2">
@@ -14531,7 +14759,7 @@
         <v>12</v>
       </c>
       <c r="F509" s="16" t="s">
-        <v>96</v>
+        <v>481</v>
       </c>
     </row>
     <row r="510" spans="3:6" x14ac:dyDescent="0.2">
@@ -14555,7 +14783,7 @@
         <v>12</v>
       </c>
       <c r="F512" s="16" t="s">
-        <v>484</v>
+        <v>444</v>
       </c>
     </row>
     <row r="513" spans="3:6" x14ac:dyDescent="0.2">
@@ -14563,7 +14791,7 @@
         <v>12</v>
       </c>
       <c r="F513" s="16" t="s">
-        <v>485</v>
+        <v>445</v>
       </c>
     </row>
     <row r="514" spans="3:6" x14ac:dyDescent="0.2">
@@ -14571,7 +14799,7 @@
         <v>12</v>
       </c>
       <c r="F514" s="16" t="s">
-        <v>486</v>
+        <v>446</v>
       </c>
     </row>
     <row r="515" spans="3:6" x14ac:dyDescent="0.2">
@@ -14579,7 +14807,7 @@
         <v>12</v>
       </c>
       <c r="F515" s="16" t="s">
-        <v>487</v>
+        <v>447</v>
       </c>
     </row>
     <row r="516" spans="3:6" x14ac:dyDescent="0.2">
@@ -14587,7 +14815,7 @@
         <v>12</v>
       </c>
       <c r="F516" s="16" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
     </row>
     <row r="517" spans="3:6" x14ac:dyDescent="0.2">
@@ -14595,7 +14823,7 @@
         <v>12</v>
       </c>
       <c r="F517" s="16" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
     </row>
     <row r="518" spans="3:6" x14ac:dyDescent="0.2">
@@ -14603,7 +14831,7 @@
         <v>12</v>
       </c>
       <c r="F518" s="16" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
     </row>
     <row r="519" spans="3:6" x14ac:dyDescent="0.2">
@@ -14611,7 +14839,7 @@
         <v>12</v>
       </c>
       <c r="F519" s="16" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
     </row>
     <row r="520" spans="3:6" x14ac:dyDescent="0.2">
@@ -14619,7 +14847,7 @@
         <v>12</v>
       </c>
       <c r="F520" s="16" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
     </row>
     <row r="521" spans="3:6" x14ac:dyDescent="0.2">
@@ -14627,7 +14855,7 @@
         <v>12</v>
       </c>
       <c r="F521" s="16" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
     </row>
     <row r="522" spans="3:6" x14ac:dyDescent="0.2">
@@ -14635,7 +14863,7 @@
         <v>12</v>
       </c>
       <c r="F522" s="16" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
     </row>
     <row r="523" spans="3:6" x14ac:dyDescent="0.2">
@@ -14643,7 +14871,7 @@
         <v>12</v>
       </c>
       <c r="F523" s="16" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
     </row>
     <row r="524" spans="3:6" x14ac:dyDescent="0.2">
@@ -14651,7 +14879,7 @@
         <v>12</v>
       </c>
       <c r="F524" s="16" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
     </row>
     <row r="525" spans="3:6" x14ac:dyDescent="0.2">
@@ -14659,7 +14887,7 @@
         <v>12</v>
       </c>
       <c r="F525" s="16" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
     </row>
     <row r="526" spans="3:6" x14ac:dyDescent="0.2">
@@ -14667,7 +14895,7 @@
         <v>12</v>
       </c>
       <c r="F526" s="16" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
     </row>
     <row r="527" spans="3:6" x14ac:dyDescent="0.2">
@@ -14675,7 +14903,7 @@
         <v>12</v>
       </c>
       <c r="F527" s="16" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="528" spans="3:6" x14ac:dyDescent="0.2">
@@ -14683,7 +14911,7 @@
         <v>12</v>
       </c>
       <c r="F528" s="16" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
     </row>
     <row r="529" spans="3:6" x14ac:dyDescent="0.2">
@@ -14691,7 +14919,7 @@
         <v>12</v>
       </c>
       <c r="F529" s="16" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
     </row>
     <row r="530" spans="3:6" x14ac:dyDescent="0.2">
@@ -14699,7 +14927,7 @@
         <v>12</v>
       </c>
       <c r="F530" s="16" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
     </row>
     <row r="531" spans="3:6" x14ac:dyDescent="0.2">
@@ -14707,7 +14935,7 @@
         <v>12</v>
       </c>
       <c r="F531" s="16" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
     </row>
     <row r="532" spans="3:6" x14ac:dyDescent="0.2">
@@ -14715,7 +14943,7 @@
         <v>12</v>
       </c>
       <c r="F532" s="16" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
     </row>
     <row r="533" spans="3:6" x14ac:dyDescent="0.2">
@@ -14723,7 +14951,7 @@
         <v>12</v>
       </c>
       <c r="F533" s="16" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
     </row>
     <row r="534" spans="3:6" x14ac:dyDescent="0.2">
@@ -14731,7 +14959,7 @@
         <v>12</v>
       </c>
       <c r="F534" s="16" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
     </row>
     <row r="535" spans="3:6" x14ac:dyDescent="0.2">
@@ -14739,15 +14967,7 @@
         <v>12</v>
       </c>
       <c r="F535" s="16" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="536" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C536" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F536" s="16" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="537" spans="3:6" x14ac:dyDescent="0.2">
@@ -14755,7 +14975,7 @@
         <v>12</v>
       </c>
       <c r="F537" s="16" t="s">
-        <v>467</v>
+        <v>8</v>
       </c>
     </row>
     <row r="538" spans="3:6" x14ac:dyDescent="0.2">
@@ -14763,7 +14983,7 @@
         <v>12</v>
       </c>
       <c r="F538" s="16" t="s">
-        <v>468</v>
+        <v>9</v>
       </c>
     </row>
     <row r="539" spans="3:6" x14ac:dyDescent="0.2">
@@ -14771,7 +14991,15 @@
         <v>12</v>
       </c>
       <c r="F539" s="16" t="s">
-        <v>469</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="540" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C540" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F540" s="16" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="541" spans="3:6" x14ac:dyDescent="0.2">
@@ -14779,7 +15007,7 @@
         <v>12</v>
       </c>
       <c r="F541" s="16" t="s">
-        <v>8</v>
+        <v>485</v>
       </c>
     </row>
     <row r="542" spans="3:6" x14ac:dyDescent="0.2">
@@ -14787,7 +15015,7 @@
         <v>12</v>
       </c>
       <c r="F542" s="16" t="s">
-        <v>9</v>
+        <v>486</v>
       </c>
     </row>
     <row r="543" spans="3:6" x14ac:dyDescent="0.2">
@@ -14795,7 +15023,7 @@
         <v>12</v>
       </c>
       <c r="F543" s="16" t="s">
-        <v>96</v>
+        <v>487</v>
       </c>
     </row>
     <row r="544" spans="3:6" x14ac:dyDescent="0.2">
@@ -15007,19 +15235,14 @@
       </c>
     </row>
     <row r="570" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C570" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F570" s="16" t="s">
-        <v>514</v>
-      </c>
+      <c r="F570" s="16"/>
     </row>
     <row r="571" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C571" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F571" s="16" t="s">
-        <v>515</v>
+        <v>8</v>
       </c>
     </row>
     <row r="572" spans="3:6" x14ac:dyDescent="0.2">
@@ -15027,7 +15250,7 @@
         <v>12</v>
       </c>
       <c r="F572" s="16" t="s">
-        <v>516</v>
+        <v>9</v>
       </c>
     </row>
     <row r="573" spans="3:6" x14ac:dyDescent="0.2">
@@ -15035,18 +15258,23 @@
         <v>12</v>
       </c>
       <c r="F573" s="16" t="s">
-        <v>517</v>
+        <v>96</v>
       </c>
     </row>
     <row r="574" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="F574" s="16"/>
+      <c r="C574" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F574" s="16" t="s">
+        <v>514</v>
+      </c>
     </row>
     <row r="575" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C575" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F575" s="16" t="s">
-        <v>8</v>
+        <v>515</v>
       </c>
     </row>
     <row r="576" spans="3:6" x14ac:dyDescent="0.2">
@@ -15054,7 +15282,7 @@
         <v>12</v>
       </c>
       <c r="F576" s="16" t="s">
-        <v>9</v>
+        <v>516</v>
       </c>
     </row>
     <row r="577" spans="3:6" x14ac:dyDescent="0.2">
@@ -15062,7 +15290,7 @@
         <v>12</v>
       </c>
       <c r="F577" s="16" t="s">
-        <v>96</v>
+        <v>517</v>
       </c>
     </row>
     <row r="578" spans="3:6" x14ac:dyDescent="0.2">
@@ -15273,20 +15501,12 @@
         <v>543</v>
       </c>
     </row>
-    <row r="604" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C604" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F604" s="16" t="s">
-        <v>544</v>
-      </c>
-    </row>
     <row r="605" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C605" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F605" s="16" t="s">
-        <v>545</v>
+        <v>8</v>
       </c>
     </row>
     <row r="606" spans="3:6" x14ac:dyDescent="0.2">
@@ -15294,7 +15514,7 @@
         <v>12</v>
       </c>
       <c r="F606" s="16" t="s">
-        <v>546</v>
+        <v>9</v>
       </c>
     </row>
     <row r="607" spans="3:6" x14ac:dyDescent="0.2">
@@ -15302,7 +15522,15 @@
         <v>12</v>
       </c>
       <c r="F607" s="16" t="s">
-        <v>547</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="608" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C608" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F608" s="16" t="s">
+        <v>544</v>
       </c>
     </row>
     <row r="609" spans="3:6" x14ac:dyDescent="0.2">
@@ -15310,7 +15538,7 @@
         <v>12</v>
       </c>
       <c r="F609" s="16" t="s">
-        <v>8</v>
+        <v>545</v>
       </c>
     </row>
     <row r="610" spans="3:6" x14ac:dyDescent="0.2">
@@ -15318,7 +15546,7 @@
         <v>12</v>
       </c>
       <c r="F610" s="16" t="s">
-        <v>9</v>
+        <v>546</v>
       </c>
     </row>
     <row r="611" spans="3:6" x14ac:dyDescent="0.2">
@@ -15326,7 +15554,7 @@
         <v>12</v>
       </c>
       <c r="F611" s="16" t="s">
-        <v>96</v>
+        <v>547</v>
       </c>
     </row>
     <row r="612" spans="3:6" x14ac:dyDescent="0.2">
@@ -15535,38 +15763,6 @@
       </c>
       <c r="F637" s="16" t="s">
         <v>573</v>
-      </c>
-    </row>
-    <row r="638" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C638" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F638" s="16" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="639" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C639" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F639" s="16" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="640" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C640" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F640" s="16" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="641" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C641" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F641" s="16" t="s">
-        <v>577</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Anto Ali ALK LOW + Exp Amb Jerem + 40% ALK AMB
</commit_message>
<xml_diff>
--- a/Data/Spring_2023/BenthFun_Alkalinity.xlsx
+++ b/Data/Spring_2023/BenthFun_Alkalinity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremy/Library/Mobile Documents/com~apple~CloudDocs/Documents/Documents/Post-Doc/Projets/Villefranche/Projets/BenthFun – Jeremy/BenthFun/Data/Spring_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF810D2E-C701-004C-8273-FC81E93EFE0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163E1137-16C9-8D42-99B2-D3244A48FC05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$502</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1846" uniqueCount="576">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1867" uniqueCount="573">
   <si>
     <t>Operator</t>
   </si>
@@ -1357,36 +1357,24 @@
     <t>Tn_t1_LOW_tile_06b</t>
   </si>
   <si>
-    <t>Tn_t1_LOW_tile_06c</t>
-  </si>
-  <si>
     <t>Tn_t1_LOW_blank_02a</t>
   </si>
   <si>
     <t>Tn_t1_LOW_blank_02b</t>
   </si>
   <si>
-    <t>Tn_t1_LOW_blank_02c</t>
-  </si>
-  <si>
     <t>Tn_t1_AMB_tile_01a</t>
   </si>
   <si>
     <t>Tn_t1_AMB_tile_01b</t>
   </si>
   <si>
-    <t>Tn_t1_AMB_tile_01c</t>
-  </si>
-  <si>
     <t>Tn_t1_AMB_tile_02a</t>
   </si>
   <si>
     <t>Tn_t1_AMB_tile_02b</t>
   </si>
   <si>
-    <t>Tn_t1_AMB_tile_02c</t>
-  </si>
-  <si>
     <t>Tn_t1_AMB_tile_03a</t>
   </si>
   <si>
@@ -1486,9 +1474,6 @@
     <t>Tn_t0_AMB_blank_02b</t>
   </si>
   <si>
-    <t>Tn_t0_AMB_blank_02c</t>
-  </si>
-  <si>
     <t>T2_t0_ELOW_blank_01a</t>
   </si>
   <si>
@@ -1763,6 +1748,12 @@
   </si>
   <si>
     <t>PI_t6_AMB_Tile_3d</t>
+  </si>
+  <si>
+    <t>Ali e Anto</t>
+  </si>
+  <si>
+    <t>Tn_t1_LOW_blank_01d</t>
   </si>
 </sst>
 </file>
@@ -2246,11 +2237,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L637"/>
+  <dimension ref="A1:L634"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="73" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A471" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H488" sqref="H488"/>
+      <pane ySplit="1" topLeftCell="A502" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I521" sqref="I521"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13018,7 +13009,7 @@
         <v>2468.38</v>
       </c>
       <c r="F424" s="32" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
     </row>
     <row r="425" spans="1:11" x14ac:dyDescent="0.2">
@@ -13214,7 +13205,7 @@
         <v>2530.84</v>
       </c>
       <c r="F432" s="32" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
     </row>
     <row r="433" spans="1:12" x14ac:dyDescent="0.2">
@@ -13512,7 +13503,7 @@
         <v>2797.88</v>
       </c>
       <c r="F444" s="16" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="G444" s="13">
         <f>AVERAGE(E444,E446)</f>
@@ -13544,7 +13535,7 @@
         <v>2892.7</v>
       </c>
       <c r="F445" s="16" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
     </row>
     <row r="446" spans="1:12" x14ac:dyDescent="0.2">
@@ -13564,7 +13555,7 @@
         <v>2791.76</v>
       </c>
       <c r="F446" s="16" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
     </row>
     <row r="447" spans="1:12" x14ac:dyDescent="0.2">
@@ -13584,7 +13575,7 @@
         <v>2776.09</v>
       </c>
       <c r="F447" s="16" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="G447" s="13">
         <f>AVERAGE(E448,E449)</f>
@@ -13616,7 +13607,7 @@
         <v>2789.47</v>
       </c>
       <c r="F448" s="16" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
     </row>
     <row r="449" spans="1:11" x14ac:dyDescent="0.2">
@@ -13636,7 +13627,7 @@
         <v>2795.12</v>
       </c>
       <c r="F449" s="16" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
     </row>
     <row r="450" spans="1:11" x14ac:dyDescent="0.2">
@@ -13771,8 +13762,8 @@
         <v>1.8879751057678118</v>
       </c>
       <c r="K454" s="5">
-        <f>G454+$J$473</f>
-        <v>2756.6450000000004</v>
+        <f>G454+$J$472</f>
+        <v>2756.5550000000003</v>
       </c>
     </row>
     <row r="455" spans="1:11" x14ac:dyDescent="0.2">
@@ -13843,8 +13834,8 @@
         <v>4.6103362133362769</v>
       </c>
       <c r="K457" s="5">
-        <f>G457+$J$473</f>
-        <v>2786.6500000000005</v>
+        <f>G457+$J$472</f>
+        <v>2786.5600000000004</v>
       </c>
     </row>
     <row r="458" spans="1:11" x14ac:dyDescent="0.2">
@@ -13915,8 +13906,8 @@
         <v>4.9992449429890069</v>
       </c>
       <c r="K460" s="5">
-        <f>G460+$J$473</f>
-        <v>2807.5450000000001</v>
+        <f>G460+$J$472</f>
+        <v>2807.4549999999999</v>
       </c>
     </row>
     <row r="461" spans="1:11" x14ac:dyDescent="0.2">
@@ -13987,8 +13978,8 @@
         <v>4.4457882690626178</v>
       </c>
       <c r="K463" s="5">
-        <f>G463+$J$473</f>
-        <v>2825.856666666667</v>
+        <f>G463+$J$472</f>
+        <v>2825.7666666666669</v>
       </c>
     </row>
     <row r="464" spans="1:11" x14ac:dyDescent="0.2">
@@ -14059,8 +14050,8 @@
         <v>1.4849242404916856</v>
       </c>
       <c r="K466" s="5">
-        <f>G466+$J$473</f>
-        <v>2809.2200000000003</v>
+        <f>G466+$J$472</f>
+        <v>2809.13</v>
       </c>
     </row>
     <row r="467" spans="1:11" x14ac:dyDescent="0.2">
@@ -14131,8 +14122,8 @@
         <v>1.4778531726799873</v>
       </c>
       <c r="K469" s="5">
-        <f>G469+$J$473</f>
-        <v>2788.0050000000001</v>
+        <f>G469+$J$472</f>
+        <v>2787.915</v>
       </c>
     </row>
     <row r="470" spans="1:11" x14ac:dyDescent="0.2">
@@ -14176,8 +14167,43 @@
       </c>
     </row>
     <row r="472" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C472" s="10"/>
-      <c r="F472" s="16"/>
+      <c r="A472" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B472" s="31">
+        <v>45091</v>
+      </c>
+      <c r="C472" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D472" s="5">
+        <v>54.11</v>
+      </c>
+      <c r="E472" s="5">
+        <v>2234.58</v>
+      </c>
+      <c r="F472" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G472" s="13">
+        <f>AVERAGE(E472,E474)</f>
+        <v>2235.73</v>
+      </c>
+      <c r="H472" s="18">
+        <f>STDEV(E472,E474)</f>
+        <v>1.626345596729188</v>
+      </c>
+      <c r="I472" s="3">
+        <v>2226.44</v>
+      </c>
+      <c r="J472" s="4">
+        <f>I472-G472</f>
+        <v>-9.2899999999999636</v>
+      </c>
+      <c r="K472" s="5">
+        <f>G472+J472</f>
+        <v>2226.44</v>
+      </c>
     </row>
     <row r="473" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A473" s="9" t="s">
@@ -14190,32 +14216,13 @@
         <v>12</v>
       </c>
       <c r="D473" s="5">
-        <v>54.11</v>
+        <v>51.07</v>
       </c>
       <c r="E473" s="5">
-        <v>2234.4899999999998</v>
+        <v>2230.42</v>
       </c>
       <c r="F473" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="G473" s="13">
-        <f>AVERAGE(E473,E475)</f>
-        <v>2235.64</v>
-      </c>
-      <c r="H473" s="18">
-        <f>STDEV(E473,E475)</f>
-        <v>1.626345596729188</v>
-      </c>
-      <c r="I473" s="3">
-        <v>2226.44</v>
-      </c>
-      <c r="J473" s="4">
-        <f>I473-G473</f>
-        <v>-9.1999999999998181</v>
-      </c>
-      <c r="K473" s="5">
-        <f>G473+J473</f>
-        <v>2226.44</v>
+        <v>9</v>
       </c>
     </row>
     <row r="474" spans="1:11" x14ac:dyDescent="0.2">
@@ -14229,18 +14236,18 @@
         <v>12</v>
       </c>
       <c r="D474" s="5">
-        <v>51.07</v>
+        <v>55.91</v>
       </c>
       <c r="E474" s="5">
-        <v>2230.34</v>
+        <v>2236.88</v>
       </c>
       <c r="F474" s="16" t="s">
-        <v>9</v>
+        <v>96</v>
       </c>
     </row>
     <row r="475" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A475" s="9" t="s">
-        <v>152</v>
+        <v>11</v>
       </c>
       <c r="B475" s="31">
         <v>45091</v>
@@ -14249,13 +14256,25 @@
         <v>12</v>
       </c>
       <c r="D475" s="5">
-        <v>55.91</v>
+        <v>50.54</v>
       </c>
       <c r="E475" s="5">
-        <v>2236.79</v>
+        <v>2724.69</v>
       </c>
       <c r="F475" s="16" t="s">
-        <v>96</v>
+        <v>470</v>
+      </c>
+      <c r="G475" s="13">
+        <f>AVERAGE(E475:E476)</f>
+        <v>2723.1849999999999</v>
+      </c>
+      <c r="H475" s="18">
+        <f>STDEV(E475,E476)</f>
+        <v>2.1283914113716627</v>
+      </c>
+      <c r="K475" s="5">
+        <f>G475+$J$472</f>
+        <v>2713.895</v>
       </c>
     </row>
     <row r="476" spans="1:11" x14ac:dyDescent="0.2">
@@ -14269,25 +14288,13 @@
         <v>12</v>
       </c>
       <c r="D476" s="5">
-        <v>50.54</v>
+        <v>48.78</v>
       </c>
       <c r="E476" s="5">
-        <v>2724.69</v>
+        <v>2721.68</v>
       </c>
       <c r="F476" s="16" t="s">
-        <v>474</v>
-      </c>
-      <c r="G476" s="13">
-        <f>AVERAGE(E476:E477)</f>
-        <v>2723.1849999999999</v>
-      </c>
-      <c r="H476" s="18">
-        <f>STDEV(E476,E477)</f>
-        <v>2.1283914113716627</v>
-      </c>
-      <c r="K476" s="5">
-        <f>G476+$J$473</f>
-        <v>2713.9850000000001</v>
+        <v>471</v>
       </c>
     </row>
     <row r="477" spans="1:11" x14ac:dyDescent="0.2">
@@ -14301,13 +14308,25 @@
         <v>12</v>
       </c>
       <c r="D477" s="5">
-        <v>48.78</v>
+        <v>49.21</v>
       </c>
       <c r="E477" s="5">
-        <v>2721.68</v>
+        <v>2703.56</v>
       </c>
       <c r="F477" s="16" t="s">
-        <v>475</v>
+        <v>472</v>
+      </c>
+      <c r="G477" s="13">
+        <f>AVERAGE(E477,E479)</f>
+        <v>2680.0749999999998</v>
+      </c>
+      <c r="H477" s="18">
+        <f>STDEV(E477,E478)</f>
+        <v>4.0305086527631921</v>
+      </c>
+      <c r="K477" s="5">
+        <f>G477+$J$472</f>
+        <v>2670.7849999999999</v>
       </c>
     </row>
     <row r="478" spans="1:11" x14ac:dyDescent="0.2">
@@ -14321,25 +14340,13 @@
         <v>12</v>
       </c>
       <c r="D478" s="5">
-        <v>49.21</v>
+        <v>49.8</v>
       </c>
       <c r="E478" s="5">
-        <v>2703.56</v>
+        <v>2697.86</v>
       </c>
       <c r="F478" s="16" t="s">
-        <v>476</v>
-      </c>
-      <c r="G478" s="13">
-        <f>AVERAGE(E478,E480)</f>
-        <v>2680.0749999999998</v>
-      </c>
-      <c r="H478" s="18">
-        <f>STDEV(E478,E479)</f>
-        <v>4.0305086527631921</v>
-      </c>
-      <c r="K478" s="5">
-        <f>G478+$J$473</f>
-        <v>2670.875</v>
+        <v>473</v>
       </c>
     </row>
     <row r="479" spans="1:11" x14ac:dyDescent="0.2">
@@ -14353,13 +14360,25 @@
         <v>12</v>
       </c>
       <c r="D479" s="5">
-        <v>49.8</v>
-      </c>
-      <c r="E479" s="5">
-        <v>2697.86</v>
+        <v>51.62</v>
+      </c>
+      <c r="E479" s="14">
+        <v>2656.59</v>
       </c>
       <c r="F479" s="16" t="s">
-        <v>477</v>
+        <v>422</v>
+      </c>
+      <c r="G479" s="13">
+        <f>AVERAGE(E480,E481)</f>
+        <v>2647.81</v>
+      </c>
+      <c r="H479" s="18">
+        <f>STDEV(E480,E481)</f>
+        <v>0.82024386617629219</v>
+      </c>
+      <c r="K479" s="5">
+        <f>G479+$J$472</f>
+        <v>2638.52</v>
       </c>
     </row>
     <row r="480" spans="1:11" x14ac:dyDescent="0.2">
@@ -14373,25 +14392,13 @@
         <v>12</v>
       </c>
       <c r="D480" s="5">
-        <v>51.62</v>
-      </c>
-      <c r="E480" s="14">
-        <v>2656.59</v>
+        <v>49.21</v>
+      </c>
+      <c r="E480" s="5">
+        <v>2647.23</v>
       </c>
       <c r="F480" s="16" t="s">
-        <v>422</v>
-      </c>
-      <c r="G480" s="13">
-        <f>AVERAGE(E481,E482)</f>
-        <v>2647.81</v>
-      </c>
-      <c r="H480" s="18">
-        <f>STDEV(E481,E482)</f>
-        <v>0.82024386617629219</v>
-      </c>
-      <c r="K480" s="5">
-        <f>G480+$J$473</f>
-        <v>2638.61</v>
+        <v>423</v>
       </c>
     </row>
     <row r="481" spans="1:11" x14ac:dyDescent="0.2">
@@ -14405,13 +14412,13 @@
         <v>12</v>
       </c>
       <c r="D481" s="5">
-        <v>49.21</v>
+        <v>48.69</v>
       </c>
       <c r="E481" s="5">
-        <v>2647.23</v>
+        <v>2648.39</v>
       </c>
       <c r="F481" s="16" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="482" spans="1:11" x14ac:dyDescent="0.2">
@@ -14425,13 +14432,25 @@
         <v>12</v>
       </c>
       <c r="D482" s="5">
-        <v>48.69</v>
+        <v>51.12</v>
       </c>
       <c r="E482" s="5">
-        <v>2648.39</v>
+        <v>2656.91</v>
       </c>
       <c r="F482" s="16" t="s">
-        <v>424</v>
+        <v>425</v>
+      </c>
+      <c r="G482" s="13">
+        <f>AVERAGE(E482,E483)</f>
+        <v>2656.1099999999997</v>
+      </c>
+      <c r="H482" s="18">
+        <f>STDEV(E482,E483)</f>
+        <v>1.1313708498984119</v>
+      </c>
+      <c r="K482" s="5">
+        <f>G482+$J$472</f>
+        <v>2646.8199999999997</v>
       </c>
     </row>
     <row r="483" spans="1:11" x14ac:dyDescent="0.2">
@@ -14445,25 +14464,13 @@
         <v>12</v>
       </c>
       <c r="D483" s="5">
-        <v>51.12</v>
+        <v>51.4</v>
       </c>
       <c r="E483" s="5">
-        <v>2656.91</v>
+        <v>2655.31</v>
       </c>
       <c r="F483" s="16" t="s">
-        <v>425</v>
-      </c>
-      <c r="G483" s="13">
-        <f>AVERAGE(E483,E484)</f>
-        <v>2656.1099999999997</v>
-      </c>
-      <c r="H483" s="18">
-        <f>STDEV(E483,E484)</f>
-        <v>1.1313708498984119</v>
-      </c>
-      <c r="K483" s="5">
-        <f>G483+$J$473</f>
-        <v>2646.91</v>
+        <v>426</v>
       </c>
     </row>
     <row r="484" spans="1:11" x14ac:dyDescent="0.2">
@@ -14477,13 +14484,25 @@
         <v>12</v>
       </c>
       <c r="D484" s="5">
-        <v>51.4</v>
+        <v>49.41</v>
       </c>
       <c r="E484" s="5">
-        <v>2655.31</v>
+        <v>2684.74</v>
       </c>
       <c r="F484" s="16" t="s">
-        <v>426</v>
+        <v>427</v>
+      </c>
+      <c r="G484" s="13">
+        <f>AVERAGE(E484,E485)</f>
+        <v>2684.2649999999999</v>
+      </c>
+      <c r="H484" s="18">
+        <f>STDEV(E484,E485)</f>
+        <v>0.67175144212709148</v>
+      </c>
+      <c r="K484" s="5">
+        <f>G484+$J$472</f>
+        <v>2674.9749999999999</v>
       </c>
     </row>
     <row r="485" spans="1:11" x14ac:dyDescent="0.2">
@@ -14497,25 +14516,13 @@
         <v>12</v>
       </c>
       <c r="D485" s="5">
-        <v>49.41</v>
+        <v>49.72</v>
       </c>
       <c r="E485" s="5">
-        <v>2684.74</v>
+        <v>2683.79</v>
       </c>
       <c r="F485" s="16" t="s">
-        <v>427</v>
-      </c>
-      <c r="G485" s="13">
-        <f>AVERAGE(E485,E486)</f>
-        <v>2684.2649999999999</v>
-      </c>
-      <c r="H485" s="18">
-        <f>STDEV(E485,E486)</f>
-        <v>0.67175144212709148</v>
-      </c>
-      <c r="K485" s="5">
-        <f>G485+$J$473</f>
-        <v>2675.0650000000001</v>
+        <v>428</v>
       </c>
     </row>
     <row r="486" spans="1:11" x14ac:dyDescent="0.2">
@@ -14529,13 +14536,25 @@
         <v>12</v>
       </c>
       <c r="D486" s="5">
-        <v>49.72</v>
-      </c>
-      <c r="E486" s="5">
-        <v>2683.79</v>
+        <v>50.83</v>
+      </c>
+      <c r="E486" s="14">
+        <v>2735.14</v>
       </c>
       <c r="F486" s="16" t="s">
-        <v>428</v>
+        <v>429</v>
+      </c>
+      <c r="G486" s="13">
+        <f>AVERAGE(E487,E489)</f>
+        <v>2724.0650000000001</v>
+      </c>
+      <c r="H486" s="18">
+        <f>STDEV(E487,E489)</f>
+        <v>1.0960155108392773</v>
+      </c>
+      <c r="K486" s="5">
+        <f>G486+$J$472</f>
+        <v>2714.7750000000001</v>
       </c>
     </row>
     <row r="487" spans="1:11" x14ac:dyDescent="0.2">
@@ -14549,25 +14568,13 @@
         <v>12</v>
       </c>
       <c r="D487" s="5">
-        <v>50.83</v>
-      </c>
-      <c r="E487" s="14">
-        <v>2735.14</v>
+        <v>48.96</v>
+      </c>
+      <c r="E487" s="5">
+        <v>2723.29</v>
       </c>
       <c r="F487" s="16" t="s">
-        <v>429</v>
-      </c>
-      <c r="G487" s="13">
-        <f>AVERAGE(E487,E488)</f>
-        <v>2729.2150000000001</v>
-      </c>
-      <c r="H487" s="18">
-        <f>STDEV(E487,E488)</f>
-        <v>8.3792153570605237</v>
-      </c>
-      <c r="K487" s="5">
-        <f>G487+$J$473</f>
-        <v>2720.0150000000003</v>
+        <v>430</v>
       </c>
     </row>
     <row r="488" spans="1:11" x14ac:dyDescent="0.2">
@@ -14581,132 +14588,364 @@
         <v>12</v>
       </c>
       <c r="D488" s="5">
-        <v>48.96</v>
-      </c>
-      <c r="E488" s="5">
-        <v>2723.29</v>
+        <v>50.39</v>
+      </c>
+      <c r="E488" s="14">
+        <v>2558.9699999999998</v>
       </c>
       <c r="F488" s="16" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="489" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A489" s="9" t="s">
-        <v>11</v>
+        <v>571</v>
       </c>
       <c r="B489" s="31">
-        <v>45091</v>
+        <v>45092</v>
       </c>
       <c r="C489" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D489" s="5">
-        <v>50.39</v>
-      </c>
-      <c r="E489" s="14">
-        <v>2558.9699999999998</v>
+        <v>53.63</v>
+      </c>
+      <c r="E489" s="5">
+        <v>2724.84</v>
       </c>
       <c r="F489" s="16" t="s">
-        <v>431</v>
+        <v>572</v>
       </c>
     </row>
     <row r="490" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A490" s="9" t="s">
+        <v>571</v>
+      </c>
+      <c r="B490" s="31">
+        <v>45092</v>
+      </c>
       <c r="C490" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D490" s="5">
+        <v>50.86</v>
+      </c>
+      <c r="E490" s="5">
+        <v>2237.83</v>
+      </c>
       <c r="F490" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G490" s="13">
+        <f>AVERAGE(E490:E491)</f>
+        <v>2236.6949999999997</v>
+      </c>
+      <c r="H490" s="18">
+        <f>STDEV(E490:E491)</f>
+        <v>1.60513239329345</v>
+      </c>
+      <c r="I490" s="3">
+        <v>2226.44</v>
+      </c>
+      <c r="J490" s="4">
+        <f>I490-G490</f>
+        <v>-10.254999999999654</v>
+      </c>
+      <c r="K490" s="5">
+        <f>G490+J490</f>
+        <v>2226.44</v>
+      </c>
+    </row>
+    <row r="491" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A491" s="9" t="s">
+        <v>571</v>
+      </c>
+      <c r="B491" s="31">
+        <v>45092</v>
+      </c>
+      <c r="C491" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D491" s="5">
+        <v>50.82</v>
+      </c>
+      <c r="E491" s="5">
+        <v>2235.56</v>
+      </c>
+      <c r="F491" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="492" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A492" s="9" t="s">
+        <v>571</v>
+      </c>
+      <c r="B492" s="31">
+        <v>45092</v>
+      </c>
+      <c r="C492" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D492" s="5">
+        <v>50.73</v>
+      </c>
+      <c r="E492" s="14">
+        <v>2249.09</v>
+      </c>
+      <c r="F492" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="493" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A493" s="9" t="s">
+        <v>571</v>
+      </c>
+      <c r="B493" s="31">
+        <v>45092</v>
+      </c>
+      <c r="C493" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D493" s="5">
+        <v>53.5</v>
+      </c>
+      <c r="E493" s="5">
+        <v>2646.16</v>
+      </c>
+      <c r="F493" s="16" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="491" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C491" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F491" s="16" t="s">
+      <c r="G493" s="13">
+        <f>AVERAGE(E493:E494)</f>
+        <v>2648.3599999999997</v>
+      </c>
+      <c r="H493" s="18">
+        <f>STDEV(E493:E494)</f>
+        <v>3.1112698372208736</v>
+      </c>
+      <c r="K493" s="5">
+        <f>G493+$J$472</f>
+        <v>2639.0699999999997</v>
+      </c>
+    </row>
+    <row r="494" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A494" s="9" t="s">
+        <v>571</v>
+      </c>
+      <c r="B494" s="31">
+        <v>45092</v>
+      </c>
+      <c r="C494" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D494" s="5">
+        <v>53.83</v>
+      </c>
+      <c r="E494" s="5">
+        <v>2650.56</v>
+      </c>
+      <c r="F494" s="16" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="492" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C492" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F492" s="16" t="s">
+    <row r="495" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A495" s="9" t="s">
+        <v>571</v>
+      </c>
+      <c r="B495" s="31">
+        <v>45092</v>
+      </c>
+      <c r="C495" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D495" s="5">
+        <v>51.93</v>
+      </c>
+      <c r="E495" s="14">
+        <v>2665.89</v>
+      </c>
+      <c r="F495" s="16" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="493" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C493" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F493" s="16" t="s">
+    <row r="496" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A496" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B496" s="31">
+        <v>45092</v>
+      </c>
+      <c r="C496" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D496" s="5">
+        <v>48.59</v>
+      </c>
+      <c r="E496" s="14">
+        <v>2623.61</v>
+      </c>
+      <c r="F496" s="16" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="494" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C494" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F494" s="16" t="s">
+      <c r="G496" s="13">
+        <f>AVERAGE(E497:E498)</f>
+        <v>2562.915</v>
+      </c>
+      <c r="H496" s="18">
+        <f>STDEV(E497:E498)</f>
+        <v>1.2798632739476123</v>
+      </c>
+      <c r="K496" s="5">
+        <f>G496+$J$472</f>
+        <v>2553.625</v>
+      </c>
+    </row>
+    <row r="497" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A497" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B497" s="31">
+        <v>45092</v>
+      </c>
+      <c r="C497" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D497" s="5">
+        <v>50.54</v>
+      </c>
+      <c r="E497" s="5">
+        <v>2563.8200000000002</v>
+      </c>
+      <c r="F497" s="16" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="495" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C495" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F495" s="16" t="s">
+    <row r="498" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A498" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B498" s="31">
+        <v>45092</v>
+      </c>
+      <c r="C498" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D498" s="5">
+        <v>51.73</v>
+      </c>
+      <c r="E498" s="5">
+        <v>2562.0100000000002</v>
+      </c>
+      <c r="F498" s="16" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="496" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C496" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F496" s="16" t="s">
+    <row r="499" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A499" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B499" s="31">
+        <v>45092</v>
+      </c>
+      <c r="C499" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D499" s="5">
+        <v>50.45</v>
+      </c>
+      <c r="E499" s="5">
+        <v>2596.41</v>
+      </c>
+      <c r="F499" s="16" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="497" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C497" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F497" s="16" t="s">
+      <c r="G499" s="13">
+        <f>AVERAGE(E499:E500)</f>
+        <v>2595.605</v>
+      </c>
+      <c r="H499" s="18">
+        <f>STDEV(E499:E500)</f>
+        <v>1.1384419177101099</v>
+      </c>
+      <c r="K499" s="5">
+        <f>G499+$J$472</f>
+        <v>2586.3150000000001</v>
+      </c>
+    </row>
+    <row r="500" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A500" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B500" s="31">
+        <v>45092</v>
+      </c>
+      <c r="C500" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D500" s="5">
+        <v>49.91</v>
+      </c>
+      <c r="E500" s="5">
+        <v>2594.8000000000002</v>
+      </c>
+      <c r="F500" s="16" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="498" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C498" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F498" s="16" t="s">
+    <row r="501" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A501" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B501" s="31">
+        <v>45092</v>
+      </c>
+      <c r="C501" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D501" s="5">
+        <v>49.75</v>
+      </c>
+      <c r="E501" s="5">
+        <v>2716.89</v>
+      </c>
+      <c r="F501" s="16" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="499" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C499" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F499" s="16" t="s">
+      <c r="G501" s="13">
+        <f>AVERAGE(E501:E502)</f>
+        <v>2715.01</v>
+      </c>
+      <c r="H501" s="18">
+        <f>STDEV(E501:E502)</f>
+        <v>2.6587214972612516</v>
+      </c>
+      <c r="K501" s="5">
+        <f>G501+$J$472</f>
+        <v>2705.7200000000003</v>
+      </c>
+    </row>
+    <row r="502" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A502" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B502" s="31">
+        <v>45092</v>
+      </c>
+      <c r="C502" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D502" s="5">
+        <v>51.38</v>
+      </c>
+      <c r="E502" s="5">
+        <v>2713.13</v>
+      </c>
+      <c r="F502" s="16" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="500" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C500" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F500" s="16" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="501" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C501" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F501" s="16" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="503" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="503" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A503" s="9"/>
       <c r="C503" s="10" t="s">
         <v>12</v>
       </c>
@@ -14714,7 +14953,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="504" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="504" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A504" s="9"/>
       <c r="C504" s="10" t="s">
         <v>12</v>
       </c>
@@ -14722,7 +14962,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="505" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="505" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A505" s="9"/>
       <c r="C505" s="10" t="s">
         <v>12</v>
       </c>
@@ -14730,188 +14971,344 @@
         <v>96</v>
       </c>
     </row>
-    <row r="506" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="506" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A506" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B506" s="31">
+        <v>45092</v>
+      </c>
       <c r="C506" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D506" s="5">
+        <v>50.1</v>
+      </c>
+      <c r="E506" s="14">
+        <v>2667.86</v>
+      </c>
       <c r="F506" s="16" t="s">
+        <v>474</v>
+      </c>
+      <c r="G506" s="13">
+        <f>AVERAGE(E507:E508)</f>
+        <v>2658.04</v>
+      </c>
+      <c r="H506" s="18">
+        <f>STDEV(E507:E508)</f>
+        <v>1.9657568516984221</v>
+      </c>
+      <c r="K506" s="5">
+        <f>G506+$J$472</f>
+        <v>2648.75</v>
+      </c>
+    </row>
+    <row r="507" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A507" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B507" s="31">
+        <v>45092</v>
+      </c>
+      <c r="C507" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D507" s="5">
+        <v>49.52</v>
+      </c>
+      <c r="E507" s="5">
+        <v>2656.65</v>
+      </c>
+      <c r="F507" s="16" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="508" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A508" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B508" s="31">
+        <v>45092</v>
+      </c>
+      <c r="C508" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D508" s="5">
+        <v>49.55</v>
+      </c>
+      <c r="E508" s="5">
+        <v>2659.43</v>
+      </c>
+      <c r="F508" s="16" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="509" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A509" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B509" s="31">
+        <v>45092</v>
+      </c>
+      <c r="C509" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D509" s="5">
+        <v>48.88</v>
+      </c>
+      <c r="E509" s="5">
+        <v>2642.93</v>
+      </c>
+      <c r="F509" s="16" t="s">
+        <v>477</v>
+      </c>
+      <c r="G509" s="13">
+        <f>AVERAGE(E509:E510)</f>
+        <v>2640.355</v>
+      </c>
+      <c r="H509" s="18">
+        <f>STDEV(E509:E510)</f>
+        <v>3.6415999231104625</v>
+      </c>
+      <c r="K509" s="5">
+        <f>G509+$J$472</f>
+        <v>2631.0650000000001</v>
+      </c>
+    </row>
+    <row r="510" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A510" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B510" s="31">
+        <v>45092</v>
+      </c>
+      <c r="C510" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D510" s="5">
+        <v>50.76</v>
+      </c>
+      <c r="E510" s="5">
+        <v>2637.78</v>
+      </c>
+      <c r="F510" s="16" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="507" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C507" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F507" s="16" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="508" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C508" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F508" s="16" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="509" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C509" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F509" s="16" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="510" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C510" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F510" s="16" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="511" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="511" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A511" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B511" s="31">
+        <v>45092</v>
+      </c>
       <c r="C511" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D511" s="5">
+        <v>50.53</v>
+      </c>
+      <c r="E511" s="5">
+        <v>2563.23</v>
+      </c>
       <c r="F511" s="16" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="512" spans="3:6" x14ac:dyDescent="0.2">
+        <v>442</v>
+      </c>
+      <c r="G511" s="13">
+        <f>AVERAGE(E511:E512)</f>
+        <v>2560.4749999999999</v>
+      </c>
+      <c r="H511" s="18">
+        <f>STDEV(E511:E512)</f>
+        <v>3.8961583643380311</v>
+      </c>
+      <c r="K511" s="5">
+        <f>G511+$J$472</f>
+        <v>2551.1849999999999</v>
+      </c>
+    </row>
+    <row r="512" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A512" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B512" s="31">
+        <v>45092</v>
+      </c>
       <c r="C512" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D512" s="5">
+        <v>50.23</v>
+      </c>
+      <c r="E512" s="5">
+        <v>2557.7199999999998</v>
+      </c>
       <c r="F512" s="16" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="513" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A513" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B513" s="31">
+        <v>45092</v>
+      </c>
+      <c r="C513" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D513" s="5">
+        <v>49.45</v>
+      </c>
+      <c r="E513" s="5">
+        <v>2567.5</v>
+      </c>
+      <c r="F513" s="16" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="513" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C513" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F513" s="16" t="s">
+      <c r="G513" s="13">
+        <f>AVERAGE(E513:E514)</f>
+        <v>2567.0150000000003</v>
+      </c>
+      <c r="H513" s="18">
+        <f>STDEV(E513:E514)</f>
+        <v>0.68589357775080961</v>
+      </c>
+      <c r="K513" s="5">
+        <f>G513+$J$472</f>
+        <v>2557.7250000000004</v>
+      </c>
+    </row>
+    <row r="514" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A514" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B514" s="31">
+        <v>45092</v>
+      </c>
+      <c r="C514" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D514" s="5">
+        <v>48.68</v>
+      </c>
+      <c r="E514" s="5">
+        <v>2566.5300000000002</v>
+      </c>
+      <c r="F514" s="16" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="514" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C514" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F514" s="16" t="s">
+    <row r="515" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C515" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F515" s="16" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="515" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C515" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F515" s="16" t="s">
+    <row r="516" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C516" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F516" s="16" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="516" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C516" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F516" s="16" t="s">
+    <row r="517" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C517" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F517" s="16" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="517" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C517" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F517" s="16" t="s">
+    <row r="518" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C518" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F518" s="16" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="518" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C518" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F518" s="16" t="s">
+    <row r="519" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C519" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F519" s="16" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="519" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C519" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F519" s="16" t="s">
+    <row r="520" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C520" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F520" s="16" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="520" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C520" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F520" s="16" t="s">
+    <row r="521" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C521" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F521" s="16" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="521" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C521" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F521" s="16" t="s">
+    <row r="522" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C522" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F522" s="16" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="522" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C522" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F522" s="16" t="s">
+    <row r="523" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C523" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F523" s="16" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="523" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C523" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F523" s="16" t="s">
+    <row r="524" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C524" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F524" s="16" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="524" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C524" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F524" s="16" t="s">
+    <row r="525" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C525" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F525" s="16" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="525" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C525" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F525" s="16" t="s">
+    <row r="526" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C526" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F526" s="16" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="526" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C526" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F526" s="16" t="s">
+    <row r="527" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C527" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F527" s="16" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="527" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C527" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F527" s="16" t="s">
+    <row r="528" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C528" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F528" s="16" t="s">
         <v>459</v>
-      </c>
-    </row>
-    <row r="528" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C528" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F528" s="16" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="529" spans="3:6" x14ac:dyDescent="0.2">
@@ -14919,7 +15316,7 @@
         <v>12</v>
       </c>
       <c r="F529" s="16" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="530" spans="3:6" x14ac:dyDescent="0.2">
@@ -14927,7 +15324,7 @@
         <v>12</v>
       </c>
       <c r="F530" s="16" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="531" spans="3:6" x14ac:dyDescent="0.2">
@@ -14935,7 +15332,7 @@
         <v>12</v>
       </c>
       <c r="F531" s="16" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="532" spans="3:6" x14ac:dyDescent="0.2">
@@ -14943,15 +15340,7 @@
         <v>12</v>
       </c>
       <c r="F532" s="16" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="533" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C533" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F533" s="16" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="534" spans="3:6" x14ac:dyDescent="0.2">
@@ -14959,7 +15348,7 @@
         <v>12</v>
       </c>
       <c r="F534" s="16" t="s">
-        <v>466</v>
+        <v>8</v>
       </c>
     </row>
     <row r="535" spans="3:6" x14ac:dyDescent="0.2">
@@ -14967,7 +15356,15 @@
         <v>12</v>
       </c>
       <c r="F535" s="16" t="s">
-        <v>467</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="536" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C536" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F536" s="16" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="537" spans="3:6" x14ac:dyDescent="0.2">
@@ -14975,7 +15372,7 @@
         <v>12</v>
       </c>
       <c r="F537" s="16" t="s">
-        <v>8</v>
+        <v>479</v>
       </c>
     </row>
     <row r="538" spans="3:6" x14ac:dyDescent="0.2">
@@ -14983,7 +15380,7 @@
         <v>12</v>
       </c>
       <c r="F538" s="16" t="s">
-        <v>9</v>
+        <v>480</v>
       </c>
     </row>
     <row r="539" spans="3:6" x14ac:dyDescent="0.2">
@@ -14991,7 +15388,7 @@
         <v>12</v>
       </c>
       <c r="F539" s="16" t="s">
-        <v>96</v>
+        <v>481</v>
       </c>
     </row>
     <row r="540" spans="3:6" x14ac:dyDescent="0.2">
@@ -14999,7 +15396,7 @@
         <v>12</v>
       </c>
       <c r="F540" s="16" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="541" spans="3:6" x14ac:dyDescent="0.2">
@@ -15007,7 +15404,7 @@
         <v>12</v>
       </c>
       <c r="F541" s="16" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="542" spans="3:6" x14ac:dyDescent="0.2">
@@ -15015,7 +15412,7 @@
         <v>12</v>
       </c>
       <c r="F542" s="16" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="543" spans="3:6" x14ac:dyDescent="0.2">
@@ -15023,7 +15420,7 @@
         <v>12</v>
       </c>
       <c r="F543" s="16" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="544" spans="3:6" x14ac:dyDescent="0.2">
@@ -15031,7 +15428,7 @@
         <v>12</v>
       </c>
       <c r="F544" s="16" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="545" spans="3:6" x14ac:dyDescent="0.2">
@@ -15039,7 +15436,7 @@
         <v>12</v>
       </c>
       <c r="F545" s="16" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="546" spans="3:6" x14ac:dyDescent="0.2">
@@ -15047,7 +15444,7 @@
         <v>12</v>
       </c>
       <c r="F546" s="16" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="547" spans="3:6" x14ac:dyDescent="0.2">
@@ -15055,7 +15452,7 @@
         <v>12</v>
       </c>
       <c r="F547" s="16" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="548" spans="3:6" x14ac:dyDescent="0.2">
@@ -15063,7 +15460,7 @@
         <v>12</v>
       </c>
       <c r="F548" s="16" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="549" spans="3:6" x14ac:dyDescent="0.2">
@@ -15071,7 +15468,7 @@
         <v>12</v>
       </c>
       <c r="F549" s="16" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="550" spans="3:6" x14ac:dyDescent="0.2">
@@ -15079,7 +15476,7 @@
         <v>12</v>
       </c>
       <c r="F550" s="16" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="551" spans="3:6" x14ac:dyDescent="0.2">
@@ -15087,7 +15484,7 @@
         <v>12</v>
       </c>
       <c r="F551" s="16" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="552" spans="3:6" x14ac:dyDescent="0.2">
@@ -15095,7 +15492,7 @@
         <v>12</v>
       </c>
       <c r="F552" s="16" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="553" spans="3:6" x14ac:dyDescent="0.2">
@@ -15103,7 +15500,7 @@
         <v>12</v>
       </c>
       <c r="F553" s="16" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="554" spans="3:6" x14ac:dyDescent="0.2">
@@ -15111,7 +15508,7 @@
         <v>12</v>
       </c>
       <c r="F554" s="16" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="555" spans="3:6" x14ac:dyDescent="0.2">
@@ -15119,7 +15516,7 @@
         <v>12</v>
       </c>
       <c r="F555" s="16" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="556" spans="3:6" x14ac:dyDescent="0.2">
@@ -15127,7 +15524,7 @@
         <v>12</v>
       </c>
       <c r="F556" s="16" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="557" spans="3:6" x14ac:dyDescent="0.2">
@@ -15135,7 +15532,7 @@
         <v>12</v>
       </c>
       <c r="F557" s="16" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="558" spans="3:6" x14ac:dyDescent="0.2">
@@ -15143,7 +15540,7 @@
         <v>12</v>
       </c>
       <c r="F558" s="16" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="559" spans="3:6" x14ac:dyDescent="0.2">
@@ -15151,7 +15548,7 @@
         <v>12</v>
       </c>
       <c r="F559" s="16" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="560" spans="3:6" x14ac:dyDescent="0.2">
@@ -15159,7 +15556,7 @@
         <v>12</v>
       </c>
       <c r="F560" s="16" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="561" spans="3:6" x14ac:dyDescent="0.2">
@@ -15167,7 +15564,7 @@
         <v>12</v>
       </c>
       <c r="F561" s="16" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="562" spans="3:6" x14ac:dyDescent="0.2">
@@ -15175,7 +15572,7 @@
         <v>12</v>
       </c>
       <c r="F562" s="16" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="563" spans="3:6" x14ac:dyDescent="0.2">
@@ -15183,7 +15580,7 @@
         <v>12</v>
       </c>
       <c r="F563" s="16" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="564" spans="3:6" x14ac:dyDescent="0.2">
@@ -15191,7 +15588,7 @@
         <v>12</v>
       </c>
       <c r="F564" s="16" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="565" spans="3:6" x14ac:dyDescent="0.2">
@@ -15199,7 +15596,7 @@
         <v>12</v>
       </c>
       <c r="F565" s="16" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="566" spans="3:6" x14ac:dyDescent="0.2">
@@ -15207,23 +15604,18 @@
         <v>12</v>
       </c>
       <c r="F566" s="16" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="567" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C567" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F567" s="16" t="s">
-        <v>511</v>
-      </c>
+      <c r="F567" s="16"/>
     </row>
     <row r="568" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C568" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F568" s="16" t="s">
-        <v>512</v>
+        <v>8</v>
       </c>
     </row>
     <row r="569" spans="3:6" x14ac:dyDescent="0.2">
@@ -15231,18 +15623,23 @@
         <v>12</v>
       </c>
       <c r="F569" s="16" t="s">
-        <v>513</v>
+        <v>9</v>
       </c>
     </row>
     <row r="570" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="F570" s="16"/>
+      <c r="C570" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F570" s="16" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="571" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C571" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F571" s="16" t="s">
-        <v>8</v>
+        <v>509</v>
       </c>
     </row>
     <row r="572" spans="3:6" x14ac:dyDescent="0.2">
@@ -15250,7 +15647,7 @@
         <v>12</v>
       </c>
       <c r="F572" s="16" t="s">
-        <v>9</v>
+        <v>510</v>
       </c>
     </row>
     <row r="573" spans="3:6" x14ac:dyDescent="0.2">
@@ -15258,7 +15655,7 @@
         <v>12</v>
       </c>
       <c r="F573" s="16" t="s">
-        <v>96</v>
+        <v>511</v>
       </c>
     </row>
     <row r="574" spans="3:6" x14ac:dyDescent="0.2">
@@ -15266,7 +15663,7 @@
         <v>12</v>
       </c>
       <c r="F574" s="16" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="575" spans="3:6" x14ac:dyDescent="0.2">
@@ -15274,7 +15671,7 @@
         <v>12</v>
       </c>
       <c r="F575" s="16" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="576" spans="3:6" x14ac:dyDescent="0.2">
@@ -15282,7 +15679,7 @@
         <v>12</v>
       </c>
       <c r="F576" s="16" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="577" spans="3:6" x14ac:dyDescent="0.2">
@@ -15290,7 +15687,7 @@
         <v>12</v>
       </c>
       <c r="F577" s="16" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="578" spans="3:6" x14ac:dyDescent="0.2">
@@ -15298,7 +15695,7 @@
         <v>12</v>
       </c>
       <c r="F578" s="16" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="579" spans="3:6" x14ac:dyDescent="0.2">
@@ -15306,7 +15703,7 @@
         <v>12</v>
       </c>
       <c r="F579" s="16" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="580" spans="3:6" x14ac:dyDescent="0.2">
@@ -15314,7 +15711,7 @@
         <v>12</v>
       </c>
       <c r="F580" s="16" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="581" spans="3:6" x14ac:dyDescent="0.2">
@@ -15322,7 +15719,7 @@
         <v>12</v>
       </c>
       <c r="F581" s="16" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="582" spans="3:6" x14ac:dyDescent="0.2">
@@ -15330,7 +15727,7 @@
         <v>12</v>
       </c>
       <c r="F582" s="16" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="583" spans="3:6" x14ac:dyDescent="0.2">
@@ -15338,7 +15735,7 @@
         <v>12</v>
       </c>
       <c r="F583" s="16" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="584" spans="3:6" x14ac:dyDescent="0.2">
@@ -15346,7 +15743,7 @@
         <v>12</v>
       </c>
       <c r="F584" s="16" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="585" spans="3:6" x14ac:dyDescent="0.2">
@@ -15354,7 +15751,7 @@
         <v>12</v>
       </c>
       <c r="F585" s="16" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="586" spans="3:6" x14ac:dyDescent="0.2">
@@ -15362,7 +15759,7 @@
         <v>12</v>
       </c>
       <c r="F586" s="16" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="587" spans="3:6" x14ac:dyDescent="0.2">
@@ -15370,7 +15767,7 @@
         <v>12</v>
       </c>
       <c r="F587" s="16" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="588" spans="3:6" x14ac:dyDescent="0.2">
@@ -15378,7 +15775,7 @@
         <v>12</v>
       </c>
       <c r="F588" s="16" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="589" spans="3:6" x14ac:dyDescent="0.2">
@@ -15386,7 +15783,7 @@
         <v>12</v>
       </c>
       <c r="F589" s="16" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="590" spans="3:6" x14ac:dyDescent="0.2">
@@ -15394,7 +15791,7 @@
         <v>12</v>
       </c>
       <c r="F590" s="16" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="591" spans="3:6" x14ac:dyDescent="0.2">
@@ -15402,7 +15799,7 @@
         <v>12</v>
       </c>
       <c r="F591" s="16" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="592" spans="3:6" x14ac:dyDescent="0.2">
@@ -15410,7 +15807,7 @@
         <v>12</v>
       </c>
       <c r="F592" s="16" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="593" spans="3:6" x14ac:dyDescent="0.2">
@@ -15418,7 +15815,7 @@
         <v>12</v>
       </c>
       <c r="F593" s="16" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="594" spans="3:6" x14ac:dyDescent="0.2">
@@ -15426,7 +15823,7 @@
         <v>12</v>
       </c>
       <c r="F594" s="16" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="595" spans="3:6" x14ac:dyDescent="0.2">
@@ -15434,7 +15831,7 @@
         <v>12</v>
       </c>
       <c r="F595" s="16" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="596" spans="3:6" x14ac:dyDescent="0.2">
@@ -15442,7 +15839,7 @@
         <v>12</v>
       </c>
       <c r="F596" s="16" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="597" spans="3:6" x14ac:dyDescent="0.2">
@@ -15450,7 +15847,7 @@
         <v>12</v>
       </c>
       <c r="F597" s="16" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="598" spans="3:6" x14ac:dyDescent="0.2">
@@ -15458,7 +15855,7 @@
         <v>12</v>
       </c>
       <c r="F598" s="16" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="599" spans="3:6" x14ac:dyDescent="0.2">
@@ -15466,7 +15863,7 @@
         <v>12</v>
       </c>
       <c r="F599" s="16" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="600" spans="3:6" x14ac:dyDescent="0.2">
@@ -15474,15 +15871,7 @@
         <v>12</v>
       </c>
       <c r="F600" s="16" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="601" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C601" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F601" s="16" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
     </row>
     <row r="602" spans="3:6" x14ac:dyDescent="0.2">
@@ -15490,7 +15879,7 @@
         <v>12</v>
       </c>
       <c r="F602" s="16" t="s">
-        <v>542</v>
+        <v>8</v>
       </c>
     </row>
     <row r="603" spans="3:6" x14ac:dyDescent="0.2">
@@ -15498,7 +15887,15 @@
         <v>12</v>
       </c>
       <c r="F603" s="16" t="s">
-        <v>543</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="604" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C604" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F604" s="16" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="605" spans="3:6" x14ac:dyDescent="0.2">
@@ -15506,7 +15903,7 @@
         <v>12</v>
       </c>
       <c r="F605" s="16" t="s">
-        <v>8</v>
+        <v>539</v>
       </c>
     </row>
     <row r="606" spans="3:6" x14ac:dyDescent="0.2">
@@ -15514,7 +15911,7 @@
         <v>12</v>
       </c>
       <c r="F606" s="16" t="s">
-        <v>9</v>
+        <v>540</v>
       </c>
     </row>
     <row r="607" spans="3:6" x14ac:dyDescent="0.2">
@@ -15522,7 +15919,7 @@
         <v>12</v>
       </c>
       <c r="F607" s="16" t="s">
-        <v>96</v>
+        <v>541</v>
       </c>
     </row>
     <row r="608" spans="3:6" x14ac:dyDescent="0.2">
@@ -15530,7 +15927,7 @@
         <v>12</v>
       </c>
       <c r="F608" s="16" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="609" spans="3:6" x14ac:dyDescent="0.2">
@@ -15538,7 +15935,7 @@
         <v>12</v>
       </c>
       <c r="F609" s="16" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="610" spans="3:6" x14ac:dyDescent="0.2">
@@ -15546,7 +15943,7 @@
         <v>12</v>
       </c>
       <c r="F610" s="16" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="611" spans="3:6" x14ac:dyDescent="0.2">
@@ -15554,7 +15951,7 @@
         <v>12</v>
       </c>
       <c r="F611" s="16" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="612" spans="3:6" x14ac:dyDescent="0.2">
@@ -15562,7 +15959,7 @@
         <v>12</v>
       </c>
       <c r="F612" s="16" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="613" spans="3:6" x14ac:dyDescent="0.2">
@@ -15570,7 +15967,7 @@
         <v>12</v>
       </c>
       <c r="F613" s="16" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="614" spans="3:6" x14ac:dyDescent="0.2">
@@ -15578,7 +15975,7 @@
         <v>12</v>
       </c>
       <c r="F614" s="16" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="615" spans="3:6" x14ac:dyDescent="0.2">
@@ -15586,7 +15983,7 @@
         <v>12</v>
       </c>
       <c r="F615" s="16" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="616" spans="3:6" x14ac:dyDescent="0.2">
@@ -15594,7 +15991,7 @@
         <v>12</v>
       </c>
       <c r="F616" s="16" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="617" spans="3:6" x14ac:dyDescent="0.2">
@@ -15602,7 +15999,7 @@
         <v>12</v>
       </c>
       <c r="F617" s="16" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="618" spans="3:6" x14ac:dyDescent="0.2">
@@ -15610,7 +16007,7 @@
         <v>12</v>
       </c>
       <c r="F618" s="16" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="619" spans="3:6" x14ac:dyDescent="0.2">
@@ -15618,7 +16015,7 @@
         <v>12</v>
       </c>
       <c r="F619" s="16" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="620" spans="3:6" x14ac:dyDescent="0.2">
@@ -15626,7 +16023,7 @@
         <v>12</v>
       </c>
       <c r="F620" s="16" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="621" spans="3:6" x14ac:dyDescent="0.2">
@@ -15634,7 +16031,7 @@
         <v>12</v>
       </c>
       <c r="F621" s="16" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="622" spans="3:6" x14ac:dyDescent="0.2">
@@ -15642,7 +16039,7 @@
         <v>12</v>
       </c>
       <c r="F622" s="16" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="623" spans="3:6" x14ac:dyDescent="0.2">
@@ -15650,7 +16047,7 @@
         <v>12</v>
       </c>
       <c r="F623" s="16" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="624" spans="3:6" x14ac:dyDescent="0.2">
@@ -15658,7 +16055,7 @@
         <v>12</v>
       </c>
       <c r="F624" s="16" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="625" spans="3:6" x14ac:dyDescent="0.2">
@@ -15666,7 +16063,7 @@
         <v>12</v>
       </c>
       <c r="F625" s="16" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="626" spans="3:6" x14ac:dyDescent="0.2">
@@ -15674,7 +16071,7 @@
         <v>12</v>
       </c>
       <c r="F626" s="16" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="627" spans="3:6" x14ac:dyDescent="0.2">
@@ -15682,7 +16079,7 @@
         <v>12</v>
       </c>
       <c r="F627" s="16" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="628" spans="3:6" x14ac:dyDescent="0.2">
@@ -15690,7 +16087,7 @@
         <v>12</v>
       </c>
       <c r="F628" s="16" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="629" spans="3:6" x14ac:dyDescent="0.2">
@@ -15698,7 +16095,7 @@
         <v>12</v>
       </c>
       <c r="F629" s="16" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="630" spans="3:6" x14ac:dyDescent="0.2">
@@ -15706,7 +16103,7 @@
         <v>12</v>
       </c>
       <c r="F630" s="16" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="631" spans="3:6" x14ac:dyDescent="0.2">
@@ -15714,7 +16111,7 @@
         <v>12</v>
       </c>
       <c r="F631" s="16" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="632" spans="3:6" x14ac:dyDescent="0.2">
@@ -15722,7 +16119,7 @@
         <v>12</v>
       </c>
       <c r="F632" s="16" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="633" spans="3:6" x14ac:dyDescent="0.2">
@@ -15730,7 +16127,7 @@
         <v>12</v>
       </c>
       <c r="F633" s="16" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="634" spans="3:6" x14ac:dyDescent="0.2">
@@ -15738,35 +16135,11 @@
         <v>12</v>
       </c>
       <c r="F634" s="16" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="635" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C635" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F635" s="16" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="636" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C636" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F636" s="16" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="637" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C637" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F637" s="16" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:L502" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
End historic tile experiment ALK
</commit_message>
<xml_diff>
--- a/Data/Spring_2023/BenthFun_Alkalinity.xlsx
+++ b/Data/Spring_2023/BenthFun_Alkalinity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremy/Library/Mobile Documents/com~apple~CloudDocs/Documents/Documents/Post-Doc/Projets/Villefranche/Projets/BenthFun – Jeremy/BenthFun/Data/Spring_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163E1137-16C9-8D42-99B2-D3244A48FC05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204A6D97-AFB6-6E48-93D5-A3E79B5789CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1867" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1885" uniqueCount="570">
   <si>
     <t>Operator</t>
   </si>
@@ -1381,9 +1381,6 @@
     <t>Tn_t1_AMB_tile_03b</t>
   </si>
   <si>
-    <t>Tn_t1_AMB_tile_03c</t>
-  </si>
-  <si>
     <t>Tn_t1_AMB_blank_01a</t>
   </si>
   <si>
@@ -1417,16 +1414,10 @@
     <t>Tn_t1_AMB_tile_06b</t>
   </si>
   <si>
-    <t>Tn_t1_AMB_tile_06c</t>
-  </si>
-  <si>
     <t>Tn_t1_AMB_blank_02a</t>
   </si>
   <si>
     <t>Tn_t1_AMB_blank_02b</t>
-  </si>
-  <si>
-    <t>Tn_t1_AMB_blank_02c</t>
   </si>
   <si>
     <t>Tn_t0_ELOW_blank_01a</t>
@@ -2237,11 +2228,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L634"/>
+  <dimension ref="A1:L630"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="73" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A502" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I521" sqref="I521"/>
+      <pane ySplit="1" topLeftCell="A504" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M517" sqref="M517"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13009,7 +13000,7 @@
         <v>2468.38</v>
       </c>
       <c r="F424" s="32" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
     </row>
     <row r="425" spans="1:11" x14ac:dyDescent="0.2">
@@ -13205,7 +13196,7 @@
         <v>2530.84</v>
       </c>
       <c r="F432" s="32" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
     </row>
     <row r="433" spans="1:12" x14ac:dyDescent="0.2">
@@ -13503,7 +13494,7 @@
         <v>2797.88</v>
       </c>
       <c r="F444" s="16" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="G444" s="13">
         <f>AVERAGE(E444,E446)</f>
@@ -13535,7 +13526,7 @@
         <v>2892.7</v>
       </c>
       <c r="F445" s="16" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
     </row>
     <row r="446" spans="1:12" x14ac:dyDescent="0.2">
@@ -13555,7 +13546,7 @@
         <v>2791.76</v>
       </c>
       <c r="F446" s="16" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
     </row>
     <row r="447" spans="1:12" x14ac:dyDescent="0.2">
@@ -13575,7 +13566,7 @@
         <v>2776.09</v>
       </c>
       <c r="F447" s="16" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="G447" s="13">
         <f>AVERAGE(E448,E449)</f>
@@ -13607,7 +13598,7 @@
         <v>2789.47</v>
       </c>
       <c r="F448" s="16" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="449" spans="1:11" x14ac:dyDescent="0.2">
@@ -13627,7 +13618,7 @@
         <v>2795.12</v>
       </c>
       <c r="F449" s="16" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="450" spans="1:11" x14ac:dyDescent="0.2">
@@ -14262,7 +14253,7 @@
         <v>2724.69</v>
       </c>
       <c r="F475" s="16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="G475" s="13">
         <f>AVERAGE(E475:E476)</f>
@@ -14294,7 +14285,7 @@
         <v>2721.68</v>
       </c>
       <c r="F476" s="16" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
     </row>
     <row r="477" spans="1:11" x14ac:dyDescent="0.2">
@@ -14314,7 +14305,7 @@
         <v>2703.56</v>
       </c>
       <c r="F477" s="16" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="G477" s="13">
         <f>AVERAGE(E477,E479)</f>
@@ -14346,7 +14337,7 @@
         <v>2697.86</v>
       </c>
       <c r="F478" s="16" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
     </row>
     <row r="479" spans="1:11" x14ac:dyDescent="0.2">
@@ -14599,7 +14590,7 @@
     </row>
     <row r="489" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A489" s="9" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="B489" s="31">
         <v>45092</v>
@@ -14614,12 +14605,12 @@
         <v>2724.84</v>
       </c>
       <c r="F489" s="16" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
     </row>
     <row r="490" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A490" s="9" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="B490" s="31">
         <v>45092</v>
@@ -14658,7 +14649,7 @@
     </row>
     <row r="491" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A491" s="9" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="B491" s="31">
         <v>45092</v>
@@ -14678,7 +14669,7 @@
     </row>
     <row r="492" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A492" s="9" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="B492" s="31">
         <v>45092</v>
@@ -14698,7 +14689,7 @@
     </row>
     <row r="493" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A493" s="9" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="B493" s="31">
         <v>45092</v>
@@ -14724,13 +14715,13 @@
         <v>3.1112698372208736</v>
       </c>
       <c r="K493" s="5">
-        <f>G493+$J$472</f>
-        <v>2639.0699999999997</v>
+        <f>G493+$J$490</f>
+        <v>2638.105</v>
       </c>
     </row>
     <row r="494" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A494" s="9" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="B494" s="31">
         <v>45092</v>
@@ -14750,7 +14741,7 @@
     </row>
     <row r="495" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A495" s="9" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="B495" s="31">
         <v>45092</v>
@@ -14796,8 +14787,8 @@
         <v>1.2798632739476123</v>
       </c>
       <c r="K496" s="5">
-        <f>G496+$J$472</f>
-        <v>2553.625</v>
+        <f>G496+$J$490</f>
+        <v>2552.6600000000003</v>
       </c>
     </row>
     <row r="497" spans="1:11" x14ac:dyDescent="0.2">
@@ -14868,8 +14859,8 @@
         <v>1.1384419177101099</v>
       </c>
       <c r="K499" s="5">
-        <f>G499+$J$472</f>
-        <v>2586.3150000000001</v>
+        <f>G499+$J$490</f>
+        <v>2585.3500000000004</v>
       </c>
     </row>
     <row r="500" spans="1:11" x14ac:dyDescent="0.2">
@@ -14920,8 +14911,8 @@
         <v>2.6587214972612516</v>
       </c>
       <c r="K501" s="5">
-        <f>G501+$J$472</f>
-        <v>2705.7200000000003</v>
+        <f>G501+$J$490</f>
+        <v>2704.7550000000006</v>
       </c>
     </row>
     <row r="502" spans="1:11" x14ac:dyDescent="0.2">
@@ -14945,30 +14936,94 @@
       </c>
     </row>
     <row r="503" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A503" s="9"/>
+      <c r="A503" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B503" s="31">
+        <v>45093</v>
+      </c>
       <c r="C503" s="10" t="s">
         <v>12</v>
+      </c>
+      <c r="D503" s="5">
+        <v>51.01</v>
+      </c>
+      <c r="E503" s="5">
+        <v>2223.71</v>
       </c>
       <c r="F503" s="16" t="s">
         <v>8</v>
       </c>
+      <c r="G503" s="13">
+        <f>AVERAGE(E503:E504)</f>
+        <v>2226.5150000000003</v>
+      </c>
+      <c r="H503" s="18">
+        <f>STDEV(E503:E504)</f>
+        <v>3.9668690424566218</v>
+      </c>
+      <c r="I503" s="3">
+        <v>2226.44</v>
+      </c>
+      <c r="J503" s="4">
+        <f>I503-G503</f>
+        <v>-7.5000000000272848E-2</v>
+      </c>
+      <c r="K503" s="5">
+        <f>G503+J503</f>
+        <v>2226.44</v>
+      </c>
     </row>
     <row r="504" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A504" s="9"/>
+      <c r="A504" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B504" s="31">
+        <v>45093</v>
+      </c>
       <c r="C504" s="10" t="s">
         <v>12</v>
+      </c>
+      <c r="D504" s="5">
+        <v>51.14</v>
+      </c>
+      <c r="E504" s="5">
+        <v>2229.3200000000002</v>
       </c>
       <c r="F504" s="16" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="505" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A505" s="9"/>
+      <c r="A505" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B505" s="31">
+        <v>45092</v>
+      </c>
       <c r="C505" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D505" s="5">
+        <v>50.1</v>
+      </c>
+      <c r="E505" s="14">
+        <v>2667.86</v>
+      </c>
       <c r="F505" s="16" t="s">
-        <v>96</v>
+        <v>471</v>
+      </c>
+      <c r="G505" s="13">
+        <f>AVERAGE(E506:E507)</f>
+        <v>2658.04</v>
+      </c>
+      <c r="H505" s="18">
+        <f>STDEV(E506:E507)</f>
+        <v>1.9657568516984221</v>
+      </c>
+      <c r="K505" s="5">
+        <f>G505+$J$490</f>
+        <v>2647.7850000000003</v>
       </c>
     </row>
     <row r="506" spans="1:11" x14ac:dyDescent="0.2">
@@ -14982,25 +15037,13 @@
         <v>12</v>
       </c>
       <c r="D506" s="5">
-        <v>50.1</v>
-      </c>
-      <c r="E506" s="14">
-        <v>2667.86</v>
+        <v>49.52</v>
+      </c>
+      <c r="E506" s="5">
+        <v>2656.65</v>
       </c>
       <c r="F506" s="16" t="s">
-        <v>474</v>
-      </c>
-      <c r="G506" s="13">
-        <f>AVERAGE(E507:E508)</f>
-        <v>2658.04</v>
-      </c>
-      <c r="H506" s="18">
-        <f>STDEV(E507:E508)</f>
-        <v>1.9657568516984221</v>
-      </c>
-      <c r="K506" s="5">
-        <f>G506+$J$472</f>
-        <v>2648.75</v>
+        <v>472</v>
       </c>
     </row>
     <row r="507" spans="1:11" x14ac:dyDescent="0.2">
@@ -15014,13 +15057,13 @@
         <v>12</v>
       </c>
       <c r="D507" s="5">
-        <v>49.52</v>
+        <v>49.55</v>
       </c>
       <c r="E507" s="5">
-        <v>2656.65</v>
+        <v>2659.43</v>
       </c>
       <c r="F507" s="16" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="508" spans="1:11" x14ac:dyDescent="0.2">
@@ -15034,13 +15077,25 @@
         <v>12</v>
       </c>
       <c r="D508" s="5">
-        <v>49.55</v>
+        <v>48.88</v>
       </c>
       <c r="E508" s="5">
-        <v>2659.43</v>
+        <v>2642.93</v>
       </c>
       <c r="F508" s="16" t="s">
-        <v>476</v>
+        <v>474</v>
+      </c>
+      <c r="G508" s="13">
+        <f>AVERAGE(E508:E509)</f>
+        <v>2640.355</v>
+      </c>
+      <c r="H508" s="18">
+        <f>STDEV(E508:E509)</f>
+        <v>3.6415999231104625</v>
+      </c>
+      <c r="K508" s="5">
+        <f>G508+$J$490</f>
+        <v>2630.1000000000004</v>
       </c>
     </row>
     <row r="509" spans="1:11" x14ac:dyDescent="0.2">
@@ -15054,25 +15109,13 @@
         <v>12</v>
       </c>
       <c r="D509" s="5">
-        <v>48.88</v>
+        <v>50.76</v>
       </c>
       <c r="E509" s="5">
-        <v>2642.93</v>
+        <v>2637.78</v>
       </c>
       <c r="F509" s="16" t="s">
-        <v>477</v>
-      </c>
-      <c r="G509" s="13">
-        <f>AVERAGE(E509:E510)</f>
-        <v>2640.355</v>
-      </c>
-      <c r="H509" s="18">
-        <f>STDEV(E509:E510)</f>
-        <v>3.6415999231104625</v>
-      </c>
-      <c r="K509" s="5">
-        <f>G509+$J$472</f>
-        <v>2631.0650000000001</v>
+        <v>475</v>
       </c>
     </row>
     <row r="510" spans="1:11" x14ac:dyDescent="0.2">
@@ -15086,13 +15129,25 @@
         <v>12</v>
       </c>
       <c r="D510" s="5">
-        <v>50.76</v>
+        <v>50.53</v>
       </c>
       <c r="E510" s="5">
-        <v>2637.78</v>
+        <v>2563.23</v>
       </c>
       <c r="F510" s="16" t="s">
-        <v>478</v>
+        <v>442</v>
+      </c>
+      <c r="G510" s="13">
+        <f>AVERAGE(E510:E511)</f>
+        <v>2560.4749999999999</v>
+      </c>
+      <c r="H510" s="18">
+        <f>STDEV(E510:E511)</f>
+        <v>3.8961583643380311</v>
+      </c>
+      <c r="K510" s="5">
+        <f>G510+$J$490</f>
+        <v>2550.2200000000003</v>
       </c>
     </row>
     <row r="511" spans="1:11" x14ac:dyDescent="0.2">
@@ -15106,25 +15161,13 @@
         <v>12</v>
       </c>
       <c r="D511" s="5">
-        <v>50.53</v>
+        <v>50.23</v>
       </c>
       <c r="E511" s="5">
-        <v>2563.23</v>
+        <v>2557.7199999999998</v>
       </c>
       <c r="F511" s="16" t="s">
-        <v>442</v>
-      </c>
-      <c r="G511" s="13">
-        <f>AVERAGE(E511:E512)</f>
-        <v>2560.4749999999999</v>
-      </c>
-      <c r="H511" s="18">
-        <f>STDEV(E511:E512)</f>
-        <v>3.8961583643380311</v>
-      </c>
-      <c r="K511" s="5">
-        <f>G511+$J$472</f>
-        <v>2551.1849999999999</v>
+        <v>443</v>
       </c>
     </row>
     <row r="512" spans="1:11" x14ac:dyDescent="0.2">
@@ -15138,13 +15181,25 @@
         <v>12</v>
       </c>
       <c r="D512" s="5">
-        <v>50.23</v>
+        <v>49.45</v>
       </c>
       <c r="E512" s="5">
-        <v>2557.7199999999998</v>
+        <v>2567.5</v>
       </c>
       <c r="F512" s="16" t="s">
-        <v>443</v>
+        <v>444</v>
+      </c>
+      <c r="G512" s="13">
+        <f>AVERAGE(E512:E513)</f>
+        <v>2567.0150000000003</v>
+      </c>
+      <c r="H512" s="18">
+        <f>STDEV(E512:E513)</f>
+        <v>0.68589357775080961</v>
+      </c>
+      <c r="K512" s="5">
+        <f>G512+$J$490</f>
+        <v>2556.7600000000007</v>
       </c>
     </row>
     <row r="513" spans="1:11" x14ac:dyDescent="0.2">
@@ -15158,25 +15213,13 @@
         <v>12</v>
       </c>
       <c r="D513" s="5">
-        <v>49.45</v>
+        <v>48.68</v>
       </c>
       <c r="E513" s="5">
-        <v>2567.5</v>
+        <v>2566.5300000000002</v>
       </c>
       <c r="F513" s="16" t="s">
-        <v>444</v>
-      </c>
-      <c r="G513" s="13">
-        <f>AVERAGE(E513:E514)</f>
-        <v>2567.0150000000003</v>
-      </c>
-      <c r="H513" s="18">
-        <f>STDEV(E513:E514)</f>
-        <v>0.68589357775080961</v>
-      </c>
-      <c r="K513" s="5">
-        <f>G513+$J$472</f>
-        <v>2557.7250000000004</v>
+        <v>445</v>
       </c>
     </row>
     <row r="514" spans="1:11" x14ac:dyDescent="0.2">
@@ -15184,138 +15227,367 @@
         <v>11</v>
       </c>
       <c r="B514" s="31">
-        <v>45092</v>
+        <v>45093</v>
       </c>
       <c r="C514" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D514" s="5">
-        <v>48.68</v>
+        <v>48.97</v>
       </c>
       <c r="E514" s="5">
-        <v>2566.5300000000002</v>
+        <v>2517.75</v>
       </c>
       <c r="F514" s="16" t="s">
-        <v>445</v>
+        <v>446</v>
+      </c>
+      <c r="G514" s="13">
+        <f>AVERAGE(E514:E515)</f>
+        <v>2517.4049999999997</v>
+      </c>
+      <c r="H514" s="18">
+        <f>STDEV(E514:E515)</f>
+        <v>0.48790367901875636</v>
+      </c>
+      <c r="K514" s="5">
+        <f>G514+$J$503</f>
+        <v>2517.3299999999995</v>
       </c>
     </row>
     <row r="515" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A515" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B515" s="31">
+        <v>45093</v>
+      </c>
       <c r="C515" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D515" s="5">
+        <v>49.58</v>
+      </c>
+      <c r="E515" s="5">
+        <v>2517.06</v>
+      </c>
       <c r="F515" s="16" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="516" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A516" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B516" s="31">
+        <v>45093</v>
+      </c>
       <c r="C516" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D516" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="E516" s="5" t="s">
+        <v>153</v>
+      </c>
       <c r="F516" s="16" t="s">
-        <v>447</v>
+        <v>448</v>
+      </c>
+      <c r="G516" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="H516" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="K516" s="5" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="517" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A517" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B517" s="31">
+        <v>45093</v>
+      </c>
       <c r="C517" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D517" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="E517" s="5" t="s">
+        <v>153</v>
+      </c>
       <c r="F517" s="16" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="518" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A518" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B518" s="31">
+        <v>45093</v>
+      </c>
       <c r="C518" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D518" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="E518" s="5" t="s">
+        <v>153</v>
+      </c>
       <c r="F518" s="16" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="519" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A519" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B519" s="31">
+        <v>45093</v>
+      </c>
       <c r="C519" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D519" s="5">
+        <v>50.4</v>
+      </c>
+      <c r="E519" s="5">
+        <v>2507.29</v>
+      </c>
       <c r="F519" s="16" t="s">
-        <v>450</v>
+        <v>451</v>
+      </c>
+      <c r="G519" s="13">
+        <f>AVERAGE(E519,E521)</f>
+        <v>2506.02</v>
+      </c>
+      <c r="H519" s="18">
+        <f>STDEV(E519,E521)</f>
+        <v>1.7960512242138049</v>
+      </c>
+      <c r="K519" s="5">
+        <f>G519+$J$503</f>
+        <v>2505.9449999999997</v>
       </c>
     </row>
     <row r="520" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A520" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B520" s="31">
+        <v>45093</v>
+      </c>
       <c r="C520" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D520" s="5">
+        <v>49.48</v>
+      </c>
+      <c r="E520" s="14">
+        <v>2496.6</v>
+      </c>
       <c r="F520" s="16" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="521" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A521" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B521" s="31">
+        <v>45093</v>
+      </c>
       <c r="C521" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D521" s="5">
+        <v>48.81</v>
+      </c>
+      <c r="E521" s="5">
+        <v>2504.75</v>
+      </c>
       <c r="F521" s="16" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="522" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A522" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B522" s="31">
+        <v>45093</v>
+      </c>
       <c r="C522" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D522" s="5">
+        <v>48.83</v>
+      </c>
+      <c r="E522" s="5">
+        <v>2568.86</v>
+      </c>
       <c r="F522" s="16" t="s">
-        <v>453</v>
+        <v>454</v>
+      </c>
+      <c r="G522" s="13">
+        <f>AVERAGE(E522,E524)</f>
+        <v>2567.92</v>
+      </c>
+      <c r="H522" s="18">
+        <f>STDEV(E522,E524)</f>
+        <v>1.3293607486307866</v>
+      </c>
+      <c r="K522" s="5">
+        <f>G522+$J$503</f>
+        <v>2567.8449999999998</v>
       </c>
     </row>
     <row r="523" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A523" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B523" s="31">
+        <v>45093</v>
+      </c>
       <c r="C523" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D523" s="5">
+        <v>51.07</v>
+      </c>
+      <c r="E523" s="14">
+        <v>2558.5700000000002</v>
+      </c>
       <c r="F523" s="16" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="524" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A524" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B524" s="31">
+        <v>45093</v>
+      </c>
       <c r="C524" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D524" s="5">
+        <v>49.28</v>
+      </c>
+      <c r="E524" s="5">
+        <v>2566.98</v>
+      </c>
       <c r="F524" s="16" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="525" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A525" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B525" s="31">
+        <v>45093</v>
+      </c>
       <c r="C525" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D525" s="5">
+        <v>50.65</v>
+      </c>
+      <c r="E525" s="5">
+        <v>2515.42</v>
+      </c>
       <c r="F525" s="16" t="s">
-        <v>456</v>
+        <v>457</v>
+      </c>
+      <c r="G525" s="13">
+        <f>AVERAGE(E525:E526)</f>
+        <v>2516.4650000000001</v>
+      </c>
+      <c r="H525" s="18">
+        <f>STDEV(E525:E526)</f>
+        <v>1.4778531726799873</v>
+      </c>
+      <c r="K525" s="5">
+        <f>G525+$J$503</f>
+        <v>2516.39</v>
       </c>
     </row>
     <row r="526" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A526" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B526" s="31">
+        <v>45093</v>
+      </c>
       <c r="C526" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D526" s="5">
+        <v>49.4</v>
+      </c>
+      <c r="E526" s="5">
+        <v>2517.5100000000002</v>
+      </c>
       <c r="F526" s="16" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="527" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A527" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B527" s="31">
+        <v>45093</v>
+      </c>
       <c r="C527" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D527" s="5">
+        <v>50.65</v>
+      </c>
+      <c r="E527" s="5">
+        <v>2632.19</v>
+      </c>
       <c r="F527" s="16" t="s">
-        <v>458</v>
+        <v>459</v>
+      </c>
+      <c r="G527" s="13">
+        <f>AVERAGE(E527:E528)</f>
+        <v>2633.46</v>
+      </c>
+      <c r="H527" s="18">
+        <f>STDEV(E527:E528)</f>
+        <v>1.7960512242138049</v>
+      </c>
+      <c r="K527" s="5">
+        <f>G527+$J$503</f>
+        <v>2633.3849999999998</v>
       </c>
     </row>
     <row r="528" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A528" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B528" s="31">
+        <v>45093</v>
+      </c>
       <c r="C528" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D528" s="5">
+        <v>49.16</v>
+      </c>
+      <c r="E528" s="5">
+        <v>2634.73</v>
+      </c>
       <c r="F528" s="16" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="529" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C529" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F529" s="16" t="s">
         <v>460</v>
       </c>
     </row>
@@ -15324,7 +15596,7 @@
         <v>12</v>
       </c>
       <c r="F530" s="16" t="s">
-        <v>461</v>
+        <v>8</v>
       </c>
     </row>
     <row r="531" spans="3:6" x14ac:dyDescent="0.2">
@@ -15332,7 +15604,7 @@
         <v>12</v>
       </c>
       <c r="F531" s="16" t="s">
-        <v>462</v>
+        <v>9</v>
       </c>
     </row>
     <row r="532" spans="3:6" x14ac:dyDescent="0.2">
@@ -15340,7 +15612,15 @@
         <v>12</v>
       </c>
       <c r="F532" s="16" t="s">
-        <v>463</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="533" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C533" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F533" s="16" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="534" spans="3:6" x14ac:dyDescent="0.2">
@@ -15348,7 +15628,7 @@
         <v>12</v>
       </c>
       <c r="F534" s="16" t="s">
-        <v>8</v>
+        <v>477</v>
       </c>
     </row>
     <row r="535" spans="3:6" x14ac:dyDescent="0.2">
@@ -15356,7 +15636,7 @@
         <v>12</v>
       </c>
       <c r="F535" s="16" t="s">
-        <v>9</v>
+        <v>478</v>
       </c>
     </row>
     <row r="536" spans="3:6" x14ac:dyDescent="0.2">
@@ -15364,7 +15644,7 @@
         <v>12</v>
       </c>
       <c r="F536" s="16" t="s">
-        <v>96</v>
+        <v>479</v>
       </c>
     </row>
     <row r="537" spans="3:6" x14ac:dyDescent="0.2">
@@ -15372,7 +15652,7 @@
         <v>12</v>
       </c>
       <c r="F537" s="16" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
     </row>
     <row r="538" spans="3:6" x14ac:dyDescent="0.2">
@@ -15380,7 +15660,7 @@
         <v>12</v>
       </c>
       <c r="F538" s="16" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="539" spans="3:6" x14ac:dyDescent="0.2">
@@ -15388,7 +15668,7 @@
         <v>12</v>
       </c>
       <c r="F539" s="16" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="540" spans="3:6" x14ac:dyDescent="0.2">
@@ -15396,7 +15676,7 @@
         <v>12</v>
       </c>
       <c r="F540" s="16" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="541" spans="3:6" x14ac:dyDescent="0.2">
@@ -15404,7 +15684,7 @@
         <v>12</v>
       </c>
       <c r="F541" s="16" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
     </row>
     <row r="542" spans="3:6" x14ac:dyDescent="0.2">
@@ -15412,7 +15692,7 @@
         <v>12</v>
       </c>
       <c r="F542" s="16" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row r="543" spans="3:6" x14ac:dyDescent="0.2">
@@ -15420,7 +15700,7 @@
         <v>12</v>
       </c>
       <c r="F543" s="16" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row r="544" spans="3:6" x14ac:dyDescent="0.2">
@@ -15428,7 +15708,7 @@
         <v>12</v>
       </c>
       <c r="F544" s="16" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row r="545" spans="3:6" x14ac:dyDescent="0.2">
@@ -15436,7 +15716,7 @@
         <v>12</v>
       </c>
       <c r="F545" s="16" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="546" spans="3:6" x14ac:dyDescent="0.2">
@@ -15444,7 +15724,7 @@
         <v>12</v>
       </c>
       <c r="F546" s="16" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row r="547" spans="3:6" x14ac:dyDescent="0.2">
@@ -15452,7 +15732,7 @@
         <v>12</v>
       </c>
       <c r="F547" s="16" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="548" spans="3:6" x14ac:dyDescent="0.2">
@@ -15460,7 +15740,7 @@
         <v>12</v>
       </c>
       <c r="F548" s="16" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="549" spans="3:6" x14ac:dyDescent="0.2">
@@ -15468,7 +15748,7 @@
         <v>12</v>
       </c>
       <c r="F549" s="16" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
     </row>
     <row r="550" spans="3:6" x14ac:dyDescent="0.2">
@@ -15476,7 +15756,7 @@
         <v>12</v>
       </c>
       <c r="F550" s="16" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
     </row>
     <row r="551" spans="3:6" x14ac:dyDescent="0.2">
@@ -15484,7 +15764,7 @@
         <v>12</v>
       </c>
       <c r="F551" s="16" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="552" spans="3:6" x14ac:dyDescent="0.2">
@@ -15492,7 +15772,7 @@
         <v>12</v>
       </c>
       <c r="F552" s="16" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="553" spans="3:6" x14ac:dyDescent="0.2">
@@ -15500,7 +15780,7 @@
         <v>12</v>
       </c>
       <c r="F553" s="16" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="554" spans="3:6" x14ac:dyDescent="0.2">
@@ -15508,7 +15788,7 @@
         <v>12</v>
       </c>
       <c r="F554" s="16" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="555" spans="3:6" x14ac:dyDescent="0.2">
@@ -15516,7 +15796,7 @@
         <v>12</v>
       </c>
       <c r="F555" s="16" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="556" spans="3:6" x14ac:dyDescent="0.2">
@@ -15524,7 +15804,7 @@
         <v>12</v>
       </c>
       <c r="F556" s="16" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row r="557" spans="3:6" x14ac:dyDescent="0.2">
@@ -15532,7 +15812,7 @@
         <v>12</v>
       </c>
       <c r="F557" s="16" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="558" spans="3:6" x14ac:dyDescent="0.2">
@@ -15540,7 +15820,7 @@
         <v>12</v>
       </c>
       <c r="F558" s="16" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
     </row>
     <row r="559" spans="3:6" x14ac:dyDescent="0.2">
@@ -15548,7 +15828,7 @@
         <v>12</v>
       </c>
       <c r="F559" s="16" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="560" spans="3:6" x14ac:dyDescent="0.2">
@@ -15556,7 +15836,7 @@
         <v>12</v>
       </c>
       <c r="F560" s="16" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="561" spans="3:6" x14ac:dyDescent="0.2">
@@ -15564,7 +15844,7 @@
         <v>12</v>
       </c>
       <c r="F561" s="16" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row r="562" spans="3:6" x14ac:dyDescent="0.2">
@@ -15572,23 +15852,18 @@
         <v>12</v>
       </c>
       <c r="F562" s="16" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
     </row>
     <row r="563" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C563" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F563" s="16" t="s">
-        <v>505</v>
-      </c>
+      <c r="F563" s="16"/>
     </row>
     <row r="564" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C564" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F564" s="16" t="s">
-        <v>506</v>
+        <v>8</v>
       </c>
     </row>
     <row r="565" spans="3:6" x14ac:dyDescent="0.2">
@@ -15596,7 +15871,7 @@
         <v>12</v>
       </c>
       <c r="F565" s="16" t="s">
-        <v>507</v>
+        <v>9</v>
       </c>
     </row>
     <row r="566" spans="3:6" x14ac:dyDescent="0.2">
@@ -15604,18 +15879,23 @@
         <v>12</v>
       </c>
       <c r="F566" s="16" t="s">
-        <v>508</v>
+        <v>96</v>
       </c>
     </row>
     <row r="567" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="F567" s="16"/>
+      <c r="C567" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F567" s="16" t="s">
+        <v>506</v>
+      </c>
     </row>
     <row r="568" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C568" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F568" s="16" t="s">
-        <v>8</v>
+        <v>507</v>
       </c>
     </row>
     <row r="569" spans="3:6" x14ac:dyDescent="0.2">
@@ -15623,7 +15903,7 @@
         <v>12</v>
       </c>
       <c r="F569" s="16" t="s">
-        <v>9</v>
+        <v>508</v>
       </c>
     </row>
     <row r="570" spans="3:6" x14ac:dyDescent="0.2">
@@ -15631,7 +15911,7 @@
         <v>12</v>
       </c>
       <c r="F570" s="16" t="s">
-        <v>96</v>
+        <v>509</v>
       </c>
     </row>
     <row r="571" spans="3:6" x14ac:dyDescent="0.2">
@@ -15639,7 +15919,7 @@
         <v>12</v>
       </c>
       <c r="F571" s="16" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row r="572" spans="3:6" x14ac:dyDescent="0.2">
@@ -15647,7 +15927,7 @@
         <v>12</v>
       </c>
       <c r="F572" s="16" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="573" spans="3:6" x14ac:dyDescent="0.2">
@@ -15655,7 +15935,7 @@
         <v>12</v>
       </c>
       <c r="F573" s="16" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="574" spans="3:6" x14ac:dyDescent="0.2">
@@ -15663,7 +15943,7 @@
         <v>12</v>
       </c>
       <c r="F574" s="16" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="575" spans="3:6" x14ac:dyDescent="0.2">
@@ -15671,7 +15951,7 @@
         <v>12</v>
       </c>
       <c r="F575" s="16" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row r="576" spans="3:6" x14ac:dyDescent="0.2">
@@ -15679,7 +15959,7 @@
         <v>12</v>
       </c>
       <c r="F576" s="16" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="577" spans="3:6" x14ac:dyDescent="0.2">
@@ -15687,7 +15967,7 @@
         <v>12</v>
       </c>
       <c r="F577" s="16" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="578" spans="3:6" x14ac:dyDescent="0.2">
@@ -15695,7 +15975,7 @@
         <v>12</v>
       </c>
       <c r="F578" s="16" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="579" spans="3:6" x14ac:dyDescent="0.2">
@@ -15703,7 +15983,7 @@
         <v>12</v>
       </c>
       <c r="F579" s="16" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="580" spans="3:6" x14ac:dyDescent="0.2">
@@ -15711,7 +15991,7 @@
         <v>12</v>
       </c>
       <c r="F580" s="16" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="581" spans="3:6" x14ac:dyDescent="0.2">
@@ -15719,7 +15999,7 @@
         <v>12</v>
       </c>
       <c r="F581" s="16" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="582" spans="3:6" x14ac:dyDescent="0.2">
@@ -15727,7 +16007,7 @@
         <v>12</v>
       </c>
       <c r="F582" s="16" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="583" spans="3:6" x14ac:dyDescent="0.2">
@@ -15735,7 +16015,7 @@
         <v>12</v>
       </c>
       <c r="F583" s="16" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row r="584" spans="3:6" x14ac:dyDescent="0.2">
@@ -15743,7 +16023,7 @@
         <v>12</v>
       </c>
       <c r="F584" s="16" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row r="585" spans="3:6" x14ac:dyDescent="0.2">
@@ -15751,7 +16031,7 @@
         <v>12</v>
       </c>
       <c r="F585" s="16" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="586" spans="3:6" x14ac:dyDescent="0.2">
@@ -15759,7 +16039,7 @@
         <v>12</v>
       </c>
       <c r="F586" s="16" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
     </row>
     <row r="587" spans="3:6" x14ac:dyDescent="0.2">
@@ -15767,7 +16047,7 @@
         <v>12</v>
       </c>
       <c r="F587" s="16" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="588" spans="3:6" x14ac:dyDescent="0.2">
@@ -15775,7 +16055,7 @@
         <v>12</v>
       </c>
       <c r="F588" s="16" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="589" spans="3:6" x14ac:dyDescent="0.2">
@@ -15783,7 +16063,7 @@
         <v>12</v>
       </c>
       <c r="F589" s="16" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row r="590" spans="3:6" x14ac:dyDescent="0.2">
@@ -15791,7 +16071,7 @@
         <v>12</v>
       </c>
       <c r="F590" s="16" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="591" spans="3:6" x14ac:dyDescent="0.2">
@@ -15799,7 +16079,7 @@
         <v>12</v>
       </c>
       <c r="F591" s="16" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="592" spans="3:6" x14ac:dyDescent="0.2">
@@ -15807,7 +16087,7 @@
         <v>12</v>
       </c>
       <c r="F592" s="16" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
     <row r="593" spans="3:6" x14ac:dyDescent="0.2">
@@ -15815,7 +16095,7 @@
         <v>12</v>
       </c>
       <c r="F593" s="16" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
     </row>
     <row r="594" spans="3:6" x14ac:dyDescent="0.2">
@@ -15823,7 +16103,7 @@
         <v>12</v>
       </c>
       <c r="F594" s="16" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
     <row r="595" spans="3:6" x14ac:dyDescent="0.2">
@@ -15831,7 +16111,7 @@
         <v>12</v>
       </c>
       <c r="F595" s="16" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="596" spans="3:6" x14ac:dyDescent="0.2">
@@ -15839,14 +16119,6 @@
         <v>12</v>
       </c>
       <c r="F596" s="16" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="597" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C597" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F597" s="16" t="s">
         <v>535</v>
       </c>
     </row>
@@ -15855,7 +16127,7 @@
         <v>12</v>
       </c>
       <c r="F598" s="16" t="s">
-        <v>536</v>
+        <v>8</v>
       </c>
     </row>
     <row r="599" spans="3:6" x14ac:dyDescent="0.2">
@@ -15863,7 +16135,7 @@
         <v>12</v>
       </c>
       <c r="F599" s="16" t="s">
-        <v>537</v>
+        <v>9</v>
       </c>
     </row>
     <row r="600" spans="3:6" x14ac:dyDescent="0.2">
@@ -15871,7 +16143,15 @@
         <v>12</v>
       </c>
       <c r="F600" s="16" t="s">
-        <v>538</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="601" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C601" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F601" s="16" t="s">
+        <v>536</v>
       </c>
     </row>
     <row r="602" spans="3:6" x14ac:dyDescent="0.2">
@@ -15879,7 +16159,7 @@
         <v>12</v>
       </c>
       <c r="F602" s="16" t="s">
-        <v>8</v>
+        <v>537</v>
       </c>
     </row>
     <row r="603" spans="3:6" x14ac:dyDescent="0.2">
@@ -15887,7 +16167,7 @@
         <v>12</v>
       </c>
       <c r="F603" s="16" t="s">
-        <v>9</v>
+        <v>538</v>
       </c>
     </row>
     <row r="604" spans="3:6" x14ac:dyDescent="0.2">
@@ -15895,7 +16175,7 @@
         <v>12</v>
       </c>
       <c r="F604" s="16" t="s">
-        <v>96</v>
+        <v>539</v>
       </c>
     </row>
     <row r="605" spans="3:6" x14ac:dyDescent="0.2">
@@ -15903,7 +16183,7 @@
         <v>12</v>
       </c>
       <c r="F605" s="16" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="606" spans="3:6" x14ac:dyDescent="0.2">
@@ -15911,7 +16191,7 @@
         <v>12</v>
       </c>
       <c r="F606" s="16" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="607" spans="3:6" x14ac:dyDescent="0.2">
@@ -15919,7 +16199,7 @@
         <v>12</v>
       </c>
       <c r="F607" s="16" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="608" spans="3:6" x14ac:dyDescent="0.2">
@@ -15927,7 +16207,7 @@
         <v>12</v>
       </c>
       <c r="F608" s="16" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="609" spans="3:6" x14ac:dyDescent="0.2">
@@ -15935,7 +16215,7 @@
         <v>12</v>
       </c>
       <c r="F609" s="16" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
     </row>
     <row r="610" spans="3:6" x14ac:dyDescent="0.2">
@@ -15943,7 +16223,7 @@
         <v>12</v>
       </c>
       <c r="F610" s="16" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
     <row r="611" spans="3:6" x14ac:dyDescent="0.2">
@@ -15951,7 +16231,7 @@
         <v>12</v>
       </c>
       <c r="F611" s="16" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="612" spans="3:6" x14ac:dyDescent="0.2">
@@ -15959,7 +16239,7 @@
         <v>12</v>
       </c>
       <c r="F612" s="16" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
     <row r="613" spans="3:6" x14ac:dyDescent="0.2">
@@ -15967,7 +16247,7 @@
         <v>12</v>
       </c>
       <c r="F613" s="16" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="614" spans="3:6" x14ac:dyDescent="0.2">
@@ -15975,7 +16255,7 @@
         <v>12</v>
       </c>
       <c r="F614" s="16" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="615" spans="3:6" x14ac:dyDescent="0.2">
@@ -15983,7 +16263,7 @@
         <v>12</v>
       </c>
       <c r="F615" s="16" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="616" spans="3:6" x14ac:dyDescent="0.2">
@@ -15991,7 +16271,7 @@
         <v>12</v>
       </c>
       <c r="F616" s="16" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="617" spans="3:6" x14ac:dyDescent="0.2">
@@ -15999,7 +16279,7 @@
         <v>12</v>
       </c>
       <c r="F617" s="16" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="618" spans="3:6" x14ac:dyDescent="0.2">
@@ -16007,7 +16287,7 @@
         <v>12</v>
       </c>
       <c r="F618" s="16" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
     <row r="619" spans="3:6" x14ac:dyDescent="0.2">
@@ -16015,7 +16295,7 @@
         <v>12</v>
       </c>
       <c r="F619" s="16" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="620" spans="3:6" x14ac:dyDescent="0.2">
@@ -16023,7 +16303,7 @@
         <v>12</v>
       </c>
       <c r="F620" s="16" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row r="621" spans="3:6" x14ac:dyDescent="0.2">
@@ -16031,7 +16311,7 @@
         <v>12</v>
       </c>
       <c r="F621" s="16" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
     <row r="622" spans="3:6" x14ac:dyDescent="0.2">
@@ -16039,7 +16319,7 @@
         <v>12</v>
       </c>
       <c r="F622" s="16" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="623" spans="3:6" x14ac:dyDescent="0.2">
@@ -16047,7 +16327,7 @@
         <v>12</v>
       </c>
       <c r="F623" s="16" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="624" spans="3:6" x14ac:dyDescent="0.2">
@@ -16055,7 +16335,7 @@
         <v>12</v>
       </c>
       <c r="F624" s="16" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
     </row>
     <row r="625" spans="3:6" x14ac:dyDescent="0.2">
@@ -16063,7 +16343,7 @@
         <v>12</v>
       </c>
       <c r="F625" s="16" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row r="626" spans="3:6" x14ac:dyDescent="0.2">
@@ -16071,7 +16351,7 @@
         <v>12</v>
       </c>
       <c r="F626" s="16" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="627" spans="3:6" x14ac:dyDescent="0.2">
@@ -16079,7 +16359,7 @@
         <v>12</v>
       </c>
       <c r="F627" s="16" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="628" spans="3:6" x14ac:dyDescent="0.2">
@@ -16087,7 +16367,7 @@
         <v>12</v>
       </c>
       <c r="F628" s="16" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="629" spans="3:6" x14ac:dyDescent="0.2">
@@ -16095,7 +16375,7 @@
         <v>12</v>
       </c>
       <c r="F629" s="16" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
     </row>
     <row r="630" spans="3:6" x14ac:dyDescent="0.2">
@@ -16103,39 +16383,7 @@
         <v>12</v>
       </c>
       <c r="F630" s="16" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="631" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C631" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F631" s="16" t="s">
         <v>565</v>
-      </c>
-    </row>
-    <row r="632" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C632" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F632" s="16" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="633" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C633" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F633" s="16" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="634" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C634" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F634" s="16" t="s">
-        <v>568</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ALK AMB T2 + Light + O2 End T2 experiment
</commit_message>
<xml_diff>
--- a/Data/Spring_2023/BenthFun_Alkalinity.xlsx
+++ b/Data/Spring_2023/BenthFun_Alkalinity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremy/Library/Mobile Documents/com~apple~CloudDocs/Documents/Documents/Post-Doc/Projets/Villefranche/Projets/BenthFun – Jeremy/BenthFun/Data/Spring_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3523E394-14DB-F04A-925D-73E1DAF31A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F9120FB-345B-6549-95A6-3C6B6EB30F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1923" uniqueCount="558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1944" uniqueCount="555">
   <si>
     <t>Operator</t>
   </si>
@@ -1621,9 +1621,6 @@
     <t>T2_t0_AMB_blank_02b</t>
   </si>
   <si>
-    <t>T2_t0_AMB_blank_02c</t>
-  </si>
-  <si>
     <t>T2_t1_AMB_tile_01a</t>
   </si>
   <si>
@@ -1636,9 +1633,6 @@
     <t>T2_t1_AMB_tile_02a</t>
   </si>
   <si>
-    <t>T2_t1_AMB_tile_02b</t>
-  </si>
-  <si>
     <t>T2_t1_AMB_tile_02c</t>
   </si>
   <si>
@@ -1657,9 +1651,6 @@
     <t>T2_t1_AMB_blank_01b</t>
   </si>
   <si>
-    <t>T2_t1_AMB_blank_01c</t>
-  </si>
-  <si>
     <t>T2_t1_AMB_tile_04a</t>
   </si>
   <si>
@@ -1684,18 +1675,12 @@
     <t>T2_t1_AMB_tile_06b</t>
   </si>
   <si>
-    <t>T2_t1_AMB_tile_06c</t>
-  </si>
-  <si>
     <t>T2_t1_AMB_blank_02a</t>
   </si>
   <si>
     <t>T2_t1_AMB_blank_02b</t>
   </si>
   <si>
-    <t>T2_t1_AMB_blank_02c</t>
-  </si>
-  <si>
     <t>PI_t5_AMB_Tile_3d</t>
   </si>
   <si>
@@ -1709,6 +1694,12 @@
   </si>
   <si>
     <t>T2_t1_LOW_blank_01d</t>
+  </si>
+  <si>
+    <t>T2_t1_AMB_tile_02e</t>
+  </si>
+  <si>
+    <t>T2_t1_AMB_tile_06e</t>
   </si>
 </sst>
 </file>
@@ -2192,11 +2183,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L616"/>
+  <dimension ref="A1:L612"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="73" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A552" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K584" sqref="K584"/>
+      <pane ySplit="1" topLeftCell="A585" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G596" sqref="G596"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12964,7 +12955,7 @@
         <v>2468.38</v>
       </c>
       <c r="F424" s="32" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
     </row>
     <row r="425" spans="1:11" x14ac:dyDescent="0.2">
@@ -13160,7 +13151,7 @@
         <v>2530.84</v>
       </c>
       <c r="F432" s="32" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="433" spans="1:12" x14ac:dyDescent="0.2">
@@ -14557,7 +14548,7 @@
     </row>
     <row r="489" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A489" s="9" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="B489" s="31">
         <v>45092</v>
@@ -14572,12 +14563,12 @@
         <v>2724.84</v>
       </c>
       <c r="F489" s="16" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
     </row>
     <row r="490" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A490" s="9" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="B490" s="31">
         <v>45092</v>
@@ -14619,7 +14610,7 @@
     </row>
     <row r="491" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A491" s="9" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="B491" s="31">
         <v>45092</v>
@@ -14639,7 +14630,7 @@
     </row>
     <row r="492" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A492" s="9" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="B492" s="31">
         <v>45092</v>
@@ -14659,7 +14650,7 @@
     </row>
     <row r="493" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A493" s="9" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="B493" s="31">
         <v>45092</v>
@@ -14691,7 +14682,7 @@
     </row>
     <row r="494" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A494" s="9" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="B494" s="31">
         <v>45092</v>
@@ -14711,7 +14702,7 @@
     </row>
     <row r="495" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A495" s="9" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="B495" s="31">
         <v>45092</v>
@@ -16714,7 +16705,7 @@
         <v>2700.17</v>
       </c>
       <c r="F574" s="16" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
     </row>
     <row r="575" spans="1:12" x14ac:dyDescent="0.2">
@@ -17008,247 +16999,663 @@
       </c>
     </row>
     <row r="586" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C586" s="10"/>
-      <c r="F586" s="16"/>
+      <c r="A586" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B586" s="31">
+        <v>45099</v>
+      </c>
+      <c r="C586" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D586" s="5">
+        <v>49.98</v>
+      </c>
+      <c r="E586" s="14">
+        <v>2715.04</v>
+      </c>
+      <c r="F586" s="16" t="s">
+        <v>523</v>
+      </c>
+      <c r="G586" s="13">
+        <f>AVERAGE(E587:E588)</f>
+        <v>2693.16</v>
+      </c>
+      <c r="H586" s="18">
+        <f>STDEV(E587:E588)</f>
+        <v>0.33941125496955571</v>
+      </c>
+      <c r="K586" s="5">
+        <f>G586+$J$575</f>
+        <v>2684.3249999999998</v>
+      </c>
     </row>
     <row r="587" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A587" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B587" s="31">
+        <v>45099</v>
+      </c>
       <c r="C587" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D587" s="5">
+        <v>50.43</v>
+      </c>
+      <c r="E587" s="5">
+        <v>2692.92</v>
+      </c>
       <c r="F587" s="16" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="588" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A588" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B588" s="31">
+        <v>45099</v>
+      </c>
       <c r="C588" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D588" s="5">
+        <v>50.15</v>
+      </c>
+      <c r="E588" s="5">
+        <v>2693.4</v>
+      </c>
       <c r="F588" s="16" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
     </row>
     <row r="589" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A589" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B589" s="31">
+        <v>45099</v>
+      </c>
       <c r="C589" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D589" s="5">
+        <v>50.55</v>
+      </c>
+      <c r="E589" s="5">
+        <v>2686.54</v>
+      </c>
       <c r="F589" s="16" t="s">
-        <v>525</v>
+        <v>526</v>
+      </c>
+      <c r="G589" s="13">
+        <f>AVERAGE(E589:E590)</f>
+        <v>2684.17</v>
+      </c>
+      <c r="H589" s="18">
+        <f>STDEV(E589:E590)</f>
+        <v>3.3516861428240809</v>
+      </c>
+      <c r="K589" s="5">
+        <f>G589+$J$575</f>
+        <v>2675.335</v>
       </c>
     </row>
     <row r="590" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A590" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B590" s="31">
+        <v>45099</v>
+      </c>
       <c r="C590" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D590" s="5">
+        <v>50.75</v>
+      </c>
+      <c r="E590" s="5">
+        <v>2681.8</v>
+      </c>
       <c r="F590" s="16" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="591" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A591" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B591" s="31">
+        <v>45099</v>
+      </c>
       <c r="C591" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D591" s="5">
+        <v>49.37</v>
+      </c>
+      <c r="E591" s="5">
+        <v>2538.7600000000002</v>
+      </c>
       <c r="F591" s="16" t="s">
-        <v>527</v>
+        <v>528</v>
+      </c>
+      <c r="G591" s="13">
+        <f>AVERAGE(E591,E593)</f>
+        <v>2539.2200000000003</v>
+      </c>
+      <c r="H591" s="18">
+        <f>STDEV(E591,E593)</f>
+        <v>0.65053823869135363</v>
+      </c>
+      <c r="K591" s="5">
+        <f>G591+$J$575</f>
+        <v>2530.3850000000002</v>
       </c>
     </row>
     <row r="592" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A592" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B592" s="31">
+        <v>45099</v>
+      </c>
       <c r="C592" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D592" s="5">
+        <v>50.21</v>
+      </c>
+      <c r="E592" s="14">
+        <v>2524.25</v>
+      </c>
       <c r="F592" s="16" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="593" spans="3:6" x14ac:dyDescent="0.2">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="593" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A593" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B593" s="31">
+        <v>45099</v>
+      </c>
       <c r="C593" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D593" s="5">
+        <v>48.43</v>
+      </c>
+      <c r="E593" s="5">
+        <v>2539.6799999999998</v>
+      </c>
       <c r="F593" s="16" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="594" spans="3:6" x14ac:dyDescent="0.2">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="594" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A594" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B594" s="31">
+        <v>45099</v>
+      </c>
       <c r="C594" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D594" s="5">
+        <v>50.41</v>
+      </c>
+      <c r="E594" s="14">
+        <v>2578.7800000000002</v>
+      </c>
       <c r="F594" s="16" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="595" spans="3:6" x14ac:dyDescent="0.2">
+        <v>531</v>
+      </c>
+      <c r="G594" s="13">
+        <f>AVERAGE(E595:E596)</f>
+        <v>2590.33</v>
+      </c>
+      <c r="H594" s="18">
+        <f>STDEV(E595:E596)</f>
+        <v>3.0688434303497192</v>
+      </c>
+      <c r="K594" s="5">
+        <f>G594+$J$575</f>
+        <v>2581.4949999999999</v>
+      </c>
+    </row>
+    <row r="595" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A595" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B595" s="31">
+        <v>45099</v>
+      </c>
       <c r="C595" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D595" s="5">
+        <v>49.38</v>
+      </c>
+      <c r="E595" s="5">
+        <v>2592.5</v>
+      </c>
       <c r="F595" s="16" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="596" spans="3:6" x14ac:dyDescent="0.2">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="596" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A596" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B596" s="31">
+        <v>45099</v>
+      </c>
       <c r="C596" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D596" s="5">
+        <v>49.42</v>
+      </c>
+      <c r="E596" s="5">
+        <v>2588.16</v>
+      </c>
       <c r="F596" s="16" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="597" spans="3:6" x14ac:dyDescent="0.2">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="597" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A597" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B597" s="31">
+        <v>45099</v>
+      </c>
       <c r="C597" s="10" t="s">
         <v>12</v>
+      </c>
+      <c r="D597" s="5">
+        <v>51.38</v>
+      </c>
+      <c r="E597" s="14">
+        <v>2545.4299999999998</v>
       </c>
       <c r="F597" s="16" t="s">
         <v>533</v>
       </c>
-    </row>
-    <row r="598" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="G597" s="13">
+        <f>AVERAGE(E598:E599)</f>
+        <v>2558.52</v>
+      </c>
+      <c r="H597" s="18">
+        <f>STDEV(E598:E599)</f>
+        <v>3.1112698372205521</v>
+      </c>
+      <c r="K597" s="5">
+        <f>G597+$J$575</f>
+        <v>2549.6849999999999</v>
+      </c>
+    </row>
+    <row r="598" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A598" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B598" s="31">
+        <v>45099</v>
+      </c>
       <c r="C598" s="10" t="s">
         <v>12</v>
+      </c>
+      <c r="D598" s="5">
+        <v>51.28</v>
+      </c>
+      <c r="E598" s="5">
+        <v>2560.7199999999998</v>
       </c>
       <c r="F598" s="16" t="s">
         <v>534</v>
       </c>
     </row>
-    <row r="599" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="599" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A599" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B599" s="31">
+        <v>45099</v>
+      </c>
       <c r="C599" s="10" t="s">
         <v>12</v>
+      </c>
+      <c r="D599" s="5">
+        <v>50.12</v>
+      </c>
+      <c r="E599" s="5">
+        <v>2556.3200000000002</v>
       </c>
       <c r="F599" s="16" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="600" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="600" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A600" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B600" s="31">
+        <v>45099</v>
+      </c>
       <c r="C600" s="10" t="s">
         <v>12</v>
+      </c>
+      <c r="D600" s="5">
+        <v>51.33</v>
+      </c>
+      <c r="E600" s="5">
+        <v>2680.89</v>
       </c>
       <c r="F600" s="16" t="s">
         <v>536</v>
       </c>
-    </row>
-    <row r="601" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="G600" s="13">
+        <f>AVERAGE(E600:E601)</f>
+        <v>2678.87</v>
+      </c>
+      <c r="H600" s="18">
+        <f>STDEV(E600:E601)</f>
+        <v>2.8567113959936261</v>
+      </c>
+      <c r="K600" s="5">
+        <f>G600+$J$575</f>
+        <v>2670.0349999999999</v>
+      </c>
+    </row>
+    <row r="601" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A601" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B601" s="31">
+        <v>45099</v>
+      </c>
       <c r="C601" s="10" t="s">
         <v>12</v>
+      </c>
+      <c r="D601" s="5">
+        <v>51.22</v>
+      </c>
+      <c r="E601" s="5">
+        <v>2676.85</v>
       </c>
       <c r="F601" s="16" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="602" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="602" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A602" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B602" s="31">
+        <v>45099</v>
+      </c>
       <c r="C602" s="10" t="s">
         <v>12</v>
+      </c>
+      <c r="D602" s="5">
+        <v>53.6</v>
+      </c>
+      <c r="E602" s="14">
+        <v>2626.42</v>
       </c>
       <c r="F602" s="16" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="603" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="G602" s="13">
+        <f>AVERAGE(E603:E604)</f>
+        <v>2616.3000000000002</v>
+      </c>
+      <c r="H602" s="18">
+        <f>STDEV(E603:E604)</f>
+        <v>3.8466608896548569</v>
+      </c>
+      <c r="K602" s="5">
+        <f>G602+$J$575</f>
+        <v>2607.4650000000001</v>
+      </c>
+    </row>
+    <row r="603" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A603" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B603" s="31">
+        <v>45099</v>
+      </c>
       <c r="C603" s="10" t="s">
         <v>12</v>
+      </c>
+      <c r="D603" s="5">
+        <v>51.26</v>
+      </c>
+      <c r="E603" s="5">
+        <v>2613.58</v>
       </c>
       <c r="F603" s="16" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="604" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="604" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A604" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B604" s="31">
+        <v>45099</v>
+      </c>
       <c r="C604" s="10" t="s">
         <v>12</v>
+      </c>
+      <c r="D604" s="5">
+        <v>50.69</v>
+      </c>
+      <c r="E604" s="5">
+        <v>2619.02</v>
       </c>
       <c r="F604" s="16" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="605" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="605" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A605" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B605" s="31">
+        <v>45099</v>
+      </c>
       <c r="C605" s="10" t="s">
         <v>12</v>
+      </c>
+      <c r="D605" s="5">
+        <v>53.95</v>
+      </c>
+      <c r="E605" s="5">
+        <v>2543.17</v>
       </c>
       <c r="F605" s="16" t="s">
         <v>541</v>
       </c>
-    </row>
-    <row r="606" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="G605" s="13">
+        <f>AVERAGE(E605,E607)</f>
+        <v>2545.9499999999998</v>
+      </c>
+      <c r="H605" s="18">
+        <f>STDEV(E605,E607)</f>
+        <v>3.9315137033971657</v>
+      </c>
+      <c r="K605" s="5">
+        <f>G605+$J$575</f>
+        <v>2537.1149999999998</v>
+      </c>
+    </row>
+    <row r="606" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A606" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B606" s="31">
+        <v>45099</v>
+      </c>
       <c r="C606" s="10" t="s">
         <v>12</v>
+      </c>
+      <c r="D606" s="5">
+        <v>51</v>
+      </c>
+      <c r="E606" s="14">
+        <v>2532.25</v>
       </c>
       <c r="F606" s="16" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="607" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="607" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A607" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B607" s="31">
+        <v>45099</v>
+      </c>
       <c r="C607" s="10" t="s">
         <v>12</v>
+      </c>
+      <c r="D607" s="5">
+        <v>50.84</v>
+      </c>
+      <c r="E607" s="5">
+        <v>2548.73</v>
       </c>
       <c r="F607" s="16" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="608" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="608" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A608" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B608" s="31">
+        <v>45099</v>
+      </c>
       <c r="C608" s="10" t="s">
         <v>12</v>
+      </c>
+      <c r="D608" s="5">
+        <v>50.39</v>
+      </c>
+      <c r="E608" s="14">
+        <v>2552.04</v>
       </c>
       <c r="F608" s="16" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="609" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="G608" s="13">
+        <f>AVERAGE(E609:E610)</f>
+        <v>2595.13</v>
+      </c>
+      <c r="H608" s="18">
+        <f>STDEV(E609:E610)</f>
+        <v>2.3475945135394536</v>
+      </c>
+      <c r="K608" s="5">
+        <f>G608+$J$575</f>
+        <v>2586.2950000000001</v>
+      </c>
+    </row>
+    <row r="609" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A609" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B609" s="31">
+        <v>45099</v>
+      </c>
       <c r="C609" s="10" t="s">
         <v>12</v>
+      </c>
+      <c r="D609" s="5">
+        <v>49.68</v>
+      </c>
+      <c r="E609" s="5">
+        <v>2593.4699999999998</v>
       </c>
       <c r="F609" s="16" t="s">
         <v>545</v>
       </c>
     </row>
-    <row r="610" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="610" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A610" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B610" s="31">
+        <v>45099</v>
+      </c>
       <c r="C610" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="D610" s="5">
+        <v>50.42</v>
+      </c>
+      <c r="E610" s="5">
+        <v>2596.79</v>
+      </c>
       <c r="F610" s="16" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="611" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A611" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B611" s="31">
+        <v>45099</v>
+      </c>
+      <c r="C611" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D611" s="5">
+        <v>51.14</v>
+      </c>
+      <c r="E611" s="5">
+        <v>2689.54</v>
+      </c>
+      <c r="F611" s="16" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="611" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C611" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F611" s="16" t="s">
+      <c r="G611" s="13">
+        <f>AVERAGE(E611:E612)</f>
+        <v>2687.41</v>
+      </c>
+      <c r="H611" s="18">
+        <f>STDEV(E611:E612)</f>
+        <v>3.0122748878545251</v>
+      </c>
+      <c r="K611" s="5">
+        <f>G611+$J$575</f>
+        <v>2678.5749999999998</v>
+      </c>
+    </row>
+    <row r="612" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A612" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B612" s="31">
+        <v>45099</v>
+      </c>
+      <c r="C612" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D612" s="5">
+        <v>50.5</v>
+      </c>
+      <c r="E612" s="5">
+        <v>2685.28</v>
+      </c>
+      <c r="F612" s="16" t="s">
         <v>547</v>
-      </c>
-    </row>
-    <row r="612" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C612" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F612" s="16" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="613" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C613" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F613" s="16" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="614" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C614" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F614" s="16" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="615" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C615" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F615" s="16" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="616" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C616" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F616" s="16" t="s">
-        <v>552</v>
       </c>
     </row>
   </sheetData>

</xml_diff>